<commit_message>
RET-2771: Modified challenge question sheet name and added answers
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\bmchugh\ccd_defs\et-ccd-definitions-englandwales\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\pmum\projects\et-ccd-definitions-englandwales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40028929-3D50-4EFB-81BD-3777229C9CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209657FE-C4F2-46F0-8F98-96ECD907C485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="3" r:id="rId1"/>
@@ -3508,7 +3508,7 @@
     <t>Unique identifer for each question MaxLenght:40</t>
   </si>
   <si>
-    <t>ChallengeQuestionTab</t>
+    <t>ChallengeQuestion</t>
   </si>
 </sst>
 </file>
@@ -5362,16 +5362,16 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="1014" width="10.44140625" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="1014" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5387,7 +5387,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="158.4">
+    <row r="2" spans="1:6" ht="153">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
@@ -5453,24 +5453,24 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.9" customHeight="1">
+    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="73" t="s">
         <v>691</v>
       </c>
@@ -5489,7 +5489,7 @@
       <c r="H1" s="78"/>
       <c r="I1" s="77"/>
     </row>
-    <row r="2" spans="1:11" ht="66.900000000000006" customHeight="1">
+    <row r="2" spans="1:11" ht="66.95" customHeight="1">
       <c r="A2" s="79" t="s">
         <v>692</v>
       </c>
@@ -11681,16 +11681,16 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="46" style="211" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" style="219" customWidth="1"/>
-    <col min="3" max="3" width="91.5546875" style="211" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="211" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="211"/>
+    <col min="2" max="2" width="28.85546875" style="219" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" style="211" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="211" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="211"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="206" t="s">
         <v>734</v>
       </c>
@@ -11704,7 +11704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="79.2">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="A2" s="212" t="s">
         <v>735</v>
       </c>
@@ -15657,19 +15657,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="43.44140625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="1021" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="28.8">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="36">
       <c r="A1" s="86" t="s">
         <v>741</v>
       </c>
@@ -15687,7 +15687,7 @@
       <c r="G1" s="90"/>
       <c r="H1" s="168"/>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="66.599999999999994">
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="75">
       <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
@@ -15711,7 +15711,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="91" t="s">
         <v>39</v>
       </c>
@@ -15737,86 +15737,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.4">
+    <row r="4" spans="1:8" ht="15">
       <c r="E4" s="8"/>
       <c r="F4" s="169"/>
       <c r="G4" s="13"/>
       <c r="H4" s="163"/>
     </row>
-    <row r="5" spans="1:8" ht="14.4">
+    <row r="5" spans="1:8" ht="15">
       <c r="E5" s="8"/>
       <c r="F5" s="169"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="14.4">
+    <row r="6" spans="1:8" ht="15">
       <c r="E6" s="8"/>
       <c r="F6" s="169"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="14.4">
+    <row r="7" spans="1:8" ht="15">
       <c r="E7" s="8"/>
       <c r="F7" s="169"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="14.4">
+    <row r="8" spans="1:8" ht="15">
       <c r="E8" s="8"/>
       <c r="F8" s="169"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.4">
+    <row r="9" spans="1:8" ht="15">
       <c r="E9" s="8"/>
       <c r="F9" s="169"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="14.4">
+    <row r="10" spans="1:8" ht="15">
       <c r="E10" s="8"/>
       <c r="F10" s="169"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="14.4">
+    <row r="11" spans="1:8" ht="15">
       <c r="E11" s="8"/>
       <c r="F11" s="169"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="14.4">
+    <row r="12" spans="1:8" ht="15">
       <c r="E12" s="8"/>
       <c r="F12" s="169"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="14.4">
+    <row r="13" spans="1:8" ht="15">
       <c r="D13" s="247"/>
       <c r="E13" s="8"/>
       <c r="F13" s="169"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="14.4">
+    <row r="14" spans="1:8" ht="15">
       <c r="E14" s="8"/>
       <c r="F14" s="169"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="14.4">
+    <row r="15" spans="1:8" ht="15">
       <c r="C15" s="57"/>
       <c r="E15" s="8"/>
       <c r="F15" s="169"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="14.4">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="57"/>
       <c r="E16" s="8"/>
       <c r="F16" s="169"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="14.4">
+    <row r="17" spans="2:8" ht="15">
       <c r="E17" s="8"/>
       <c r="F17" s="169"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="14.4">
+    <row r="18" spans="2:8" ht="15">
       <c r="E18" s="8"/>
       <c r="F18" s="169"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="14.4">
+    <row r="19" spans="2:8" ht="15">
       <c r="E19" s="8"/>
       <c r="H19" s="169"/>
     </row>
@@ -15857,18 +15857,18 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="67" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.5546875" customWidth="1"/>
-    <col min="8" max="1013" width="8.44140625" customWidth="1"/>
+    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="67" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="17.399999999999999">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="18">
       <c r="A1" s="86" t="s">
         <v>745</v>
       </c>
@@ -15885,7 +15885,7 @@
       <c r="F1" s="164"/>
       <c r="G1" s="165"/>
     </row>
-    <row r="2" spans="1:7" s="9" customFormat="1" ht="86.4">
+    <row r="2" spans="1:7" s="9" customFormat="1" ht="90">
       <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
@@ -15906,7 +15906,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.4">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="91" t="s">
         <v>39</v>
       </c>
@@ -16014,19 +16014,19 @@
       <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
-    <col min="2" max="3" width="31.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="8" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" customWidth="1"/>
-    <col min="9" max="1022" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="96" t="s">
         <v>749</v>
       </c>
@@ -16044,7 +16044,7 @@
       <c r="G1" s="164"/>
       <c r="H1" s="165"/>
     </row>
-    <row r="2" spans="1:8" ht="92.4">
+    <row r="2" spans="1:8" ht="76.5">
       <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
@@ -16068,7 +16068,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="91" t="s">
         <v>39</v>
       </c>
@@ -16094,19 +16094,19 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.4">
+    <row r="4" spans="1:8" ht="15">
       <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="137"/>
     </row>
-    <row r="6" spans="1:8" ht="13.8">
+    <row r="6" spans="1:8" ht="14.25">
       <c r="D6" s="145"/>
     </row>
-    <row r="7" spans="1:8" ht="13.8">
+    <row r="7" spans="1:8" ht="14.25">
       <c r="D7" s="145"/>
     </row>
-    <row r="8" spans="1:8" ht="13.8">
+    <row r="8" spans="1:8" ht="14.25">
       <c r="D8" s="145"/>
     </row>
     <row r="9" spans="1:8">
@@ -16166,18 +16166,18 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="3" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="8" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="1008" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="54" t="s">
         <v>750</v>
       </c>
@@ -16194,7 +16194,7 @@
       <c r="F1" s="164"/>
       <c r="G1" s="165"/>
     </row>
-    <row r="2" spans="1:7" ht="86.4">
+    <row r="2" spans="1:7" ht="105">
       <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
@@ -16215,7 +16215,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.4">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="91" t="s">
         <v>39</v>
       </c>
@@ -16238,7 +16238,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="D6" s="145"/>
     </row>
     <row r="10" spans="1:7">
@@ -16297,21 +16297,21 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="176" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="176" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="176" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" style="176" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="176" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" style="176" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="176" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="176" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="176" customWidth="1"/>
-    <col min="10" max="16384" width="10.88671875" style="176"/>
+    <col min="1" max="1" width="31.85546875" style="176" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="176" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="176" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="176" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="176" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="176" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="176" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="176" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="176" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="176"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="171" t="s">
         <v>927</v>
       </c>
@@ -16330,7 +16330,7 @@
       <c r="H1" s="175"/>
       <c r="I1" s="175"/>
     </row>
-    <row r="2" spans="1:9" ht="39.6">
+    <row r="2" spans="1:9" ht="38.25">
       <c r="A2" s="177"/>
       <c r="B2" s="177"/>
       <c r="C2" s="178" t="s">
@@ -16349,7 +16349,7 @@
       <c r="H2" s="177"/>
       <c r="I2" s="177"/>
     </row>
-    <row r="3" spans="1:9" ht="14.4">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="179" t="s">
         <v>19</v>
       </c>
@@ -16378,7 +16378,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="181"/>
       <c r="B4" s="182"/>
       <c r="C4" s="175"/>
@@ -16389,7 +16389,7 @@
       <c r="H4" s="182"/>
       <c r="I4" s="182"/>
     </row>
-    <row r="5" spans="1:9" ht="14.4">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="181"/>
       <c r="B5" s="182"/>
       <c r="C5" s="175"/>
@@ -16400,7 +16400,7 @@
       <c r="H5" s="175"/>
       <c r="I5" s="182"/>
     </row>
-    <row r="6" spans="1:9" ht="14.4">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="181"/>
       <c r="B6" s="182"/>
       <c r="C6" s="175"/>
@@ -16411,7 +16411,7 @@
       <c r="H6" s="175"/>
       <c r="I6" s="182"/>
     </row>
-    <row r="7" spans="1:9" ht="14.4">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="181"/>
       <c r="B7" s="182"/>
       <c r="C7" s="175"/>
@@ -16422,7 +16422,7 @@
       <c r="H7" s="175"/>
       <c r="I7" s="182"/>
     </row>
-    <row r="8" spans="1:9" ht="14.4">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="181"/>
       <c r="B8" s="182"/>
       <c r="C8" s="175"/>
@@ -16433,7 +16433,7 @@
       <c r="H8" s="175"/>
       <c r="I8" s="182"/>
     </row>
-    <row r="9" spans="1:9" ht="14.4">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="181"/>
       <c r="B9" s="182"/>
       <c r="C9" s="175"/>
@@ -16461,15 +16461,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.44140625" customWidth="1"/>
+    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="41" t="s">
         <v>12</v>
       </c>
@@ -16483,7 +16483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="79.2">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="B2" s="23" t="s">
         <v>751</v>
       </c>
@@ -16494,7 +16494,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39.6">
+    <row r="3" spans="1:4" ht="38.25">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -16585,17 +16585,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="176" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="176" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" style="176" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" style="176" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="176" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" style="176" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" style="176" customWidth="1"/>
-    <col min="8" max="1025" width="8.88671875" style="176" customWidth="1"/>
-    <col min="1026" max="16384" width="8.88671875" style="176"/>
+    <col min="1" max="1" width="16.140625" style="176" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="176" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="176" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="176" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="176" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="176" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="176" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="176" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="176"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -16614,7 +16614,7 @@
       <c r="E1" s="187"/>
       <c r="F1" s="187"/>
     </row>
-    <row r="2" spans="1:6" s="191" customFormat="1" ht="39.6">
+    <row r="2" spans="1:6" s="191" customFormat="1" ht="38.25">
       <c r="A2" s="188" t="s">
         <v>14</v>
       </c>
@@ -16634,7 +16634,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.65" customHeight="1">
+    <row r="3" spans="1:6" ht="13.7" customHeight="1">
       <c r="A3" s="192" t="s">
         <v>19</v>
       </c>
@@ -16654,28 +16654,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.65" customHeight="1">
+    <row r="4" spans="1:6" ht="13.7" customHeight="1">
       <c r="A4" s="195"/>
       <c r="B4" s="195"/>
     </row>
-    <row r="5" spans="1:6" ht="13.65" customHeight="1">
+    <row r="5" spans="1:6" ht="13.7" customHeight="1">
       <c r="A5" s="195"/>
       <c r="B5" s="195"/>
     </row>
-    <row r="6" spans="1:6" ht="13.65" customHeight="1">
+    <row r="6" spans="1:6" ht="13.7" customHeight="1">
       <c r="A6" s="195"/>
       <c r="B6" s="195"/>
     </row>
-    <row r="7" spans="1:6" ht="13.65" customHeight="1">
+    <row r="7" spans="1:6" ht="13.7" customHeight="1">
       <c r="A7" s="195"/>
       <c r="B7" s="195"/>
     </row>
-    <row r="8" spans="1:6" ht="13.65" customHeight="1">
+    <row r="8" spans="1:6" ht="13.7" customHeight="1">
       <c r="A8" s="195"/>
       <c r="B8" s="195"/>
     </row>
-    <row r="9" spans="1:6" ht="13.65" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.65" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16694,12 +16694,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="8" customWidth="1"/>
-    <col min="4" max="775" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="8" customWidth="1"/>
+    <col min="4" max="775" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -16716,7 +16716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="184.8">
+    <row r="2" spans="1:5" ht="178.5">
       <c r="A2" s="37" t="s">
         <v>759</v>
       </c>
@@ -16784,17 +16784,17 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
-    <col min="4" max="5" width="21.109375" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.88671875" customWidth="1"/>
-    <col min="8" max="1011" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
@@ -16813,7 +16813,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" ht="211.2">
+    <row r="2" spans="1:9" ht="191.25">
       <c r="A2" s="23" t="s">
         <v>14</v>
       </c>
@@ -16842,7 +16842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39.6">
+    <row r="3" spans="1:9" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>19</v>
       </c>
@@ -16910,12 +16910,12 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="8" customWidth="1"/>
-    <col min="4" max="773" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="8" customWidth="1"/>
+    <col min="4" max="773" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="66" customFormat="1" ht="18" customHeight="1">
@@ -16929,7 +16929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="66" customFormat="1" ht="79.2">
+    <row r="2" spans="1:3" s="66" customFormat="1" ht="76.5">
       <c r="A2" s="24" t="s">
         <v>766</v>
       </c>
@@ -17002,17 +17002,17 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="49.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="8" customWidth="1"/>
-    <col min="5" max="1011" width="8.44140625" customWidth="1"/>
-    <col min="1012" max="1015" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="8" customWidth="1"/>
+    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="66" customFormat="1" ht="17.399999999999999">
+    <row r="1" spans="1:4" s="66" customFormat="1" ht="18">
       <c r="A1" s="111" t="s">
         <v>769</v>
       </c>
@@ -17026,7 +17026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="66" customFormat="1" ht="52.8">
+    <row r="2" spans="1:4" s="66" customFormat="1" ht="51">
       <c r="A2" s="24" t="s">
         <v>759</v>
       </c>
@@ -18935,16 +18935,16 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="8" customWidth="1"/>
-    <col min="5" max="774" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="8" customWidth="1"/>
+    <col min="5" max="774" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="66" customFormat="1" ht="17.399999999999999">
+    <row r="1" spans="1:4" s="66" customFormat="1" ht="18">
       <c r="A1" s="41" t="s">
         <v>771</v>
       </c>
@@ -18958,7 +18958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="66" customFormat="1" ht="66">
+    <row r="2" spans="1:4" s="66" customFormat="1" ht="63.75">
       <c r="A2" s="24" t="s">
         <v>766</v>
       </c>
@@ -19436,15 +19436,15 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="50" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="50" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="50" customWidth="1"/>
     <col min="3" max="3" width="62" style="50" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" style="51" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="66" customFormat="1" ht="17.399999999999999">
+    <row r="1" spans="1:4" s="66" customFormat="1" ht="18">
       <c r="A1" s="119" t="s">
         <v>773</v>
       </c>
@@ -19458,7 +19458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="66" customFormat="1" ht="52.8">
+    <row r="2" spans="1:4" s="66" customFormat="1" ht="51">
       <c r="A2" s="24" t="s">
         <v>759</v>
       </c>
@@ -19676,17 +19676,17 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="31" t="s">
         <v>32</v>
       </c>
@@ -19702,7 +19702,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:6" ht="92.4">
+    <row r="2" spans="1:6" ht="89.25">
       <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
@@ -19722,7 +19722,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.4">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="28" t="s">
         <v>39</v>
       </c>
@@ -19819,22 +19819,22 @@
       <selection activeCell="A4" sqref="A4:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
-    <col min="8" max="8" width="49.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="11" max="1015" width="8.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="1015" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="41" t="s">
         <v>42</v>
       </c>
@@ -19852,7 +19852,7 @@
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
     </row>
-    <row r="2" spans="1:10" ht="92.4">
+    <row r="2" spans="1:10" ht="102">
       <c r="A2" s="24" t="s">
         <v>33</v>
       </c>
@@ -19884,7 +19884,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="39.6">
+    <row r="3" spans="1:10" ht="38.25">
       <c r="A3" s="48" t="s">
         <v>39</v>
       </c>
@@ -20497,27 +20497,27 @@
       <selection activeCell="F4" sqref="A4:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="15" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="55.44140625" customWidth="1"/>
-    <col min="8" max="8" width="47.88671875" customWidth="1"/>
-    <col min="9" max="9" width="52.44140625" customWidth="1"/>
-    <col min="10" max="10" width="81.5546875" customWidth="1"/>
-    <col min="11" max="11" width="93.5546875" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" customWidth="1"/>
-    <col min="13" max="13" width="23.44140625" customWidth="1"/>
-    <col min="14" max="15" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="18.44140625" style="8" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" customWidth="1"/>
-    <col min="18" max="18" width="20.44140625" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" customWidth="1"/>
-    <col min="20" max="1013" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" customWidth="1"/>
+    <col min="10" max="10" width="81.5703125" customWidth="1"/>
+    <col min="11" max="11" width="93.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" customHeight="1">
@@ -20549,7 +20549,7 @@
       <c r="R1" s="58"/>
       <c r="S1" s="58"/>
     </row>
-    <row r="2" spans="1:19" ht="132">
+    <row r="2" spans="1:19" ht="114.75">
       <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
@@ -20590,7 +20590,7 @@
       <c r="R2" s="38"/>
       <c r="S2" s="38"/>
     </row>
-    <row r="3" spans="1:19" ht="39.6">
+    <row r="3" spans="1:19" ht="38.25">
       <c r="A3" s="48" t="s">
         <v>39</v>
       </c>
@@ -20649,7 +20649,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.8">
+    <row r="4" spans="1:19" ht="14.25">
       <c r="I4" s="126"/>
       <c r="J4" s="126"/>
       <c r="L4" s="57"/>
@@ -20657,7 +20657,7 @@
       <c r="R4" s="150"/>
       <c r="S4" s="150"/>
     </row>
-    <row r="5" spans="1:19" ht="13.8">
+    <row r="5" spans="1:19" ht="14.25">
       <c r="F5" s="9"/>
       <c r="J5" s="167"/>
       <c r="K5" s="57"/>
@@ -20666,7 +20666,7 @@
       <c r="R5" s="150"/>
       <c r="S5" s="150"/>
     </row>
-    <row r="6" spans="1:19" ht="13.8">
+    <row r="6" spans="1:19" ht="14.25">
       <c r="F6" s="9"/>
       <c r="G6" s="247"/>
       <c r="I6" s="204"/>
@@ -20676,7 +20676,7 @@
       <c r="R6" s="150"/>
       <c r="S6" s="150"/>
     </row>
-    <row r="7" spans="1:19" ht="13.8">
+    <row r="7" spans="1:19" ht="14.25">
       <c r="F7" s="9"/>
       <c r="G7" s="287"/>
       <c r="H7" s="9"/>
@@ -20687,7 +20687,7 @@
       <c r="R7" s="150"/>
       <c r="S7" s="150"/>
     </row>
-    <row r="8" spans="1:19" ht="13.8">
+    <row r="8" spans="1:19" ht="14.25">
       <c r="F8" s="9"/>
       <c r="G8" s="287"/>
       <c r="H8" s="9"/>
@@ -20698,7 +20698,7 @@
       <c r="R8" s="150"/>
       <c r="S8" s="150"/>
     </row>
-    <row r="9" spans="1:19" ht="13.8">
+    <row r="9" spans="1:19" ht="14.25">
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -20710,7 +20710,7 @@
       <c r="R9" s="150"/>
       <c r="S9" s="150"/>
     </row>
-    <row r="10" spans="1:19" ht="13.8">
+    <row r="10" spans="1:19" ht="14.25">
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -20722,7 +20722,7 @@
       <c r="R10" s="150"/>
       <c r="S10" s="150"/>
     </row>
-    <row r="11" spans="1:19" ht="13.8">
+    <row r="11" spans="1:19" ht="14.25">
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="288"/>
@@ -20734,7 +20734,7 @@
       <c r="R11" s="150"/>
       <c r="S11" s="150"/>
     </row>
-    <row r="12" spans="1:19" ht="13.8">
+    <row r="12" spans="1:19" ht="14.25">
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="288"/>
@@ -20746,7 +20746,7 @@
       <c r="R12" s="150"/>
       <c r="S12" s="150"/>
     </row>
-    <row r="13" spans="1:19" ht="13.8">
+    <row r="13" spans="1:19" ht="14.25">
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -20758,7 +20758,7 @@
       <c r="R13" s="150"/>
       <c r="S13" s="150"/>
     </row>
-    <row r="14" spans="1:19" ht="13.8">
+    <row r="14" spans="1:19" ht="14.25">
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -20770,7 +20770,7 @@
       <c r="R14" s="150"/>
       <c r="S14" s="150"/>
     </row>
-    <row r="15" spans="1:19" ht="13.8">
+    <row r="15" spans="1:19" ht="14.25">
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -20782,7 +20782,7 @@
       <c r="R15" s="150"/>
       <c r="S15" s="150"/>
     </row>
-    <row r="16" spans="1:19" ht="13.8">
+    <row r="16" spans="1:19" ht="14.25">
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -20794,7 +20794,7 @@
       <c r="R16" s="150"/>
       <c r="S16" s="150"/>
     </row>
-    <row r="17" spans="6:19" ht="13.8">
+    <row r="17" spans="6:19" ht="14.25">
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -20806,7 +20806,7 @@
       <c r="R17" s="150"/>
       <c r="S17" s="150"/>
     </row>
-    <row r="18" spans="6:19" ht="13.8">
+    <row r="18" spans="6:19" ht="14.25">
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -20818,7 +20818,7 @@
       <c r="R18" s="150"/>
       <c r="S18" s="150"/>
     </row>
-    <row r="19" spans="6:19" ht="13.8">
+    <row r="19" spans="6:19" ht="14.25">
       <c r="F19" s="9"/>
       <c r="I19" s="301"/>
       <c r="J19" s="243"/>
@@ -20828,7 +20828,7 @@
       <c r="R19" s="150"/>
       <c r="S19" s="150"/>
     </row>
-    <row r="20" spans="6:19" ht="13.8">
+    <row r="20" spans="6:19" ht="14.25">
       <c r="F20" s="9"/>
       <c r="J20" s="126"/>
       <c r="L20" s="57"/>
@@ -20836,7 +20836,7 @@
       <c r="R20" s="150"/>
       <c r="S20" s="150"/>
     </row>
-    <row r="21" spans="6:19" ht="13.8">
+    <row r="21" spans="6:19" ht="14.25">
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="288"/>
@@ -20847,7 +20847,7 @@
       <c r="R21" s="150"/>
       <c r="S21" s="150"/>
     </row>
-    <row r="22" spans="6:19" ht="13.8">
+    <row r="22" spans="6:19" ht="14.25">
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="288"/>
@@ -20859,7 +20859,7 @@
       <c r="R22" s="150"/>
       <c r="S22" s="150"/>
     </row>
-    <row r="23" spans="6:19" ht="13.8">
+    <row r="23" spans="6:19" ht="14.25">
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="288"/>
@@ -20871,7 +20871,7 @@
       <c r="R23" s="150"/>
       <c r="S23" s="150"/>
     </row>
-    <row r="24" spans="6:19" ht="13.8">
+    <row r="24" spans="6:19" ht="14.25">
       <c r="J24" s="127"/>
       <c r="L24" s="57"/>
       <c r="M24" s="61"/>
@@ -20879,7 +20879,7 @@
       <c r="R24" s="150"/>
       <c r="S24" s="150"/>
     </row>
-    <row r="25" spans="6:19" ht="13.8">
+    <row r="25" spans="6:19" ht="14.25">
       <c r="F25" s="9"/>
       <c r="I25" s="126"/>
       <c r="J25" s="126"/>
@@ -20890,7 +20890,7 @@
       <c r="R25" s="150"/>
       <c r="S25" s="150"/>
     </row>
-    <row r="26" spans="6:19" ht="13.8">
+    <row r="26" spans="6:19" ht="14.25">
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="I26" s="126"/>
@@ -20902,7 +20902,7 @@
       <c r="R26" s="150"/>
       <c r="S26" s="150"/>
     </row>
-    <row r="27" spans="6:19" ht="13.8">
+    <row r="27" spans="6:19" ht="14.25">
       <c r="F27" s="9"/>
       <c r="I27" s="126"/>
       <c r="J27" s="126"/>
@@ -20913,7 +20913,7 @@
       <c r="R27" s="150"/>
       <c r="S27" s="150"/>
     </row>
-    <row r="28" spans="6:19" ht="13.8">
+    <row r="28" spans="6:19" ht="14.25">
       <c r="F28" s="9"/>
       <c r="J28" s="126"/>
       <c r="K28" s="126"/>
@@ -20923,7 +20923,7 @@
       <c r="R28" s="150"/>
       <c r="S28" s="150"/>
     </row>
-    <row r="29" spans="6:19" ht="13.8">
+    <row r="29" spans="6:19" ht="14.25">
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="I29" s="126"/>
@@ -20934,7 +20934,7 @@
       <c r="R29" s="150"/>
       <c r="S29" s="150"/>
     </row>
-    <row r="30" spans="6:19" ht="13.8">
+    <row r="30" spans="6:19" ht="14.25">
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="I30" s="126"/>
@@ -20945,7 +20945,7 @@
       <c r="R30" s="150"/>
       <c r="S30" s="150"/>
     </row>
-    <row r="31" spans="6:19" ht="13.8">
+    <row r="31" spans="6:19" ht="14.25">
       <c r="F31" s="289"/>
       <c r="H31" s="9"/>
       <c r="I31" s="126"/>
@@ -20956,7 +20956,7 @@
       <c r="R31" s="150"/>
       <c r="S31" s="150"/>
     </row>
-    <row r="32" spans="6:19" ht="13.8">
+    <row r="32" spans="6:19" ht="14.25">
       <c r="G32" s="9"/>
       <c r="I32" s="204"/>
       <c r="J32" s="167"/>
@@ -20966,7 +20966,7 @@
       <c r="R32" s="150"/>
       <c r="S32" s="150"/>
     </row>
-    <row r="33" spans="1:19" ht="13.8">
+    <row r="33" spans="1:19" ht="14.25">
       <c r="C33" s="167"/>
       <c r="J33" s="126"/>
       <c r="K33" s="126"/>
@@ -20976,7 +20976,7 @@
       <c r="R33" s="150"/>
       <c r="S33" s="150"/>
     </row>
-    <row r="34" spans="1:19" ht="13.8">
+    <row r="34" spans="1:19" ht="14.25">
       <c r="G34" s="9"/>
       <c r="J34" s="126"/>
       <c r="K34" s="126"/>
@@ -20986,7 +20986,7 @@
       <c r="R34" s="150"/>
       <c r="S34" s="150"/>
     </row>
-    <row r="35" spans="1:19" ht="13.8">
+    <row r="35" spans="1:19" ht="14.25">
       <c r="A35" s="167"/>
       <c r="B35" s="167"/>
       <c r="C35" s="167"/>
@@ -21005,7 +21005,7 @@
       <c r="Q35" s="150"/>
       <c r="S35" s="150"/>
     </row>
-    <row r="36" spans="1:19" ht="13.8">
+    <row r="36" spans="1:19" ht="14.25">
       <c r="A36" s="167"/>
       <c r="B36" s="167"/>
       <c r="C36" s="167"/>
@@ -21240,7 +21240,7 @@
       <c r="R47" s="150"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="1:19" ht="13.8">
+    <row r="48" spans="1:19" ht="14.25">
       <c r="B48" s="167"/>
       <c r="C48" s="167"/>
       <c r="D48" s="167"/>
@@ -21406,23 +21406,23 @@
       <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="58.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="58.5703125" customWidth="1"/>
     <col min="9" max="9" width="100" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="87.109375" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="87.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.399999999999999">
+    <row r="1" spans="1:16" ht="18">
       <c r="A1" s="41" t="s">
         <v>106</v>
       </c>
@@ -21442,7 +21442,7 @@
       <c r="O1" s="42"/>
       <c r="P1" s="62"/>
     </row>
-    <row r="2" spans="1:16" ht="57.9" customHeight="1">
+    <row r="2" spans="1:16" ht="57.95" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>33</v>
       </c>
@@ -21490,7 +21490,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="39.6">
+    <row r="3" spans="1:16" ht="38.25">
       <c r="A3" s="28" t="s">
         <v>39</v>
       </c>
@@ -24358,23 +24358,23 @@
       <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="41" t="s">
         <v>136</v>
       </c>
@@ -24388,7 +24388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93.9" customHeight="1">
+    <row r="2" spans="1:10" ht="93.95" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>33</v>
       </c>
@@ -24420,7 +24420,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="48" t="s">
         <v>39</v>
       </c>
@@ -30247,27 +30247,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243AEE7-DA61-4CDF-84FC-CA2502F211A6}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="314" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="314"/>
-    <col min="3" max="3" width="54.77734375" style="314" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="314" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="314" customWidth="1"/>
-    <col min="7" max="7" width="44.33203125" style="314" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="314" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="314" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="314"/>
+    <col min="3" max="3" width="54.7109375" style="314" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="314" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="314" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="314" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="314" customWidth="1"/>
     <col min="9" max="9" width="37" style="314" customWidth="1"/>
-    <col min="10" max="10" width="43.6640625" style="314" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" style="314" customWidth="1"/>
-    <col min="12" max="1025" width="10.88671875" style="314"/>
-    <col min="1026" max="16384" width="10.88671875" style="313"/>
+    <col min="10" max="10" width="43.7109375" style="314" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="314" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" style="314"/>
+    <col min="1026" max="16384" width="10.85546875" style="313"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.399999999999999">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="330" t="s">
         <v>1117</v>
       </c>
@@ -30290,7 +30290,7 @@
       <c r="L1" s="315"/>
       <c r="M1" s="315"/>
     </row>
-    <row r="2" spans="1:13" ht="79.2">
+    <row r="2" spans="1:13" ht="63.75">
       <c r="A2" s="326" t="s">
         <v>14</v>
       </c>
@@ -30325,7 +30325,7 @@
       <c r="L2" s="322"/>
       <c r="M2" s="322"/>
     </row>
-    <row r="3" spans="1:13" ht="15.6">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="321" t="s">
         <v>19</v>
       </c>
@@ -30453,23 +30453,23 @@
       <selection pane="bottomLeft" activeCell="A328" sqref="A328:XFD563"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" customWidth="1"/>
-    <col min="6" max="6" width="53.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.399999999999999">
+    <row r="1" spans="1:14" ht="18">
       <c r="A1" s="41" t="s">
         <v>192</v>
       </c>
@@ -30492,7 +30492,7 @@
       <c r="L1" s="68"/>
       <c r="N1" s="42"/>
     </row>
-    <row r="2" spans="1:14" ht="54.9" customHeight="1">
+    <row r="2" spans="1:14" ht="54.95" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>193</v>
       </c>
@@ -30532,7 +30532,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="52.8">
+    <row r="3" spans="1:14" ht="51">
       <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
@@ -32071,7 +32071,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="9.9" customHeight="1">
+    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -36840,7 +36840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14">
+    <row r="279" spans="1:14" ht="13.5">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -39316,7 +39316,7 @@
       <c r="H508" s="250"/>
       <c r="I508" s="158"/>
     </row>
-    <row r="509" spans="1:10">
+    <row r="509" spans="1:10" ht="13.5">
       <c r="A509" s="155"/>
       <c r="B509" s="306"/>
       <c r="C509" s="155"/>
@@ -39327,7 +39327,7 @@
       <c r="I509" s="67"/>
       <c r="J509" s="67"/>
     </row>
-    <row r="510" spans="1:10">
+    <row r="510" spans="1:10" ht="13.5">
       <c r="A510" s="155"/>
       <c r="B510" s="306"/>
       <c r="C510" s="155"/>
@@ -39338,7 +39338,7 @@
       <c r="I510" s="158"/>
       <c r="J510" s="67"/>
     </row>
-    <row r="511" spans="1:10" s="167" customFormat="1">
+    <row r="511" spans="1:10" s="167" customFormat="1" ht="13.5">
       <c r="A511" s="246"/>
       <c r="B511" s="312"/>
       <c r="C511" s="246"/>

</xml_diff>

<commit_message>
Ret 3878 - Migrate ET from IDAM to RAS (#571)
* Refactor AuthCaseType tab

* Update ccd-template

* Add role to access profiles tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\england feature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CD371A-DFD9-4C63-991F-569EF1A0D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58D9F30E-AAEA-41A8-A0CE-9A8D08395E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="966" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="966" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="3" r:id="rId1"/>
@@ -23,43 +23,44 @@
     <sheet name="ChallengeQuestion" sheetId="35" r:id="rId8"/>
     <sheet name="ComplexTypes" sheetId="26" r:id="rId9"/>
     <sheet name="EventToComplexTypes" sheetId="29" r:id="rId10"/>
-    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId11"/>
-    <sheet name="SearchInputFields" sheetId="13" r:id="rId12"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId13"/>
-    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId14"/>
-    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId15"/>
-    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId16"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId17"/>
-    <sheet name="CaseRoles" sheetId="31" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId20"/>
-    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId23"/>
+    <sheet name="RoleToAccessProfiles" sheetId="36" r:id="rId11"/>
+    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
+    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId16"/>
+    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId17"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId18"/>
+    <sheet name="CaseRoles" sheetId="31" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CaseEvent!$A$3:$S$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseEventToFields!$A$3:$Q$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseField!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">CaseRoles!$A$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CaseType!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseTypeTab!$A$3:$J$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jurisdiction!$A$3:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">State!$A$3:$F$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">UserProfile!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">UserProfile!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3684" uniqueCount="1125">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3515,6 +3516,21 @@
   </si>
   <si>
     <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>A comma-separated list of AccessProfiles that should be assigned to the user if their RoleName, ReadOnly value (and optional Authorisations) match.</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
   </si>
 </sst>
 </file>
@@ -4160,7 +4176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -4174,8 +4190,9 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4678,8 +4695,15 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
     <cellStyle name="Excel Built-in Explanatory Text 1" xfId="4" xr:uid="{5353AD2F-8751-B54D-A42A-F1E5A519675A}"/>
     <cellStyle name="Excel Built-in Explanatory Text 2" xfId="5" xr:uid="{B27B4066-0F1E-E149-8491-1AE49358B0E8}"/>
@@ -4690,6 +4714,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="6" xr:uid="{368B2A22-AC2F-7043-9063-FDD22315830C}"/>
     <cellStyle name="Normal 2 2" xfId="7" xr:uid="{BB3D72ED-A2C7-E24E-AB25-3911206CD18F}"/>
+    <cellStyle name="Normal 2 2 2" xfId="13" xr:uid="{A5CB6139-F93D-4B14-A914-C827AFF33C59}"/>
     <cellStyle name="Normal 2 3" xfId="9" xr:uid="{DE4FBD9B-2287-384A-AEB1-B7A407276E39}"/>
     <cellStyle name="Normal 2 4" xfId="11" xr:uid="{4DC5648C-A706-458A-9740-2045DCF780E4}"/>
     <cellStyle name="Normal 3" xfId="10" xr:uid="{AACD9C3A-6E51-46AD-9056-7604EA32DDD9}"/>
@@ -11531,6 +11556,809 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAE9FA2-52B9-4405-9114-F66593C32E66}">
+  <dimension ref="A1:E249"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="169">
+      <c r="A2" s="257" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>761</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.5">
+      <c r="A3" s="258" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D3" s="259" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E3" s="259" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="14"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="14"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="14"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="14"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="14"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="14"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="14"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="14"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="14"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="14"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="14"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="14"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="14"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="14"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="14"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="14"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="14"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="14"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="14"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="14"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="14"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="14"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="14"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="14"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="14"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="14"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="14"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="14"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="14"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="14"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="14"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="14"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="14"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="14"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="14"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="14"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="14"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="14"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="14"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="14"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="14"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="14"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="14"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="14"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="14"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="14"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="14"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="14"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="14"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="14"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="14"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="14"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="14"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="14"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="14"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="14"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="14"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="14"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="14"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="14"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="14"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="14"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="14"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="14"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="14"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="14"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="14"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="14"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="14"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="14"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="14"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="14"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="14"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="14"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="14"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="14"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="14"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="14"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="14"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="14"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="14"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="14"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="14"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="14"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="14"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="14"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="14"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="14"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="14"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="14"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="14"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="14"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="14"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="14"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="14"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="14"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="14"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="14"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="14"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="14"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="14"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="14"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="14"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="14"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="14"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="14"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="14"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="14"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="14"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="14"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="14"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="14"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="14"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="14"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="14"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="14"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="14"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="14"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="14"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="14"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="14"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="14"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="14"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="14"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="14"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="14"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="14"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="14"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="14"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="14"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="14"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="14"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="14"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="14"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="14"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="14"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="14"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="14"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="14"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="14"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="14"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="14"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="14"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="14"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="14"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="14"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="14"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="14"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="14"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="14"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="14"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="14"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="14"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="14"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="14"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="14"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="14"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="14"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="14"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="14"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="14"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="14"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="14"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="14"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="14"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="14"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="14"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="14"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="14"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="14"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="14"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="14"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="14"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="14"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="14"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="14"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="14"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="14"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="14"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="14"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="14"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="14"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="14"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="14"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="14"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="14"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="14"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="14"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="14"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="14"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="14"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="14"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="14"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="14"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="14"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="14"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="14"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="14"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="14"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="14"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="14"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="14"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="14"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="14"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="14"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="14"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="14"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="14"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="14"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="14"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="14"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="14"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="14"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="14"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="14"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="14"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="14"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="14"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="14"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="14"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="14"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="14"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="14"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="14"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="14"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="14"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="14"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="14"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="14"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="14"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="14"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="14"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="14"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="14"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="14"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="14"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="14"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="14"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="14"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="14"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="14"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="14"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="14"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="14"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="14"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABABBB7-6A1E-0B4E-82BF-6CDF21C8BDBC}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -15504,7 +16332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H25"/>
@@ -15704,7 +16532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:G27"/>
@@ -15861,7 +16689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:H28"/>
@@ -16013,7 +16841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:G27"/>
@@ -16145,7 +16973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -16308,7 +17136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D13"/>
@@ -16423,12 +17251,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B5A0B4-9586-D946-AB25-20C3418D4E9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -16527,96 +17355,6 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>758</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="175.5">
-      <c r="A2" s="23" t="s">
-        <v>759</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>760</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>761</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13">
-      <c r="A3" s="78" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" t="s">
-        <v>763</v>
-      </c>
-      <c r="E3" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="60"/>
-      <c r="C5" s="81"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="60"/>
-      <c r="C6" s="81"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="60"/>
-      <c r="C7" s="81"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -16748,6 +17486,96 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet18"/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>758</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="175.5">
+      <c r="A2" s="23" t="s">
+        <v>759</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>760</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>761</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13">
+      <c r="A3" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>763</v>
+      </c>
+      <c r="E3" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="60"/>
+      <c r="C5" s="81"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="60"/>
+      <c r="C6" s="81"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="60"/>
+      <c r="C7" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:C10"/>
@@ -16836,7 +17664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:D484"/>
@@ -18531,7 +19359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D120"/>
@@ -19023,7 +19851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D32"/>
@@ -20685,10 +21513,10 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
RET-2501: Postmerge Tidy Up
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\england feature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-englandwales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58D9F30E-AAEA-41A8-A0CE-9A8D08395E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9527F8B0-B2A3-48B2-A001-E24F22450B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="966" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="966" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3684" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3686" uniqueCount="1125">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -5250,13 +5250,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="1014" width="10.453125" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="1014" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -5274,7 +5274,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="143">
+    <row r="2" spans="1:6" ht="153">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13">
+    <row r="3" spans="1:6">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -5333,29 +5333,29 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EE7EEF-305D-1145-A07B-3D132F6E2765}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:K402"/>
+  <dimension ref="A1:L402"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1">
+    <row r="1" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -5374,7 +5374,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:11" ht="67" customHeight="1">
+    <row r="2" spans="1:12" ht="66.95" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -5400,8 +5400,11 @@
       <c r="I2" s="55" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="13">
+      <c r="L2" s="22" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
@@ -5435,8 +5438,11 @@
       <c r="K3" s="226" t="s">
         <v>1080</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="256" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5464,7 +5470,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5492,7 +5498,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5520,7 +5526,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5548,7 +5554,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5576,7 +5582,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5604,7 +5610,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5627,7 +5633,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5652,7 +5658,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5675,7 +5681,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5698,7 +5704,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5723,7 +5729,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="47" t="s">
         <v>1019</v>
       </c>
@@ -5748,7 +5754,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="47" t="s">
         <v>1019</v>
       </c>
@@ -11559,17 +11565,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAE9FA2-52B9-4405-9114-F66593C32E66}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -11583,7 +11589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="169">
+    <row r="2" spans="1:5" ht="165.75">
       <c r="A2" s="257" t="s">
         <v>14</v>
       </c>
@@ -11597,7 +11603,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="258" t="s">
         <v>19</v>
       </c>
@@ -12369,13 +12375,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.54296875" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.453125" style="170"/>
+    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -12392,7 +12398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="78">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -12406,7 +12412,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="173" t="s">
         <v>6</v>
       </c>
@@ -16341,19 +16347,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.453125" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" customWidth="1"/>
-    <col min="7" max="7" width="43.453125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="1021" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="29.5">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -16371,7 +16377,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="65.5">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -16395,7 +16401,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -16421,86 +16427,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5">
+    <row r="4" spans="1:8" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="133"/>
       <c r="G4" s="12"/>
       <c r="H4" s="128"/>
     </row>
-    <row r="5" spans="1:8" ht="14.5">
+    <row r="5" spans="1:8" ht="15">
       <c r="E5" s="7"/>
       <c r="F5" s="133"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="14.5">
+    <row r="6" spans="1:8" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="133"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="14.5">
+    <row r="7" spans="1:8" ht="15">
       <c r="E7" s="7"/>
       <c r="F7" s="133"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="14.5">
+    <row r="8" spans="1:8" ht="15">
       <c r="E8" s="7"/>
       <c r="F8" s="133"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.5">
+    <row r="9" spans="1:8" ht="15">
       <c r="E9" s="7"/>
       <c r="F9" s="133"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="14.5">
+    <row r="10" spans="1:8" ht="15">
       <c r="E10" s="7"/>
       <c r="F10" s="133"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="14.5">
+    <row r="11" spans="1:8" ht="15">
       <c r="E11" s="7"/>
       <c r="F11" s="133"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="14.5">
+    <row r="12" spans="1:8" ht="15">
       <c r="E12" s="7"/>
       <c r="F12" s="133"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="14.5">
+    <row r="13" spans="1:8" ht="15">
       <c r="D13" s="202"/>
       <c r="E13" s="7"/>
       <c r="F13" s="133"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="14.5">
+    <row r="14" spans="1:8" ht="15">
       <c r="E14" s="7"/>
       <c r="F14" s="133"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="14.5">
+    <row r="15" spans="1:8" ht="15">
       <c r="C15" s="31"/>
       <c r="E15" s="7"/>
       <c r="F15" s="133"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="14.5">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="31"/>
       <c r="E16" s="7"/>
       <c r="F16" s="133"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="14.5">
+    <row r="17" spans="2:8" ht="15">
       <c r="E17" s="7"/>
       <c r="F17" s="133"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="14.5">
+    <row r="18" spans="2:8" ht="15">
       <c r="E18" s="7"/>
       <c r="F18" s="133"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="14.5">
+    <row r="19" spans="2:8" ht="15">
       <c r="E19" s="7"/>
       <c r="H19" s="133"/>
     </row>
@@ -16541,15 +16547,15 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" customWidth="1"/>
-    <col min="7" max="7" width="29.54296875" customWidth="1"/>
-    <col min="8" max="1013" width="8.453125" customWidth="1"/>
+    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
@@ -16569,7 +16575,7 @@
       <c r="F1" s="129"/>
       <c r="G1" s="130"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="87">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -16590,7 +16596,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -16698,19 +16704,19 @@
       <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="3" width="31.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="7" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" customWidth="1"/>
-    <col min="9" max="1022" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="72" t="s">
         <v>749</v>
       </c>
@@ -16728,7 +16734,7 @@
       <c r="G1" s="129"/>
       <c r="H1" s="130"/>
     </row>
-    <row r="2" spans="1:8" ht="78">
+    <row r="2" spans="1:8" ht="76.5">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -16752,7 +16758,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -16778,19 +16784,19 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5">
+    <row r="4" spans="1:8" ht="15">
       <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="107"/>
     </row>
-    <row r="6" spans="1:8" ht="14">
+    <row r="6" spans="1:8" ht="14.25">
       <c r="D6" s="114"/>
     </row>
-    <row r="7" spans="1:8" ht="14">
+    <row r="7" spans="1:8" ht="14.25">
       <c r="D7" s="114"/>
     </row>
-    <row r="8" spans="1:8" ht="14">
+    <row r="8" spans="1:8" ht="14.25">
       <c r="D8" s="114"/>
     </row>
     <row r="9" spans="1:8">
@@ -16850,15 +16856,15 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="3" width="27.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" customWidth="1"/>
-    <col min="8" max="1008" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
@@ -16878,7 +16884,7 @@
       <c r="F1" s="129"/>
       <c r="G1" s="130"/>
     </row>
-    <row r="2" spans="1:7" ht="87">
+    <row r="2" spans="1:7" ht="105">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -16899,7 +16905,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -16922,7 +16928,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="D6" s="114"/>
     </row>
     <row r="10" spans="1:7">
@@ -16981,18 +16987,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="140"/>
+    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -17014,7 +17020,7 @@
       <c r="H1" s="139"/>
       <c r="I1" s="139"/>
     </row>
-    <row r="2" spans="1:9" ht="39">
+    <row r="2" spans="1:9" ht="38.25">
       <c r="A2" s="141"/>
       <c r="B2" s="141"/>
       <c r="C2" s="142" t="s">
@@ -17033,7 +17039,7 @@
       <c r="H2" s="141"/>
       <c r="I2" s="141"/>
     </row>
-    <row r="3" spans="1:9" ht="14.5">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="143" t="s">
         <v>19</v>
       </c>
@@ -17062,7 +17068,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.5">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="145"/>
       <c r="B4" s="146"/>
       <c r="C4" s="139"/>
@@ -17073,7 +17079,7 @@
       <c r="H4" s="146"/>
       <c r="I4" s="146"/>
     </row>
-    <row r="5" spans="1:9" ht="14.5">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="145"/>
       <c r="B5" s="146"/>
       <c r="C5" s="139"/>
@@ -17084,7 +17090,7 @@
       <c r="H5" s="139"/>
       <c r="I5" s="146"/>
     </row>
-    <row r="6" spans="1:9" ht="14.5">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="145"/>
       <c r="B6" s="146"/>
       <c r="C6" s="139"/>
@@ -17095,7 +17101,7 @@
       <c r="H6" s="139"/>
       <c r="I6" s="146"/>
     </row>
-    <row r="7" spans="1:9" ht="14.5">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="145"/>
       <c r="B7" s="146"/>
       <c r="C7" s="139"/>
@@ -17106,7 +17112,7 @@
       <c r="H7" s="139"/>
       <c r="I7" s="146"/>
     </row>
-    <row r="8" spans="1:9" ht="14.5">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="145"/>
       <c r="B8" s="146"/>
       <c r="C8" s="139"/>
@@ -17117,7 +17123,7 @@
       <c r="H8" s="139"/>
       <c r="I8" s="146"/>
     </row>
-    <row r="9" spans="1:9" ht="14.5">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="145"/>
       <c r="B9" s="146"/>
       <c r="C9" s="139"/>
@@ -17145,12 +17151,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.453125" customWidth="1"/>
+    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -17167,7 +17173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="65">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -17178,7 +17184,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39">
+    <row r="3" spans="1:4" ht="38.25">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -17259,17 +17265,17 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.81640625" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="140"/>
+    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -17288,7 +17294,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="39">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -17308,7 +17314,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.75" customHeight="1">
+    <row r="3" spans="1:6" ht="13.7" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -17328,28 +17334,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1">
+    <row r="4" spans="1:6" ht="13.7" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1">
+    <row r="5" spans="1:6" ht="13.7" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1">
+    <row r="6" spans="1:6" ht="13.7" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1">
+    <row r="7" spans="1:6" ht="13.7" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1">
+    <row r="8" spans="1:6" ht="13.7" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -17368,14 +17374,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="5" width="21.1796875" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.81640625" customWidth="1"/>
-    <col min="8" max="1011" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -17397,7 +17403,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="195">
+    <row r="2" spans="1:9" ht="191.25">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -17426,7 +17432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39">
+    <row r="3" spans="1:9" ht="38.25">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -17494,12 +17500,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -17516,7 +17522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="175.5">
+    <row r="2" spans="1:5" ht="178.5">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -17533,7 +17539,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13">
+    <row r="3" spans="1:5">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -17584,12 +17590,12 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1">
@@ -17603,7 +17609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="78">
+    <row r="2" spans="1:3" ht="76.5">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -17614,7 +17620,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13">
+    <row r="3" spans="1:3">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -17673,14 +17679,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.453125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -17697,7 +17703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -17711,7 +17717,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -19368,13 +19374,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.453125" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -19391,7 +19397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="63.75">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -19405,7 +19411,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -19860,12 +19866,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -19882,7 +19888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -19896,7 +19902,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -20071,14 +20077,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -20097,7 +20103,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="91">
+    <row r="2" spans="1:6" ht="89.25">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -20117,7 +20123,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -20211,19 +20217,19 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.54296875" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" customWidth="1"/>
-    <col min="8" max="8" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" customWidth="1"/>
-    <col min="11" max="1015" width="8.54296875" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="1015" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -20244,7 +20250,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="88">
+    <row r="2" spans="1:10" ht="102">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -20276,7 +20282,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="39">
+    <row r="3" spans="1:10" ht="38.25">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -20805,27 +20811,27 @@
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="55.453125" customWidth="1"/>
-    <col min="8" max="8" width="47.81640625" customWidth="1"/>
-    <col min="9" max="9" width="52.453125" customWidth="1"/>
-    <col min="10" max="10" width="81.54296875" customWidth="1"/>
-    <col min="11" max="11" width="93.54296875" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="23.453125" customWidth="1"/>
-    <col min="14" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="18.453125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" customWidth="1"/>
-    <col min="18" max="18" width="20.453125" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" customWidth="1"/>
-    <col min="20" max="1013" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" customWidth="1"/>
+    <col min="10" max="10" width="81.5703125" customWidth="1"/>
+    <col min="11" max="11" width="93.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" customHeight="1">
@@ -20857,7 +20863,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:20" ht="117">
+    <row r="2" spans="1:20" ht="114.75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -20901,7 +20907,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="39">
+    <row r="3" spans="1:20" ht="38.25">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -20963,7 +20969,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14">
+    <row r="4" spans="1:20" ht="14.25">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -20971,7 +20977,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:20" ht="14">
+    <row r="5" spans="1:20" ht="14.25">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -20979,7 +20985,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:20" ht="14">
+    <row r="6" spans="1:20" ht="14.25">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -20989,7 +20995,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:20" ht="14">
+    <row r="7" spans="1:20" ht="14.25">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -21000,7 +21006,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:20" ht="14">
+    <row r="8" spans="1:20" ht="14.25">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -21011,7 +21017,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:20" ht="14">
+    <row r="9" spans="1:20" ht="14.25">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -21023,7 +21029,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:20" ht="14">
+    <row r="10" spans="1:20" ht="14.25">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -21035,7 +21041,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:20" ht="14">
+    <row r="11" spans="1:20" ht="14.25">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -21047,7 +21053,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:20" ht="14">
+    <row r="12" spans="1:20" ht="14.25">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -21059,7 +21065,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:20" ht="14">
+    <row r="13" spans="1:20" ht="14.25">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -21071,7 +21077,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:20" ht="14">
+    <row r="14" spans="1:20" ht="14.25">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -21083,7 +21089,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:20" ht="14">
+    <row r="15" spans="1:20" ht="14.25">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -21095,7 +21101,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:20" ht="14">
+    <row r="16" spans="1:20" ht="14.25">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -21107,7 +21113,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14">
+    <row r="17" spans="6:19" ht="14.25">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -21119,7 +21125,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14">
+    <row r="18" spans="6:19" ht="14.25">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -21131,7 +21137,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14">
+    <row r="19" spans="6:19" ht="14.25">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -21141,7 +21147,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14">
+    <row r="20" spans="6:19" ht="14.25">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -21149,7 +21155,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14">
+    <row r="21" spans="6:19" ht="14.25">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -21160,7 +21166,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14">
+    <row r="22" spans="6:19" ht="14.25">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -21172,7 +21178,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14">
+    <row r="23" spans="6:19" ht="14.25">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -21184,7 +21190,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14">
+    <row r="24" spans="6:19" ht="14.25">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -21192,7 +21198,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14">
+    <row r="25" spans="6:19" ht="14.25">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -21203,7 +21209,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14">
+    <row r="26" spans="6:19" ht="14.25">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -21215,7 +21221,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14">
+    <row r="27" spans="6:19" ht="14.25">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -21226,7 +21232,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14">
+    <row r="28" spans="6:19" ht="14.25">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -21236,7 +21242,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14">
+    <row r="29" spans="6:19" ht="14.25">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -21247,7 +21253,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14">
+    <row r="30" spans="6:19" ht="14.25">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -21258,7 +21264,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14">
+    <row r="31" spans="6:19" ht="14.25">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -21269,7 +21275,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14">
+    <row r="32" spans="6:19" ht="14.25">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -21278,7 +21284,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14">
+    <row r="33" spans="6:19" ht="14.25">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -21287,7 +21293,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14">
+    <row r="34" spans="6:19" ht="14.25">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -21297,7 +21303,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14">
+    <row r="35" spans="6:19" ht="14.25">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -21306,7 +21312,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14">
+    <row r="36" spans="6:19" ht="14.25">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -21422,7 +21428,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14">
+    <row r="48" spans="6:19" ht="14.25">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -21519,20 +21525,20 @@
       <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="8" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="58.54296875" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="58.5703125" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.54296875" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="87.1796875" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="87.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18">
@@ -21556,7 +21562,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:18" ht="58" customHeight="1">
+    <row r="2" spans="1:18" ht="57.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -21608,7 +21614,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="39">
+    <row r="3" spans="1:18" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -23675,20 +23681,20 @@
       <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -23705,7 +23711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="94" customHeight="1">
+    <row r="2" spans="1:10" ht="93.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -23737,7 +23743,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13">
+    <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -29462,20 +29468,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="239"/>
-    <col min="3" max="3" width="54.7265625" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7265625" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.26953125" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="239"/>
+    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7265625" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.81640625" style="239"/>
-    <col min="1026" max="16384" width="10.81640625" style="238"/>
+    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" style="239"/>
+    <col min="1026" max="16384" width="10.85546875" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -29501,7 +29507,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="52">
+    <row r="2" spans="1:13" ht="63.75">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -29536,7 +29542,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.5">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -29588,7 +29594,7 @@
       <c r="L4" s="240"/>
       <c r="M4" s="240"/>
     </row>
-    <row r="5" spans="1:13" ht="13">
+    <row r="5" spans="1:13">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="242"/>
@@ -29603,7 +29609,7 @@
       <c r="L5" s="240"/>
       <c r="M5" s="240"/>
     </row>
-    <row r="6" spans="1:13" ht="13">
+    <row r="6" spans="1:13">
       <c r="A6" s="241"/>
       <c r="B6" s="241"/>
       <c r="D6" s="240"/>
@@ -29617,7 +29623,7 @@
       <c r="L6" s="240"/>
       <c r="M6" s="240"/>
     </row>
-    <row r="7" spans="1:13" ht="13">
+    <row r="7" spans="1:13">
       <c r="A7" s="241"/>
       <c r="B7" s="241"/>
       <c r="D7" s="240"/>
@@ -29664,20 +29670,20 @@
       <selection pane="bottomLeft" activeCell="A328" sqref="A328:XFD563"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" customWidth="1"/>
-    <col min="6" max="6" width="53.81640625" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
@@ -29703,7 +29709,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:14" ht="55" customHeight="1">
+    <row r="2" spans="1:14" ht="54.95" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -29743,7 +29749,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="52">
+    <row r="3" spans="1:14" ht="51">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -29881,7 +29887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="13">
+    <row r="9" spans="1:14">
       <c r="A9" s="121" t="s">
         <v>1036</v>
       </c>
@@ -29972,7 +29978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="13">
+    <row r="14" spans="1:14">
       <c r="A14" s="121" t="s">
         <v>1037</v>
       </c>
@@ -30137,7 +30143,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13">
+    <row r="22" spans="1:9">
       <c r="A22" s="121" t="s">
         <v>1062</v>
       </c>
@@ -30182,7 +30188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13">
+    <row r="24" spans="1:9">
       <c r="A24" s="121" t="s">
         <v>1063</v>
       </c>
@@ -30223,7 +30229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13">
+    <row r="26" spans="1:9">
       <c r="A26" s="121" t="s">
         <v>1023</v>
       </c>
@@ -30431,7 +30437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13">
+    <row r="36" spans="1:9">
       <c r="A36" s="121" t="s">
         <v>1018</v>
       </c>
@@ -30786,7 +30792,7 @@
       <c r="J50" s="43"/>
       <c r="K50" s="43"/>
     </row>
-    <row r="51" spans="1:11" ht="13">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -30813,7 +30819,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
     </row>
-    <row r="52" spans="1:11" ht="13">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -30840,7 +30846,7 @@
       <c r="J52" s="43"/>
       <c r="K52" s="43"/>
     </row>
-    <row r="53" spans="1:11" ht="13">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -31238,7 +31244,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="13">
+    <row r="69" spans="1:9">
       <c r="A69" s="121" t="s">
         <v>80</v>
       </c>
@@ -31259,7 +31265,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.15" customHeight="1">
+    <row r="70" spans="1:9" ht="14.1" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -31282,7 +31288,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="10" customHeight="1">
+    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -31488,7 +31494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="13">
+    <row r="81" spans="1:14">
       <c r="A81" s="121" t="s">
         <v>1020</v>
       </c>
@@ -31579,7 +31585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="13">
+    <row r="85" spans="1:14">
       <c r="A85" s="121" t="s">
         <v>1056</v>
       </c>
@@ -31649,7 +31655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="13">
+    <row r="88" spans="1:14">
       <c r="A88" s="121" t="s">
         <v>1040</v>
       </c>
@@ -31710,7 +31716,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="13">
+    <row r="91" spans="1:14">
       <c r="A91" s="121" t="s">
         <v>1065</v>
       </c>
@@ -31731,7 +31737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="13">
+    <row r="92" spans="1:14">
       <c r="A92" s="121" t="s">
         <v>1065</v>
       </c>
@@ -31752,7 +31758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="13">
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
         <v>1014</v>
       </c>
@@ -31781,7 +31787,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="13">
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
         <v>1014</v>
       </c>
@@ -31807,7 +31813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="13">
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
         <v>1014</v>
       </c>
@@ -31827,7 +31833,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="13">
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
         <v>1014</v>
       </c>
@@ -31853,7 +31859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="13">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>1014</v>
       </c>
@@ -31873,7 +31879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="13">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>1014</v>
       </c>
@@ -32082,7 +32088,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="13">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>1014</v>
       </c>
@@ -32108,7 +32114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="13">
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>1014</v>
       </c>
@@ -32149,7 +32155,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="13">
+    <row r="111" spans="1:9">
       <c r="A111" s="121" t="s">
         <v>1014</v>
       </c>
@@ -32335,7 +32341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="13">
+    <row r="119" spans="1:13">
       <c r="A119" s="121" t="s">
         <v>1003</v>
       </c>
@@ -32439,7 +32445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="13">
+    <row r="124" spans="1:13">
       <c r="A124" s="121" t="s">
         <v>998</v>
       </c>
@@ -32630,7 +32636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="13">
+    <row r="133" spans="1:9">
       <c r="A133" s="121" t="s">
         <v>1064</v>
       </c>
@@ -32711,7 +32717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="13">
+    <row r="137" spans="1:9">
       <c r="A137" s="121" t="s">
         <v>883</v>
       </c>
@@ -32912,7 +32918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="13">
+    <row r="147" spans="1:14">
       <c r="A147" s="121" t="s">
         <v>884</v>
       </c>
@@ -32996,7 +33002,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="13">
+    <row r="151" spans="1:14">
       <c r="A151" s="121" t="s">
         <v>885</v>
       </c>
@@ -33017,7 +33023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="13">
+    <row r="152" spans="1:14">
       <c r="A152" s="121" t="s">
         <v>1076</v>
       </c>
@@ -33038,7 +33044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="13">
+    <row r="153" spans="1:14">
       <c r="A153" s="121" t="s">
         <v>1066</v>
       </c>
@@ -33102,7 +33108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="13">
+    <row r="156" spans="1:14">
       <c r="A156" s="121" t="s">
         <v>936</v>
       </c>
@@ -33170,7 +33176,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="13">
+    <row r="159" spans="1:14">
       <c r="A159" s="121" t="s">
         <v>946</v>
       </c>
@@ -33215,7 +33221,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="13">
+    <row r="161" spans="1:9">
       <c r="A161" s="121" t="s">
         <v>953</v>
       </c>
@@ -33331,7 +33337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="13">
+    <row r="166" spans="1:9">
       <c r="A166" s="121" t="s">
         <v>956</v>
       </c>
@@ -33456,7 +33462,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="13">
+    <row r="172" spans="1:9">
       <c r="A172" s="121" t="s">
         <v>986</v>
       </c>
@@ -35156,7 +35162,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="13">
+    <row r="243" spans="1:11">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -35182,7 +35188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="13">
+    <row r="244" spans="1:11">
       <c r="A244" s="121" t="s">
         <v>0</v>
       </c>
@@ -35229,7 +35235,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
     </row>
-    <row r="246" spans="1:11" ht="13">
+    <row r="246" spans="1:11">
       <c r="A246" t="s">
         <v>861</v>
       </c>
@@ -35256,7 +35262,7 @@
       <c r="J246" s="43"/>
       <c r="K246" s="43"/>
     </row>
-    <row r="247" spans="1:11" ht="13">
+    <row r="247" spans="1:11">
       <c r="A247" t="s">
         <v>861</v>
       </c>
@@ -35283,7 +35289,7 @@
       <c r="J247" s="43"/>
       <c r="K247" s="43"/>
     </row>
-    <row r="248" spans="1:11" ht="13">
+    <row r="248" spans="1:11">
       <c r="A248" t="s">
         <v>861</v>
       </c>
@@ -35312,7 +35318,7 @@
       <c r="J248" s="43"/>
       <c r="K248" s="43"/>
     </row>
-    <row r="249" spans="1:11" ht="13">
+    <row r="249" spans="1:11">
       <c r="A249" t="s">
         <v>861</v>
       </c>
@@ -35341,7 +35347,7 @@
       <c r="J249" s="43"/>
       <c r="K249" s="43"/>
     </row>
-    <row r="250" spans="1:11" ht="13">
+    <row r="250" spans="1:11">
       <c r="A250" s="121" t="s">
         <v>861</v>
       </c>
@@ -35695,7 +35701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="13">
+    <row r="265" spans="1:14">
       <c r="A265" s="121" t="s">
         <v>1034</v>
       </c>
@@ -35959,7 +35965,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="13">
+    <row r="275" spans="1:14">
       <c r="A275" s="121" t="s">
         <v>1033</v>
       </c>
@@ -36051,7 +36057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13">
+    <row r="279" spans="1:14" ht="13.5">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -36223,7 +36229,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="13">
+    <row r="287" spans="1:14">
       <c r="A287" t="s">
         <v>102</v>
       </c>
@@ -36246,7 +36252,7 @@
       <c r="J287" s="43"/>
       <c r="K287" s="43"/>
     </row>
-    <row r="288" spans="1:14" ht="13">
+    <row r="288" spans="1:14">
       <c r="A288" s="121" t="s">
         <v>102</v>
       </c>
@@ -36806,7 +36812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="13">
+    <row r="309" spans="1:9">
       <c r="A309" s="121" t="s">
         <v>103</v>
       </c>
@@ -36831,7 +36837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:9" ht="13">
+    <row r="310" spans="1:9">
       <c r="A310" s="121" t="s">
         <v>103</v>
       </c>
@@ -37321,7 +37327,7 @@
       <c r="G329" s="31"/>
       <c r="H329" s="31"/>
     </row>
-    <row r="330" spans="1:9" ht="13">
+    <row r="330" spans="1:9">
       <c r="A330" s="121"/>
       <c r="B330" s="121"/>
       <c r="C330" s="121"/>
@@ -37332,7 +37338,7 @@
       <c r="H330" s="205"/>
       <c r="I330" s="124"/>
     </row>
-    <row r="331" spans="1:9" ht="13">
+    <row r="331" spans="1:9">
       <c r="A331" s="121"/>
       <c r="B331" s="121"/>
       <c r="C331" s="121"/>
@@ -37348,7 +37354,7 @@
       <c r="G332" s="31"/>
       <c r="H332" s="31"/>
     </row>
-    <row r="333" spans="1:9" ht="13">
+    <row r="333" spans="1:9">
       <c r="A333" s="121"/>
       <c r="B333" s="121"/>
       <c r="C333" s="121"/>
@@ -37376,7 +37382,7 @@
       <c r="G336" s="31"/>
       <c r="H336" s="31"/>
     </row>
-    <row r="337" spans="1:9" ht="13">
+    <row r="337" spans="1:9">
       <c r="A337" s="121"/>
       <c r="B337" s="121"/>
       <c r="C337" s="121"/>
@@ -37410,7 +37416,7 @@
       <c r="G341" s="31"/>
       <c r="H341" s="31"/>
     </row>
-    <row r="342" spans="1:9" ht="13">
+    <row r="342" spans="1:9">
       <c r="A342" s="121"/>
       <c r="B342" s="121"/>
       <c r="C342" s="121"/>
@@ -37421,7 +37427,7 @@
       <c r="H342" s="205"/>
       <c r="I342" s="124"/>
     </row>
-    <row r="343" spans="1:9" ht="13">
+    <row r="343" spans="1:9">
       <c r="A343" s="105"/>
       <c r="B343" s="121"/>
       <c r="E343" s="117"/>
@@ -37429,7 +37435,7 @@
       <c r="G343" s="31"/>
       <c r="H343" s="31"/>
     </row>
-    <row r="344" spans="1:9" ht="13">
+    <row r="344" spans="1:9">
       <c r="A344" s="105"/>
       <c r="B344" s="121"/>
       <c r="E344" s="117"/>
@@ -37437,28 +37443,28 @@
       <c r="G344" s="31"/>
       <c r="H344" s="31"/>
     </row>
-    <row r="345" spans="1:9" ht="13">
+    <row r="345" spans="1:9">
       <c r="A345" s="105"/>
       <c r="E345" s="117"/>
       <c r="F345" s="31"/>
       <c r="G345" s="31"/>
       <c r="H345" s="31"/>
     </row>
-    <row r="346" spans="1:9" ht="13">
+    <row r="346" spans="1:9">
       <c r="A346" s="105"/>
       <c r="E346" s="117"/>
       <c r="F346" s="31"/>
       <c r="G346" s="31"/>
       <c r="H346" s="31"/>
     </row>
-    <row r="347" spans="1:9" ht="13">
+    <row r="347" spans="1:9">
       <c r="A347" s="105"/>
       <c r="E347" s="117"/>
       <c r="F347" s="31"/>
       <c r="G347" s="31"/>
       <c r="H347" s="31"/>
     </row>
-    <row r="348" spans="1:9" ht="13">
+    <row r="348" spans="1:9">
       <c r="A348" s="121"/>
       <c r="B348" s="121"/>
       <c r="C348" s="121"/>
@@ -38310,7 +38316,7 @@
       <c r="G474" s="31"/>
       <c r="H474" s="31"/>
     </row>
-    <row r="475" spans="1:9" ht="13">
+    <row r="475" spans="1:9">
       <c r="A475" s="121"/>
       <c r="B475" s="121"/>
       <c r="C475" s="121"/>
@@ -38321,7 +38327,7 @@
       <c r="H475" s="205"/>
       <c r="I475" s="124"/>
     </row>
-    <row r="476" spans="1:9" ht="13">
+    <row r="476" spans="1:9">
       <c r="A476" s="121"/>
       <c r="B476" s="121"/>
       <c r="C476" s="121"/>
@@ -38332,55 +38338,55 @@
       <c r="H476" s="31"/>
       <c r="I476" s="124"/>
     </row>
-    <row r="477" spans="1:9" ht="13">
+    <row r="477" spans="1:9">
       <c r="A477" s="105"/>
       <c r="E477" s="117"/>
       <c r="F477" s="105"/>
       <c r="G477" s="31"/>
     </row>
-    <row r="478" spans="1:9" ht="13">
+    <row r="478" spans="1:9">
       <c r="A478" s="105"/>
       <c r="E478" s="117"/>
       <c r="F478" s="105"/>
       <c r="G478" s="31"/>
     </row>
-    <row r="479" spans="1:9" ht="13">
+    <row r="479" spans="1:9">
       <c r="A479" s="105"/>
       <c r="E479" s="117"/>
       <c r="F479" s="105"/>
       <c r="G479" s="31"/>
     </row>
-    <row r="480" spans="1:9" ht="13">
+    <row r="480" spans="1:9">
       <c r="A480" s="105"/>
       <c r="E480" s="117"/>
       <c r="F480" s="105"/>
       <c r="G480" s="31"/>
     </row>
-    <row r="481" spans="1:8" ht="13">
+    <row r="481" spans="1:8">
       <c r="A481" s="105"/>
       <c r="E481" s="117"/>
       <c r="F481" s="105"/>
       <c r="G481" s="31"/>
     </row>
-    <row r="482" spans="1:8" ht="13">
+    <row r="482" spans="1:8">
       <c r="A482" s="105"/>
       <c r="E482" s="117"/>
       <c r="F482" s="105"/>
       <c r="G482" s="31"/>
     </row>
-    <row r="483" spans="1:8" ht="13">
+    <row r="483" spans="1:8">
       <c r="A483" s="105"/>
       <c r="E483" s="117"/>
       <c r="F483" s="105"/>
       <c r="G483" s="31"/>
     </row>
-    <row r="484" spans="1:8" ht="13">
+    <row r="484" spans="1:8">
       <c r="A484" s="105"/>
       <c r="E484" s="117"/>
       <c r="F484" s="105"/>
       <c r="G484" s="31"/>
     </row>
-    <row r="485" spans="1:8" ht="13">
+    <row r="485" spans="1:8">
       <c r="A485" s="105"/>
       <c r="E485" s="117"/>
       <c r="F485" s="105"/>
@@ -38496,7 +38502,7 @@
       <c r="G507" s="31"/>
       <c r="H507" s="31"/>
     </row>
-    <row r="508" spans="1:10" ht="13">
+    <row r="508" spans="1:10">
       <c r="A508" s="121"/>
       <c r="B508" s="121"/>
       <c r="C508" s="121"/>
@@ -38507,7 +38513,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13">
+    <row r="509" spans="1:10" ht="13.5">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -38518,7 +38524,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13">
+    <row r="510" spans="1:10" ht="13.5">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -38529,7 +38535,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13">
+    <row r="511" spans="1:10" ht="13.5">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -38611,7 +38617,7 @@
       <c r="G525" s="31"/>
       <c r="H525" s="31"/>
     </row>
-    <row r="526" spans="1:9" ht="13">
+    <row r="526" spans="1:9">
       <c r="A526" s="121"/>
       <c r="B526" s="121"/>
       <c r="C526" s="121"/>
@@ -38732,7 +38738,7 @@
       <c r="G546" s="31"/>
       <c r="H546" s="31"/>
     </row>
-    <row r="547" spans="1:9" ht="13">
+    <row r="547" spans="1:9">
       <c r="A547" s="121"/>
       <c r="B547" s="121"/>
       <c r="C547" s="121"/>
@@ -38819,7 +38825,7 @@
       <c r="G562" s="31"/>
       <c r="H562" s="31"/>
     </row>
-    <row r="563" spans="1:9" ht="13">
+    <row r="563" spans="1:9">
       <c r="A563" s="121"/>
       <c r="B563" s="121"/>
       <c r="C563" s="121"/>

</xml_diff>

<commit_message>
RET-0000: Tidy up after merge
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-englandwales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C0F65-4BD5-42A8-96D1-B85D582DE939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81542D7B-9885-429C-8B46-5A68316E0E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="549" firstSheet="18" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2895" windowWidth="29040" windowHeight="15840" tabRatio="549" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="ChallengeQuestion" sheetId="35" r:id="rId10"/>
     <sheet name="ComplexTypes" sheetId="26" r:id="rId11"/>
     <sheet name="EventToComplexTypes" sheetId="29" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="38" r:id="rId13"/>
+    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId13"/>
     <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId14"/>
     <sheet name="SearchInputFields" sheetId="13" r:id="rId15"/>
     <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
@@ -21078,8 +21078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B407BCC-AC89-45D9-AD51-F07E4F87B419}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -29347,7 +29347,7 @@
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RET-4288: nonprod.json support and CaseFlags nonprod.json example (#659)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-englandwales\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-englandwales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7DB5CB-85A6-49C0-87F1-5E22B00B421C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC1D55-4FB8-444B-9E45-F7CC0D4BE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="500" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="1470" windowWidth="36660" windowHeight="19395" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$P$217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$Q$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$J$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseType!$A$3:$I$3</definedName>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3708" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="1143">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -21065,7 +21065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -31197,12 +31197,12 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E75101-AE74-3B43-A771-FE940D099A52}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:P217"/>
+  <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD217"/>
+      <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -31210,18 +31210,18 @@
     <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="58.42578125" customWidth="1"/>
-    <col min="9" max="9" width="100" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="87.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="58.42578125" customWidth="1"/>
+    <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="87.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18">
+    <row r="1" spans="1:17" ht="18">
       <c r="A1" s="30" t="s">
         <v>106</v>
       </c>
@@ -31229,19 +31229,20 @@
         <v>1</v>
       </c>
       <c r="D1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="G1" s="31"/>
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="34"/>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
-      <c r="P1" s="34"/>
-    </row>
-    <row r="2" spans="1:16" ht="57.95" customHeight="1">
+      <c r="P1" s="31"/>
+      <c r="Q1" s="34"/>
+    </row>
+    <row r="2" spans="1:17" ht="57.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31254,42 +31255,43 @@
       <c r="D2" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="H2" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="M2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="N2" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="O2" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="P2" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="38.25">
+    <row r="3" spans="1:17" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -31302,44 +31304,47 @@
       <c r="D3" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="G3" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="I3" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="J3" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="K3" s="26" t="s">
         <v>1080</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="L3" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="M3" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="N3" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="O3" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="P3" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="Q3" s="26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>1103</v>
       </c>
@@ -31352,25 +31357,25 @@
       <c r="D4" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
       <c r="F4" s="7">
         <v>1</v>
       </c>
       <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="L4" s="77"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="7">
+      <c r="M4" s="77"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
@@ -31383,24 +31388,24 @@
       <c r="D5" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
       <c r="F5" s="7">
         <v>1</v>
       </c>
       <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
         <v>2</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="7">
+      <c r="N5" s="42"/>
+      <c r="O5" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>1103</v>
       </c>
@@ -31413,24 +31418,24 @@
       <c r="D6" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
       <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
         <v>3</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M6" s="42"/>
-      <c r="N6" s="7">
+      <c r="N6" s="42"/>
+      <c r="O6" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -31443,30 +31448,30 @@
       <c r="D7" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
         <v>4</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>800</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>740</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M7" s="42"/>
-      <c r="N7" s="7">
+      <c r="N7" s="42"/>
+      <c r="O7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>1103</v>
       </c>
@@ -31479,30 +31484,30 @@
       <c r="D8" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <v>5</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>800</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>1075</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M8" s="42"/>
-      <c r="N8" s="7">
+      <c r="N8" s="42"/>
+      <c r="O8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>1103</v>
       </c>
@@ -31515,30 +31520,30 @@
       <c r="D9" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
         <v>6</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>800</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>1075</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="7">
+      <c r="N9" s="42"/>
+      <c r="O9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>1103</v>
       </c>
@@ -31551,30 +31556,30 @@
       <c r="D10" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
       <c r="F10" s="7">
         <v>1</v>
       </c>
       <c r="G10" s="7">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
         <v>7</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>800</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>1075</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="L10" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M10" s="42"/>
-      <c r="N10" s="7">
+      <c r="N10" s="42"/>
+      <c r="O10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>1103</v>
       </c>
@@ -31587,1735 +31592,1749 @@
       <c r="D11" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
       <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
         <v>8</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>800</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>1075</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="L11" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M11" s="42"/>
-      <c r="N11" s="7">
+      <c r="N11" s="42"/>
+      <c r="O11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="E12" s="7"/>
+    <row r="12" spans="1:17">
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="E13" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="E14" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="77"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="E15" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="E16" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="5:14">
-      <c r="E17" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="6:15">
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="5:14">
-      <c r="E18" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="6:15">
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="5:14">
-      <c r="E19" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="6:15">
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="5:14">
-      <c r="E20" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="6:15">
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="5:14">
-      <c r="E21" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="6:15">
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="5:14">
-      <c r="E22" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="6:15">
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="5:14">
-      <c r="E23" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="6:15">
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="5:14">
-      <c r="E24" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="6:15">
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="7"/>
-    </row>
-    <row r="25" spans="5:14">
-      <c r="E25" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="6:15">
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="5:14">
-      <c r="E26" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="6:15">
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="7"/>
-    </row>
-    <row r="27" spans="5:14">
-      <c r="E27" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="6:15">
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="7"/>
-    </row>
-    <row r="28" spans="5:14">
-      <c r="E28" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="6:15">
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="7"/>
-    </row>
-    <row r="29" spans="5:14">
-      <c r="E29" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="6:15">
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="7"/>
-    </row>
-    <row r="30" spans="5:14">
-      <c r="E30" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="6:15">
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="7"/>
-    </row>
-    <row r="31" spans="5:14">
-      <c r="E31" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="6:15">
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="7"/>
-    </row>
-    <row r="32" spans="5:14">
-      <c r="E32" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="6:15">
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="7"/>
-    </row>
-    <row r="33" spans="5:14">
-      <c r="E33" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="6:15">
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="5:14">
-      <c r="E34" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="6:15">
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="7"/>
-    </row>
-    <row r="35" spans="5:14">
-      <c r="E35" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="6:15">
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="7"/>
-    </row>
-    <row r="36" spans="5:14">
-      <c r="E36" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="6:15">
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="7"/>
-    </row>
-    <row r="37" spans="5:14">
-      <c r="E37" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="6:15">
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="7"/>
-    </row>
-    <row r="38" spans="5:14">
-      <c r="E38" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="6:15">
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="7"/>
-    </row>
-    <row r="39" spans="5:14">
-      <c r="E39" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="6:15">
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="7"/>
-    </row>
-    <row r="40" spans="5:14">
-      <c r="E40" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="N39" s="42"/>
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="6:15">
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="7"/>
-    </row>
-    <row r="41" spans="5:14">
-      <c r="E41" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="6:15">
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="7"/>
-    </row>
-    <row r="42" spans="5:14">
-      <c r="E42" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" spans="6:15">
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="7"/>
-    </row>
-    <row r="43" spans="5:14">
-      <c r="E43" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="6:15">
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="7"/>
-    </row>
-    <row r="44" spans="5:14">
-      <c r="E44" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="6:15">
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="M44" s="42"/>
-      <c r="N44" s="7"/>
-    </row>
-    <row r="45" spans="5:14">
-      <c r="E45" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="N44" s="42"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="6:15">
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="77"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="7"/>
-    </row>
-    <row r="46" spans="5:14">
-      <c r="E46" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="77"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="7"/>
+    </row>
+    <row r="46" spans="6:15">
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="77"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="7"/>
-    </row>
-    <row r="47" spans="5:14">
-      <c r="E47" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="77"/>
+      <c r="N46" s="42"/>
+      <c r="O46" s="7"/>
+    </row>
+    <row r="47" spans="6:15">
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="M47" s="42"/>
-      <c r="N47" s="7"/>
-    </row>
-    <row r="48" spans="5:14">
-      <c r="E48" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="N47" s="42"/>
+      <c r="O47" s="7"/>
+    </row>
+    <row r="48" spans="6:15">
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="7"/>
-    </row>
-    <row r="49" spans="5:14">
-      <c r="E49" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="N48" s="42"/>
+      <c r="O48" s="7"/>
+    </row>
+    <row r="49" spans="6:15">
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="M49" s="42"/>
-      <c r="N49" s="7"/>
-    </row>
-    <row r="50" spans="5:14">
-      <c r="E50" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="N49" s="42"/>
+      <c r="O49" s="7"/>
+    </row>
+    <row r="50" spans="6:15">
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="M50" s="42"/>
-      <c r="N50" s="7"/>
-    </row>
-    <row r="51" spans="5:14">
-      <c r="E51" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="7"/>
+    </row>
+    <row r="51" spans="6:15">
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="M51" s="42"/>
-      <c r="N51" s="7"/>
-    </row>
-    <row r="52" spans="5:14">
-      <c r="E52" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="N51" s="42"/>
+      <c r="O51" s="7"/>
+    </row>
+    <row r="52" spans="6:15">
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="M52" s="42"/>
-      <c r="N52" s="7"/>
-    </row>
-    <row r="53" spans="5:14">
-      <c r="E53" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="7"/>
+    </row>
+    <row r="53" spans="6:15">
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="M53" s="42"/>
-      <c r="N53" s="7"/>
-    </row>
-    <row r="54" spans="5:14">
-      <c r="E54" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="7"/>
+    </row>
+    <row r="54" spans="6:15">
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="M54" s="42"/>
-      <c r="N54" s="7"/>
-    </row>
-    <row r="55" spans="5:14">
-      <c r="E55" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="N54" s="42"/>
+      <c r="O54" s="7"/>
+    </row>
+    <row r="55" spans="6:15">
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="M55" s="42"/>
-      <c r="N55" s="7"/>
-    </row>
-    <row r="56" spans="5:14">
-      <c r="E56" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="N55" s="42"/>
+      <c r="O55" s="7"/>
+    </row>
+    <row r="56" spans="6:15">
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="M56" s="42"/>
-      <c r="N56" s="7"/>
-    </row>
-    <row r="57" spans="5:14">
-      <c r="E57" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="N56" s="42"/>
+      <c r="O56" s="7"/>
+    </row>
+    <row r="57" spans="6:15">
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="M57" s="42"/>
-      <c r="N57" s="7"/>
-    </row>
-    <row r="58" spans="5:14">
-      <c r="E58" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="N57" s="42"/>
+      <c r="O57" s="7"/>
+    </row>
+    <row r="58" spans="6:15">
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="M58" s="42"/>
-      <c r="N58" s="7"/>
-    </row>
-    <row r="59" spans="5:14">
-      <c r="E59" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="N58" s="42"/>
+      <c r="O58" s="7"/>
+    </row>
+    <row r="59" spans="6:15">
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="M59" s="42"/>
-      <c r="N59" s="7"/>
-    </row>
-    <row r="60" spans="5:14">
-      <c r="E60" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="N59" s="42"/>
+      <c r="O59" s="7"/>
+    </row>
+    <row r="60" spans="6:15">
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="M60" s="42"/>
-      <c r="N60" s="7"/>
-    </row>
-    <row r="61" spans="5:14">
-      <c r="E61" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="N60" s="42"/>
+      <c r="O60" s="7"/>
+    </row>
+    <row r="61" spans="6:15">
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="7"/>
-    </row>
-    <row r="62" spans="5:14">
-      <c r="E62" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="N61" s="42"/>
+      <c r="O61" s="7"/>
+    </row>
+    <row r="62" spans="6:15">
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="M62" s="42"/>
-      <c r="N62" s="7"/>
-    </row>
-    <row r="63" spans="5:14">
-      <c r="E63" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="N62" s="42"/>
+      <c r="O62" s="7"/>
+    </row>
+    <row r="63" spans="6:15">
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="M63" s="42"/>
-      <c r="N63" s="7"/>
-    </row>
-    <row r="64" spans="5:14">
-      <c r="E64" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="N63" s="42"/>
+      <c r="O63" s="7"/>
+    </row>
+    <row r="64" spans="6:15">
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
-      <c r="K64" s="7"/>
-      <c r="M64" s="42"/>
-      <c r="N64" s="7"/>
-    </row>
-    <row r="65" spans="5:14">
-      <c r="E65" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="N64" s="42"/>
+      <c r="O64" s="7"/>
+    </row>
+    <row r="65" spans="6:15">
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="M65" s="42"/>
-      <c r="N65" s="7"/>
-    </row>
-    <row r="66" spans="5:14">
-      <c r="E66" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="N65" s="42"/>
+      <c r="O65" s="7"/>
+    </row>
+    <row r="66" spans="6:15">
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
-      <c r="K66" s="7"/>
-      <c r="M66" s="42"/>
-      <c r="N66" s="7"/>
-    </row>
-    <row r="67" spans="5:14">
-      <c r="E67" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="7"/>
+    </row>
+    <row r="67" spans="6:15">
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="77"/>
-      <c r="M67" s="42"/>
-      <c r="N67" s="7"/>
-    </row>
-    <row r="68" spans="5:14">
-      <c r="E68" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="77"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="7"/>
+    </row>
+    <row r="68" spans="6:15">
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="M68" s="42"/>
-      <c r="N68" s="7"/>
-    </row>
-    <row r="69" spans="5:14">
-      <c r="E69" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="N68" s="42"/>
+      <c r="O68" s="7"/>
+    </row>
+    <row r="69" spans="6:15">
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="M69" s="42"/>
-      <c r="N69" s="7"/>
-    </row>
-    <row r="70" spans="5:14">
-      <c r="E70" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="N69" s="42"/>
+      <c r="O69" s="7"/>
+    </row>
+    <row r="70" spans="6:15">
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="77"/>
-      <c r="M70" s="42"/>
-      <c r="N70" s="7"/>
-    </row>
-    <row r="71" spans="5:14">
-      <c r="E71" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="77"/>
+      <c r="N70" s="42"/>
+      <c r="O70" s="7"/>
+    </row>
+    <row r="71" spans="6:15">
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="42"/>
-      <c r="N71" s="7"/>
-    </row>
-    <row r="72" spans="5:14">
-      <c r="E72" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="77"/>
+      <c r="N71" s="42"/>
+      <c r="O71" s="7"/>
+    </row>
+    <row r="72" spans="6:15">
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="42"/>
-      <c r="N72" s="7"/>
-    </row>
-    <row r="73" spans="5:14">
-      <c r="E73" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="77"/>
+      <c r="N72" s="42"/>
+      <c r="O72" s="7"/>
+    </row>
+    <row r="73" spans="6:15">
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="77"/>
-      <c r="M73" s="42"/>
-      <c r="N73" s="7"/>
-    </row>
-    <row r="74" spans="5:14">
-      <c r="E74" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="77"/>
+      <c r="N73" s="42"/>
+      <c r="O73" s="7"/>
+    </row>
+    <row r="74" spans="6:15">
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="77"/>
-      <c r="M74" s="42"/>
-      <c r="N74" s="7"/>
-    </row>
-    <row r="75" spans="5:14">
-      <c r="E75" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="77"/>
+      <c r="N74" s="42"/>
+      <c r="O74" s="7"/>
+    </row>
+    <row r="75" spans="6:15">
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="77"/>
-      <c r="M75" s="42"/>
-      <c r="N75" s="7"/>
-    </row>
-    <row r="76" spans="5:14">
-      <c r="E76" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="77"/>
+      <c r="N75" s="42"/>
+      <c r="O75" s="7"/>
+    </row>
+    <row r="76" spans="6:15">
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="77"/>
-      <c r="M76" s="42"/>
-      <c r="N76" s="7"/>
-    </row>
-    <row r="77" spans="5:14">
-      <c r="E77" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="77"/>
+      <c r="N76" s="42"/>
+      <c r="O76" s="7"/>
+    </row>
+    <row r="77" spans="6:15">
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="77"/>
-      <c r="M77" s="42"/>
-      <c r="N77" s="7"/>
-    </row>
-    <row r="78" spans="5:14">
-      <c r="E78" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="77"/>
+      <c r="N77" s="42"/>
+      <c r="O77" s="7"/>
+    </row>
+    <row r="78" spans="6:15">
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="77"/>
-      <c r="M78" s="42"/>
-      <c r="N78" s="7"/>
-    </row>
-    <row r="79" spans="5:14">
-      <c r="E79" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="77"/>
+      <c r="N78" s="42"/>
+      <c r="O78" s="7"/>
+    </row>
+    <row r="79" spans="6:15">
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="42"/>
-      <c r="N79" s="7"/>
-    </row>
-    <row r="80" spans="5:14">
-      <c r="E80" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="77"/>
+      <c r="N79" s="42"/>
+      <c r="O79" s="7"/>
+    </row>
+    <row r="80" spans="6:15">
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="77"/>
-      <c r="M80" s="42"/>
-      <c r="N80" s="7"/>
-    </row>
-    <row r="81" spans="3:14">
+      <c r="H80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="77"/>
+      <c r="N80" s="42"/>
+      <c r="O80" s="7"/>
+    </row>
+    <row r="81" spans="3:15">
       <c r="C81" s="105"/>
-      <c r="E81" s="7"/>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="77"/>
-      <c r="M81" s="42"/>
-      <c r="N81" s="7"/>
-    </row>
-    <row r="82" spans="3:14">
+      <c r="H81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="77"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="7"/>
+    </row>
+    <row r="82" spans="3:15">
       <c r="C82" s="105"/>
-      <c r="E82" s="7"/>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
-      <c r="K82" s="7"/>
-      <c r="L82" s="77"/>
-      <c r="M82" s="42"/>
-      <c r="N82" s="7"/>
-    </row>
-    <row r="83" spans="3:14">
-      <c r="E83" s="7"/>
+      <c r="H82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="77"/>
+      <c r="N82" s="42"/>
+      <c r="O82" s="7"/>
+    </row>
+    <row r="83" spans="3:15">
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="77"/>
-      <c r="M83" s="42"/>
-      <c r="N83" s="7"/>
-    </row>
-    <row r="84" spans="3:14">
-      <c r="E84" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="77"/>
+      <c r="N83" s="42"/>
+      <c r="O83" s="7"/>
+    </row>
+    <row r="84" spans="3:15">
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
-      <c r="K84" s="7"/>
-      <c r="L84" s="77"/>
-      <c r="M84" s="42"/>
-      <c r="N84" s="7"/>
-    </row>
-    <row r="85" spans="3:14">
-      <c r="E85" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="77"/>
+      <c r="N84" s="42"/>
+      <c r="O84" s="7"/>
+    </row>
+    <row r="85" spans="3:15">
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
-      <c r="K85" s="7"/>
-      <c r="L85" s="77"/>
-      <c r="M85" s="42"/>
-      <c r="N85" s="7"/>
-    </row>
-    <row r="86" spans="3:14">
-      <c r="E86" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="77"/>
+      <c r="N85" s="42"/>
+      <c r="O85" s="7"/>
+    </row>
+    <row r="86" spans="3:15">
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="77"/>
-      <c r="M86" s="42"/>
-      <c r="N86" s="7"/>
-    </row>
-    <row r="87" spans="3:14">
-      <c r="E87" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="77"/>
+      <c r="N86" s="42"/>
+      <c r="O86" s="7"/>
+    </row>
+    <row r="87" spans="3:15">
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="77"/>
-      <c r="M87" s="42"/>
-      <c r="N87" s="7"/>
-    </row>
-    <row r="88" spans="3:14">
-      <c r="E88" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="77"/>
+      <c r="N87" s="42"/>
+      <c r="O87" s="7"/>
+    </row>
+    <row r="88" spans="3:15">
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="77"/>
-      <c r="M88" s="42"/>
-      <c r="N88" s="7"/>
-    </row>
-    <row r="89" spans="3:14">
-      <c r="E89" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="77"/>
+      <c r="N88" s="42"/>
+      <c r="O88" s="7"/>
+    </row>
+    <row r="89" spans="3:15">
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
-      <c r="K89" s="7"/>
-      <c r="L89" s="77"/>
-      <c r="M89" s="42"/>
-      <c r="N89" s="7"/>
-    </row>
-    <row r="90" spans="3:14">
-      <c r="E90" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="77"/>
+      <c r="N89" s="42"/>
+      <c r="O89" s="7"/>
+    </row>
+    <row r="90" spans="3:15">
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
-      <c r="K90" s="7"/>
-      <c r="L90" s="77"/>
-      <c r="M90" s="42"/>
-      <c r="N90" s="7"/>
-    </row>
-    <row r="91" spans="3:14">
-      <c r="E91" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="77"/>
+      <c r="N90" s="42"/>
+      <c r="O90" s="7"/>
+    </row>
+    <row r="91" spans="3:15">
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
-      <c r="K91" s="7"/>
-      <c r="L91" s="77"/>
-      <c r="M91" s="42"/>
-      <c r="N91" s="7"/>
-    </row>
-    <row r="92" spans="3:14">
-      <c r="E92" s="7"/>
+      <c r="H91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="77"/>
+      <c r="N91" s="42"/>
+      <c r="O91" s="7"/>
+    </row>
+    <row r="92" spans="3:15">
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
-      <c r="K92" s="7"/>
-      <c r="L92" s="77"/>
-      <c r="M92" s="42"/>
-      <c r="N92" s="7"/>
-    </row>
-    <row r="93" spans="3:14">
-      <c r="E93" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="77"/>
+      <c r="N92" s="42"/>
+      <c r="O92" s="7"/>
+    </row>
+    <row r="93" spans="3:15">
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="77"/>
-      <c r="M93" s="42"/>
-      <c r="N93" s="7"/>
-    </row>
-    <row r="94" spans="3:14">
-      <c r="E94" s="7"/>
+      <c r="H93" s="7"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="77"/>
+      <c r="N93" s="42"/>
+      <c r="O93" s="7"/>
+    </row>
+    <row r="94" spans="3:15">
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="77"/>
-      <c r="M94" s="42"/>
-      <c r="N94" s="7"/>
-    </row>
-    <row r="95" spans="3:14">
-      <c r="E95" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="77"/>
+      <c r="N94" s="42"/>
+      <c r="O94" s="7"/>
+    </row>
+    <row r="95" spans="3:15">
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="77"/>
-      <c r="M95" s="42"/>
-      <c r="N95" s="7"/>
-    </row>
-    <row r="96" spans="3:14">
+      <c r="H95" s="7"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="77"/>
+      <c r="N95" s="42"/>
+      <c r="O95" s="7"/>
+    </row>
+    <row r="96" spans="3:15">
       <c r="C96" s="121"/>
-      <c r="E96" s="7"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
-      <c r="K96" s="7"/>
-      <c r="L96" s="77"/>
-      <c r="M96" s="42"/>
-      <c r="N96" s="7"/>
-    </row>
-    <row r="97" spans="5:14">
-      <c r="E97" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="L96" s="7"/>
+      <c r="M96" s="77"/>
+      <c r="N96" s="42"/>
+      <c r="O96" s="7"/>
+    </row>
+    <row r="97" spans="6:15">
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="77"/>
-      <c r="M97" s="42"/>
-      <c r="N97" s="7"/>
-    </row>
-    <row r="98" spans="5:14">
-      <c r="E98" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="77"/>
+      <c r="N97" s="42"/>
+      <c r="O97" s="7"/>
+    </row>
+    <row r="98" spans="6:15">
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
-      <c r="K98" s="7"/>
-      <c r="M98" s="42"/>
-      <c r="N98" s="7"/>
-    </row>
-    <row r="99" spans="5:14">
-      <c r="E99" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="L98" s="7"/>
+      <c r="N98" s="42"/>
+      <c r="O98" s="7"/>
+    </row>
+    <row r="99" spans="6:15">
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
-      <c r="K99" s="7"/>
-      <c r="M99" s="42"/>
-      <c r="N99" s="7"/>
-    </row>
-    <row r="100" spans="5:14">
-      <c r="E100" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="N99" s="42"/>
+      <c r="O99" s="7"/>
+    </row>
+    <row r="100" spans="6:15">
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
-      <c r="K100" s="7"/>
-      <c r="M100" s="42"/>
-      <c r="N100" s="7"/>
-    </row>
-    <row r="101" spans="5:14">
-      <c r="E101" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="L100" s="7"/>
+      <c r="N100" s="42"/>
+      <c r="O100" s="7"/>
+    </row>
+    <row r="101" spans="6:15">
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
-      <c r="K101" s="7"/>
-      <c r="M101" s="42"/>
-      <c r="N101" s="7"/>
-    </row>
-    <row r="102" spans="5:14">
-      <c r="E102" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="N101" s="42"/>
+      <c r="O101" s="7"/>
+    </row>
+    <row r="102" spans="6:15">
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
-      <c r="K102" s="7"/>
-      <c r="M102" s="42"/>
-      <c r="N102" s="7"/>
-    </row>
-    <row r="103" spans="5:14">
-      <c r="E103" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="L102" s="7"/>
+      <c r="N102" s="42"/>
+      <c r="O102" s="7"/>
+    </row>
+    <row r="103" spans="6:15">
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
-      <c r="K103" s="7"/>
-      <c r="M103" s="42"/>
-      <c r="N103" s="7"/>
-    </row>
-    <row r="104" spans="5:14">
-      <c r="E104" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="N103" s="42"/>
+      <c r="O103" s="7"/>
+    </row>
+    <row r="104" spans="6:15">
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
-      <c r="K104" s="7"/>
-      <c r="N104" s="7"/>
-    </row>
-    <row r="105" spans="5:14">
-      <c r="E105" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="L104" s="7"/>
+      <c r="O104" s="7"/>
+    </row>
+    <row r="105" spans="6:15">
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
-      <c r="K105" s="7"/>
-      <c r="L105" s="77"/>
-      <c r="M105" s="42"/>
-      <c r="N105" s="7"/>
-    </row>
-    <row r="106" spans="5:14">
-      <c r="E106" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="77"/>
+      <c r="N105" s="42"/>
+      <c r="O105" s="7"/>
+    </row>
+    <row r="106" spans="6:15">
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
-      <c r="K106" s="7"/>
-      <c r="M106" s="42"/>
-      <c r="N106" s="7"/>
-    </row>
-    <row r="107" spans="5:14">
-      <c r="E107" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="L106" s="7"/>
+      <c r="N106" s="42"/>
+      <c r="O106" s="7"/>
+    </row>
+    <row r="107" spans="6:15">
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
-      <c r="K107" s="7"/>
-      <c r="M107" s="42"/>
-      <c r="N107" s="7"/>
-    </row>
-    <row r="108" spans="5:14">
-      <c r="E108" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="N107" s="42"/>
+      <c r="O107" s="7"/>
+    </row>
+    <row r="108" spans="6:15">
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
-      <c r="K108" s="7"/>
-      <c r="N108" s="7"/>
-    </row>
-    <row r="109" spans="5:14">
-      <c r="E109" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="L108" s="7"/>
+      <c r="O108" s="7"/>
+    </row>
+    <row r="109" spans="6:15">
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
-      <c r="K109" s="7"/>
-      <c r="N109" s="7"/>
-    </row>
-    <row r="110" spans="5:14">
-      <c r="E110" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="O109" s="7"/>
+    </row>
+    <row r="110" spans="6:15">
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
-      <c r="K110" s="7"/>
-      <c r="N110" s="7"/>
-    </row>
-    <row r="111" spans="5:14">
-      <c r="E111" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="L110" s="7"/>
+      <c r="O110" s="7"/>
+    </row>
+    <row r="111" spans="6:15">
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
-      <c r="K111" s="7"/>
-      <c r="N111" s="7"/>
-    </row>
-    <row r="112" spans="5:14">
-      <c r="E112" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="O111" s="7"/>
+    </row>
+    <row r="112" spans="6:15">
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
-      <c r="K112" s="7"/>
-      <c r="N112" s="7"/>
-    </row>
-    <row r="113" spans="2:14">
-      <c r="E113" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="L112" s="7"/>
+      <c r="O112" s="7"/>
+    </row>
+    <row r="113" spans="2:15">
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
-      <c r="K113" s="7"/>
-      <c r="L113" s="111"/>
-      <c r="N113" s="7"/>
-    </row>
-    <row r="114" spans="2:14">
-      <c r="E114" s="7"/>
+      <c r="H113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="111"/>
+      <c r="O113" s="7"/>
+    </row>
+    <row r="114" spans="2:15">
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
-      <c r="K114" s="7"/>
-      <c r="N114" s="7"/>
-    </row>
-    <row r="115" spans="2:14">
-      <c r="E115" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="L114" s="7"/>
+      <c r="O114" s="7"/>
+    </row>
+    <row r="115" spans="2:15">
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
-      <c r="K115" s="7"/>
-      <c r="N115" s="7"/>
-    </row>
-    <row r="116" spans="2:14">
-      <c r="E116" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="O115" s="7"/>
+    </row>
+    <row r="116" spans="2:15">
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
-      <c r="K116" s="7"/>
-      <c r="N116" s="7"/>
-    </row>
-    <row r="117" spans="2:14">
-      <c r="E117" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="L116" s="7"/>
+      <c r="O116" s="7"/>
+    </row>
+    <row r="117" spans="2:15">
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
-      <c r="K117" s="7"/>
-      <c r="N117" s="7"/>
-    </row>
-    <row r="118" spans="2:14">
-      <c r="E118" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="O117" s="7"/>
+    </row>
+    <row r="118" spans="2:15">
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
-      <c r="K118" s="7"/>
-      <c r="N118" s="7"/>
-    </row>
-    <row r="119" spans="2:14">
-      <c r="E119" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="L118" s="7"/>
+      <c r="O118" s="7"/>
+    </row>
+    <row r="119" spans="2:15">
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
-      <c r="K119" s="7"/>
-      <c r="N119" s="7"/>
-    </row>
-    <row r="120" spans="2:14">
+      <c r="H119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="O119" s="7"/>
+    </row>
+    <row r="120" spans="2:15">
       <c r="B120" s="31"/>
       <c r="C120" s="31"/>
-      <c r="E120" s="7"/>
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
-      <c r="K120" s="7"/>
-      <c r="N120" s="7"/>
-    </row>
-    <row r="121" spans="2:14">
+      <c r="H120" s="7"/>
+      <c r="L120" s="7"/>
+      <c r="O120" s="7"/>
+    </row>
+    <row r="121" spans="2:15">
       <c r="B121" s="31"/>
       <c r="C121" s="31"/>
-      <c r="E121" s="7"/>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
-      <c r="K121" s="7"/>
-      <c r="N121" s="7"/>
-    </row>
-    <row r="122" spans="2:14">
+      <c r="H121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="O121" s="7"/>
+    </row>
+    <row r="122" spans="2:15">
       <c r="B122" s="31"/>
       <c r="C122" s="31"/>
-      <c r="E122" s="7"/>
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
-      <c r="K122" s="7"/>
-      <c r="N122" s="7"/>
-    </row>
-    <row r="123" spans="2:14">
+      <c r="H122" s="7"/>
+      <c r="L122" s="7"/>
+      <c r="O122" s="7"/>
+    </row>
+    <row r="123" spans="2:15">
       <c r="B123" s="31"/>
       <c r="C123" s="31"/>
-      <c r="E123" s="7"/>
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
-      <c r="K123" s="7"/>
-      <c r="N123" s="7"/>
-    </row>
-    <row r="124" spans="2:14">
+      <c r="H123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="O123" s="7"/>
+    </row>
+    <row r="124" spans="2:15">
       <c r="B124" s="31"/>
       <c r="C124" s="31"/>
-      <c r="E124" s="7"/>
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
-      <c r="K124" s="7"/>
-      <c r="N124" s="7"/>
-    </row>
-    <row r="125" spans="2:14">
-      <c r="E125" s="7"/>
+      <c r="H124" s="7"/>
+      <c r="L124" s="7"/>
+      <c r="O124" s="7"/>
+    </row>
+    <row r="125" spans="2:15">
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
-      <c r="K125" s="7"/>
-      <c r="N125" s="7"/>
-    </row>
-    <row r="126" spans="2:14">
-      <c r="E126" s="7"/>
+      <c r="H125" s="7"/>
+      <c r="L125" s="7"/>
+      <c r="O125" s="7"/>
+    </row>
+    <row r="126" spans="2:15">
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
-      <c r="K126" s="7"/>
-      <c r="N126" s="7"/>
-    </row>
-    <row r="127" spans="2:14">
+      <c r="H126" s="7"/>
+      <c r="L126" s="7"/>
+      <c r="O126" s="7"/>
+    </row>
+    <row r="127" spans="2:15">
       <c r="C127" s="31"/>
-      <c r="E127" s="7"/>
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
-      <c r="K127" s="7"/>
-      <c r="N127" s="7"/>
-    </row>
-    <row r="128" spans="2:14">
+      <c r="H127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="O127" s="7"/>
+    </row>
+    <row r="128" spans="2:15">
       <c r="C128" s="31"/>
-      <c r="E128" s="7"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
-      <c r="K128" s="7"/>
-      <c r="N128" s="7"/>
-    </row>
-    <row r="129" spans="2:14">
-      <c r="E129" s="7"/>
+      <c r="H128" s="7"/>
+      <c r="L128" s="7"/>
+      <c r="O128" s="7"/>
+    </row>
+    <row r="129" spans="2:15">
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
-      <c r="K129" s="7"/>
-      <c r="N129" s="7"/>
-    </row>
-    <row r="130" spans="2:14">
+      <c r="H129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="O129" s="7"/>
+    </row>
+    <row r="130" spans="2:15">
       <c r="B130" s="31"/>
       <c r="C130" s="31"/>
-      <c r="E130" s="7"/>
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
-      <c r="K130" s="7"/>
-      <c r="N130" s="7"/>
-    </row>
-    <row r="131" spans="2:14">
+      <c r="H130" s="7"/>
+      <c r="L130" s="7"/>
+      <c r="O130" s="7"/>
+    </row>
+    <row r="131" spans="2:15">
       <c r="B131" s="31"/>
       <c r="C131" s="31"/>
-      <c r="E131" s="7"/>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
-      <c r="K131" s="7"/>
-      <c r="N131" s="7"/>
-    </row>
-    <row r="132" spans="2:14">
+      <c r="H131" s="7"/>
+      <c r="L131" s="7"/>
+      <c r="O131" s="7"/>
+    </row>
+    <row r="132" spans="2:15">
       <c r="B132" s="31"/>
       <c r="C132" s="31"/>
-      <c r="E132" s="7"/>
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
-      <c r="K132" s="7"/>
-      <c r="N132" s="7"/>
-    </row>
-    <row r="133" spans="2:14">
-      <c r="E133" s="7"/>
+      <c r="H132" s="7"/>
+      <c r="L132" s="7"/>
+      <c r="O132" s="7"/>
+    </row>
+    <row r="133" spans="2:15">
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
-      <c r="K133" s="7"/>
-      <c r="M133" s="42"/>
-      <c r="N133" s="7"/>
-    </row>
-    <row r="134" spans="2:14">
-      <c r="E134" s="7"/>
+      <c r="H133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="N133" s="42"/>
+      <c r="O133" s="7"/>
+    </row>
+    <row r="134" spans="2:15">
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
-      <c r="K134" s="7"/>
-      <c r="M134" s="42"/>
-      <c r="N134" s="7"/>
-    </row>
-    <row r="135" spans="2:14">
-      <c r="E135" s="7"/>
+      <c r="H134" s="7"/>
+      <c r="L134" s="7"/>
+      <c r="N134" s="42"/>
+      <c r="O134" s="7"/>
+    </row>
+    <row r="135" spans="2:15">
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
-      <c r="K135" s="7"/>
-      <c r="M135" s="42"/>
-      <c r="N135" s="7"/>
-    </row>
-    <row r="136" spans="2:14">
-      <c r="E136" s="7"/>
+      <c r="H135" s="7"/>
+      <c r="L135" s="7"/>
+      <c r="N135" s="42"/>
+      <c r="O135" s="7"/>
+    </row>
+    <row r="136" spans="2:15">
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
-      <c r="K136" s="7"/>
-      <c r="M136" s="42"/>
-      <c r="N136" s="7"/>
-    </row>
-    <row r="137" spans="2:14">
-      <c r="E137" s="7"/>
+      <c r="H136" s="7"/>
+      <c r="L136" s="7"/>
+      <c r="N136" s="42"/>
+      <c r="O136" s="7"/>
+    </row>
+    <row r="137" spans="2:15">
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
-      <c r="K137" s="7"/>
-      <c r="M137" s="42"/>
-      <c r="N137" s="7"/>
-    </row>
-    <row r="138" spans="2:14">
-      <c r="E138" s="7"/>
+      <c r="H137" s="7"/>
+      <c r="L137" s="7"/>
+      <c r="N137" s="42"/>
+      <c r="O137" s="7"/>
+    </row>
+    <row r="138" spans="2:15">
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
-      <c r="K138" s="7"/>
-      <c r="N138" s="7"/>
-    </row>
-    <row r="139" spans="2:14">
-      <c r="E139" s="7"/>
+      <c r="H138" s="7"/>
+      <c r="L138" s="7"/>
+      <c r="O138" s="7"/>
+    </row>
+    <row r="139" spans="2:15">
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
-      <c r="K139" s="7"/>
-      <c r="N139" s="7"/>
-    </row>
-    <row r="140" spans="2:14">
-      <c r="E140" s="7"/>
+      <c r="H139" s="7"/>
+      <c r="L139" s="7"/>
+      <c r="O139" s="7"/>
+    </row>
+    <row r="140" spans="2:15">
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
-      <c r="K140" s="7"/>
-      <c r="N140" s="7"/>
-    </row>
-    <row r="141" spans="2:14">
-      <c r="E141" s="7"/>
+      <c r="H140" s="7"/>
+      <c r="L140" s="7"/>
+      <c r="O140" s="7"/>
+    </row>
+    <row r="141" spans="2:15">
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
-      <c r="K141" s="7"/>
-      <c r="N141" s="7"/>
-    </row>
-    <row r="142" spans="2:14">
-      <c r="E142" s="7"/>
+      <c r="H141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="O141" s="7"/>
+    </row>
+    <row r="142" spans="2:15">
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
-      <c r="K142" s="7"/>
-      <c r="N142" s="7"/>
-    </row>
-    <row r="143" spans="2:14">
-      <c r="E143" s="7"/>
+      <c r="H142" s="7"/>
+      <c r="L142" s="7"/>
+      <c r="O142" s="7"/>
+    </row>
+    <row r="143" spans="2:15">
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
-      <c r="K143" s="7"/>
-      <c r="N143" s="7"/>
-    </row>
-    <row r="144" spans="2:14">
-      <c r="E144" s="7"/>
+      <c r="H143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="O143" s="7"/>
+    </row>
+    <row r="144" spans="2:15">
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
-      <c r="K144" s="7"/>
-      <c r="N144" s="7"/>
-    </row>
-    <row r="145" spans="5:14">
-      <c r="E145" s="7"/>
+      <c r="H144" s="7"/>
+      <c r="L144" s="7"/>
+      <c r="O144" s="7"/>
+    </row>
+    <row r="145" spans="6:15">
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
-      <c r="K145" s="7"/>
-      <c r="N145" s="7"/>
-    </row>
-    <row r="146" spans="5:14">
-      <c r="E146" s="7"/>
+      <c r="H145" s="7"/>
+      <c r="L145" s="7"/>
+      <c r="O145" s="7"/>
+    </row>
+    <row r="146" spans="6:15">
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
-      <c r="K146" s="7"/>
-      <c r="N146" s="7"/>
-    </row>
-    <row r="147" spans="5:14">
-      <c r="E147" s="7"/>
+      <c r="H146" s="7"/>
+      <c r="L146" s="7"/>
+      <c r="O146" s="7"/>
+    </row>
+    <row r="147" spans="6:15">
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
-      <c r="K147" s="7"/>
-      <c r="N147" s="7"/>
-    </row>
-    <row r="148" spans="5:14">
-      <c r="E148" s="7"/>
+      <c r="H147" s="7"/>
+      <c r="L147" s="7"/>
+      <c r="O147" s="7"/>
+    </row>
+    <row r="148" spans="6:15">
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
-      <c r="K148" s="7"/>
-      <c r="N148" s="7"/>
-    </row>
-    <row r="149" spans="5:14">
-      <c r="E149" s="7"/>
+      <c r="H148" s="7"/>
+      <c r="L148" s="7"/>
+      <c r="O148" s="7"/>
+    </row>
+    <row r="149" spans="6:15">
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
-      <c r="K149" s="7"/>
-      <c r="N149" s="7"/>
-    </row>
-    <row r="150" spans="5:14">
-      <c r="E150" s="7"/>
+      <c r="H149" s="7"/>
+      <c r="L149" s="7"/>
+      <c r="O149" s="7"/>
+    </row>
+    <row r="150" spans="6:15">
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
-      <c r="K150" s="7"/>
-      <c r="N150" s="7"/>
-    </row>
-    <row r="151" spans="5:14">
-      <c r="E151" s="7"/>
+      <c r="H150" s="7"/>
+      <c r="L150" s="7"/>
+      <c r="O150" s="7"/>
+    </row>
+    <row r="151" spans="6:15">
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
-      <c r="K151" s="7"/>
-      <c r="N151" s="7"/>
-    </row>
-    <row r="152" spans="5:14">
-      <c r="E152" s="7"/>
+      <c r="H151" s="7"/>
+      <c r="L151" s="7"/>
+      <c r="O151" s="7"/>
+    </row>
+    <row r="152" spans="6:15">
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
-      <c r="K152" s="7"/>
-      <c r="N152" s="7"/>
-    </row>
-    <row r="153" spans="5:14">
-      <c r="E153" s="7"/>
+      <c r="H152" s="7"/>
+      <c r="L152" s="7"/>
+      <c r="O152" s="7"/>
+    </row>
+    <row r="153" spans="6:15">
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
-      <c r="K153" s="7"/>
-      <c r="N153" s="7"/>
-    </row>
-    <row r="154" spans="5:14">
-      <c r="E154" s="7"/>
+      <c r="H153" s="7"/>
+      <c r="L153" s="7"/>
+      <c r="O153" s="7"/>
+    </row>
+    <row r="154" spans="6:15">
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
-      <c r="K154" s="7"/>
-      <c r="N154" s="7"/>
-    </row>
-    <row r="155" spans="5:14">
-      <c r="E155" s="7"/>
+      <c r="H154" s="7"/>
+      <c r="L154" s="7"/>
+      <c r="O154" s="7"/>
+    </row>
+    <row r="155" spans="6:15">
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
-      <c r="K155" s="7"/>
-      <c r="L155" s="77"/>
-      <c r="N155" s="7"/>
-    </row>
-    <row r="156" spans="5:14">
-      <c r="E156" s="7"/>
+      <c r="H155" s="7"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="77"/>
+      <c r="O155" s="7"/>
+    </row>
+    <row r="156" spans="6:15">
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
-      <c r="K156" s="7"/>
-      <c r="L156" s="77"/>
-      <c r="N156" s="7"/>
-    </row>
-    <row r="157" spans="5:14">
-      <c r="E157" s="7"/>
+      <c r="H156" s="7"/>
+      <c r="L156" s="7"/>
+      <c r="M156" s="77"/>
+      <c r="O156" s="7"/>
+    </row>
+    <row r="157" spans="6:15">
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
-      <c r="K157" s="7"/>
-      <c r="L157" s="37"/>
-      <c r="N157" s="7"/>
-    </row>
-    <row r="158" spans="5:14">
-      <c r="E158" s="7"/>
+      <c r="H157" s="7"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="37"/>
+      <c r="O157" s="7"/>
+    </row>
+    <row r="158" spans="6:15">
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
-      <c r="K158" s="7"/>
-      <c r="L158" s="37"/>
-      <c r="N158" s="7"/>
-    </row>
-    <row r="159" spans="5:14">
-      <c r="E159" s="7"/>
+      <c r="H158" s="7"/>
+      <c r="L158" s="7"/>
+      <c r="M158" s="37"/>
+      <c r="O158" s="7"/>
+    </row>
+    <row r="159" spans="6:15">
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
-      <c r="K159" s="7"/>
-      <c r="L159" s="37"/>
-      <c r="N159" s="7"/>
-    </row>
-    <row r="160" spans="5:14">
-      <c r="E160" s="7"/>
+      <c r="H159" s="7"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="37"/>
+      <c r="O159" s="7"/>
+    </row>
+    <row r="160" spans="6:15">
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
-      <c r="K160" s="7"/>
-      <c r="L160" s="37"/>
-      <c r="N160" s="7"/>
-    </row>
-    <row r="161" spans="2:14">
-      <c r="E161" s="7"/>
+      <c r="H160" s="7"/>
+      <c r="L160" s="7"/>
+      <c r="M160" s="37"/>
+      <c r="O160" s="7"/>
+    </row>
+    <row r="161" spans="2:15">
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
-      <c r="K161" s="7"/>
-      <c r="L161" s="37"/>
-      <c r="N161" s="7"/>
-    </row>
-    <row r="162" spans="2:14">
-      <c r="E162" s="7"/>
+      <c r="H161" s="7"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="37"/>
+      <c r="O161" s="7"/>
+    </row>
+    <row r="162" spans="2:15">
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
-      <c r="K162" s="7"/>
-      <c r="L162" s="37"/>
-      <c r="N162" s="7"/>
-    </row>
-    <row r="163" spans="2:14">
-      <c r="E163" s="7"/>
+      <c r="H162" s="7"/>
+      <c r="L162" s="7"/>
+      <c r="M162" s="37"/>
+      <c r="O162" s="7"/>
+    </row>
+    <row r="163" spans="2:15">
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
-      <c r="K163" s="7"/>
-      <c r="L163" s="99"/>
-      <c r="N163" s="7"/>
-    </row>
-    <row r="164" spans="2:14">
-      <c r="E164" s="7"/>
+      <c r="H163" s="7"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="99"/>
+      <c r="O163" s="7"/>
+    </row>
+    <row r="164" spans="2:15">
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
-      <c r="K164" s="7"/>
-      <c r="N164" s="7"/>
-    </row>
-    <row r="165" spans="2:14">
+      <c r="H164" s="7"/>
+      <c r="L164" s="7"/>
+      <c r="O164" s="7"/>
+    </row>
+    <row r="165" spans="2:15">
       <c r="B165" s="105"/>
-      <c r="E165" s="7"/>
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
-      <c r="K165" s="7"/>
-      <c r="N165" s="7"/>
-    </row>
-    <row r="166" spans="2:14">
+      <c r="H165" s="7"/>
+      <c r="L165" s="7"/>
+      <c r="O165" s="7"/>
+    </row>
+    <row r="166" spans="2:15">
       <c r="B166" s="105"/>
-      <c r="E166" s="7"/>
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
-      <c r="K166" s="7"/>
-      <c r="N166" s="7"/>
-    </row>
-    <row r="167" spans="2:14">
+      <c r="H166" s="7"/>
+      <c r="L166" s="7"/>
+      <c r="O166" s="7"/>
+    </row>
+    <row r="167" spans="2:15">
       <c r="B167" s="105"/>
-      <c r="E167" s="7"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
-      <c r="K167" s="7"/>
-      <c r="N167" s="7"/>
-    </row>
-    <row r="168" spans="2:14">
+      <c r="H167" s="7"/>
+      <c r="L167" s="7"/>
+      <c r="O167" s="7"/>
+    </row>
+    <row r="168" spans="2:15">
       <c r="B168" s="105"/>
-      <c r="E168" s="7"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
-      <c r="K168" s="7"/>
-      <c r="N168" s="7"/>
-    </row>
-    <row r="169" spans="2:14">
+      <c r="H168" s="7"/>
+      <c r="L168" s="7"/>
+      <c r="O168" s="7"/>
+    </row>
+    <row r="169" spans="2:15">
       <c r="B169" s="105"/>
-      <c r="E169" s="7"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
-      <c r="K169" s="7"/>
-      <c r="N169" s="7"/>
-    </row>
-    <row r="170" spans="2:14">
+      <c r="H169" s="7"/>
+      <c r="L169" s="7"/>
+      <c r="O169" s="7"/>
+    </row>
+    <row r="170" spans="2:15">
       <c r="B170" s="105"/>
       <c r="C170" s="105"/>
       <c r="D170" s="105"/>
-      <c r="E170" s="7"/>
+      <c r="E170" s="105"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
-      <c r="K170" s="7"/>
-      <c r="N170" s="7"/>
-    </row>
-    <row r="171" spans="2:14">
+      <c r="H170" s="7"/>
+      <c r="L170" s="7"/>
+      <c r="O170" s="7"/>
+    </row>
+    <row r="171" spans="2:15">
       <c r="C171" s="31"/>
       <c r="D171" s="105"/>
-      <c r="E171" s="7"/>
+      <c r="E171" s="105"/>
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
-      <c r="K171" s="7"/>
-      <c r="N171" s="7"/>
-    </row>
-    <row r="172" spans="2:14">
+      <c r="H171" s="7"/>
+      <c r="L171" s="7"/>
+      <c r="O171" s="7"/>
+    </row>
+    <row r="172" spans="2:15">
       <c r="C172" s="31"/>
-      <c r="E172" s="7"/>
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
-      <c r="K172" s="7"/>
-      <c r="N172" s="7"/>
-    </row>
-    <row r="173" spans="2:14">
+      <c r="H172" s="7"/>
+      <c r="L172" s="7"/>
+      <c r="O172" s="7"/>
+    </row>
+    <row r="173" spans="2:15">
       <c r="D173" s="105"/>
-      <c r="E173" s="7"/>
+      <c r="E173" s="105"/>
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
-      <c r="K173" s="7"/>
-      <c r="N173" s="7"/>
-    </row>
-    <row r="174" spans="2:14">
+      <c r="H173" s="7"/>
+      <c r="L173" s="7"/>
+      <c r="O173" s="7"/>
+    </row>
+    <row r="174" spans="2:15">
       <c r="D174" s="105"/>
-      <c r="E174" s="7"/>
+      <c r="E174" s="105"/>
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
-      <c r="K174" s="7"/>
-      <c r="N174" s="7"/>
-    </row>
-    <row r="175" spans="2:14">
+      <c r="H174" s="7"/>
+      <c r="L174" s="7"/>
+      <c r="O174" s="7"/>
+    </row>
+    <row r="175" spans="2:15">
       <c r="D175" s="105"/>
-      <c r="E175" s="7"/>
+      <c r="E175" s="105"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
-      <c r="K175" s="7"/>
-      <c r="N175" s="7"/>
-    </row>
-    <row r="176" spans="2:14">
+      <c r="H175" s="7"/>
+      <c r="L175" s="7"/>
+      <c r="O175" s="7"/>
+    </row>
+    <row r="176" spans="2:15">
       <c r="D176" s="105"/>
-      <c r="E176" s="7"/>
+      <c r="E176" s="105"/>
       <c r="F176" s="7"/>
       <c r="G176" s="7"/>
-      <c r="K176" s="7"/>
-      <c r="N176" s="7"/>
-    </row>
-    <row r="177" spans="3:14">
+      <c r="H176" s="7"/>
+      <c r="L176" s="7"/>
+      <c r="O176" s="7"/>
+    </row>
+    <row r="177" spans="3:15">
       <c r="C177" s="31"/>
       <c r="D177" s="105"/>
-      <c r="E177" s="7"/>
+      <c r="E177" s="105"/>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
-      <c r="K177" s="7"/>
-      <c r="L177" s="77"/>
-      <c r="N177" s="7"/>
-    </row>
-    <row r="178" spans="3:14">
-      <c r="E178" s="7"/>
+      <c r="H177" s="7"/>
+      <c r="L177" s="7"/>
+      <c r="M177" s="77"/>
+      <c r="O177" s="7"/>
+    </row>
+    <row r="178" spans="3:15">
       <c r="F178" s="7"/>
       <c r="G178" s="7"/>
-      <c r="K178" s="7"/>
-      <c r="L178" s="77"/>
-      <c r="N178" s="7"/>
-    </row>
-    <row r="179" spans="3:14">
-      <c r="E179" s="7"/>
+      <c r="H178" s="7"/>
+      <c r="L178" s="7"/>
+      <c r="M178" s="77"/>
+      <c r="O178" s="7"/>
+    </row>
+    <row r="179" spans="3:15">
       <c r="F179" s="7"/>
       <c r="G179" s="7"/>
-      <c r="K179" s="7"/>
-      <c r="N179" s="7"/>
-    </row>
-    <row r="180" spans="3:14">
-      <c r="E180" s="7"/>
+      <c r="H179" s="7"/>
+      <c r="L179" s="7"/>
+      <c r="O179" s="7"/>
+    </row>
+    <row r="180" spans="3:15">
       <c r="F180" s="7"/>
       <c r="G180" s="7"/>
-      <c r="H180" s="225"/>
-      <c r="K180" s="7"/>
-      <c r="N180" s="7"/>
-    </row>
-    <row r="181" spans="3:14">
-      <c r="E181" s="7"/>
+      <c r="H180" s="7"/>
+      <c r="I180" s="225"/>
+      <c r="L180" s="7"/>
+      <c r="O180" s="7"/>
+    </row>
+    <row r="181" spans="3:15">
       <c r="F181" s="7"/>
       <c r="G181" s="7"/>
-      <c r="H181" s="31"/>
-      <c r="K181" s="7"/>
-      <c r="N181" s="7"/>
-    </row>
-    <row r="182" spans="3:14">
-      <c r="E182" s="7"/>
+      <c r="H181" s="7"/>
+      <c r="I181" s="31"/>
+      <c r="L181" s="7"/>
+      <c r="O181" s="7"/>
+    </row>
+    <row r="182" spans="3:15">
       <c r="F182" s="7"/>
       <c r="G182" s="7"/>
-      <c r="H182" s="31"/>
-      <c r="K182" s="7"/>
-      <c r="N182" s="7"/>
-    </row>
-    <row r="183" spans="3:14">
-      <c r="E183" s="7"/>
+      <c r="H182" s="7"/>
+      <c r="I182" s="31"/>
+      <c r="L182" s="7"/>
+      <c r="O182" s="7"/>
+    </row>
+    <row r="183" spans="3:15">
       <c r="F183" s="7"/>
       <c r="G183" s="7"/>
-      <c r="H183" s="31"/>
-      <c r="K183" s="7"/>
-      <c r="L183" s="77"/>
-      <c r="N183" s="7"/>
-    </row>
-    <row r="184" spans="3:14">
+      <c r="H183" s="7"/>
+      <c r="I183" s="31"/>
+      <c r="L183" s="7"/>
+      <c r="M183" s="77"/>
+      <c r="O183" s="7"/>
+    </row>
+    <row r="184" spans="3:15">
       <c r="C184" s="31"/>
-      <c r="E184" s="7"/>
       <c r="F184" s="7"/>
       <c r="G184" s="7"/>
-      <c r="H184" s="31"/>
-      <c r="K184" s="7"/>
-      <c r="L184" s="77"/>
-      <c r="N184" s="7"/>
-    </row>
-    <row r="185" spans="3:14">
-      <c r="E185" s="7"/>
+      <c r="H184" s="7"/>
+      <c r="I184" s="31"/>
+      <c r="L184" s="7"/>
+      <c r="M184" s="77"/>
+      <c r="O184" s="7"/>
+    </row>
+    <row r="185" spans="3:15">
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
-      <c r="H185" s="31"/>
-      <c r="K185" s="7"/>
-      <c r="L185" s="77"/>
-      <c r="N185" s="7"/>
-    </row>
-    <row r="186" spans="3:14">
+      <c r="H185" s="7"/>
+      <c r="I185" s="31"/>
+      <c r="L185" s="7"/>
+      <c r="M185" s="77"/>
+      <c r="O185" s="7"/>
+    </row>
+    <row r="186" spans="3:15">
       <c r="C186" s="31"/>
-      <c r="E186" s="7"/>
       <c r="F186" s="7"/>
       <c r="G186" s="7"/>
-      <c r="H186" s="31"/>
-      <c r="K186" s="7"/>
-      <c r="L186" s="77"/>
-      <c r="N186" s="7"/>
-    </row>
-    <row r="187" spans="3:14">
+      <c r="H186" s="7"/>
+      <c r="I186" s="31"/>
+      <c r="L186" s="7"/>
+      <c r="M186" s="77"/>
+      <c r="O186" s="7"/>
+    </row>
+    <row r="187" spans="3:15">
       <c r="C187" s="31"/>
-      <c r="E187" s="7"/>
       <c r="F187" s="7"/>
       <c r="G187" s="7"/>
-      <c r="H187" s="31"/>
-      <c r="K187" s="7"/>
-      <c r="L187" s="77"/>
-      <c r="N187" s="7"/>
-    </row>
-    <row r="188" spans="3:14">
+      <c r="H187" s="7"/>
+      <c r="I187" s="31"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="77"/>
+      <c r="O187" s="7"/>
+    </row>
+    <row r="188" spans="3:15">
       <c r="C188" s="31"/>
-      <c r="E188" s="7"/>
       <c r="F188" s="7"/>
       <c r="G188" s="7"/>
-      <c r="H188" s="31"/>
-      <c r="K188" s="7"/>
-      <c r="L188" s="77"/>
-      <c r="N188" s="7"/>
-    </row>
-    <row r="189" spans="3:14">
+      <c r="H188" s="7"/>
+      <c r="I188" s="31"/>
+      <c r="L188" s="7"/>
+      <c r="M188" s="77"/>
+      <c r="O188" s="7"/>
+    </row>
+    <row r="189" spans="3:15">
       <c r="C189" s="31"/>
-      <c r="E189" s="7"/>
       <c r="F189" s="7"/>
       <c r="G189" s="7"/>
-      <c r="H189" s="31"/>
+      <c r="H189" s="7"/>
       <c r="I189" s="31"/>
-      <c r="K189" s="7"/>
-      <c r="L189" s="77"/>
-      <c r="N189" s="7"/>
-    </row>
-    <row r="190" spans="3:14">
+      <c r="J189" s="31"/>
+      <c r="L189" s="7"/>
+      <c r="M189" s="77"/>
+      <c r="O189" s="7"/>
+    </row>
+    <row r="190" spans="3:15">
       <c r="C190" s="31"/>
-      <c r="E190" s="7"/>
       <c r="F190" s="7"/>
       <c r="G190" s="7"/>
-      <c r="I190" s="31"/>
-      <c r="K190" s="7"/>
-      <c r="L190" s="77"/>
-      <c r="N190" s="7"/>
-    </row>
-    <row r="191" spans="3:14">
-      <c r="E191" s="7"/>
+      <c r="H190" s="7"/>
+      <c r="J190" s="31"/>
+      <c r="L190" s="7"/>
+      <c r="M190" s="77"/>
+      <c r="O190" s="7"/>
+    </row>
+    <row r="191" spans="3:15">
       <c r="F191" s="7"/>
       <c r="G191" s="7"/>
-      <c r="K191" s="7"/>
-      <c r="L191" s="77"/>
-      <c r="N191" s="7"/>
-    </row>
-    <row r="192" spans="3:14">
+      <c r="H191" s="7"/>
+      <c r="L191" s="7"/>
+      <c r="M191" s="77"/>
+      <c r="O191" s="7"/>
+    </row>
+    <row r="192" spans="3:15">
       <c r="C192" s="31"/>
-      <c r="E192" s="7"/>
       <c r="F192" s="7"/>
       <c r="G192" s="7"/>
-      <c r="K192" s="7"/>
-      <c r="L192" s="77"/>
-      <c r="N192" s="7"/>
-    </row>
-    <row r="193" spans="2:14">
+      <c r="H192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="77"/>
+      <c r="O192" s="7"/>
+    </row>
+    <row r="193" spans="2:15">
       <c r="D193" s="105"/>
-      <c r="E193" s="7"/>
+      <c r="E193" s="105"/>
       <c r="F193" s="7"/>
       <c r="G193" s="7"/>
-      <c r="K193" s="7"/>
-      <c r="N193" s="7"/>
-    </row>
-    <row r="194" spans="2:14">
+      <c r="H193" s="7"/>
+      <c r="L193" s="7"/>
+      <c r="O193" s="7"/>
+    </row>
+    <row r="194" spans="2:15">
       <c r="D194" s="105"/>
-      <c r="E194" s="7"/>
+      <c r="E194" s="105"/>
       <c r="F194" s="7"/>
       <c r="G194" s="7"/>
-      <c r="K194" s="7"/>
-      <c r="N194" s="7"/>
-    </row>
-    <row r="195" spans="2:14">
+      <c r="H194" s="7"/>
+      <c r="L194" s="7"/>
+      <c r="O194" s="7"/>
+    </row>
+    <row r="195" spans="2:15">
       <c r="D195" s="105"/>
-      <c r="E195" s="7"/>
+      <c r="E195" s="105"/>
       <c r="F195" s="7"/>
       <c r="G195" s="7"/>
-      <c r="K195" s="7"/>
-      <c r="N195" s="7"/>
-    </row>
-    <row r="196" spans="2:14">
+      <c r="H195" s="7"/>
+      <c r="L195" s="7"/>
+      <c r="O195" s="7"/>
+    </row>
+    <row r="196" spans="2:15">
       <c r="D196" s="105"/>
-      <c r="E196" s="7"/>
+      <c r="E196" s="105"/>
       <c r="F196" s="7"/>
       <c r="G196" s="7"/>
-      <c r="K196" s="7"/>
-      <c r="N196" s="7"/>
-    </row>
-    <row r="197" spans="2:14">
+      <c r="H196" s="7"/>
+      <c r="L196" s="7"/>
+      <c r="O196" s="7"/>
+    </row>
+    <row r="197" spans="2:15">
       <c r="D197" s="105"/>
-      <c r="E197" s="7"/>
+      <c r="E197" s="105"/>
       <c r="F197" s="7"/>
       <c r="G197" s="7"/>
-      <c r="K197" s="7"/>
-      <c r="L197" s="77"/>
-      <c r="N197" s="7"/>
-    </row>
-    <row r="198" spans="2:14">
+      <c r="H197" s="7"/>
+      <c r="L197" s="7"/>
+      <c r="M197" s="77"/>
+      <c r="O197" s="7"/>
+    </row>
+    <row r="198" spans="2:15">
       <c r="D198" s="105"/>
-      <c r="E198" s="7"/>
+      <c r="E198" s="105"/>
       <c r="F198" s="7"/>
       <c r="G198" s="7"/>
-      <c r="K198" s="7"/>
-      <c r="N198" s="7"/>
-    </row>
-    <row r="199" spans="2:14">
+      <c r="H198" s="7"/>
+      <c r="L198" s="7"/>
+      <c r="O198" s="7"/>
+    </row>
+    <row r="199" spans="2:15">
       <c r="D199" s="105"/>
-      <c r="E199" s="7"/>
+      <c r="E199" s="105"/>
       <c r="F199" s="7"/>
       <c r="G199" s="7"/>
-      <c r="K199" s="7"/>
-      <c r="L199" s="77"/>
-      <c r="N199" s="7"/>
-    </row>
-    <row r="200" spans="2:14">
+      <c r="H199" s="7"/>
+      <c r="L199" s="7"/>
+      <c r="M199" s="77"/>
+      <c r="O199" s="7"/>
+    </row>
+    <row r="200" spans="2:15">
       <c r="B200" s="31"/>
       <c r="C200" s="31"/>
-      <c r="E200" s="7"/>
       <c r="F200" s="7"/>
       <c r="G200" s="7"/>
-      <c r="K200" s="7"/>
-      <c r="N200" s="7"/>
-    </row>
-    <row r="201" spans="2:14">
+      <c r="H200" s="7"/>
+      <c r="L200" s="7"/>
+      <c r="O200" s="7"/>
+    </row>
+    <row r="201" spans="2:15">
       <c r="B201" s="31"/>
       <c r="C201" s="31"/>
-      <c r="E201" s="7"/>
       <c r="F201" s="7"/>
       <c r="G201" s="7"/>
-      <c r="K201" s="7"/>
-      <c r="N201" s="7"/>
-    </row>
-    <row r="202" spans="2:14">
+      <c r="H201" s="7"/>
+      <c r="L201" s="7"/>
+      <c r="O201" s="7"/>
+    </row>
+    <row r="202" spans="2:15">
       <c r="B202" s="31"/>
       <c r="C202" s="31"/>
-      <c r="E202" s="7"/>
       <c r="F202" s="7"/>
       <c r="G202" s="7"/>
-      <c r="K202" s="7"/>
-      <c r="N202" s="7"/>
-    </row>
-    <row r="203" spans="2:14">
+      <c r="H202" s="7"/>
+      <c r="L202" s="7"/>
+      <c r="O202" s="7"/>
+    </row>
+    <row r="203" spans="2:15">
       <c r="B203" s="31"/>
       <c r="C203" s="31"/>
-      <c r="E203" s="7"/>
       <c r="F203" s="7"/>
       <c r="G203" s="7"/>
-      <c r="K203" s="7"/>
-      <c r="N203" s="7"/>
-    </row>
-    <row r="204" spans="2:14">
-      <c r="E204" s="7"/>
+      <c r="H203" s="7"/>
+      <c r="L203" s="7"/>
+      <c r="O203" s="7"/>
+    </row>
+    <row r="204" spans="2:15">
       <c r="F204" s="7"/>
       <c r="G204" s="7"/>
-      <c r="K204" s="7"/>
-      <c r="N204" s="7"/>
-    </row>
-    <row r="205" spans="2:14">
-      <c r="E205" s="7"/>
+      <c r="H204" s="7"/>
+      <c r="L204" s="7"/>
+      <c r="O204" s="7"/>
+    </row>
+    <row r="205" spans="2:15">
       <c r="F205" s="7"/>
       <c r="G205" s="7"/>
-      <c r="K205" s="7"/>
-      <c r="N205" s="7"/>
-    </row>
-    <row r="206" spans="2:14">
-      <c r="E206" s="7"/>
+      <c r="H205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="O205" s="7"/>
+    </row>
+    <row r="206" spans="2:15">
       <c r="F206" s="7"/>
       <c r="G206" s="7"/>
-      <c r="K206" s="7"/>
-      <c r="N206" s="7"/>
-    </row>
-    <row r="207" spans="2:14">
-      <c r="E207" s="7"/>
+      <c r="H206" s="7"/>
+      <c r="L206" s="7"/>
+      <c r="O206" s="7"/>
+    </row>
+    <row r="207" spans="2:15">
       <c r="F207" s="7"/>
       <c r="G207" s="7"/>
-      <c r="K207" s="7"/>
-      <c r="N207" s="7"/>
-    </row>
-    <row r="208" spans="2:14">
-      <c r="E208" s="7"/>
+      <c r="H207" s="7"/>
+      <c r="L207" s="7"/>
+      <c r="O207" s="7"/>
+    </row>
+    <row r="208" spans="2:15">
       <c r="F208" s="7"/>
       <c r="G208" s="7"/>
-      <c r="K208" s="7"/>
-      <c r="N208" s="7"/>
-    </row>
-    <row r="209" spans="3:14">
-      <c r="E209" s="7"/>
+      <c r="H208" s="7"/>
+      <c r="L208" s="7"/>
+      <c r="O208" s="7"/>
+    </row>
+    <row r="209" spans="3:15">
       <c r="F209" s="7"/>
       <c r="G209" s="7"/>
-      <c r="H209" s="31"/>
+      <c r="H209" s="7"/>
       <c r="I209" s="31"/>
       <c r="J209" s="31"/>
-      <c r="K209" s="7"/>
-      <c r="N209" s="7"/>
-    </row>
-    <row r="210" spans="3:14">
-      <c r="E210" s="7"/>
+      <c r="K209" s="31"/>
+      <c r="L209" s="7"/>
+      <c r="O209" s="7"/>
+    </row>
+    <row r="210" spans="3:15">
       <c r="F210" s="7"/>
       <c r="G210" s="7"/>
-      <c r="H210" s="31"/>
+      <c r="H210" s="7"/>
       <c r="I210" s="31"/>
       <c r="J210" s="31"/>
-      <c r="K210" s="7"/>
-      <c r="N210" s="7"/>
-    </row>
-    <row r="211" spans="3:14">
-      <c r="E211" s="7"/>
+      <c r="K210" s="31"/>
+      <c r="L210" s="7"/>
+      <c r="O210" s="7"/>
+    </row>
+    <row r="211" spans="3:15">
       <c r="F211" s="7"/>
       <c r="G211" s="7"/>
-      <c r="H211" s="31"/>
+      <c r="H211" s="7"/>
       <c r="I211" s="31"/>
       <c r="J211" s="31"/>
-      <c r="K211" s="7"/>
-      <c r="N211" s="7"/>
-    </row>
-    <row r="212" spans="3:14">
-      <c r="E212" s="7"/>
+      <c r="K211" s="31"/>
+      <c r="L211" s="7"/>
+      <c r="O211" s="7"/>
+    </row>
+    <row r="212" spans="3:15">
       <c r="F212" s="7"/>
       <c r="G212" s="7"/>
-      <c r="H212" s="31"/>
+      <c r="H212" s="7"/>
       <c r="I212" s="31"/>
       <c r="J212" s="31"/>
-      <c r="K212" s="7"/>
-      <c r="N212" s="7"/>
-    </row>
-    <row r="213" spans="3:14">
+      <c r="K212" s="31"/>
+      <c r="L212" s="7"/>
+      <c r="O212" s="7"/>
+    </row>
+    <row r="213" spans="3:15">
       <c r="C213" s="31"/>
-      <c r="E213" s="7"/>
       <c r="F213" s="7"/>
       <c r="G213" s="7"/>
-      <c r="H213" s="31"/>
+      <c r="H213" s="7"/>
       <c r="I213" s="31"/>
       <c r="J213" s="31"/>
-      <c r="K213" s="7"/>
-      <c r="N213" s="7"/>
-    </row>
-    <row r="214" spans="3:14">
+      <c r="K213" s="31"/>
+      <c r="L213" s="7"/>
+      <c r="O213" s="7"/>
+    </row>
+    <row r="214" spans="3:15">
       <c r="C214" s="31"/>
-      <c r="E214" s="7"/>
       <c r="F214" s="7"/>
       <c r="G214" s="7"/>
-      <c r="H214" s="31"/>
+      <c r="H214" s="7"/>
       <c r="I214" s="31"/>
       <c r="J214" s="31"/>
-      <c r="K214" s="7"/>
-      <c r="N214" s="7"/>
-    </row>
-    <row r="215" spans="3:14">
+      <c r="K214" s="31"/>
+      <c r="L214" s="7"/>
+      <c r="O214" s="7"/>
+    </row>
+    <row r="215" spans="3:15">
       <c r="C215" s="31"/>
-      <c r="E215" s="7"/>
       <c r="F215" s="7"/>
       <c r="G215" s="7"/>
-      <c r="H215" s="31"/>
+      <c r="H215" s="7"/>
       <c r="I215" s="31"/>
       <c r="J215" s="31"/>
-      <c r="K215" s="7"/>
-      <c r="N215" s="7"/>
-    </row>
-    <row r="216" spans="3:14">
+      <c r="K215" s="31"/>
+      <c r="L215" s="7"/>
+      <c r="O215" s="7"/>
+    </row>
+    <row r="216" spans="3:15">
       <c r="C216" s="31"/>
-      <c r="E216" s="7"/>
       <c r="F216" s="7"/>
       <c r="G216" s="7"/>
-      <c r="H216" s="31"/>
+      <c r="H216" s="7"/>
       <c r="I216" s="31"/>
       <c r="J216" s="31"/>
-      <c r="K216" s="7"/>
-      <c r="N216" s="7"/>
-    </row>
-    <row r="217" spans="3:14">
-      <c r="E217" s="7"/>
+      <c r="K216" s="31"/>
+      <c r="L216" s="7"/>
+      <c r="O216" s="7"/>
+    </row>
+    <row r="217" spans="3:15">
       <c r="F217" s="7"/>
       <c r="G217" s="7"/>
-      <c r="K217" s="7"/>
-      <c r="L217" s="77"/>
-      <c r="N217" s="7"/>
+      <c r="H217" s="7"/>
+      <c r="L217" s="7"/>
+      <c r="M217" s="77"/>
+      <c r="O217" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:P217" xr:uid="{CC7C3B69-9998-624E-A306-40140D5C2988}"/>
+  <autoFilter ref="A3:Q217" xr:uid="{CC7C3B69-9998-624E-A306-40140D5C2988}"/>
   <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Feature flag case file view
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-englandwales\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC1D55-4FB8-444B-9E45-F7CC0D4BE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF576B99-775F-47A7-8355-F168B63163BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1470" windowWidth="36660" windowHeight="19395" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1905" yWindow="-18165" windowWidth="28800" windowHeight="15315" tabRatio="500" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -22,47 +22,48 @@
     <sheet name="CaseEvent" sheetId="23" r:id="rId7"/>
     <sheet name="CaseEventToFields" sheetId="24" r:id="rId8"/>
     <sheet name="CaseField" sheetId="25" r:id="rId9"/>
-    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId10"/>
-    <sheet name="ComplexTypes" sheetId="26" r:id="rId11"/>
-    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId12"/>
-    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId13"/>
-    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId14"/>
-    <sheet name="SearchInputFields" sheetId="13" r:id="rId15"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId17"/>
-    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId18"/>
-    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
-    <sheet name="CaseRoles" sheetId="31" r:id="rId21"/>
-    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId22"/>
-    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId23"/>
-    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId24"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId25"/>
-    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId26"/>
+    <sheet name="Categories" sheetId="39" r:id="rId10"/>
+    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId11"/>
+    <sheet name="ComplexTypes" sheetId="26" r:id="rId12"/>
+    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId13"/>
+    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId14"/>
+    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId15"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId16"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId17"/>
+    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId18"/>
+    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId19"/>
+    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId20"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId21"/>
+    <sheet name="CaseRoles" sheetId="31" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId23"/>
+    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId24"/>
+    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId25"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId26"/>
+    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId27"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$Q$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CaseRoles!$A$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseType!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseTypeTab!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Jurisdiction!$A$3:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">State!$A$3:$F$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">UserProfile!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">UserProfile!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1152">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3595,6 +3596,35 @@
   </si>
   <si>
     <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Unique ID that identifies the category
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label that gets displayed in the UI. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Specifies the display order for the category.</t>
+  </si>
+  <si>
+    <t>Identifies the parent category id for a sub-category.</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>CategoryLabel</t>
+  </si>
+  <si>
+    <t>ParentCategoryID</t>
+  </si>
+  <si>
+    <t>ID that identifies the document category
+MaxLength: 70</t>
   </si>
 </sst>
 </file>
@@ -4350,7 +4380,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4890,6 +4920,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -5371,14 +5404,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="17.5">
       <c r="A1" s="267" t="s">
         <v>1137</v>
       </c>
@@ -5386,7 +5419,7 @@
       <c r="C1" s="271"/>
       <c r="D1" s="270"/>
     </row>
-    <row r="2" spans="1:4" ht="102.75">
+    <row r="2" spans="1:4" ht="88.5">
       <c r="A2" s="269" t="s">
         <v>1133</v>
       </c>
@@ -5424,6 +5457,65 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5E47D-EB2A-4FD0-8353-2773316B4A69}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="12.5"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="65">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13">
+      <c r="A3" s="276" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C3" s="276" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243AEE7-DA61-4CDF-84FC-CA2502F211A6}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -5431,20 +5523,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="239"/>
-    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="239"/>
+    <col min="3" max="3" width="54.7265625" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.7265625" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.26953125" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" style="239"/>
-    <col min="1026" max="16384" width="10.85546875" style="238"/>
+    <col min="10" max="10" width="43.7265625" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.81640625" style="239"/>
+    <col min="1026" max="16384" width="10.81640625" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -5470,7 +5562,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="63.75">
+    <row r="2" spans="1:13" ht="52">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -5505,7 +5597,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75">
+    <row r="3" spans="1:13" ht="15.5">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -5557,7 +5649,7 @@
       <c r="L4" s="240"/>
       <c r="M4" s="240"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="13">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="242"/>
@@ -5572,7 +5664,7 @@
       <c r="L5" s="240"/>
       <c r="M5" s="240"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="13">
       <c r="A6" s="241"/>
       <c r="B6" s="241"/>
       <c r="D6" s="240"/>
@@ -5586,7 +5678,7 @@
       <c r="L6" s="240"/>
       <c r="M6" s="240"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="13">
       <c r="A7" s="241"/>
       <c r="B7" s="241"/>
       <c r="D7" s="240"/>
@@ -5622,34 +5714,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC74BE-16DE-BC4E-A66A-E3A520C8B91F}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:N563"/>
+  <dimension ref="A1:O563"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A328" sqref="A328:XFD563"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="53.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" customWidth="1"/>
+    <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="30" t="s">
         <v>192</v>
       </c>
@@ -5672,7 +5765,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:14" ht="54.95" customHeight="1">
+    <row r="2" spans="1:15" ht="55" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -5711,8 +5804,11 @@
       <c r="N2" s="24" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="51">
+      <c r="O2" s="22" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="52">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -5755,8 +5851,11 @@
       <c r="N3" s="26" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="26" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1036</v>
       </c>
@@ -5776,7 +5875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>1036</v>
       </c>
@@ -5799,7 +5898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>1036</v>
       </c>
@@ -5816,7 +5915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1036</v>
       </c>
@@ -5833,7 +5932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>1036</v>
       </c>
@@ -5850,7 +5949,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15" ht="13">
       <c r="A9" s="121" t="s">
         <v>1036</v>
       </c>
@@ -5873,7 +5972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>1037</v>
       </c>
@@ -5890,7 +5989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>1037</v>
       </c>
@@ -5907,7 +6006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>1037</v>
       </c>
@@ -5924,7 +6023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>1037</v>
       </c>
@@ -5941,7 +6040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15" ht="13">
       <c r="A14" s="121" t="s">
         <v>1037</v>
       </c>
@@ -5964,7 +6063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>1062</v>
       </c>
@@ -5981,7 +6080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="105" t="s">
         <v>1062</v>
       </c>
@@ -6106,7 +6205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="13">
       <c r="A22" s="121" t="s">
         <v>1062</v>
       </c>
@@ -6151,7 +6250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="13">
       <c r="A24" s="121" t="s">
         <v>1063</v>
       </c>
@@ -6192,7 +6291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="13">
       <c r="A26" s="121" t="s">
         <v>1023</v>
       </c>
@@ -6400,7 +6499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" ht="13">
       <c r="A36" s="121" t="s">
         <v>1018</v>
       </c>
@@ -6755,7 +6854,7 @@
       <c r="J50" s="43"/>
       <c r="K50" s="43"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" ht="13">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -6782,7 +6881,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" ht="13">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -6809,7 +6908,7 @@
       <c r="J52" s="43"/>
       <c r="K52" s="43"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" ht="13">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -7207,7 +7306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" ht="13">
       <c r="A69" s="121" t="s">
         <v>80</v>
       </c>
@@ -7228,7 +7327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.1" customHeight="1">
+    <row r="70" spans="1:9" ht="14.15" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -7251,7 +7350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
+    <row r="71" spans="1:9" ht="10" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -7457,7 +7556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" ht="13">
       <c r="A81" s="121" t="s">
         <v>1020</v>
       </c>
@@ -7548,7 +7647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" ht="13">
       <c r="A85" s="121" t="s">
         <v>1056</v>
       </c>
@@ -7618,7 +7717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" ht="13">
       <c r="A88" s="121" t="s">
         <v>1040</v>
       </c>
@@ -7679,7 +7778,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" ht="13">
       <c r="A91" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7700,7 +7799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" ht="13">
       <c r="A92" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7721,7 +7820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" ht="13">
       <c r="A93" t="s">
         <v>1014</v>
       </c>
@@ -7750,7 +7849,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" ht="13">
       <c r="A94" t="s">
         <v>1014</v>
       </c>
@@ -7776,7 +7875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" ht="13">
       <c r="A95" t="s">
         <v>1014</v>
       </c>
@@ -7796,7 +7895,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" ht="13">
       <c r="A96" t="s">
         <v>1014</v>
       </c>
@@ -7822,7 +7921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:15" ht="13">
       <c r="A97" t="s">
         <v>1014</v>
       </c>
@@ -7842,7 +7941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:15" ht="13">
       <c r="A98" t="s">
         <v>1014</v>
       </c>
@@ -7864,7 +7963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>1014</v>
       </c>
@@ -7883,7 +7982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>1014</v>
       </c>
@@ -7902,7 +8001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>1014</v>
       </c>
@@ -7921,7 +8020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>1014</v>
       </c>
@@ -7944,7 +8043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>1014</v>
       </c>
@@ -7963,7 +8062,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>1014</v>
       </c>
@@ -7986,7 +8085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>1014</v>
       </c>
@@ -8005,7 +8104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>1014</v>
       </c>
@@ -8028,7 +8127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>1014</v>
       </c>
@@ -8051,7 +8150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:15" ht="13">
       <c r="A108" t="s">
         <v>1014</v>
       </c>
@@ -8076,8 +8175,9 @@
       <c r="I108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="O108" s="233"/>
+    </row>
+    <row r="109" spans="1:15" ht="13">
       <c r="A109" t="s">
         <v>1014</v>
       </c>
@@ -8099,7 +8199,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>1014</v>
       </c>
@@ -8118,7 +8218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:15" ht="13">
       <c r="A111" s="121" t="s">
         <v>1014</v>
       </c>
@@ -8138,7 +8238,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>1003</v>
       </c>
@@ -8304,7 +8404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" ht="13">
       <c r="A119" s="121" t="s">
         <v>1003</v>
       </c>
@@ -8408,7 +8508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" ht="13">
       <c r="A124" s="121" t="s">
         <v>998</v>
       </c>
@@ -8599,7 +8699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" ht="13">
       <c r="A133" s="121" t="s">
         <v>1064</v>
       </c>
@@ -8680,7 +8780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" ht="13">
       <c r="A137" s="121" t="s">
         <v>883</v>
       </c>
@@ -8881,7 +8981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:14" ht="13">
       <c r="A147" s="121" t="s">
         <v>884</v>
       </c>
@@ -8965,7 +9065,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:14" ht="13">
       <c r="A151" s="121" t="s">
         <v>885</v>
       </c>
@@ -8986,7 +9086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:14" ht="13">
       <c r="A152" s="121" t="s">
         <v>1076</v>
       </c>
@@ -9007,7 +9107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:14" ht="13">
       <c r="A153" s="121" t="s">
         <v>1066</v>
       </c>
@@ -9071,7 +9171,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:14" ht="13">
       <c r="A156" s="121" t="s">
         <v>936</v>
       </c>
@@ -9139,7 +9239,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:14" ht="13">
       <c r="A159" s="121" t="s">
         <v>946</v>
       </c>
@@ -9184,7 +9284,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" ht="13">
       <c r="A161" s="121" t="s">
         <v>953</v>
       </c>
@@ -9300,7 +9400,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" ht="13">
       <c r="A166" s="121" t="s">
         <v>956</v>
       </c>
@@ -9425,7 +9525,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" ht="13">
       <c r="A172" s="121" t="s">
         <v>986</v>
       </c>
@@ -11125,7 +11225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" ht="13">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -11151,7 +11251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" ht="13">
       <c r="A244" s="121" t="s">
         <v>0</v>
       </c>
@@ -11198,7 +11298,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" ht="13">
       <c r="A246" t="s">
         <v>861</v>
       </c>
@@ -11225,7 +11325,7 @@
       <c r="J246" s="43"/>
       <c r="K246" s="43"/>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" ht="13">
       <c r="A247" t="s">
         <v>861</v>
       </c>
@@ -11252,7 +11352,7 @@
       <c r="J247" s="43"/>
       <c r="K247" s="43"/>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" ht="13">
       <c r="A248" t="s">
         <v>861</v>
       </c>
@@ -11281,7 +11381,7 @@
       <c r="J248" s="43"/>
       <c r="K248" s="43"/>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" ht="13">
       <c r="A249" t="s">
         <v>861</v>
       </c>
@@ -11310,7 +11410,7 @@
       <c r="J249" s="43"/>
       <c r="K249" s="43"/>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" ht="13">
       <c r="A250" s="121" t="s">
         <v>861</v>
       </c>
@@ -11664,7 +11764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:14">
+    <row r="265" spans="1:14" ht="13">
       <c r="A265" s="121" t="s">
         <v>1034</v>
       </c>
@@ -11928,7 +12028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:14">
+    <row r="275" spans="1:14" ht="13">
       <c r="A275" s="121" t="s">
         <v>1033</v>
       </c>
@@ -12020,7 +12120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13.5">
+    <row r="279" spans="1:14" ht="13">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -12192,7 +12292,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:14">
+    <row r="287" spans="1:14" ht="13">
       <c r="A287" t="s">
         <v>102</v>
       </c>
@@ -12215,7 +12315,7 @@
       <c r="J287" s="43"/>
       <c r="K287" s="43"/>
     </row>
-    <row r="288" spans="1:14">
+    <row r="288" spans="1:14" ht="13">
       <c r="A288" s="121" t="s">
         <v>102</v>
       </c>
@@ -12775,7 +12875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" ht="13">
       <c r="A309" s="121" t="s">
         <v>103</v>
       </c>
@@ -12800,7 +12900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" ht="13">
       <c r="A310" s="121" t="s">
         <v>103</v>
       </c>
@@ -13290,7 +13390,7 @@
       <c r="G329" s="31"/>
       <c r="H329" s="31"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" ht="13">
       <c r="A330" s="121"/>
       <c r="B330" s="121"/>
       <c r="C330" s="121"/>
@@ -13301,7 +13401,7 @@
       <c r="H330" s="205"/>
       <c r="I330" s="124"/>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" ht="13">
       <c r="A331" s="121"/>
       <c r="B331" s="121"/>
       <c r="C331" s="121"/>
@@ -13317,7 +13417,7 @@
       <c r="G332" s="31"/>
       <c r="H332" s="31"/>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" ht="13">
       <c r="A333" s="121"/>
       <c r="B333" s="121"/>
       <c r="C333" s="121"/>
@@ -13345,7 +13445,7 @@
       <c r="G336" s="31"/>
       <c r="H336" s="31"/>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" ht="13">
       <c r="A337" s="121"/>
       <c r="B337" s="121"/>
       <c r="C337" s="121"/>
@@ -13379,7 +13479,7 @@
       <c r="G341" s="31"/>
       <c r="H341" s="31"/>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" ht="13">
       <c r="A342" s="121"/>
       <c r="B342" s="121"/>
       <c r="C342" s="121"/>
@@ -13390,7 +13490,7 @@
       <c r="H342" s="205"/>
       <c r="I342" s="124"/>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" ht="13">
       <c r="A343" s="105"/>
       <c r="B343" s="121"/>
       <c r="E343" s="117"/>
@@ -13398,7 +13498,7 @@
       <c r="G343" s="31"/>
       <c r="H343" s="31"/>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" ht="13">
       <c r="A344" s="105"/>
       <c r="B344" s="121"/>
       <c r="E344" s="117"/>
@@ -13406,28 +13506,28 @@
       <c r="G344" s="31"/>
       <c r="H344" s="31"/>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" ht="13">
       <c r="A345" s="105"/>
       <c r="E345" s="117"/>
       <c r="F345" s="31"/>
       <c r="G345" s="31"/>
       <c r="H345" s="31"/>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" ht="13">
       <c r="A346" s="105"/>
       <c r="E346" s="117"/>
       <c r="F346" s="31"/>
       <c r="G346" s="31"/>
       <c r="H346" s="31"/>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" ht="13">
       <c r="A347" s="105"/>
       <c r="E347" s="117"/>
       <c r="F347" s="31"/>
       <c r="G347" s="31"/>
       <c r="H347" s="31"/>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" ht="13">
       <c r="A348" s="121"/>
       <c r="B348" s="121"/>
       <c r="C348" s="121"/>
@@ -14279,7 +14379,7 @@
       <c r="G474" s="31"/>
       <c r="H474" s="31"/>
     </row>
-    <row r="475" spans="1:9">
+    <row r="475" spans="1:9" ht="13">
       <c r="A475" s="121"/>
       <c r="B475" s="121"/>
       <c r="C475" s="121"/>
@@ -14290,7 +14390,7 @@
       <c r="H475" s="205"/>
       <c r="I475" s="124"/>
     </row>
-    <row r="476" spans="1:9">
+    <row r="476" spans="1:9" ht="13">
       <c r="A476" s="121"/>
       <c r="B476" s="121"/>
       <c r="C476" s="121"/>
@@ -14301,55 +14401,55 @@
       <c r="H476" s="31"/>
       <c r="I476" s="124"/>
     </row>
-    <row r="477" spans="1:9">
+    <row r="477" spans="1:9" ht="13">
       <c r="A477" s="105"/>
       <c r="E477" s="117"/>
       <c r="F477" s="105"/>
       <c r="G477" s="31"/>
     </row>
-    <row r="478" spans="1:9">
+    <row r="478" spans="1:9" ht="13">
       <c r="A478" s="105"/>
       <c r="E478" s="117"/>
       <c r="F478" s="105"/>
       <c r="G478" s="31"/>
     </row>
-    <row r="479" spans="1:9">
+    <row r="479" spans="1:9" ht="13">
       <c r="A479" s="105"/>
       <c r="E479" s="117"/>
       <c r="F479" s="105"/>
       <c r="G479" s="31"/>
     </row>
-    <row r="480" spans="1:9">
+    <row r="480" spans="1:9" ht="13">
       <c r="A480" s="105"/>
       <c r="E480" s="117"/>
       <c r="F480" s="105"/>
       <c r="G480" s="31"/>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" ht="13">
       <c r="A481" s="105"/>
       <c r="E481" s="117"/>
       <c r="F481" s="105"/>
       <c r="G481" s="31"/>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" ht="13">
       <c r="A482" s="105"/>
       <c r="E482" s="117"/>
       <c r="F482" s="105"/>
       <c r="G482" s="31"/>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" ht="13">
       <c r="A483" s="105"/>
       <c r="E483" s="117"/>
       <c r="F483" s="105"/>
       <c r="G483" s="31"/>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" ht="13">
       <c r="A484" s="105"/>
       <c r="E484" s="117"/>
       <c r="F484" s="105"/>
       <c r="G484" s="31"/>
     </row>
-    <row r="485" spans="1:8">
+    <row r="485" spans="1:8" ht="13">
       <c r="A485" s="105"/>
       <c r="E485" s="117"/>
       <c r="F485" s="105"/>
@@ -14465,7 +14565,7 @@
       <c r="G507" s="31"/>
       <c r="H507" s="31"/>
     </row>
-    <row r="508" spans="1:10">
+    <row r="508" spans="1:10" ht="13">
       <c r="A508" s="121"/>
       <c r="B508" s="121"/>
       <c r="C508" s="121"/>
@@ -14476,7 +14576,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13.5">
+    <row r="509" spans="1:10" ht="13">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -14487,7 +14587,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13.5">
+    <row r="510" spans="1:10" ht="13">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -14498,7 +14598,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13.5">
+    <row r="511" spans="1:10" ht="13">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -14580,7 +14680,7 @@
       <c r="G525" s="31"/>
       <c r="H525" s="31"/>
     </row>
-    <row r="526" spans="1:9">
+    <row r="526" spans="1:9" ht="13">
       <c r="A526" s="121"/>
       <c r="B526" s="121"/>
       <c r="C526" s="121"/>
@@ -14701,7 +14801,7 @@
       <c r="G546" s="31"/>
       <c r="H546" s="31"/>
     </row>
-    <row r="547" spans="1:9">
+    <row r="547" spans="1:9" ht="13">
       <c r="A547" s="121"/>
       <c r="B547" s="121"/>
       <c r="C547" s="121"/>
@@ -14788,7 +14888,7 @@
       <c r="G562" s="31"/>
       <c r="H562" s="31"/>
     </row>
-    <row r="563" spans="1:9">
+    <row r="563" spans="1:9" ht="13">
       <c r="A563" s="121"/>
       <c r="B563" s="121"/>
       <c r="C563" s="121"/>
@@ -14836,7 +14936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EE7EEF-305D-1145-A07B-3D132F6E2765}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K402"/>
@@ -14847,21 +14947,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:11" ht="40" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -14880,7 +14980,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:11" ht="66.95" customHeight="1">
+    <row r="2" spans="1:11" ht="67" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -14907,7 +15007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="13">
       <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
@@ -21061,7 +21161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
@@ -21069,13 +21169,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -21089,7 +21189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165.75">
+    <row r="2" spans="1:5" ht="169">
       <c r="A2" s="273" t="s">
         <v>14</v>
       </c>
@@ -21103,7 +21203,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="14.5">
       <c r="A3" s="274" t="s">
         <v>19</v>
       </c>
@@ -21863,7 +21963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABABBB7-6A1E-0B4E-82BF-6CDF21C8BDBC}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -21874,13 +21974,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.42578125" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="170"/>
+    <col min="2" max="2" width="28.81640625" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.453125" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.453125" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21897,7 +21997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="78">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -21911,7 +22011,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="173" t="s">
         <v>6</v>
       </c>
@@ -25837,7 +25937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H25"/>
@@ -25846,19 +25946,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.453125" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="43.453125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="1021" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="29.5">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -25876,7 +25976,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="65.5">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -25900,7 +26000,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -25926,86 +26026,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" ht="14.5">
       <c r="E4" s="7"/>
       <c r="F4" s="133"/>
       <c r="G4" s="12"/>
       <c r="H4" s="128"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" ht="14.5">
       <c r="E5" s="7"/>
       <c r="F5" s="133"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" ht="14.5">
       <c r="E6" s="7"/>
       <c r="F6" s="133"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" ht="14.5">
       <c r="E7" s="7"/>
       <c r="F7" s="133"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" ht="14.5">
       <c r="E8" s="7"/>
       <c r="F8" s="133"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" ht="14.5">
       <c r="E9" s="7"/>
       <c r="F9" s="133"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" ht="14.5">
       <c r="E10" s="7"/>
       <c r="F10" s="133"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" ht="14.5">
       <c r="E11" s="7"/>
       <c r="F11" s="133"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" ht="14.5">
       <c r="E12" s="7"/>
       <c r="F12" s="133"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" ht="14.5">
       <c r="D13" s="202"/>
       <c r="E13" s="7"/>
       <c r="F13" s="133"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" ht="14.5">
       <c r="E14" s="7"/>
       <c r="F14" s="133"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8" ht="14.5">
       <c r="C15" s="31"/>
       <c r="E15" s="7"/>
       <c r="F15" s="133"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" ht="14.5">
       <c r="C16" s="31"/>
       <c r="E16" s="7"/>
       <c r="F16" s="133"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="15">
+    <row r="17" spans="2:8" ht="14.5">
       <c r="E17" s="7"/>
       <c r="F17" s="133"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="15">
+    <row r="18" spans="2:8" ht="14.5">
       <c r="E18" s="7"/>
       <c r="F18" s="133"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="15">
+    <row r="19" spans="2:8" ht="14.5">
       <c r="E19" s="7"/>
       <c r="H19" s="133"/>
     </row>
@@ -26027,163 +26127,6 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="105"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
-      <c r="A1" s="62" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
-      <c r="A2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>746</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
-        <v>747</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
-        <v>925</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15">
-      <c r="A3" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="67" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="7"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="105"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="105"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="105"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="105"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="105"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="105"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="105"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="105"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="105"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="105"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26195,69 +26138,64 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="7" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="29.453125" customWidth="1"/>
+    <col min="8" max="1013" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="72" t="s">
-        <v>749</v>
-      </c>
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
+      <c r="A1" s="62" t="s">
+        <v>745</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
-    </row>
-    <row r="2" spans="1:8" ht="76.5">
+      <c r="E1" s="34"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="87">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>744</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="131" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
         <v>925</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:7" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26273,33 +26211,46 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="128" t="s">
-        <v>58</v>
+      <c r="F3" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="H4" s="68"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="D5" s="107"/>
-    </row>
-    <row r="6" spans="1:8" ht="14.25">
-      <c r="D6" s="114"/>
-    </row>
-    <row r="7" spans="1:8" ht="14.25">
-      <c r="D7" s="114"/>
-    </row>
-    <row r="8" spans="1:8" ht="14.25">
-      <c r="D8" s="114"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" s="37"/>
+    <row r="4" spans="1:7">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26333,9 +26284,6 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26347,64 +26295,69 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="3" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" customWidth="1"/>
+    <col min="9" max="1022" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="30" t="s">
-        <v>750</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:8" ht="18.5">
+      <c r="A1" s="72" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" ht="105">
+      <c r="E1" s="76"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="130"/>
+    </row>
+    <row r="2" spans="1:8" ht="78">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
+        <v>744</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="131" t="s">
         <v>925</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:8" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26420,21 +26373,33 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="4" spans="1:8" ht="14.5">
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" s="107"/>
+    </row>
+    <row r="6" spans="1:8" ht="14">
       <c r="D6" s="114"/>
     </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
+    <row r="7" spans="1:8" ht="14">
+      <c r="D7" s="114"/>
+    </row>
+    <row r="8" spans="1:8" ht="14">
+      <c r="D8" s="114"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="F9" s="37"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26468,6 +26433,9 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26479,162 +26447,131 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="140"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" customWidth="1"/>
+    <col min="8" max="1008" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="135" t="s">
-        <v>927</v>
-      </c>
-      <c r="B1" s="136" t="s">
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>750</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="137" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-    </row>
-    <row r="2" spans="1:9" ht="38.25">
-      <c r="A2" s="141"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142" t="s">
-        <v>928</v>
-      </c>
-      <c r="D2" s="142" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" ht="87">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>746</v>
       </c>
-      <c r="E2" s="142" t="s">
-        <v>929</v>
-      </c>
-      <c r="F2" s="141" t="s">
-        <v>930</v>
-      </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-    </row>
-    <row r="3" spans="1:9" ht="15">
-      <c r="A3" s="143" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="144" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
+        <v>925</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.5">
+      <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="B3" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="143" t="s">
+      <c r="C3" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="143" t="s">
+      <c r="F3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="143" t="s">
-        <v>931</v>
-      </c>
-      <c r="I3" s="143" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15">
-      <c r="A4" s="145"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-    </row>
-    <row r="5" spans="1:9" ht="15">
-      <c r="A5" s="145"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="146"/>
-    </row>
-    <row r="6" spans="1:9" ht="15">
-      <c r="A6" s="145"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="139"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="146"/>
-    </row>
-    <row r="7" spans="1:9" ht="15">
-      <c r="A7" s="145"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="146"/>
-    </row>
-    <row r="8" spans="1:9" ht="15">
-      <c r="A8" s="145"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="146"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="145"/>
-      <c r="B9" s="146"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="146"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="146"/>
+      <c r="G3" s="12" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14">
+      <c r="D6" s="114"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="105"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="105"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="105"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="105"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="105"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="105"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="105"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="105"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="105"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="105"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="105"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
   </headerFooter>
@@ -26649,14 +26586,14 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:10" ht="17.5">
       <c r="A1" s="267" t="s">
         <v>1134</v>
       </c>
@@ -26741,6 +26678,169 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="140"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="135" t="s">
+        <v>927</v>
+      </c>
+      <c r="B1" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="138" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+    </row>
+    <row r="2" spans="1:9" ht="39">
+      <c r="A2" s="141"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="142" t="s">
+        <v>928</v>
+      </c>
+      <c r="D2" s="142" t="s">
+        <v>746</v>
+      </c>
+      <c r="E2" s="142" t="s">
+        <v>929</v>
+      </c>
+      <c r="F2" s="141" t="s">
+        <v>930</v>
+      </c>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.5">
+      <c r="A3" s="143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="144" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="143" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="143" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="143" t="s">
+        <v>931</v>
+      </c>
+      <c r="I3" s="143" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.5">
+      <c r="A4" s="145"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.5">
+      <c r="A5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="146"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.5">
+      <c r="A6" s="145"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="146"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.5">
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="146"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.5">
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="146"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.5">
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="146"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D13"/>
@@ -26749,12 +26849,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
+    <col min="4" max="1013" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -26771,7 +26871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="65">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -26782,7 +26882,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.25">
+    <row r="3" spans="1:4" ht="39">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -26855,7 +26955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B5A0B4-9586-D946-AB25-20C3418D4E9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -26863,17 +26963,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="140"/>
+    <col min="1" max="1" width="16.1796875" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.81640625" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -26892,7 +26992,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="39">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -26912,7 +27012,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.7" customHeight="1">
+    <row r="3" spans="1:6" ht="13.75" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -26932,28 +27032,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.7" customHeight="1">
+    <row r="4" spans="1:6" ht="13.75" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.7" customHeight="1">
+    <row r="5" spans="1:6" ht="13.75" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.7" customHeight="1">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.7" customHeight="1">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.7" customHeight="1">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -26963,7 +27063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E7"/>
@@ -26972,12 +27072,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -26994,7 +27094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="178.5">
+    <row r="2" spans="1:5" ht="175.5">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27011,7 +27111,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="13">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -27043,95 +27143,6 @@
     <row r="7" spans="1:5">
       <c r="B7" s="60"/>
       <c r="C7" s="81"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="76.5">
-      <c r="A2" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="78" t="s">
-        <v>768</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>763</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="60"/>
-      <c r="C5" s="81"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="81"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="61"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="81"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="61"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -27143,6 +27154,95 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="48.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>765</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="78">
+      <c r="A2" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>761</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13">
+      <c r="A3" s="78" t="s">
+        <v>768</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="60"/>
+      <c r="C5" s="81"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="60"/>
+      <c r="C7" s="81"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="61"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="81"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="61"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:D484"/>
@@ -27151,14 +27251,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.453125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -27175,7 +27275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27189,7 +27289,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -28837,7 +28937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D120"/>
@@ -28846,13 +28946,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -28869,7 +28969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="63.75">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -28883,7 +28983,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -29329,7 +29429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D32"/>
@@ -29338,12 +29438,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -29360,7 +29460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -29374,7 +29474,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -29549,12 +29649,12 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="1014" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="1014" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29572,7 +29672,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="153">
+    <row r="2" spans="1:6" ht="143">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -29592,7 +29692,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="13">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -29637,14 +29737,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="5" width="21.1796875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.85546875" customWidth="1"/>
-    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="58.81640625" customWidth="1"/>
+    <col min="8" max="1011" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -29666,7 +29766,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="191.25">
+    <row r="2" spans="1:9" ht="195">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29695,7 +29795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25">
+    <row r="3" spans="1:9" ht="39">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29763,14 +29863,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29789,7 +29889,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="89.25">
+    <row r="2" spans="1:6" ht="91">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29809,7 +29909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="26">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -29903,19 +30003,19 @@
       <selection activeCell="A4" sqref="A4:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="49.453125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
-    <col min="11" max="1015" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.453125" customWidth="1"/>
+    <col min="11" max="1015" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -29936,7 +30036,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="102">
+    <row r="2" spans="1:10" ht="88">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29968,7 +30068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25">
+    <row r="3" spans="1:10" ht="39">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30497,27 +30597,27 @@
       <selection activeCell="F4" sqref="A4:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="55.42578125" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" customWidth="1"/>
-    <col min="10" max="10" width="81.42578125" customWidth="1"/>
-    <col min="11" max="11" width="93.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="15" width="8.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="55.453125" customWidth="1"/>
+    <col min="8" max="8" width="47.81640625" customWidth="1"/>
+    <col min="9" max="9" width="52.453125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
+    <col min="11" max="11" width="93.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" customWidth="1"/>
+    <col min="14" max="15" width="8.453125" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" customWidth="1"/>
+    <col min="18" max="18" width="20.453125" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" customWidth="1"/>
+    <col min="20" max="1013" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" customHeight="1">
@@ -30549,7 +30649,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:19" ht="114.75">
+    <row r="2" spans="1:19" ht="117">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30590,7 +30690,7 @@
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
     </row>
-    <row r="3" spans="1:19" ht="38.25">
+    <row r="3" spans="1:19" ht="39">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30649,7 +30749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.25">
+    <row r="4" spans="1:19" ht="14">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -30657,7 +30757,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:19" ht="14.25">
+    <row r="5" spans="1:19" ht="14">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -30665,7 +30765,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25">
+    <row r="6" spans="1:19" ht="14">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -30675,7 +30775,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:19" ht="14.25">
+    <row r="7" spans="1:19" ht="14">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30686,7 +30786,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:19" ht="14.25">
+    <row r="8" spans="1:19" ht="14">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30697,7 +30797,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:19" ht="14.25">
+    <row r="9" spans="1:19" ht="14">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30709,7 +30809,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:19" ht="14.25">
+    <row r="10" spans="1:19" ht="14">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30721,7 +30821,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:19" ht="14.25">
+    <row r="11" spans="1:19" ht="14">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30733,7 +30833,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:19" ht="14.25">
+    <row r="12" spans="1:19" ht="14">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30745,7 +30845,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:19" ht="14.25">
+    <row r="13" spans="1:19" ht="14">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30757,7 +30857,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:19" ht="14.25">
+    <row r="14" spans="1:19" ht="14">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30769,7 +30869,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:19" ht="14.25">
+    <row r="15" spans="1:19" ht="14">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30781,7 +30881,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:19" ht="14.25">
+    <row r="16" spans="1:19" ht="14">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30793,7 +30893,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14.25">
+    <row r="17" spans="6:19" ht="14">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30805,7 +30905,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14.25">
+    <row r="18" spans="6:19" ht="14">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30817,7 +30917,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14.25">
+    <row r="19" spans="6:19" ht="14">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -30827,7 +30927,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14.25">
+    <row r="20" spans="6:19" ht="14">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -30835,7 +30935,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14.25">
+    <row r="21" spans="6:19" ht="14">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30846,7 +30946,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14.25">
+    <row r="22" spans="6:19" ht="14">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30858,7 +30958,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14.25">
+    <row r="23" spans="6:19" ht="14">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -30870,7 +30970,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14.25">
+    <row r="24" spans="6:19" ht="14">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -30878,7 +30978,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14.25">
+    <row r="25" spans="6:19" ht="14">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -30889,7 +30989,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14.25">
+    <row r="26" spans="6:19" ht="14">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -30901,7 +31001,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14.25">
+    <row r="27" spans="6:19" ht="14">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -30912,7 +31012,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14.25">
+    <row r="28" spans="6:19" ht="14">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -30922,7 +31022,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14.25">
+    <row r="29" spans="6:19" ht="14">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -30933,7 +31033,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14.25">
+    <row r="30" spans="6:19" ht="14">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -30944,7 +31044,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14.25">
+    <row r="31" spans="6:19" ht="14">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -30955,7 +31055,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14.25">
+    <row r="32" spans="6:19" ht="14">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -30964,7 +31064,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14.25">
+    <row r="33" spans="6:19" ht="14">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -30973,7 +31073,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14.25">
+    <row r="34" spans="6:19" ht="14">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -30983,7 +31083,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14.25">
+    <row r="35" spans="6:19" ht="14">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -30992,7 +31092,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14.25">
+    <row r="36" spans="6:19" ht="14">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -31108,7 +31208,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14.25">
+    <row r="48" spans="6:19" ht="14">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -31199,26 +31299,26 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="58.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="58.453125" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="87.140625" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="87.1796875" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -31242,7 +31342,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:17" ht="57.95" customHeight="1">
+    <row r="2" spans="1:17" ht="58" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31291,7 +31391,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="38.25">
+    <row r="3" spans="1:17" ht="39">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -33349,29 +33449,29 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:XFD194"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD192"/>
+      <selection pane="bottomLeft" activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.1796875" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="30" t="s">
         <v>136</v>
       </c>
@@ -33385,7 +33485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93.95" customHeight="1">
+    <row r="2" spans="1:11" ht="94" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -33416,8 +33516,11 @@
       <c r="J2" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="25.5">
+      <c r="K2" s="22" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -33448,8 +33551,11 @@
       <c r="J3" s="26" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="26" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>1103</v>
       </c>
@@ -33467,7 +33573,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
@@ -33485,7 +33591,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>1103</v>
       </c>
@@ -33503,7 +33609,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -33523,7 +33629,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1103</v>
       </c>
@@ -33543,7 +33649,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>1103</v>
       </c>
@@ -33563,7 +33669,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>1103</v>
       </c>
@@ -33585,7 +33691,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>1103</v>
       </c>
@@ -33605,7 +33711,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>1103</v>
       </c>
@@ -33625,7 +33731,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>1103</v>
       </c>
@@ -33645,7 +33751,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>1103</v>
       </c>
@@ -33664,7 +33770,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>1103</v>
       </c>
@@ -33684,7 +33790,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>1103</v>
       </c>

</xml_diff>

<commit_message>
Feature flag case file view (#660)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-englandwales\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC1D55-4FB8-444B-9E45-F7CC0D4BE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF576B99-775F-47A7-8355-F168B63163BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1470" windowWidth="36660" windowHeight="19395" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1905" yWindow="-18165" windowWidth="28800" windowHeight="15315" tabRatio="500" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -22,47 +22,48 @@
     <sheet name="CaseEvent" sheetId="23" r:id="rId7"/>
     <sheet name="CaseEventToFields" sheetId="24" r:id="rId8"/>
     <sheet name="CaseField" sheetId="25" r:id="rId9"/>
-    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId10"/>
-    <sheet name="ComplexTypes" sheetId="26" r:id="rId11"/>
-    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId12"/>
-    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId13"/>
-    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId14"/>
-    <sheet name="SearchInputFields" sheetId="13" r:id="rId15"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId17"/>
-    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId18"/>
-    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
-    <sheet name="CaseRoles" sheetId="31" r:id="rId21"/>
-    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId22"/>
-    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId23"/>
-    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId24"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId25"/>
-    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId26"/>
+    <sheet name="Categories" sheetId="39" r:id="rId10"/>
+    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId11"/>
+    <sheet name="ComplexTypes" sheetId="26" r:id="rId12"/>
+    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId13"/>
+    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId14"/>
+    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId15"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId16"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId17"/>
+    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId18"/>
+    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId19"/>
+    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId20"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId21"/>
+    <sheet name="CaseRoles" sheetId="31" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId23"/>
+    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId24"/>
+    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId25"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId26"/>
+    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId27"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$Q$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CaseRoles!$A$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseType!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseTypeTab!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Jurisdiction!$A$3:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">State!$A$3:$F$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">UserProfile!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">UserProfile!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1152">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3595,6 +3596,35 @@
   </si>
   <si>
     <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Unique ID that identifies the category
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label that gets displayed in the UI. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Specifies the display order for the category.</t>
+  </si>
+  <si>
+    <t>Identifies the parent category id for a sub-category.</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>CategoryLabel</t>
+  </si>
+  <si>
+    <t>ParentCategoryID</t>
+  </si>
+  <si>
+    <t>ID that identifies the document category
+MaxLength: 70</t>
   </si>
 </sst>
 </file>
@@ -4350,7 +4380,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4890,6 +4920,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -5371,14 +5404,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="17.5">
       <c r="A1" s="267" t="s">
         <v>1137</v>
       </c>
@@ -5386,7 +5419,7 @@
       <c r="C1" s="271"/>
       <c r="D1" s="270"/>
     </row>
-    <row r="2" spans="1:4" ht="102.75">
+    <row r="2" spans="1:4" ht="88.5">
       <c r="A2" s="269" t="s">
         <v>1133</v>
       </c>
@@ -5424,6 +5457,65 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5E47D-EB2A-4FD0-8353-2773316B4A69}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="12.5"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="65">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13">
+      <c r="A3" s="276" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C3" s="276" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243AEE7-DA61-4CDF-84FC-CA2502F211A6}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -5431,20 +5523,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="239"/>
-    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="239"/>
+    <col min="3" max="3" width="54.7265625" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.7265625" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.26953125" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" style="239"/>
-    <col min="1026" max="16384" width="10.85546875" style="238"/>
+    <col min="10" max="10" width="43.7265625" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.81640625" style="239"/>
+    <col min="1026" max="16384" width="10.81640625" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -5470,7 +5562,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="63.75">
+    <row r="2" spans="1:13" ht="52">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -5505,7 +5597,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75">
+    <row r="3" spans="1:13" ht="15.5">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -5557,7 +5649,7 @@
       <c r="L4" s="240"/>
       <c r="M4" s="240"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="13">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="242"/>
@@ -5572,7 +5664,7 @@
       <c r="L5" s="240"/>
       <c r="M5" s="240"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="13">
       <c r="A6" s="241"/>
       <c r="B6" s="241"/>
       <c r="D6" s="240"/>
@@ -5586,7 +5678,7 @@
       <c r="L6" s="240"/>
       <c r="M6" s="240"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="13">
       <c r="A7" s="241"/>
       <c r="B7" s="241"/>
       <c r="D7" s="240"/>
@@ -5622,34 +5714,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC74BE-16DE-BC4E-A66A-E3A520C8B91F}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:N563"/>
+  <dimension ref="A1:O563"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A328" sqref="A328:XFD563"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="53.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" customWidth="1"/>
+    <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="30" t="s">
         <v>192</v>
       </c>
@@ -5672,7 +5765,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:14" ht="54.95" customHeight="1">
+    <row r="2" spans="1:15" ht="55" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -5711,8 +5804,11 @@
       <c r="N2" s="24" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="51">
+      <c r="O2" s="22" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="52">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -5755,8 +5851,11 @@
       <c r="N3" s="26" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="26" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1036</v>
       </c>
@@ -5776,7 +5875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>1036</v>
       </c>
@@ -5799,7 +5898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>1036</v>
       </c>
@@ -5816,7 +5915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1036</v>
       </c>
@@ -5833,7 +5932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>1036</v>
       </c>
@@ -5850,7 +5949,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15" ht="13">
       <c r="A9" s="121" t="s">
         <v>1036</v>
       </c>
@@ -5873,7 +5972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>1037</v>
       </c>
@@ -5890,7 +5989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>1037</v>
       </c>
@@ -5907,7 +6006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>1037</v>
       </c>
@@ -5924,7 +6023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>1037</v>
       </c>
@@ -5941,7 +6040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15" ht="13">
       <c r="A14" s="121" t="s">
         <v>1037</v>
       </c>
@@ -5964,7 +6063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>1062</v>
       </c>
@@ -5981,7 +6080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="105" t="s">
         <v>1062</v>
       </c>
@@ -6106,7 +6205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="13">
       <c r="A22" s="121" t="s">
         <v>1062</v>
       </c>
@@ -6151,7 +6250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="13">
       <c r="A24" s="121" t="s">
         <v>1063</v>
       </c>
@@ -6192,7 +6291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="13">
       <c r="A26" s="121" t="s">
         <v>1023</v>
       </c>
@@ -6400,7 +6499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" ht="13">
       <c r="A36" s="121" t="s">
         <v>1018</v>
       </c>
@@ -6755,7 +6854,7 @@
       <c r="J50" s="43"/>
       <c r="K50" s="43"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" ht="13">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -6782,7 +6881,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" ht="13">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -6809,7 +6908,7 @@
       <c r="J52" s="43"/>
       <c r="K52" s="43"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" ht="13">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -7207,7 +7306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" ht="13">
       <c r="A69" s="121" t="s">
         <v>80</v>
       </c>
@@ -7228,7 +7327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.1" customHeight="1">
+    <row r="70" spans="1:9" ht="14.15" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -7251,7 +7350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
+    <row r="71" spans="1:9" ht="10" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -7457,7 +7556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" ht="13">
       <c r="A81" s="121" t="s">
         <v>1020</v>
       </c>
@@ -7548,7 +7647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" ht="13">
       <c r="A85" s="121" t="s">
         <v>1056</v>
       </c>
@@ -7618,7 +7717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" ht="13">
       <c r="A88" s="121" t="s">
         <v>1040</v>
       </c>
@@ -7679,7 +7778,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" ht="13">
       <c r="A91" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7700,7 +7799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" ht="13">
       <c r="A92" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7721,7 +7820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" ht="13">
       <c r="A93" t="s">
         <v>1014</v>
       </c>
@@ -7750,7 +7849,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" ht="13">
       <c r="A94" t="s">
         <v>1014</v>
       </c>
@@ -7776,7 +7875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" ht="13">
       <c r="A95" t="s">
         <v>1014</v>
       </c>
@@ -7796,7 +7895,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" ht="13">
       <c r="A96" t="s">
         <v>1014</v>
       </c>
@@ -7822,7 +7921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:15" ht="13">
       <c r="A97" t="s">
         <v>1014</v>
       </c>
@@ -7842,7 +7941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:15" ht="13">
       <c r="A98" t="s">
         <v>1014</v>
       </c>
@@ -7864,7 +7963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>1014</v>
       </c>
@@ -7883,7 +7982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>1014</v>
       </c>
@@ -7902,7 +8001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>1014</v>
       </c>
@@ -7921,7 +8020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>1014</v>
       </c>
@@ -7944,7 +8043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>1014</v>
       </c>
@@ -7963,7 +8062,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>1014</v>
       </c>
@@ -7986,7 +8085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>1014</v>
       </c>
@@ -8005,7 +8104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>1014</v>
       </c>
@@ -8028,7 +8127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>1014</v>
       </c>
@@ -8051,7 +8150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:15" ht="13">
       <c r="A108" t="s">
         <v>1014</v>
       </c>
@@ -8076,8 +8175,9 @@
       <c r="I108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="O108" s="233"/>
+    </row>
+    <row r="109" spans="1:15" ht="13">
       <c r="A109" t="s">
         <v>1014</v>
       </c>
@@ -8099,7 +8199,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>1014</v>
       </c>
@@ -8118,7 +8218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:15" ht="13">
       <c r="A111" s="121" t="s">
         <v>1014</v>
       </c>
@@ -8138,7 +8238,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>1003</v>
       </c>
@@ -8304,7 +8404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" ht="13">
       <c r="A119" s="121" t="s">
         <v>1003</v>
       </c>
@@ -8408,7 +8508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" ht="13">
       <c r="A124" s="121" t="s">
         <v>998</v>
       </c>
@@ -8599,7 +8699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" ht="13">
       <c r="A133" s="121" t="s">
         <v>1064</v>
       </c>
@@ -8680,7 +8780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" ht="13">
       <c r="A137" s="121" t="s">
         <v>883</v>
       </c>
@@ -8881,7 +8981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:14" ht="13">
       <c r="A147" s="121" t="s">
         <v>884</v>
       </c>
@@ -8965,7 +9065,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:14" ht="13">
       <c r="A151" s="121" t="s">
         <v>885</v>
       </c>
@@ -8986,7 +9086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:14" ht="13">
       <c r="A152" s="121" t="s">
         <v>1076</v>
       </c>
@@ -9007,7 +9107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:14" ht="13">
       <c r="A153" s="121" t="s">
         <v>1066</v>
       </c>
@@ -9071,7 +9171,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:14" ht="13">
       <c r="A156" s="121" t="s">
         <v>936</v>
       </c>
@@ -9139,7 +9239,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:14" ht="13">
       <c r="A159" s="121" t="s">
         <v>946</v>
       </c>
@@ -9184,7 +9284,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" ht="13">
       <c r="A161" s="121" t="s">
         <v>953</v>
       </c>
@@ -9300,7 +9400,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" ht="13">
       <c r="A166" s="121" t="s">
         <v>956</v>
       </c>
@@ -9425,7 +9525,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" ht="13">
       <c r="A172" s="121" t="s">
         <v>986</v>
       </c>
@@ -11125,7 +11225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" ht="13">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -11151,7 +11251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" ht="13">
       <c r="A244" s="121" t="s">
         <v>0</v>
       </c>
@@ -11198,7 +11298,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" ht="13">
       <c r="A246" t="s">
         <v>861</v>
       </c>
@@ -11225,7 +11325,7 @@
       <c r="J246" s="43"/>
       <c r="K246" s="43"/>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" ht="13">
       <c r="A247" t="s">
         <v>861</v>
       </c>
@@ -11252,7 +11352,7 @@
       <c r="J247" s="43"/>
       <c r="K247" s="43"/>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" ht="13">
       <c r="A248" t="s">
         <v>861</v>
       </c>
@@ -11281,7 +11381,7 @@
       <c r="J248" s="43"/>
       <c r="K248" s="43"/>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" ht="13">
       <c r="A249" t="s">
         <v>861</v>
       </c>
@@ -11310,7 +11410,7 @@
       <c r="J249" s="43"/>
       <c r="K249" s="43"/>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" ht="13">
       <c r="A250" s="121" t="s">
         <v>861</v>
       </c>
@@ -11664,7 +11764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:14">
+    <row r="265" spans="1:14" ht="13">
       <c r="A265" s="121" t="s">
         <v>1034</v>
       </c>
@@ -11928,7 +12028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:14">
+    <row r="275" spans="1:14" ht="13">
       <c r="A275" s="121" t="s">
         <v>1033</v>
       </c>
@@ -12020,7 +12120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13.5">
+    <row r="279" spans="1:14" ht="13">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -12192,7 +12292,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:14">
+    <row r="287" spans="1:14" ht="13">
       <c r="A287" t="s">
         <v>102</v>
       </c>
@@ -12215,7 +12315,7 @@
       <c r="J287" s="43"/>
       <c r="K287" s="43"/>
     </row>
-    <row r="288" spans="1:14">
+    <row r="288" spans="1:14" ht="13">
       <c r="A288" s="121" t="s">
         <v>102</v>
       </c>
@@ -12775,7 +12875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" ht="13">
       <c r="A309" s="121" t="s">
         <v>103</v>
       </c>
@@ -12800,7 +12900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" ht="13">
       <c r="A310" s="121" t="s">
         <v>103</v>
       </c>
@@ -13290,7 +13390,7 @@
       <c r="G329" s="31"/>
       <c r="H329" s="31"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" ht="13">
       <c r="A330" s="121"/>
       <c r="B330" s="121"/>
       <c r="C330" s="121"/>
@@ -13301,7 +13401,7 @@
       <c r="H330" s="205"/>
       <c r="I330" s="124"/>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" ht="13">
       <c r="A331" s="121"/>
       <c r="B331" s="121"/>
       <c r="C331" s="121"/>
@@ -13317,7 +13417,7 @@
       <c r="G332" s="31"/>
       <c r="H332" s="31"/>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" ht="13">
       <c r="A333" s="121"/>
       <c r="B333" s="121"/>
       <c r="C333" s="121"/>
@@ -13345,7 +13445,7 @@
       <c r="G336" s="31"/>
       <c r="H336" s="31"/>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" ht="13">
       <c r="A337" s="121"/>
       <c r="B337" s="121"/>
       <c r="C337" s="121"/>
@@ -13379,7 +13479,7 @@
       <c r="G341" s="31"/>
       <c r="H341" s="31"/>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" ht="13">
       <c r="A342" s="121"/>
       <c r="B342" s="121"/>
       <c r="C342" s="121"/>
@@ -13390,7 +13490,7 @@
       <c r="H342" s="205"/>
       <c r="I342" s="124"/>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" ht="13">
       <c r="A343" s="105"/>
       <c r="B343" s="121"/>
       <c r="E343" s="117"/>
@@ -13398,7 +13498,7 @@
       <c r="G343" s="31"/>
       <c r="H343" s="31"/>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" ht="13">
       <c r="A344" s="105"/>
       <c r="B344" s="121"/>
       <c r="E344" s="117"/>
@@ -13406,28 +13506,28 @@
       <c r="G344" s="31"/>
       <c r="H344" s="31"/>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" ht="13">
       <c r="A345" s="105"/>
       <c r="E345" s="117"/>
       <c r="F345" s="31"/>
       <c r="G345" s="31"/>
       <c r="H345" s="31"/>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" ht="13">
       <c r="A346" s="105"/>
       <c r="E346" s="117"/>
       <c r="F346" s="31"/>
       <c r="G346" s="31"/>
       <c r="H346" s="31"/>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" ht="13">
       <c r="A347" s="105"/>
       <c r="E347" s="117"/>
       <c r="F347" s="31"/>
       <c r="G347" s="31"/>
       <c r="H347" s="31"/>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" ht="13">
       <c r="A348" s="121"/>
       <c r="B348" s="121"/>
       <c r="C348" s="121"/>
@@ -14279,7 +14379,7 @@
       <c r="G474" s="31"/>
       <c r="H474" s="31"/>
     </row>
-    <row r="475" spans="1:9">
+    <row r="475" spans="1:9" ht="13">
       <c r="A475" s="121"/>
       <c r="B475" s="121"/>
       <c r="C475" s="121"/>
@@ -14290,7 +14390,7 @@
       <c r="H475" s="205"/>
       <c r="I475" s="124"/>
     </row>
-    <row r="476" spans="1:9">
+    <row r="476" spans="1:9" ht="13">
       <c r="A476" s="121"/>
       <c r="B476" s="121"/>
       <c r="C476" s="121"/>
@@ -14301,55 +14401,55 @@
       <c r="H476" s="31"/>
       <c r="I476" s="124"/>
     </row>
-    <row r="477" spans="1:9">
+    <row r="477" spans="1:9" ht="13">
       <c r="A477" s="105"/>
       <c r="E477" s="117"/>
       <c r="F477" s="105"/>
       <c r="G477" s="31"/>
     </row>
-    <row r="478" spans="1:9">
+    <row r="478" spans="1:9" ht="13">
       <c r="A478" s="105"/>
       <c r="E478" s="117"/>
       <c r="F478" s="105"/>
       <c r="G478" s="31"/>
     </row>
-    <row r="479" spans="1:9">
+    <row r="479" spans="1:9" ht="13">
       <c r="A479" s="105"/>
       <c r="E479" s="117"/>
       <c r="F479" s="105"/>
       <c r="G479" s="31"/>
     </row>
-    <row r="480" spans="1:9">
+    <row r="480" spans="1:9" ht="13">
       <c r="A480" s="105"/>
       <c r="E480" s="117"/>
       <c r="F480" s="105"/>
       <c r="G480" s="31"/>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" ht="13">
       <c r="A481" s="105"/>
       <c r="E481" s="117"/>
       <c r="F481" s="105"/>
       <c r="G481" s="31"/>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" ht="13">
       <c r="A482" s="105"/>
       <c r="E482" s="117"/>
       <c r="F482" s="105"/>
       <c r="G482" s="31"/>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" ht="13">
       <c r="A483" s="105"/>
       <c r="E483" s="117"/>
       <c r="F483" s="105"/>
       <c r="G483" s="31"/>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" ht="13">
       <c r="A484" s="105"/>
       <c r="E484" s="117"/>
       <c r="F484" s="105"/>
       <c r="G484" s="31"/>
     </row>
-    <row r="485" spans="1:8">
+    <row r="485" spans="1:8" ht="13">
       <c r="A485" s="105"/>
       <c r="E485" s="117"/>
       <c r="F485" s="105"/>
@@ -14465,7 +14565,7 @@
       <c r="G507" s="31"/>
       <c r="H507" s="31"/>
     </row>
-    <row r="508" spans="1:10">
+    <row r="508" spans="1:10" ht="13">
       <c r="A508" s="121"/>
       <c r="B508" s="121"/>
       <c r="C508" s="121"/>
@@ -14476,7 +14576,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13.5">
+    <row r="509" spans="1:10" ht="13">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -14487,7 +14587,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13.5">
+    <row r="510" spans="1:10" ht="13">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -14498,7 +14598,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13.5">
+    <row r="511" spans="1:10" ht="13">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -14580,7 +14680,7 @@
       <c r="G525" s="31"/>
       <c r="H525" s="31"/>
     </row>
-    <row r="526" spans="1:9">
+    <row r="526" spans="1:9" ht="13">
       <c r="A526" s="121"/>
       <c r="B526" s="121"/>
       <c r="C526" s="121"/>
@@ -14701,7 +14801,7 @@
       <c r="G546" s="31"/>
       <c r="H546" s="31"/>
     </row>
-    <row r="547" spans="1:9">
+    <row r="547" spans="1:9" ht="13">
       <c r="A547" s="121"/>
       <c r="B547" s="121"/>
       <c r="C547" s="121"/>
@@ -14788,7 +14888,7 @@
       <c r="G562" s="31"/>
       <c r="H562" s="31"/>
     </row>
-    <row r="563" spans="1:9">
+    <row r="563" spans="1:9" ht="13">
       <c r="A563" s="121"/>
       <c r="B563" s="121"/>
       <c r="C563" s="121"/>
@@ -14836,7 +14936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EE7EEF-305D-1145-A07B-3D132F6E2765}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K402"/>
@@ -14847,21 +14947,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:11" ht="40" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -14880,7 +14980,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:11" ht="66.95" customHeight="1">
+    <row r="2" spans="1:11" ht="67" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -14907,7 +15007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="13">
       <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
@@ -21061,7 +21161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
@@ -21069,13 +21169,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -21089,7 +21189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165.75">
+    <row r="2" spans="1:5" ht="169">
       <c r="A2" s="273" t="s">
         <v>14</v>
       </c>
@@ -21103,7 +21203,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="14.5">
       <c r="A3" s="274" t="s">
         <v>19</v>
       </c>
@@ -21863,7 +21963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABABBB7-6A1E-0B4E-82BF-6CDF21C8BDBC}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -21874,13 +21974,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.42578125" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="170"/>
+    <col min="2" max="2" width="28.81640625" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.453125" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.453125" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21897,7 +21997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="78">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -21911,7 +22011,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="173" t="s">
         <v>6</v>
       </c>
@@ -25837,7 +25937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H25"/>
@@ -25846,19 +25946,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.453125" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="43.453125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="1021" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="29.5">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -25876,7 +25976,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="65.5">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -25900,7 +26000,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -25926,86 +26026,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" ht="14.5">
       <c r="E4" s="7"/>
       <c r="F4" s="133"/>
       <c r="G4" s="12"/>
       <c r="H4" s="128"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" ht="14.5">
       <c r="E5" s="7"/>
       <c r="F5" s="133"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" ht="14.5">
       <c r="E6" s="7"/>
       <c r="F6" s="133"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" ht="14.5">
       <c r="E7" s="7"/>
       <c r="F7" s="133"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" ht="14.5">
       <c r="E8" s="7"/>
       <c r="F8" s="133"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" ht="14.5">
       <c r="E9" s="7"/>
       <c r="F9" s="133"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" ht="14.5">
       <c r="E10" s="7"/>
       <c r="F10" s="133"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" ht="14.5">
       <c r="E11" s="7"/>
       <c r="F11" s="133"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" ht="14.5">
       <c r="E12" s="7"/>
       <c r="F12" s="133"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" ht="14.5">
       <c r="D13" s="202"/>
       <c r="E13" s="7"/>
       <c r="F13" s="133"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" ht="14.5">
       <c r="E14" s="7"/>
       <c r="F14" s="133"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8" ht="14.5">
       <c r="C15" s="31"/>
       <c r="E15" s="7"/>
       <c r="F15" s="133"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" ht="14.5">
       <c r="C16" s="31"/>
       <c r="E16" s="7"/>
       <c r="F16" s="133"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="15">
+    <row r="17" spans="2:8" ht="14.5">
       <c r="E17" s="7"/>
       <c r="F17" s="133"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="15">
+    <row r="18" spans="2:8" ht="14.5">
       <c r="E18" s="7"/>
       <c r="F18" s="133"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="15">
+    <row r="19" spans="2:8" ht="14.5">
       <c r="E19" s="7"/>
       <c r="H19" s="133"/>
     </row>
@@ -26027,163 +26127,6 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="105"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
-      <c r="A1" s="62" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
-      <c r="A2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>746</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
-        <v>747</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
-        <v>925</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15">
-      <c r="A3" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="67" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="7"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="105"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="105"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="105"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="105"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="105"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="105"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="105"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="105"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="105"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="105"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26195,69 +26138,64 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="7" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="29.453125" customWidth="1"/>
+    <col min="8" max="1013" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="72" t="s">
-        <v>749</v>
-      </c>
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
+      <c r="A1" s="62" t="s">
+        <v>745</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
-    </row>
-    <row r="2" spans="1:8" ht="76.5">
+      <c r="E1" s="34"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="87">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>744</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="131" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
         <v>925</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:7" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26273,33 +26211,46 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="128" t="s">
-        <v>58</v>
+      <c r="F3" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="H4" s="68"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="D5" s="107"/>
-    </row>
-    <row r="6" spans="1:8" ht="14.25">
-      <c r="D6" s="114"/>
-    </row>
-    <row r="7" spans="1:8" ht="14.25">
-      <c r="D7" s="114"/>
-    </row>
-    <row r="8" spans="1:8" ht="14.25">
-      <c r="D8" s="114"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" s="37"/>
+    <row r="4" spans="1:7">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26333,9 +26284,6 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26347,64 +26295,69 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="3" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" customWidth="1"/>
+    <col min="9" max="1022" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="30" t="s">
-        <v>750</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:8" ht="18.5">
+      <c r="A1" s="72" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" ht="105">
+      <c r="E1" s="76"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="130"/>
+    </row>
+    <row r="2" spans="1:8" ht="78">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
+        <v>744</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="131" t="s">
         <v>925</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:8" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26420,21 +26373,33 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="4" spans="1:8" ht="14.5">
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" s="107"/>
+    </row>
+    <row r="6" spans="1:8" ht="14">
       <c r="D6" s="114"/>
     </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
+    <row r="7" spans="1:8" ht="14">
+      <c r="D7" s="114"/>
+    </row>
+    <row r="8" spans="1:8" ht="14">
+      <c r="D8" s="114"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="F9" s="37"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26468,6 +26433,9 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26479,162 +26447,131 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="140"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" customWidth="1"/>
+    <col min="8" max="1008" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="135" t="s">
-        <v>927</v>
-      </c>
-      <c r="B1" s="136" t="s">
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>750</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="137" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-    </row>
-    <row r="2" spans="1:9" ht="38.25">
-      <c r="A2" s="141"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142" t="s">
-        <v>928</v>
-      </c>
-      <c r="D2" s="142" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" ht="87">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>746</v>
       </c>
-      <c r="E2" s="142" t="s">
-        <v>929</v>
-      </c>
-      <c r="F2" s="141" t="s">
-        <v>930</v>
-      </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-    </row>
-    <row r="3" spans="1:9" ht="15">
-      <c r="A3" s="143" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="144" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
+        <v>925</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.5">
+      <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="B3" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="143" t="s">
+      <c r="C3" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="143" t="s">
+      <c r="F3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="143" t="s">
-        <v>931</v>
-      </c>
-      <c r="I3" s="143" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15">
-      <c r="A4" s="145"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-    </row>
-    <row r="5" spans="1:9" ht="15">
-      <c r="A5" s="145"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="146"/>
-    </row>
-    <row r="6" spans="1:9" ht="15">
-      <c r="A6" s="145"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="139"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="146"/>
-    </row>
-    <row r="7" spans="1:9" ht="15">
-      <c r="A7" s="145"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="146"/>
-    </row>
-    <row r="8" spans="1:9" ht="15">
-      <c r="A8" s="145"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="146"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="145"/>
-      <c r="B9" s="146"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="146"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="146"/>
+      <c r="G3" s="12" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14">
+      <c r="D6" s="114"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="105"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="105"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="105"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="105"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="105"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="105"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="105"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="105"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="105"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="105"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="105"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
   </headerFooter>
@@ -26649,14 +26586,14 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:10" ht="17.5">
       <c r="A1" s="267" t="s">
         <v>1134</v>
       </c>
@@ -26741,6 +26678,169 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="140"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="135" t="s">
+        <v>927</v>
+      </c>
+      <c r="B1" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="138" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+    </row>
+    <row r="2" spans="1:9" ht="39">
+      <c r="A2" s="141"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="142" t="s">
+        <v>928</v>
+      </c>
+      <c r="D2" s="142" t="s">
+        <v>746</v>
+      </c>
+      <c r="E2" s="142" t="s">
+        <v>929</v>
+      </c>
+      <c r="F2" s="141" t="s">
+        <v>930</v>
+      </c>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.5">
+      <c r="A3" s="143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="144" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="143" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="143" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="143" t="s">
+        <v>931</v>
+      </c>
+      <c r="I3" s="143" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.5">
+      <c r="A4" s="145"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.5">
+      <c r="A5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="146"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.5">
+      <c r="A6" s="145"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="146"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.5">
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="146"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.5">
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="146"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.5">
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="146"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D13"/>
@@ -26749,12 +26849,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
+    <col min="4" max="1013" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -26771,7 +26871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="65">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -26782,7 +26882,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.25">
+    <row r="3" spans="1:4" ht="39">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -26855,7 +26955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B5A0B4-9586-D946-AB25-20C3418D4E9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -26863,17 +26963,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="140"/>
+    <col min="1" max="1" width="16.1796875" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.81640625" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -26892,7 +26992,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="39">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -26912,7 +27012,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.7" customHeight="1">
+    <row r="3" spans="1:6" ht="13.75" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -26932,28 +27032,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.7" customHeight="1">
+    <row r="4" spans="1:6" ht="13.75" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.7" customHeight="1">
+    <row r="5" spans="1:6" ht="13.75" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.7" customHeight="1">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.7" customHeight="1">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.7" customHeight="1">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -26963,7 +27063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E7"/>
@@ -26972,12 +27072,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -26994,7 +27094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="178.5">
+    <row r="2" spans="1:5" ht="175.5">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27011,7 +27111,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="13">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -27043,95 +27143,6 @@
     <row r="7" spans="1:5">
       <c r="B7" s="60"/>
       <c r="C7" s="81"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="76.5">
-      <c r="A2" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="78" t="s">
-        <v>768</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>763</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="60"/>
-      <c r="C5" s="81"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="81"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="61"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="81"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="61"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -27143,6 +27154,95 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="48.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>765</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="78">
+      <c r="A2" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>761</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13">
+      <c r="A3" s="78" t="s">
+        <v>768</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="60"/>
+      <c r="C5" s="81"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="60"/>
+      <c r="C7" s="81"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="61"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="81"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="61"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:D484"/>
@@ -27151,14 +27251,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.453125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -27175,7 +27275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27189,7 +27289,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -28837,7 +28937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D120"/>
@@ -28846,13 +28946,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -28869,7 +28969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="63.75">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -28883,7 +28983,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -29329,7 +29429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D32"/>
@@ -29338,12 +29438,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -29360,7 +29460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -29374,7 +29474,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -29549,12 +29649,12 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="1014" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="1014" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29572,7 +29672,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="153">
+    <row r="2" spans="1:6" ht="143">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -29592,7 +29692,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="13">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -29637,14 +29737,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="5" width="21.1796875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.85546875" customWidth="1"/>
-    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="58.81640625" customWidth="1"/>
+    <col min="8" max="1011" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -29666,7 +29766,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="191.25">
+    <row r="2" spans="1:9" ht="195">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29695,7 +29795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25">
+    <row r="3" spans="1:9" ht="39">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29763,14 +29863,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29789,7 +29889,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="89.25">
+    <row r="2" spans="1:6" ht="91">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29809,7 +29909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="26">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -29903,19 +30003,19 @@
       <selection activeCell="A4" sqref="A4:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="49.453125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
-    <col min="11" max="1015" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.453125" customWidth="1"/>
+    <col min="11" max="1015" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -29936,7 +30036,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="102">
+    <row r="2" spans="1:10" ht="88">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29968,7 +30068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25">
+    <row r="3" spans="1:10" ht="39">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30497,27 +30597,27 @@
       <selection activeCell="F4" sqref="A4:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="55.42578125" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" customWidth="1"/>
-    <col min="10" max="10" width="81.42578125" customWidth="1"/>
-    <col min="11" max="11" width="93.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="15" width="8.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="55.453125" customWidth="1"/>
+    <col min="8" max="8" width="47.81640625" customWidth="1"/>
+    <col min="9" max="9" width="52.453125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
+    <col min="11" max="11" width="93.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" customWidth="1"/>
+    <col min="14" max="15" width="8.453125" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" customWidth="1"/>
+    <col min="18" max="18" width="20.453125" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" customWidth="1"/>
+    <col min="20" max="1013" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" customHeight="1">
@@ -30549,7 +30649,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:19" ht="114.75">
+    <row r="2" spans="1:19" ht="117">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30590,7 +30690,7 @@
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
     </row>
-    <row r="3" spans="1:19" ht="38.25">
+    <row r="3" spans="1:19" ht="39">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30649,7 +30749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.25">
+    <row r="4" spans="1:19" ht="14">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -30657,7 +30757,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:19" ht="14.25">
+    <row r="5" spans="1:19" ht="14">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -30665,7 +30765,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25">
+    <row r="6" spans="1:19" ht="14">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -30675,7 +30775,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:19" ht="14.25">
+    <row r="7" spans="1:19" ht="14">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30686,7 +30786,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:19" ht="14.25">
+    <row r="8" spans="1:19" ht="14">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30697,7 +30797,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:19" ht="14.25">
+    <row r="9" spans="1:19" ht="14">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30709,7 +30809,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:19" ht="14.25">
+    <row r="10" spans="1:19" ht="14">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30721,7 +30821,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:19" ht="14.25">
+    <row r="11" spans="1:19" ht="14">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30733,7 +30833,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:19" ht="14.25">
+    <row r="12" spans="1:19" ht="14">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30745,7 +30845,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:19" ht="14.25">
+    <row r="13" spans="1:19" ht="14">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30757,7 +30857,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:19" ht="14.25">
+    <row r="14" spans="1:19" ht="14">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30769,7 +30869,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:19" ht="14.25">
+    <row r="15" spans="1:19" ht="14">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30781,7 +30881,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:19" ht="14.25">
+    <row r="16" spans="1:19" ht="14">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30793,7 +30893,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14.25">
+    <row r="17" spans="6:19" ht="14">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30805,7 +30905,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14.25">
+    <row r="18" spans="6:19" ht="14">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30817,7 +30917,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14.25">
+    <row r="19" spans="6:19" ht="14">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -30827,7 +30927,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14.25">
+    <row r="20" spans="6:19" ht="14">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -30835,7 +30935,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14.25">
+    <row r="21" spans="6:19" ht="14">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30846,7 +30946,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14.25">
+    <row r="22" spans="6:19" ht="14">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30858,7 +30958,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14.25">
+    <row r="23" spans="6:19" ht="14">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -30870,7 +30970,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14.25">
+    <row r="24" spans="6:19" ht="14">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -30878,7 +30978,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14.25">
+    <row r="25" spans="6:19" ht="14">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -30889,7 +30989,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14.25">
+    <row r="26" spans="6:19" ht="14">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -30901,7 +31001,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14.25">
+    <row r="27" spans="6:19" ht="14">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -30912,7 +31012,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14.25">
+    <row r="28" spans="6:19" ht="14">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -30922,7 +31022,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14.25">
+    <row r="29" spans="6:19" ht="14">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -30933,7 +31033,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14.25">
+    <row r="30" spans="6:19" ht="14">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -30944,7 +31044,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14.25">
+    <row r="31" spans="6:19" ht="14">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -30955,7 +31055,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14.25">
+    <row r="32" spans="6:19" ht="14">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -30964,7 +31064,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14.25">
+    <row r="33" spans="6:19" ht="14">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -30973,7 +31073,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14.25">
+    <row r="34" spans="6:19" ht="14">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -30983,7 +31083,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14.25">
+    <row r="35" spans="6:19" ht="14">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -30992,7 +31092,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14.25">
+    <row r="36" spans="6:19" ht="14">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -31108,7 +31208,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14.25">
+    <row r="48" spans="6:19" ht="14">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -31199,26 +31299,26 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="58.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="58.453125" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="87.140625" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="87.1796875" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -31242,7 +31342,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:17" ht="57.95" customHeight="1">
+    <row r="2" spans="1:17" ht="58" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31291,7 +31391,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="38.25">
+    <row r="3" spans="1:17" ht="39">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -33349,29 +33449,29 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:XFD194"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD192"/>
+      <selection pane="bottomLeft" activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.1796875" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="30" t="s">
         <v>136</v>
       </c>
@@ -33385,7 +33485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93.95" customHeight="1">
+    <row r="2" spans="1:11" ht="94" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -33416,8 +33516,11 @@
       <c r="J2" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="25.5">
+      <c r="K2" s="22" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -33448,8 +33551,11 @@
       <c r="J3" s="26" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="26" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>1103</v>
       </c>
@@ -33467,7 +33573,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
@@ -33485,7 +33591,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>1103</v>
       </c>
@@ -33503,7 +33609,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -33523,7 +33629,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1103</v>
       </c>
@@ -33543,7 +33649,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>1103</v>
       </c>
@@ -33563,7 +33669,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>1103</v>
       </c>
@@ -33585,7 +33691,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>1103</v>
       </c>
@@ -33605,7 +33711,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>1103</v>
       </c>
@@ -33625,7 +33731,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>1103</v>
       </c>
@@ -33645,7 +33751,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>1103</v>
       </c>
@@ -33664,7 +33770,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>1103</v>
       </c>
@@ -33684,7 +33790,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>1103</v>
       </c>

</xml_diff>

<commit_message>
Revert "Feature flag case file view (#660)"
This reverts commit 5b1079b55ce4833aa524e7ae7b270aaf9dcabe76.
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-englandwales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF576B99-775F-47A7-8355-F168B63163BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC1D55-4FB8-444B-9E45-F7CC0D4BE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1905" yWindow="-18165" windowWidth="28800" windowHeight="15315" tabRatio="500" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="1470" windowWidth="36660" windowHeight="19395" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -22,48 +22,47 @@
     <sheet name="CaseEvent" sheetId="23" r:id="rId7"/>
     <sheet name="CaseEventToFields" sheetId="24" r:id="rId8"/>
     <sheet name="CaseField" sheetId="25" r:id="rId9"/>
-    <sheet name="Categories" sheetId="39" r:id="rId10"/>
-    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId11"/>
-    <sheet name="ComplexTypes" sheetId="26" r:id="rId12"/>
-    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId13"/>
-    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId14"/>
-    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId15"/>
-    <sheet name="SearchInputFields" sheetId="13" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId17"/>
-    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId18"/>
-    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId19"/>
-    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId20"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId21"/>
-    <sheet name="CaseRoles" sheetId="31" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId23"/>
-    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId24"/>
-    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId25"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId26"/>
-    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId27"/>
+    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId10"/>
+    <sheet name="ComplexTypes" sheetId="26" r:id="rId11"/>
+    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId12"/>
+    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId13"/>
+    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId18"/>
+    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
+    <sheet name="CaseRoles" sheetId="31" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId22"/>
+    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId23"/>
+    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId24"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId25"/>
+    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId26"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$Q$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseType!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseTypeTab!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Jurisdiction!$A$3:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">State!$A$3:$F$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">UserProfile!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">UserProfile!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="1143">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3596,35 +3595,6 @@
   </si>
   <si>
     <t>AccessProfiles</t>
-  </si>
-  <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>Unique ID that identifies the category
-MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Label that gets displayed in the UI. MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Specifies the display order for the category.</t>
-  </si>
-  <si>
-    <t>Identifies the parent category id for a sub-category.</t>
-  </si>
-  <si>
-    <t>CategoryID</t>
-  </si>
-  <si>
-    <t>CategoryLabel</t>
-  </si>
-  <si>
-    <t>ParentCategoryID</t>
-  </si>
-  <si>
-    <t>ID that identifies the document category
-MaxLength: 70</t>
   </si>
 </sst>
 </file>
@@ -4380,7 +4350,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="277">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4920,9 +4890,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -5404,14 +5371,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="256"/>
+    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="267" t="s">
         <v>1137</v>
       </c>
@@ -5419,7 +5386,7 @@
       <c r="C1" s="271"/>
       <c r="D1" s="270"/>
     </row>
-    <row r="2" spans="1:4" ht="88.5">
+    <row r="2" spans="1:4" ht="102.75">
       <c r="A2" s="269" t="s">
         <v>1133</v>
       </c>
@@ -5457,65 +5424,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5E47D-EB2A-4FD0-8353-2773316B4A69}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="12.5"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18">
-      <c r="A1" s="30" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:5" ht="65">
-      <c r="A2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>1144</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13">
-      <c r="A3" s="276" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>1148</v>
-      </c>
-      <c r="C3" s="276" t="s">
-        <v>1149</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243AEE7-DA61-4CDF-84FC-CA2502F211A6}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -5523,20 +5431,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="239"/>
-    <col min="3" max="3" width="54.7265625" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7265625" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.26953125" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="239"/>
+    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7265625" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.81640625" style="239"/>
-    <col min="1026" max="16384" width="10.81640625" style="238"/>
+    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" style="239"/>
+    <col min="1026" max="16384" width="10.85546875" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -5562,7 +5470,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="52">
+    <row r="2" spans="1:13" ht="63.75">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -5597,7 +5505,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.5">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -5649,7 +5557,7 @@
       <c r="L4" s="240"/>
       <c r="M4" s="240"/>
     </row>
-    <row r="5" spans="1:13" ht="13">
+    <row r="5" spans="1:13">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="242"/>
@@ -5664,7 +5572,7 @@
       <c r="L5" s="240"/>
       <c r="M5" s="240"/>
     </row>
-    <row r="6" spans="1:13" ht="13">
+    <row r="6" spans="1:13">
       <c r="A6" s="241"/>
       <c r="B6" s="241"/>
       <c r="D6" s="240"/>
@@ -5678,7 +5586,7 @@
       <c r="L6" s="240"/>
       <c r="M6" s="240"/>
     </row>
-    <row r="7" spans="1:13" ht="13">
+    <row r="7" spans="1:13">
       <c r="A7" s="241"/>
       <c r="B7" s="241"/>
       <c r="D7" s="240"/>
@@ -5714,35 +5622,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC74BE-16DE-BC4E-A66A-E3A520C8B91F}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O563"/>
+  <dimension ref="A1:N563"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomLeft" activeCell="A328" sqref="A328:XFD563"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="6" width="53.81640625" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="15" max="15" width="35" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:14" ht="18">
       <c r="A1" s="30" t="s">
         <v>192</v>
       </c>
@@ -5765,7 +5672,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:15" ht="55" customHeight="1">
+    <row r="2" spans="1:14" ht="54.95" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -5804,11 +5711,8 @@
       <c r="N2" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="O2" s="22" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="52">
+    </row>
+    <row r="3" spans="1:14" ht="51">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -5851,11 +5755,8 @@
       <c r="N3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="26" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>1036</v>
       </c>
@@ -5875,7 +5776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>1036</v>
       </c>
@@ -5898,7 +5799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>1036</v>
       </c>
@@ -5915,7 +5816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>1036</v>
       </c>
@@ -5932,7 +5833,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>1036</v>
       </c>
@@ -5949,7 +5850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="13">
+    <row r="9" spans="1:14">
       <c r="A9" s="121" t="s">
         <v>1036</v>
       </c>
@@ -5972,7 +5873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>1037</v>
       </c>
@@ -5989,7 +5890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>1037</v>
       </c>
@@ -6006,7 +5907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>1037</v>
       </c>
@@ -6023,7 +5924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>1037</v>
       </c>
@@ -6040,7 +5941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13">
+    <row r="14" spans="1:14">
       <c r="A14" s="121" t="s">
         <v>1037</v>
       </c>
@@ -6063,7 +5964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>1062</v>
       </c>
@@ -6080,7 +5981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:14">
       <c r="A16" s="105" t="s">
         <v>1062</v>
       </c>
@@ -6205,7 +6106,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13">
+    <row r="22" spans="1:9">
       <c r="A22" s="121" t="s">
         <v>1062</v>
       </c>
@@ -6250,7 +6151,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13">
+    <row r="24" spans="1:9">
       <c r="A24" s="121" t="s">
         <v>1063</v>
       </c>
@@ -6291,7 +6192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13">
+    <row r="26" spans="1:9">
       <c r="A26" s="121" t="s">
         <v>1023</v>
       </c>
@@ -6499,7 +6400,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13">
+    <row r="36" spans="1:9">
       <c r="A36" s="121" t="s">
         <v>1018</v>
       </c>
@@ -6854,7 +6755,7 @@
       <c r="J50" s="43"/>
       <c r="K50" s="43"/>
     </row>
-    <row r="51" spans="1:11" ht="13">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -6881,7 +6782,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
     </row>
-    <row r="52" spans="1:11" ht="13">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -6908,7 +6809,7 @@
       <c r="J52" s="43"/>
       <c r="K52" s="43"/>
     </row>
-    <row r="53" spans="1:11" ht="13">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -7306,7 +7207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="13">
+    <row r="69" spans="1:9">
       <c r="A69" s="121" t="s">
         <v>80</v>
       </c>
@@ -7327,7 +7228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.15" customHeight="1">
+    <row r="70" spans="1:9" ht="14.1" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -7350,7 +7251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="10" customHeight="1">
+    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -7556,7 +7457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="13">
+    <row r="81" spans="1:14">
       <c r="A81" s="121" t="s">
         <v>1020</v>
       </c>
@@ -7647,7 +7548,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="13">
+    <row r="85" spans="1:14">
       <c r="A85" s="121" t="s">
         <v>1056</v>
       </c>
@@ -7717,7 +7618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="13">
+    <row r="88" spans="1:14">
       <c r="A88" s="121" t="s">
         <v>1040</v>
       </c>
@@ -7778,7 +7679,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="13">
+    <row r="91" spans="1:14">
       <c r="A91" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7799,7 +7700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="13">
+    <row r="92" spans="1:14">
       <c r="A92" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7820,7 +7721,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="13">
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
         <v>1014</v>
       </c>
@@ -7849,7 +7750,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="13">
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
         <v>1014</v>
       </c>
@@ -7875,7 +7776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="13">
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
         <v>1014</v>
       </c>
@@ -7895,7 +7796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="13">
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
         <v>1014</v>
       </c>
@@ -7921,7 +7822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="13">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>1014</v>
       </c>
@@ -7941,7 +7842,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="13">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>1014</v>
       </c>
@@ -7963,7 +7864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>1014</v>
       </c>
@@ -7982,7 +7883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>1014</v>
       </c>
@@ -8001,7 +7902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>1014</v>
       </c>
@@ -8020,7 +7921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>1014</v>
       </c>
@@ -8043,7 +7944,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>1014</v>
       </c>
@@ -8062,7 +7963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>1014</v>
       </c>
@@ -8085,7 +7986,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>1014</v>
       </c>
@@ -8104,7 +8005,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>1014</v>
       </c>
@@ -8127,7 +8028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>1014</v>
       </c>
@@ -8150,7 +8051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="13">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>1014</v>
       </c>
@@ -8175,9 +8076,8 @@
       <c r="I108" t="s">
         <v>31</v>
       </c>
-      <c r="O108" s="233"/>
-    </row>
-    <row r="109" spans="1:15" ht="13">
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>1014</v>
       </c>
@@ -8199,7 +8099,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>1014</v>
       </c>
@@ -8218,7 +8118,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="13">
+    <row r="111" spans="1:9">
       <c r="A111" s="121" t="s">
         <v>1014</v>
       </c>
@@ -8238,7 +8138,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>1003</v>
       </c>
@@ -8404,7 +8304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="13">
+    <row r="119" spans="1:13">
       <c r="A119" s="121" t="s">
         <v>1003</v>
       </c>
@@ -8508,7 +8408,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="13">
+    <row r="124" spans="1:13">
       <c r="A124" s="121" t="s">
         <v>998</v>
       </c>
@@ -8699,7 +8599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="13">
+    <row r="133" spans="1:9">
       <c r="A133" s="121" t="s">
         <v>1064</v>
       </c>
@@ -8780,7 +8680,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="13">
+    <row r="137" spans="1:9">
       <c r="A137" s="121" t="s">
         <v>883</v>
       </c>
@@ -8981,7 +8881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="13">
+    <row r="147" spans="1:14">
       <c r="A147" s="121" t="s">
         <v>884</v>
       </c>
@@ -9065,7 +8965,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="13">
+    <row r="151" spans="1:14">
       <c r="A151" s="121" t="s">
         <v>885</v>
       </c>
@@ -9086,7 +8986,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="13">
+    <row r="152" spans="1:14">
       <c r="A152" s="121" t="s">
         <v>1076</v>
       </c>
@@ -9107,7 +9007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="13">
+    <row r="153" spans="1:14">
       <c r="A153" s="121" t="s">
         <v>1066</v>
       </c>
@@ -9171,7 +9071,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="13">
+    <row r="156" spans="1:14">
       <c r="A156" s="121" t="s">
         <v>936</v>
       </c>
@@ -9239,7 +9139,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="13">
+    <row r="159" spans="1:14">
       <c r="A159" s="121" t="s">
         <v>946</v>
       </c>
@@ -9284,7 +9184,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="13">
+    <row r="161" spans="1:9">
       <c r="A161" s="121" t="s">
         <v>953</v>
       </c>
@@ -9400,7 +9300,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="13">
+    <row r="166" spans="1:9">
       <c r="A166" s="121" t="s">
         <v>956</v>
       </c>
@@ -9525,7 +9425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="13">
+    <row r="172" spans="1:9">
       <c r="A172" s="121" t="s">
         <v>986</v>
       </c>
@@ -11225,7 +11125,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="13">
+    <row r="243" spans="1:11">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -11251,7 +11151,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="13">
+    <row r="244" spans="1:11">
       <c r="A244" s="121" t="s">
         <v>0</v>
       </c>
@@ -11298,7 +11198,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
     </row>
-    <row r="246" spans="1:11" ht="13">
+    <row r="246" spans="1:11">
       <c r="A246" t="s">
         <v>861</v>
       </c>
@@ -11325,7 +11225,7 @@
       <c r="J246" s="43"/>
       <c r="K246" s="43"/>
     </row>
-    <row r="247" spans="1:11" ht="13">
+    <row r="247" spans="1:11">
       <c r="A247" t="s">
         <v>861</v>
       </c>
@@ -11352,7 +11252,7 @@
       <c r="J247" s="43"/>
       <c r="K247" s="43"/>
     </row>
-    <row r="248" spans="1:11" ht="13">
+    <row r="248" spans="1:11">
       <c r="A248" t="s">
         <v>861</v>
       </c>
@@ -11381,7 +11281,7 @@
       <c r="J248" s="43"/>
       <c r="K248" s="43"/>
     </row>
-    <row r="249" spans="1:11" ht="13">
+    <row r="249" spans="1:11">
       <c r="A249" t="s">
         <v>861</v>
       </c>
@@ -11410,7 +11310,7 @@
       <c r="J249" s="43"/>
       <c r="K249" s="43"/>
     </row>
-    <row r="250" spans="1:11" ht="13">
+    <row r="250" spans="1:11">
       <c r="A250" s="121" t="s">
         <v>861</v>
       </c>
@@ -11764,7 +11664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="13">
+    <row r="265" spans="1:14">
       <c r="A265" s="121" t="s">
         <v>1034</v>
       </c>
@@ -12028,7 +11928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="13">
+    <row r="275" spans="1:14">
       <c r="A275" s="121" t="s">
         <v>1033</v>
       </c>
@@ -12120,7 +12020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13">
+    <row r="279" spans="1:14" ht="13.5">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -12292,7 +12192,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="13">
+    <row r="287" spans="1:14">
       <c r="A287" t="s">
         <v>102</v>
       </c>
@@ -12315,7 +12215,7 @@
       <c r="J287" s="43"/>
       <c r="K287" s="43"/>
     </row>
-    <row r="288" spans="1:14" ht="13">
+    <row r="288" spans="1:14">
       <c r="A288" s="121" t="s">
         <v>102</v>
       </c>
@@ -12875,7 +12775,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="13">
+    <row r="309" spans="1:9">
       <c r="A309" s="121" t="s">
         <v>103</v>
       </c>
@@ -12900,7 +12800,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:9" ht="13">
+    <row r="310" spans="1:9">
       <c r="A310" s="121" t="s">
         <v>103</v>
       </c>
@@ -13390,7 +13290,7 @@
       <c r="G329" s="31"/>
       <c r="H329" s="31"/>
     </row>
-    <row r="330" spans="1:9" ht="13">
+    <row r="330" spans="1:9">
       <c r="A330" s="121"/>
       <c r="B330" s="121"/>
       <c r="C330" s="121"/>
@@ -13401,7 +13301,7 @@
       <c r="H330" s="205"/>
       <c r="I330" s="124"/>
     </row>
-    <row r="331" spans="1:9" ht="13">
+    <row r="331" spans="1:9">
       <c r="A331" s="121"/>
       <c r="B331" s="121"/>
       <c r="C331" s="121"/>
@@ -13417,7 +13317,7 @@
       <c r="G332" s="31"/>
       <c r="H332" s="31"/>
     </row>
-    <row r="333" spans="1:9" ht="13">
+    <row r="333" spans="1:9">
       <c r="A333" s="121"/>
       <c r="B333" s="121"/>
       <c r="C333" s="121"/>
@@ -13445,7 +13345,7 @@
       <c r="G336" s="31"/>
       <c r="H336" s="31"/>
     </row>
-    <row r="337" spans="1:9" ht="13">
+    <row r="337" spans="1:9">
       <c r="A337" s="121"/>
       <c r="B337" s="121"/>
       <c r="C337" s="121"/>
@@ -13479,7 +13379,7 @@
       <c r="G341" s="31"/>
       <c r="H341" s="31"/>
     </row>
-    <row r="342" spans="1:9" ht="13">
+    <row r="342" spans="1:9">
       <c r="A342" s="121"/>
       <c r="B342" s="121"/>
       <c r="C342" s="121"/>
@@ -13490,7 +13390,7 @@
       <c r="H342" s="205"/>
       <c r="I342" s="124"/>
     </row>
-    <row r="343" spans="1:9" ht="13">
+    <row r="343" spans="1:9">
       <c r="A343" s="105"/>
       <c r="B343" s="121"/>
       <c r="E343" s="117"/>
@@ -13498,7 +13398,7 @@
       <c r="G343" s="31"/>
       <c r="H343" s="31"/>
     </row>
-    <row r="344" spans="1:9" ht="13">
+    <row r="344" spans="1:9">
       <c r="A344" s="105"/>
       <c r="B344" s="121"/>
       <c r="E344" s="117"/>
@@ -13506,28 +13406,28 @@
       <c r="G344" s="31"/>
       <c r="H344" s="31"/>
     </row>
-    <row r="345" spans="1:9" ht="13">
+    <row r="345" spans="1:9">
       <c r="A345" s="105"/>
       <c r="E345" s="117"/>
       <c r="F345" s="31"/>
       <c r="G345" s="31"/>
       <c r="H345" s="31"/>
     </row>
-    <row r="346" spans="1:9" ht="13">
+    <row r="346" spans="1:9">
       <c r="A346" s="105"/>
       <c r="E346" s="117"/>
       <c r="F346" s="31"/>
       <c r="G346" s="31"/>
       <c r="H346" s="31"/>
     </row>
-    <row r="347" spans="1:9" ht="13">
+    <row r="347" spans="1:9">
       <c r="A347" s="105"/>
       <c r="E347" s="117"/>
       <c r="F347" s="31"/>
       <c r="G347" s="31"/>
       <c r="H347" s="31"/>
     </row>
-    <row r="348" spans="1:9" ht="13">
+    <row r="348" spans="1:9">
       <c r="A348" s="121"/>
       <c r="B348" s="121"/>
       <c r="C348" s="121"/>
@@ -14379,7 +14279,7 @@
       <c r="G474" s="31"/>
       <c r="H474" s="31"/>
     </row>
-    <row r="475" spans="1:9" ht="13">
+    <row r="475" spans="1:9">
       <c r="A475" s="121"/>
       <c r="B475" s="121"/>
       <c r="C475" s="121"/>
@@ -14390,7 +14290,7 @@
       <c r="H475" s="205"/>
       <c r="I475" s="124"/>
     </row>
-    <row r="476" spans="1:9" ht="13">
+    <row r="476" spans="1:9">
       <c r="A476" s="121"/>
       <c r="B476" s="121"/>
       <c r="C476" s="121"/>
@@ -14401,55 +14301,55 @@
       <c r="H476" s="31"/>
       <c r="I476" s="124"/>
     </row>
-    <row r="477" spans="1:9" ht="13">
+    <row r="477" spans="1:9">
       <c r="A477" s="105"/>
       <c r="E477" s="117"/>
       <c r="F477" s="105"/>
       <c r="G477" s="31"/>
     </row>
-    <row r="478" spans="1:9" ht="13">
+    <row r="478" spans="1:9">
       <c r="A478" s="105"/>
       <c r="E478" s="117"/>
       <c r="F478" s="105"/>
       <c r="G478" s="31"/>
     </row>
-    <row r="479" spans="1:9" ht="13">
+    <row r="479" spans="1:9">
       <c r="A479" s="105"/>
       <c r="E479" s="117"/>
       <c r="F479" s="105"/>
       <c r="G479" s="31"/>
     </row>
-    <row r="480" spans="1:9" ht="13">
+    <row r="480" spans="1:9">
       <c r="A480" s="105"/>
       <c r="E480" s="117"/>
       <c r="F480" s="105"/>
       <c r="G480" s="31"/>
     </row>
-    <row r="481" spans="1:8" ht="13">
+    <row r="481" spans="1:8">
       <c r="A481" s="105"/>
       <c r="E481" s="117"/>
       <c r="F481" s="105"/>
       <c r="G481" s="31"/>
     </row>
-    <row r="482" spans="1:8" ht="13">
+    <row r="482" spans="1:8">
       <c r="A482" s="105"/>
       <c r="E482" s="117"/>
       <c r="F482" s="105"/>
       <c r="G482" s="31"/>
     </row>
-    <row r="483" spans="1:8" ht="13">
+    <row r="483" spans="1:8">
       <c r="A483" s="105"/>
       <c r="E483" s="117"/>
       <c r="F483" s="105"/>
       <c r="G483" s="31"/>
     </row>
-    <row r="484" spans="1:8" ht="13">
+    <row r="484" spans="1:8">
       <c r="A484" s="105"/>
       <c r="E484" s="117"/>
       <c r="F484" s="105"/>
       <c r="G484" s="31"/>
     </row>
-    <row r="485" spans="1:8" ht="13">
+    <row r="485" spans="1:8">
       <c r="A485" s="105"/>
       <c r="E485" s="117"/>
       <c r="F485" s="105"/>
@@ -14565,7 +14465,7 @@
       <c r="G507" s="31"/>
       <c r="H507" s="31"/>
     </row>
-    <row r="508" spans="1:10" ht="13">
+    <row r="508" spans="1:10">
       <c r="A508" s="121"/>
       <c r="B508" s="121"/>
       <c r="C508" s="121"/>
@@ -14576,7 +14476,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13">
+    <row r="509" spans="1:10" ht="13.5">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -14587,7 +14487,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13">
+    <row r="510" spans="1:10" ht="13.5">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -14598,7 +14498,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13">
+    <row r="511" spans="1:10" ht="13.5">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -14680,7 +14580,7 @@
       <c r="G525" s="31"/>
       <c r="H525" s="31"/>
     </row>
-    <row r="526" spans="1:9" ht="13">
+    <row r="526" spans="1:9">
       <c r="A526" s="121"/>
       <c r="B526" s="121"/>
       <c r="C526" s="121"/>
@@ -14801,7 +14701,7 @@
       <c r="G546" s="31"/>
       <c r="H546" s="31"/>
     </row>
-    <row r="547" spans="1:9" ht="13">
+    <row r="547" spans="1:9">
       <c r="A547" s="121"/>
       <c r="B547" s="121"/>
       <c r="C547" s="121"/>
@@ -14888,7 +14788,7 @@
       <c r="G562" s="31"/>
       <c r="H562" s="31"/>
     </row>
-    <row r="563" spans="1:9" ht="13">
+    <row r="563" spans="1:9">
       <c r="A563" s="121"/>
       <c r="B563" s="121"/>
       <c r="C563" s="121"/>
@@ -14936,7 +14836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EE7EEF-305D-1145-A07B-3D132F6E2765}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K402"/>
@@ -14947,21 +14847,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1">
+    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -14980,7 +14880,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:11" ht="67" customHeight="1">
+    <row r="2" spans="1:11" ht="66.95" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -15007,7 +14907,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13">
+    <row r="3" spans="1:11">
       <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
@@ -21161,7 +21061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
@@ -21169,13 +21069,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -21189,7 +21089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="169">
+    <row r="2" spans="1:5" ht="165.75">
       <c r="A2" s="273" t="s">
         <v>14</v>
       </c>
@@ -21203,7 +21103,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="274" t="s">
         <v>19</v>
       </c>
@@ -21963,7 +21863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABABBB7-6A1E-0B4E-82BF-6CDF21C8BDBC}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -21974,13 +21874,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.453125" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.453125" style="170"/>
+    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21997,7 +21897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="78">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -22011,7 +21911,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="173" t="s">
         <v>6</v>
       </c>
@@ -25937,7 +25837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H25"/>
@@ -25946,19 +25846,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.453125" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" customWidth="1"/>
-    <col min="7" max="7" width="43.453125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="1021" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="29.5">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -25976,7 +25876,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="65.5">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26000,7 +25900,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26026,86 +25926,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5">
+    <row r="4" spans="1:8" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="133"/>
       <c r="G4" s="12"/>
       <c r="H4" s="128"/>
     </row>
-    <row r="5" spans="1:8" ht="14.5">
+    <row r="5" spans="1:8" ht="15">
       <c r="E5" s="7"/>
       <c r="F5" s="133"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="14.5">
+    <row r="6" spans="1:8" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="133"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="14.5">
+    <row r="7" spans="1:8" ht="15">
       <c r="E7" s="7"/>
       <c r="F7" s="133"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="14.5">
+    <row r="8" spans="1:8" ht="15">
       <c r="E8" s="7"/>
       <c r="F8" s="133"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.5">
+    <row r="9" spans="1:8" ht="15">
       <c r="E9" s="7"/>
       <c r="F9" s="133"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="14.5">
+    <row r="10" spans="1:8" ht="15">
       <c r="E10" s="7"/>
       <c r="F10" s="133"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="14.5">
+    <row r="11" spans="1:8" ht="15">
       <c r="E11" s="7"/>
       <c r="F11" s="133"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="14.5">
+    <row r="12" spans="1:8" ht="15">
       <c r="E12" s="7"/>
       <c r="F12" s="133"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="14.5">
+    <row r="13" spans="1:8" ht="15">
       <c r="D13" s="202"/>
       <c r="E13" s="7"/>
       <c r="F13" s="133"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="14.5">
+    <row r="14" spans="1:8" ht="15">
       <c r="E14" s="7"/>
       <c r="F14" s="133"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="14.5">
+    <row r="15" spans="1:8" ht="15">
       <c r="C15" s="31"/>
       <c r="E15" s="7"/>
       <c r="F15" s="133"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="14.5">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="31"/>
       <c r="E16" s="7"/>
       <c r="F16" s="133"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="14.5">
+    <row r="17" spans="2:8" ht="15">
       <c r="E17" s="7"/>
       <c r="F17" s="133"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="14.5">
+    <row r="18" spans="2:8" ht="15">
       <c r="E18" s="7"/>
       <c r="F18" s="133"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="14.5">
+    <row r="19" spans="2:8" ht="15">
       <c r="E19" s="7"/>
       <c r="H19" s="133"/>
     </row>
@@ -26127,6 +26027,163 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="105"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
+      <c r="A1" s="62" t="s">
+        <v>745</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>746</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
+        <v>925</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15">
+      <c r="A3" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="105"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="105"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="105"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="105"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="105"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="105"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="105"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="105"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="105"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="105"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26138,64 +26195,69 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" customWidth="1"/>
-    <col min="7" max="7" width="29.453125" customWidth="1"/>
-    <col min="8" max="1013" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
-      <c r="A1" s="62" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1" s="69" t="s">
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="72" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="87">
+      <c r="E1" s="76"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="130"/>
+    </row>
+    <row r="2" spans="1:8" ht="76.5">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
+        <v>744</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="131" t="s">
         <v>925</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.5">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26211,46 +26273,33 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="7"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
+    <row r="4" spans="1:8" ht="15">
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" s="107"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.25">
+      <c r="D6" s="114"/>
+    </row>
+    <row r="7" spans="1:8" ht="14.25">
+      <c r="D7" s="114"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.25">
+      <c r="D8" s="114"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="F9" s="37"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26284,6 +26333,9 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26295,69 +26347,64 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="3" width="31.453125" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="7" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" customWidth="1"/>
-    <col min="9" max="1022" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5">
-      <c r="A1" s="72" t="s">
-        <v>749</v>
-      </c>
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>750</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
-    </row>
-    <row r="2" spans="1:8" ht="78">
+      <c r="E1" s="31"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" ht="105">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>744</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="131" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
         <v>925</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26373,33 +26420,21 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="128" t="s">
-        <v>58</v>
+      <c r="F3" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5">
-      <c r="H4" s="68"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="D5" s="107"/>
-    </row>
-    <row r="6" spans="1:8" ht="14">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="D6" s="114"/>
     </row>
-    <row r="7" spans="1:8" ht="14">
-      <c r="D7" s="114"/>
-    </row>
-    <row r="8" spans="1:8" ht="14">
-      <c r="D8" s="114"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" s="37"/>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26433,9 +26468,6 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26447,131 +26479,162 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" customWidth="1"/>
-    <col min="8" max="1008" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="140"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="30" t="s">
-        <v>750</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="135" t="s">
+        <v>927</v>
+      </c>
+      <c r="B1" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" ht="87">
-      <c r="A2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="23" t="s">
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+    </row>
+    <row r="2" spans="1:9" ht="38.25">
+      <c r="A2" s="141"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="142" t="s">
+        <v>928</v>
+      </c>
+      <c r="D2" s="142" t="s">
         <v>746</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
-        <v>747</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
-        <v>925</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.5">
-      <c r="A3" s="67" t="s">
+      <c r="E2" s="142" t="s">
+        <v>929</v>
+      </c>
+      <c r="F2" s="141" t="s">
+        <v>930</v>
+      </c>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+    </row>
+    <row r="3" spans="1:9" ht="15">
+      <c r="A3" s="143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="144" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="D3" s="144" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="67" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="143" t="s">
         <v>145</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="143" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="14">
-      <c r="D6" s="114"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="105"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="105"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="105"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="105"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="105"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="105"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="105"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="105"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="105"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="105"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="105"/>
+      <c r="H3" s="143" t="s">
+        <v>931</v>
+      </c>
+      <c r="I3" s="143" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
+      <c r="A4" s="145"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+    </row>
+    <row r="5" spans="1:9" ht="15">
+      <c r="A5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="146"/>
+    </row>
+    <row r="6" spans="1:9" ht="15">
+      <c r="A6" s="145"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="146"/>
+    </row>
+    <row r="7" spans="1:9" ht="15">
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="146"/>
+    </row>
+    <row r="8" spans="1:9" ht="15">
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="146"/>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="146"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
   </headerFooter>
@@ -26586,14 +26649,14 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="256"/>
+    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="267" t="s">
         <v>1134</v>
       </c>
@@ -26678,169 +26741,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="1" width="31.81640625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="140"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="135" t="s">
-        <v>927</v>
-      </c>
-      <c r="B1" s="136" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="138" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-    </row>
-    <row r="2" spans="1:9" ht="39">
-      <c r="A2" s="141"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142" t="s">
-        <v>928</v>
-      </c>
-      <c r="D2" s="142" t="s">
-        <v>746</v>
-      </c>
-      <c r="E2" s="142" t="s">
-        <v>929</v>
-      </c>
-      <c r="F2" s="141" t="s">
-        <v>930</v>
-      </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.5">
-      <c r="A3" s="143" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="144" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="144" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="143" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="143" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="143" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="143" t="s">
-        <v>931</v>
-      </c>
-      <c r="I3" s="143" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.5">
-      <c r="A4" s="145"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-    </row>
-    <row r="5" spans="1:9" ht="14.5">
-      <c r="A5" s="145"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="146"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.5">
-      <c r="A6" s="145"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="139"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="146"/>
-    </row>
-    <row r="7" spans="1:9" ht="14.5">
-      <c r="A7" s="145"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="146"/>
-    </row>
-    <row r="8" spans="1:9" ht="14.5">
-      <c r="A8" s="145"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="146"/>
-    </row>
-    <row r="9" spans="1:9" ht="14.5">
-      <c r="A9" s="145"/>
-      <c r="B9" s="146"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="146"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="146"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D13"/>
@@ -26849,12 +26749,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.453125" customWidth="1"/>
+    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -26871,7 +26771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="65">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -26882,7 +26782,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39">
+    <row r="3" spans="1:4" ht="38.25">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -26955,7 +26855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B5A0B4-9586-D946-AB25-20C3418D4E9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -26963,17 +26863,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.81640625" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="140"/>
+    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -26992,7 +26892,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="39">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -27012,7 +26912,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.75" customHeight="1">
+    <row r="3" spans="1:6" ht="13.7" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -27032,28 +26932,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1">
+    <row r="4" spans="1:6" ht="13.7" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1">
+    <row r="5" spans="1:6" ht="13.7" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1">
+    <row r="6" spans="1:6" ht="13.7" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1">
+    <row r="7" spans="1:6" ht="13.7" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1">
+    <row r="8" spans="1:6" ht="13.7" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27063,7 +26963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E7"/>
@@ -27072,12 +26972,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -27094,7 +26994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="175.5">
+    <row r="2" spans="1:5" ht="178.5">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27111,7 +27011,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13">
+    <row r="3" spans="1:5">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -27143,6 +27043,95 @@
     <row r="7" spans="1:5">
       <c r="B7" s="60"/>
       <c r="C7" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>765</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="76.5">
+      <c r="A2" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>761</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="78" t="s">
+        <v>768</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="60"/>
+      <c r="C5" s="81"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="60"/>
+      <c r="C7" s="81"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="61"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="81"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="61"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -27154,95 +27143,6 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="78">
-      <c r="A2" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="13">
-      <c r="A3" s="78" t="s">
-        <v>768</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>763</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="60"/>
-      <c r="C5" s="81"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="81"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="61"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="81"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="61"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="81"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:D484"/>
@@ -27251,14 +27151,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.453125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -27275,7 +27175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27289,7 +27189,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -28937,7 +28837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D120"/>
@@ -28946,13 +28846,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.453125" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -28969,7 +28869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="63.75">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -28983,7 +28883,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -29429,7 +29329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D32"/>
@@ -29438,12 +29338,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -29460,7 +29360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -29474,7 +29374,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -29649,12 +29549,12 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="1014" width="10.453125" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="1014" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29672,7 +29572,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="143">
+    <row r="2" spans="1:6" ht="153">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -29692,7 +29592,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13">
+    <row r="3" spans="1:6">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -29737,14 +29637,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="5" width="21.1796875" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.81640625" customWidth="1"/>
-    <col min="8" max="1011" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -29766,7 +29666,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="195">
+    <row r="2" spans="1:9" ht="191.25">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29795,7 +29695,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39">
+    <row r="3" spans="1:9" ht="38.25">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29863,14 +29763,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29889,7 +29789,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="91">
+    <row r="2" spans="1:6" ht="89.25">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29909,7 +29809,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -30003,19 +29903,19 @@
       <selection activeCell="A4" sqref="A4:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" customWidth="1"/>
-    <col min="11" max="1015" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="1015" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -30036,7 +29936,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="88">
+    <row r="2" spans="1:10" ht="102">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30068,7 +29968,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="39">
+    <row r="3" spans="1:10" ht="38.25">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30597,27 +30497,27 @@
       <selection activeCell="F4" sqref="A4:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="55.453125" customWidth="1"/>
-    <col min="8" max="8" width="47.81640625" customWidth="1"/>
-    <col min="9" max="9" width="52.453125" customWidth="1"/>
-    <col min="10" max="10" width="81.453125" customWidth="1"/>
-    <col min="11" max="11" width="93.453125" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="23.453125" customWidth="1"/>
-    <col min="14" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="18.453125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" customWidth="1"/>
-    <col min="18" max="18" width="20.453125" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" customWidth="1"/>
-    <col min="20" max="1013" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" customWidth="1"/>
+    <col min="10" max="10" width="81.42578125" customWidth="1"/>
+    <col min="11" max="11" width="93.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" customHeight="1">
@@ -30649,7 +30549,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:19" ht="117">
+    <row r="2" spans="1:19" ht="114.75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30690,7 +30590,7 @@
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
     </row>
-    <row r="3" spans="1:19" ht="39">
+    <row r="3" spans="1:19" ht="38.25">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30749,7 +30649,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14">
+    <row r="4" spans="1:19" ht="14.25">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -30757,7 +30657,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:19" ht="14">
+    <row r="5" spans="1:19" ht="14.25">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -30765,7 +30665,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:19" ht="14">
+    <row r="6" spans="1:19" ht="14.25">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -30775,7 +30675,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:19" ht="14">
+    <row r="7" spans="1:19" ht="14.25">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30786,7 +30686,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:19" ht="14">
+    <row r="8" spans="1:19" ht="14.25">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30797,7 +30697,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:19" ht="14">
+    <row r="9" spans="1:19" ht="14.25">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30809,7 +30709,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:19" ht="14">
+    <row r="10" spans="1:19" ht="14.25">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30821,7 +30721,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:19" ht="14">
+    <row r="11" spans="1:19" ht="14.25">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30833,7 +30733,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:19" ht="14">
+    <row r="12" spans="1:19" ht="14.25">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30845,7 +30745,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:19" ht="14">
+    <row r="13" spans="1:19" ht="14.25">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30857,7 +30757,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:19" ht="14">
+    <row r="14" spans="1:19" ht="14.25">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30869,7 +30769,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:19" ht="14">
+    <row r="15" spans="1:19" ht="14.25">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30881,7 +30781,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:19" ht="14">
+    <row r="16" spans="1:19" ht="14.25">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30893,7 +30793,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14">
+    <row r="17" spans="6:19" ht="14.25">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30905,7 +30805,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14">
+    <row r="18" spans="6:19" ht="14.25">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30917,7 +30817,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14">
+    <row r="19" spans="6:19" ht="14.25">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -30927,7 +30827,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14">
+    <row r="20" spans="6:19" ht="14.25">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -30935,7 +30835,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14">
+    <row r="21" spans="6:19" ht="14.25">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30946,7 +30846,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14">
+    <row r="22" spans="6:19" ht="14.25">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30958,7 +30858,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14">
+    <row r="23" spans="6:19" ht="14.25">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -30970,7 +30870,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14">
+    <row r="24" spans="6:19" ht="14.25">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -30978,7 +30878,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14">
+    <row r="25" spans="6:19" ht="14.25">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -30989,7 +30889,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14">
+    <row r="26" spans="6:19" ht="14.25">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -31001,7 +30901,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14">
+    <row r="27" spans="6:19" ht="14.25">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -31012,7 +30912,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14">
+    <row r="28" spans="6:19" ht="14.25">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -31022,7 +30922,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14">
+    <row r="29" spans="6:19" ht="14.25">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -31033,7 +30933,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14">
+    <row r="30" spans="6:19" ht="14.25">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -31044,7 +30944,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14">
+    <row r="31" spans="6:19" ht="14.25">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -31055,7 +30955,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14">
+    <row r="32" spans="6:19" ht="14.25">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -31064,7 +30964,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14">
+    <row r="33" spans="6:19" ht="14.25">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -31073,7 +30973,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14">
+    <row r="34" spans="6:19" ht="14.25">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -31083,7 +30983,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14">
+    <row r="35" spans="6:19" ht="14.25">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -31092,7 +30992,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14">
+    <row r="36" spans="6:19" ht="14.25">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -31208,7 +31108,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14">
+    <row r="48" spans="6:19" ht="14.25">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -31299,26 +31199,26 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="8" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="58.453125" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="58.42578125" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.453125" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="87.1796875" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="87.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -31342,7 +31242,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:17" ht="58" customHeight="1">
+    <row r="2" spans="1:17" ht="57.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31391,7 +31291,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="39">
+    <row r="3" spans="1:17" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -33449,29 +33349,29 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:XFD194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="K167" sqref="K167"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.1796875" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="30" t="s">
         <v>136</v>
       </c>
@@ -33485,7 +33385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="94" customHeight="1">
+    <row r="2" spans="1:10" ht="93.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -33516,11 +33416,8 @@
       <c r="J2" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="13">
+    </row>
+    <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -33551,11 +33448,8 @@
       <c r="J3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="26" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>1103</v>
       </c>
@@ -33573,7 +33467,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
@@ -33591,7 +33485,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>1103</v>
       </c>
@@ -33609,7 +33503,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -33629,7 +33523,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>1103</v>
       </c>
@@ -33649,7 +33543,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>1103</v>
       </c>
@@ -33669,7 +33563,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>1103</v>
       </c>
@@ -33691,7 +33585,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>1103</v>
       </c>
@@ -33711,7 +33605,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>1103</v>
       </c>
@@ -33731,7 +33625,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>1103</v>
       </c>
@@ -33751,7 +33645,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>1103</v>
       </c>
@@ -33770,7 +33664,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>1103</v>
       </c>
@@ -33790,7 +33684,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>1103</v>
       </c>

</xml_diff>

<commit_message>
Ret 4284 - Feature flag case file view (#661)
* Feature flag case file view

* Fix case file view

* Make Categories prod file
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-englandwales\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC1D55-4FB8-444B-9E45-F7CC0D4BE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF576B99-775F-47A7-8355-F168B63163BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1470" windowWidth="36660" windowHeight="19395" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1905" yWindow="-18165" windowWidth="28800" windowHeight="15315" tabRatio="500" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -22,47 +22,48 @@
     <sheet name="CaseEvent" sheetId="23" r:id="rId7"/>
     <sheet name="CaseEventToFields" sheetId="24" r:id="rId8"/>
     <sheet name="CaseField" sheetId="25" r:id="rId9"/>
-    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId10"/>
-    <sheet name="ComplexTypes" sheetId="26" r:id="rId11"/>
-    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId12"/>
-    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId13"/>
-    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId14"/>
-    <sheet name="SearchInputFields" sheetId="13" r:id="rId15"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId17"/>
-    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId18"/>
-    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
-    <sheet name="CaseRoles" sheetId="31" r:id="rId21"/>
-    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId22"/>
-    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId23"/>
-    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId24"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId25"/>
-    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId26"/>
+    <sheet name="Categories" sheetId="39" r:id="rId10"/>
+    <sheet name="ChallengeQuestion" sheetId="35" r:id="rId11"/>
+    <sheet name="ComplexTypes" sheetId="26" r:id="rId12"/>
+    <sheet name="EventToComplexTypes" sheetId="29" r:id="rId13"/>
+    <sheet name="RoleToAccessProfiles" sheetId="38" r:id="rId14"/>
+    <sheet name="EnglandWales Scrubbed" sheetId="34" r:id="rId15"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId16"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId17"/>
+    <sheet name="WorkBasketInputFields" sheetId="15" r:id="rId18"/>
+    <sheet name="WorkBasketResultFields" sheetId="16" r:id="rId19"/>
+    <sheet name="SearchCaseResultFields" sheetId="30" r:id="rId20"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId21"/>
+    <sheet name="CaseRoles" sheetId="31" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="18" r:id="rId23"/>
+    <sheet name="AuthorisationCaseType" sheetId="19" r:id="rId24"/>
+    <sheet name="AuthorisationCaseField" sheetId="20" r:id="rId25"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="21" r:id="rId26"/>
+    <sheet name="AuthorisationCaseState" sheetId="22" r:id="rId27"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseField!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$Q$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CaseRoles!$A$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseType!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseTypeTab!$A$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Jurisdiction!$A$3:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">SearchCaseResultFields!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">SearchInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">SearchResultFields!$A$3:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">State!$A$3:$F$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">UserProfile!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">UserProfile!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketInputFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1152">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3595,6 +3596,35 @@
   </si>
   <si>
     <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Unique ID that identifies the category
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label that gets displayed in the UI. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Specifies the display order for the category.</t>
+  </si>
+  <si>
+    <t>Identifies the parent category id for a sub-category.</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>CategoryLabel</t>
+  </si>
+  <si>
+    <t>ParentCategoryID</t>
+  </si>
+  <si>
+    <t>ID that identifies the document category
+MaxLength: 70</t>
   </si>
 </sst>
 </file>
@@ -4350,7 +4380,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4890,6 +4920,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -5371,14 +5404,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="17.5">
       <c r="A1" s="267" t="s">
         <v>1137</v>
       </c>
@@ -5386,7 +5419,7 @@
       <c r="C1" s="271"/>
       <c r="D1" s="270"/>
     </row>
-    <row r="2" spans="1:4" ht="102.75">
+    <row r="2" spans="1:4" ht="88.5">
       <c r="A2" s="269" t="s">
         <v>1133</v>
       </c>
@@ -5424,6 +5457,65 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD5E47D-EB2A-4FD0-8353-2773316B4A69}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="12.5"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="65">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13">
+      <c r="A3" s="276" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C3" s="276" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243AEE7-DA61-4CDF-84FC-CA2502F211A6}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -5431,20 +5523,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="239"/>
-    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="239"/>
+    <col min="3" max="3" width="54.7265625" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.7265625" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.26953125" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" style="239"/>
-    <col min="1026" max="16384" width="10.85546875" style="238"/>
+    <col min="10" max="10" width="43.7265625" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.81640625" style="239"/>
+    <col min="1026" max="16384" width="10.81640625" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -5470,7 +5562,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="63.75">
+    <row r="2" spans="1:13" ht="52">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -5505,7 +5597,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75">
+    <row r="3" spans="1:13" ht="15.5">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -5557,7 +5649,7 @@
       <c r="L4" s="240"/>
       <c r="M4" s="240"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="13">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="242"/>
@@ -5572,7 +5664,7 @@
       <c r="L5" s="240"/>
       <c r="M5" s="240"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="13">
       <c r="A6" s="241"/>
       <c r="B6" s="241"/>
       <c r="D6" s="240"/>
@@ -5586,7 +5678,7 @@
       <c r="L6" s="240"/>
       <c r="M6" s="240"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="13">
       <c r="A7" s="241"/>
       <c r="B7" s="241"/>
       <c r="D7" s="240"/>
@@ -5622,34 +5714,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC74BE-16DE-BC4E-A66A-E3A520C8B91F}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:N563"/>
+  <dimension ref="A1:O563"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A328" sqref="A328:XFD563"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="53.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" customWidth="1"/>
+    <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="30" t="s">
         <v>192</v>
       </c>
@@ -5672,7 +5765,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:14" ht="54.95" customHeight="1">
+    <row r="2" spans="1:15" ht="55" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -5711,8 +5804,11 @@
       <c r="N2" s="24" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="51">
+      <c r="O2" s="22" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="52">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -5755,8 +5851,11 @@
       <c r="N3" s="26" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="26" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1036</v>
       </c>
@@ -5776,7 +5875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>1036</v>
       </c>
@@ -5799,7 +5898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>1036</v>
       </c>
@@ -5816,7 +5915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1036</v>
       </c>
@@ -5833,7 +5932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>1036</v>
       </c>
@@ -5850,7 +5949,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15" ht="13">
       <c r="A9" s="121" t="s">
         <v>1036</v>
       </c>
@@ -5873,7 +5972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>1037</v>
       </c>
@@ -5890,7 +5989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>1037</v>
       </c>
@@ -5907,7 +6006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>1037</v>
       </c>
@@ -5924,7 +6023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>1037</v>
       </c>
@@ -5941,7 +6040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15" ht="13">
       <c r="A14" s="121" t="s">
         <v>1037</v>
       </c>
@@ -5964,7 +6063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>1062</v>
       </c>
@@ -5981,7 +6080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="105" t="s">
         <v>1062</v>
       </c>
@@ -6106,7 +6205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="13">
       <c r="A22" s="121" t="s">
         <v>1062</v>
       </c>
@@ -6151,7 +6250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="13">
       <c r="A24" s="121" t="s">
         <v>1063</v>
       </c>
@@ -6192,7 +6291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="13">
       <c r="A26" s="121" t="s">
         <v>1023</v>
       </c>
@@ -6400,7 +6499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" ht="13">
       <c r="A36" s="121" t="s">
         <v>1018</v>
       </c>
@@ -6755,7 +6854,7 @@
       <c r="J50" s="43"/>
       <c r="K50" s="43"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" ht="13">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -6782,7 +6881,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" ht="13">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -6809,7 +6908,7 @@
       <c r="J52" s="43"/>
       <c r="K52" s="43"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" ht="13">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -7207,7 +7306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" ht="13">
       <c r="A69" s="121" t="s">
         <v>80</v>
       </c>
@@ -7228,7 +7327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.1" customHeight="1">
+    <row r="70" spans="1:9" ht="14.15" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -7251,7 +7350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
+    <row r="71" spans="1:9" ht="10" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -7457,7 +7556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" ht="13">
       <c r="A81" s="121" t="s">
         <v>1020</v>
       </c>
@@ -7548,7 +7647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" ht="13">
       <c r="A85" s="121" t="s">
         <v>1056</v>
       </c>
@@ -7618,7 +7717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" ht="13">
       <c r="A88" s="121" t="s">
         <v>1040</v>
       </c>
@@ -7679,7 +7778,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" ht="13">
       <c r="A91" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7700,7 +7799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" ht="13">
       <c r="A92" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7721,7 +7820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" ht="13">
       <c r="A93" t="s">
         <v>1014</v>
       </c>
@@ -7750,7 +7849,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" ht="13">
       <c r="A94" t="s">
         <v>1014</v>
       </c>
@@ -7776,7 +7875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" ht="13">
       <c r="A95" t="s">
         <v>1014</v>
       </c>
@@ -7796,7 +7895,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" ht="13">
       <c r="A96" t="s">
         <v>1014</v>
       </c>
@@ -7822,7 +7921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:15" ht="13">
       <c r="A97" t="s">
         <v>1014</v>
       </c>
@@ -7842,7 +7941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:15" ht="13">
       <c r="A98" t="s">
         <v>1014</v>
       </c>
@@ -7864,7 +7963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>1014</v>
       </c>
@@ -7883,7 +7982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>1014</v>
       </c>
@@ -7902,7 +8001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>1014</v>
       </c>
@@ -7921,7 +8020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>1014</v>
       </c>
@@ -7944,7 +8043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>1014</v>
       </c>
@@ -7963,7 +8062,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>1014</v>
       </c>
@@ -7986,7 +8085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>1014</v>
       </c>
@@ -8005,7 +8104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>1014</v>
       </c>
@@ -8028,7 +8127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>1014</v>
       </c>
@@ -8051,7 +8150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:15" ht="13">
       <c r="A108" t="s">
         <v>1014</v>
       </c>
@@ -8076,8 +8175,9 @@
       <c r="I108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="O108" s="233"/>
+    </row>
+    <row r="109" spans="1:15" ht="13">
       <c r="A109" t="s">
         <v>1014</v>
       </c>
@@ -8099,7 +8199,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>1014</v>
       </c>
@@ -8118,7 +8218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:15" ht="13">
       <c r="A111" s="121" t="s">
         <v>1014</v>
       </c>
@@ -8138,7 +8238,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>1003</v>
       </c>
@@ -8304,7 +8404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" ht="13">
       <c r="A119" s="121" t="s">
         <v>1003</v>
       </c>
@@ -8408,7 +8508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" ht="13">
       <c r="A124" s="121" t="s">
         <v>998</v>
       </c>
@@ -8599,7 +8699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" ht="13">
       <c r="A133" s="121" t="s">
         <v>1064</v>
       </c>
@@ -8680,7 +8780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" ht="13">
       <c r="A137" s="121" t="s">
         <v>883</v>
       </c>
@@ -8881,7 +8981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:14" ht="13">
       <c r="A147" s="121" t="s">
         <v>884</v>
       </c>
@@ -8965,7 +9065,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:14" ht="13">
       <c r="A151" s="121" t="s">
         <v>885</v>
       </c>
@@ -8986,7 +9086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:14" ht="13">
       <c r="A152" s="121" t="s">
         <v>1076</v>
       </c>
@@ -9007,7 +9107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:14" ht="13">
       <c r="A153" s="121" t="s">
         <v>1066</v>
       </c>
@@ -9071,7 +9171,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:14" ht="13">
       <c r="A156" s="121" t="s">
         <v>936</v>
       </c>
@@ -9139,7 +9239,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:14" ht="13">
       <c r="A159" s="121" t="s">
         <v>946</v>
       </c>
@@ -9184,7 +9284,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" ht="13">
       <c r="A161" s="121" t="s">
         <v>953</v>
       </c>
@@ -9300,7 +9400,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" ht="13">
       <c r="A166" s="121" t="s">
         <v>956</v>
       </c>
@@ -9425,7 +9525,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" ht="13">
       <c r="A172" s="121" t="s">
         <v>986</v>
       </c>
@@ -11125,7 +11225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" ht="13">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -11151,7 +11251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" ht="13">
       <c r="A244" s="121" t="s">
         <v>0</v>
       </c>
@@ -11198,7 +11298,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" ht="13">
       <c r="A246" t="s">
         <v>861</v>
       </c>
@@ -11225,7 +11325,7 @@
       <c r="J246" s="43"/>
       <c r="K246" s="43"/>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" ht="13">
       <c r="A247" t="s">
         <v>861</v>
       </c>
@@ -11252,7 +11352,7 @@
       <c r="J247" s="43"/>
       <c r="K247" s="43"/>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" ht="13">
       <c r="A248" t="s">
         <v>861</v>
       </c>
@@ -11281,7 +11381,7 @@
       <c r="J248" s="43"/>
       <c r="K248" s="43"/>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" ht="13">
       <c r="A249" t="s">
         <v>861</v>
       </c>
@@ -11310,7 +11410,7 @@
       <c r="J249" s="43"/>
       <c r="K249" s="43"/>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" ht="13">
       <c r="A250" s="121" t="s">
         <v>861</v>
       </c>
@@ -11664,7 +11764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:14">
+    <row r="265" spans="1:14" ht="13">
       <c r="A265" s="121" t="s">
         <v>1034</v>
       </c>
@@ -11928,7 +12028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:14">
+    <row r="275" spans="1:14" ht="13">
       <c r="A275" s="121" t="s">
         <v>1033</v>
       </c>
@@ -12020,7 +12120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13.5">
+    <row r="279" spans="1:14" ht="13">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -12192,7 +12292,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:14">
+    <row r="287" spans="1:14" ht="13">
       <c r="A287" t="s">
         <v>102</v>
       </c>
@@ -12215,7 +12315,7 @@
       <c r="J287" s="43"/>
       <c r="K287" s="43"/>
     </row>
-    <row r="288" spans="1:14">
+    <row r="288" spans="1:14" ht="13">
       <c r="A288" s="121" t="s">
         <v>102</v>
       </c>
@@ -12775,7 +12875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" ht="13">
       <c r="A309" s="121" t="s">
         <v>103</v>
       </c>
@@ -12800,7 +12900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" ht="13">
       <c r="A310" s="121" t="s">
         <v>103</v>
       </c>
@@ -13290,7 +13390,7 @@
       <c r="G329" s="31"/>
       <c r="H329" s="31"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" ht="13">
       <c r="A330" s="121"/>
       <c r="B330" s="121"/>
       <c r="C330" s="121"/>
@@ -13301,7 +13401,7 @@
       <c r="H330" s="205"/>
       <c r="I330" s="124"/>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" ht="13">
       <c r="A331" s="121"/>
       <c r="B331" s="121"/>
       <c r="C331" s="121"/>
@@ -13317,7 +13417,7 @@
       <c r="G332" s="31"/>
       <c r="H332" s="31"/>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" ht="13">
       <c r="A333" s="121"/>
       <c r="B333" s="121"/>
       <c r="C333" s="121"/>
@@ -13345,7 +13445,7 @@
       <c r="G336" s="31"/>
       <c r="H336" s="31"/>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" ht="13">
       <c r="A337" s="121"/>
       <c r="B337" s="121"/>
       <c r="C337" s="121"/>
@@ -13379,7 +13479,7 @@
       <c r="G341" s="31"/>
       <c r="H341" s="31"/>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" ht="13">
       <c r="A342" s="121"/>
       <c r="B342" s="121"/>
       <c r="C342" s="121"/>
@@ -13390,7 +13490,7 @@
       <c r="H342" s="205"/>
       <c r="I342" s="124"/>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" ht="13">
       <c r="A343" s="105"/>
       <c r="B343" s="121"/>
       <c r="E343" s="117"/>
@@ -13398,7 +13498,7 @@
       <c r="G343" s="31"/>
       <c r="H343" s="31"/>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" ht="13">
       <c r="A344" s="105"/>
       <c r="B344" s="121"/>
       <c r="E344" s="117"/>
@@ -13406,28 +13506,28 @@
       <c r="G344" s="31"/>
       <c r="H344" s="31"/>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" ht="13">
       <c r="A345" s="105"/>
       <c r="E345" s="117"/>
       <c r="F345" s="31"/>
       <c r="G345" s="31"/>
       <c r="H345" s="31"/>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" ht="13">
       <c r="A346" s="105"/>
       <c r="E346" s="117"/>
       <c r="F346" s="31"/>
       <c r="G346" s="31"/>
       <c r="H346" s="31"/>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" ht="13">
       <c r="A347" s="105"/>
       <c r="E347" s="117"/>
       <c r="F347" s="31"/>
       <c r="G347" s="31"/>
       <c r="H347" s="31"/>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" ht="13">
       <c r="A348" s="121"/>
       <c r="B348" s="121"/>
       <c r="C348" s="121"/>
@@ -14279,7 +14379,7 @@
       <c r="G474" s="31"/>
       <c r="H474" s="31"/>
     </row>
-    <row r="475" spans="1:9">
+    <row r="475" spans="1:9" ht="13">
       <c r="A475" s="121"/>
       <c r="B475" s="121"/>
       <c r="C475" s="121"/>
@@ -14290,7 +14390,7 @@
       <c r="H475" s="205"/>
       <c r="I475" s="124"/>
     </row>
-    <row r="476" spans="1:9">
+    <row r="476" spans="1:9" ht="13">
       <c r="A476" s="121"/>
       <c r="B476" s="121"/>
       <c r="C476" s="121"/>
@@ -14301,55 +14401,55 @@
       <c r="H476" s="31"/>
       <c r="I476" s="124"/>
     </row>
-    <row r="477" spans="1:9">
+    <row r="477" spans="1:9" ht="13">
       <c r="A477" s="105"/>
       <c r="E477" s="117"/>
       <c r="F477" s="105"/>
       <c r="G477" s="31"/>
     </row>
-    <row r="478" spans="1:9">
+    <row r="478" spans="1:9" ht="13">
       <c r="A478" s="105"/>
       <c r="E478" s="117"/>
       <c r="F478" s="105"/>
       <c r="G478" s="31"/>
     </row>
-    <row r="479" spans="1:9">
+    <row r="479" spans="1:9" ht="13">
       <c r="A479" s="105"/>
       <c r="E479" s="117"/>
       <c r="F479" s="105"/>
       <c r="G479" s="31"/>
     </row>
-    <row r="480" spans="1:9">
+    <row r="480" spans="1:9" ht="13">
       <c r="A480" s="105"/>
       <c r="E480" s="117"/>
       <c r="F480" s="105"/>
       <c r="G480" s="31"/>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" ht="13">
       <c r="A481" s="105"/>
       <c r="E481" s="117"/>
       <c r="F481" s="105"/>
       <c r="G481" s="31"/>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" ht="13">
       <c r="A482" s="105"/>
       <c r="E482" s="117"/>
       <c r="F482" s="105"/>
       <c r="G482" s="31"/>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" ht="13">
       <c r="A483" s="105"/>
       <c r="E483" s="117"/>
       <c r="F483" s="105"/>
       <c r="G483" s="31"/>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" ht="13">
       <c r="A484" s="105"/>
       <c r="E484" s="117"/>
       <c r="F484" s="105"/>
       <c r="G484" s="31"/>
     </row>
-    <row r="485" spans="1:8">
+    <row r="485" spans="1:8" ht="13">
       <c r="A485" s="105"/>
       <c r="E485" s="117"/>
       <c r="F485" s="105"/>
@@ -14465,7 +14565,7 @@
       <c r="G507" s="31"/>
       <c r="H507" s="31"/>
     </row>
-    <row r="508" spans="1:10">
+    <row r="508" spans="1:10" ht="13">
       <c r="A508" s="121"/>
       <c r="B508" s="121"/>
       <c r="C508" s="121"/>
@@ -14476,7 +14576,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13.5">
+    <row r="509" spans="1:10" ht="13">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -14487,7 +14587,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13.5">
+    <row r="510" spans="1:10" ht="13">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -14498,7 +14598,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13.5">
+    <row r="511" spans="1:10" ht="13">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -14580,7 +14680,7 @@
       <c r="G525" s="31"/>
       <c r="H525" s="31"/>
     </row>
-    <row r="526" spans="1:9">
+    <row r="526" spans="1:9" ht="13">
       <c r="A526" s="121"/>
       <c r="B526" s="121"/>
       <c r="C526" s="121"/>
@@ -14701,7 +14801,7 @@
       <c r="G546" s="31"/>
       <c r="H546" s="31"/>
     </row>
-    <row r="547" spans="1:9">
+    <row r="547" spans="1:9" ht="13">
       <c r="A547" s="121"/>
       <c r="B547" s="121"/>
       <c r="C547" s="121"/>
@@ -14788,7 +14888,7 @@
       <c r="G562" s="31"/>
       <c r="H562" s="31"/>
     </row>
-    <row r="563" spans="1:9">
+    <row r="563" spans="1:9" ht="13">
       <c r="A563" s="121"/>
       <c r="B563" s="121"/>
       <c r="C563" s="121"/>
@@ -14836,7 +14936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EE7EEF-305D-1145-A07B-3D132F6E2765}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K402"/>
@@ -14847,21 +14947,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:11" ht="40" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -14880,7 +14980,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:11" ht="66.95" customHeight="1">
+    <row r="2" spans="1:11" ht="67" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -14907,7 +15007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="13">
       <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
@@ -21061,7 +21161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
@@ -21069,13 +21169,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -21089,7 +21189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165.75">
+    <row r="2" spans="1:5" ht="169">
       <c r="A2" s="273" t="s">
         <v>14</v>
       </c>
@@ -21103,7 +21203,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="14.5">
       <c r="A3" s="274" t="s">
         <v>19</v>
       </c>
@@ -21863,7 +21963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABABBB7-6A1E-0B4E-82BF-6CDF21C8BDBC}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -21874,13 +21974,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.42578125" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="170"/>
+    <col min="2" max="2" width="28.81640625" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.453125" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.453125" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21897,7 +21997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="78">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -21911,7 +22011,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="173" t="s">
         <v>6</v>
       </c>
@@ -25837,7 +25937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H25"/>
@@ -25846,19 +25946,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.453125" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="43.453125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="1021" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="29.5">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -25876,7 +25976,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="65.5">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -25900,7 +26000,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -25926,86 +26026,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" ht="14.5">
       <c r="E4" s="7"/>
       <c r="F4" s="133"/>
       <c r="G4" s="12"/>
       <c r="H4" s="128"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" ht="14.5">
       <c r="E5" s="7"/>
       <c r="F5" s="133"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" ht="14.5">
       <c r="E6" s="7"/>
       <c r="F6" s="133"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" ht="14.5">
       <c r="E7" s="7"/>
       <c r="F7" s="133"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" ht="14.5">
       <c r="E8" s="7"/>
       <c r="F8" s="133"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" ht="14.5">
       <c r="E9" s="7"/>
       <c r="F9" s="133"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" ht="14.5">
       <c r="E10" s="7"/>
       <c r="F10" s="133"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" ht="14.5">
       <c r="E11" s="7"/>
       <c r="F11" s="133"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" ht="14.5">
       <c r="E12" s="7"/>
       <c r="F12" s="133"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" ht="14.5">
       <c r="D13" s="202"/>
       <c r="E13" s="7"/>
       <c r="F13" s="133"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" ht="14.5">
       <c r="E14" s="7"/>
       <c r="F14" s="133"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8" ht="14.5">
       <c r="C15" s="31"/>
       <c r="E15" s="7"/>
       <c r="F15" s="133"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" ht="14.5">
       <c r="C16" s="31"/>
       <c r="E16" s="7"/>
       <c r="F16" s="133"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="15">
+    <row r="17" spans="2:8" ht="14.5">
       <c r="E17" s="7"/>
       <c r="F17" s="133"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="15">
+    <row r="18" spans="2:8" ht="14.5">
       <c r="E18" s="7"/>
       <c r="F18" s="133"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="15">
+    <row r="19" spans="2:8" ht="14.5">
       <c r="E19" s="7"/>
       <c r="H19" s="133"/>
     </row>
@@ -26027,163 +26127,6 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="105"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
-      <c r="A1" s="62" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
-      <c r="A2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>746</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
-        <v>747</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
-        <v>925</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15">
-      <c r="A3" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="67" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="7"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="105"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="105"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="105"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="105"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="105"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="105"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="105"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="105"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="105"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="105"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26195,69 +26138,64 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="7" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="29.453125" customWidth="1"/>
+    <col min="8" max="1013" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="72" t="s">
-        <v>749</v>
-      </c>
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
+      <c r="A1" s="62" t="s">
+        <v>745</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
-    </row>
-    <row r="2" spans="1:8" ht="76.5">
+      <c r="E1" s="34"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="87">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>744</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="131" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
         <v>925</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:7" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26273,33 +26211,46 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="128" t="s">
-        <v>58</v>
+      <c r="F3" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="H4" s="68"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="D5" s="107"/>
-    </row>
-    <row r="6" spans="1:8" ht="14.25">
-      <c r="D6" s="114"/>
-    </row>
-    <row r="7" spans="1:8" ht="14.25">
-      <c r="D7" s="114"/>
-    </row>
-    <row r="8" spans="1:8" ht="14.25">
-      <c r="D8" s="114"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" s="37"/>
+    <row r="4" spans="1:7">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26333,9 +26284,6 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26347,64 +26295,69 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="3" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" customWidth="1"/>
+    <col min="9" max="1022" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="30" t="s">
-        <v>750</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:8" ht="18.5">
+      <c r="A1" s="72" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" ht="105">
+      <c r="E1" s="76"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="130"/>
+    </row>
+    <row r="2" spans="1:8" ht="78">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="F2" s="134" t="s">
+        <v>744</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="131" t="s">
         <v>925</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:8" ht="14.5">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26420,21 +26373,33 @@
       <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="128" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="4" spans="1:8" ht="14.5">
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" s="107"/>
+    </row>
+    <row r="6" spans="1:8" ht="14">
       <c r="D6" s="114"/>
     </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="105"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="105"/>
+    <row r="7" spans="1:8" ht="14">
+      <c r="D7" s="114"/>
+    </row>
+    <row r="8" spans="1:8" ht="14">
+      <c r="D8" s="114"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="F9" s="37"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="105"/>
@@ -26468,6 +26433,9 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="105"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26479,162 +26447,131 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="140"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" customWidth="1"/>
+    <col min="8" max="1008" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="135" t="s">
-        <v>927</v>
-      </c>
-      <c r="B1" s="136" t="s">
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="30" t="s">
+        <v>750</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="137" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-    </row>
-    <row r="2" spans="1:9" ht="38.25">
-      <c r="A2" s="141"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142" t="s">
-        <v>928</v>
-      </c>
-      <c r="D2" s="142" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+    </row>
+    <row r="2" spans="1:7" ht="87">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>746</v>
       </c>
-      <c r="E2" s="142" t="s">
-        <v>929</v>
-      </c>
-      <c r="F2" s="141" t="s">
-        <v>930</v>
-      </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-    </row>
-    <row r="3" spans="1:9" ht="15">
-      <c r="A3" s="143" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="144" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="134" t="s">
+        <v>925</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.5">
+      <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="B3" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="143" t="s">
+      <c r="C3" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="E3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="143" t="s">
+      <c r="F3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="143" t="s">
-        <v>931</v>
-      </c>
-      <c r="I3" s="143" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15">
-      <c r="A4" s="145"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-    </row>
-    <row r="5" spans="1:9" ht="15">
-      <c r="A5" s="145"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="146"/>
-    </row>
-    <row r="6" spans="1:9" ht="15">
-      <c r="A6" s="145"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="139"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="146"/>
-    </row>
-    <row r="7" spans="1:9" ht="15">
-      <c r="A7" s="145"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="146"/>
-    </row>
-    <row r="8" spans="1:9" ht="15">
-      <c r="A8" s="145"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="146"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="145"/>
-      <c r="B9" s="146"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="146"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="146"/>
+      <c r="G3" s="12" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14">
+      <c r="D6" s="114"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="105"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="105"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="105"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="105"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="105"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="105"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="105"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="105"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="105"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="105"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="105"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="105"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="105"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
   </headerFooter>
@@ -26649,14 +26586,14 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:10" ht="17.5">
       <c r="A1" s="267" t="s">
         <v>1134</v>
       </c>
@@ -26741,6 +26678,169 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802C44A7-4FE2-AB4A-86BC-DB153A3772C9}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="140"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="135" t="s">
+        <v>927</v>
+      </c>
+      <c r="B1" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="138" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+    </row>
+    <row r="2" spans="1:9" ht="39">
+      <c r="A2" s="141"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="142" t="s">
+        <v>928</v>
+      </c>
+      <c r="D2" s="142" t="s">
+        <v>746</v>
+      </c>
+      <c r="E2" s="142" t="s">
+        <v>929</v>
+      </c>
+      <c r="F2" s="141" t="s">
+        <v>930</v>
+      </c>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.5">
+      <c r="A3" s="143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="144" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="143" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="143" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="143" t="s">
+        <v>931</v>
+      </c>
+      <c r="I3" s="143" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.5">
+      <c r="A4" s="145"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.5">
+      <c r="A5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="146"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.5">
+      <c r="A6" s="145"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="146"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.5">
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="146"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.5">
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="146"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.5">
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="146"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D13"/>
@@ -26749,12 +26849,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
+    <col min="4" max="1013" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -26771,7 +26871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="65">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -26782,7 +26882,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.25">
+    <row r="3" spans="1:4" ht="39">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -26855,7 +26955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B5A0B4-9586-D946-AB25-20C3418D4E9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -26863,17 +26963,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="140"/>
+    <col min="1" max="1" width="16.1796875" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.81640625" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.81640625" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -26892,7 +26992,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="39">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -26912,7 +27012,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.7" customHeight="1">
+    <row r="3" spans="1:6" ht="13.75" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -26932,28 +27032,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.7" customHeight="1">
+    <row r="4" spans="1:6" ht="13.75" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.7" customHeight="1">
+    <row r="5" spans="1:6" ht="13.75" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.7" customHeight="1">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.7" customHeight="1">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.7" customHeight="1">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -26963,7 +27063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E7"/>
@@ -26972,12 +27072,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -26994,7 +27094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="178.5">
+    <row r="2" spans="1:5" ht="175.5">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27011,7 +27111,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="13">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -27043,95 +27143,6 @@
     <row r="7" spans="1:5">
       <c r="B7" s="60"/>
       <c r="C7" s="81"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="76.5">
-      <c r="A2" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="78" t="s">
-        <v>768</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>763</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="60"/>
-      <c r="C5" s="81"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="81"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="61"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="81"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="61"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -27143,6 +27154,95 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="48.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>765</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="78">
+      <c r="A2" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>761</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13">
+      <c r="A3" s="78" t="s">
+        <v>768</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="60"/>
+      <c r="C5" s="81"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="60"/>
+      <c r="C7" s="81"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="61"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="81"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="61"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:D484"/>
@@ -27151,14 +27251,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.453125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -27175,7 +27275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27189,7 +27289,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -28837,7 +28937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D120"/>
@@ -28846,13 +28946,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -28869,7 +28969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="63.75">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -28883,7 +28983,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -29329,7 +29429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D32"/>
@@ -29338,12 +29438,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -29360,7 +29460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="52">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -29374,7 +29474,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -29549,12 +29649,12 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="1014" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="1014" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29572,7 +29672,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="153">
+    <row r="2" spans="1:6" ht="143">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -29592,7 +29692,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="13">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -29637,14 +29737,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="5" width="21.1796875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.85546875" customWidth="1"/>
-    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="58.81640625" customWidth="1"/>
+    <col min="8" max="1011" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -29666,7 +29766,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="191.25">
+    <row r="2" spans="1:9" ht="195">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29695,7 +29795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25">
+    <row r="3" spans="1:9" ht="39">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29763,14 +29863,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29789,7 +29889,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="89.25">
+    <row r="2" spans="1:6" ht="91">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29809,7 +29909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="26">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -29903,19 +30003,19 @@
       <selection activeCell="A4" sqref="A4:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="49.453125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
-    <col min="11" max="1015" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.453125" customWidth="1"/>
+    <col min="11" max="1015" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -29936,7 +30036,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="102">
+    <row r="2" spans="1:10" ht="88">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29968,7 +30068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25">
+    <row r="3" spans="1:10" ht="39">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30497,27 +30597,27 @@
       <selection activeCell="F4" sqref="A4:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="55.42578125" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" customWidth="1"/>
-    <col min="10" max="10" width="81.42578125" customWidth="1"/>
-    <col min="11" max="11" width="93.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="15" width="8.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="55.453125" customWidth="1"/>
+    <col min="8" max="8" width="47.81640625" customWidth="1"/>
+    <col min="9" max="9" width="52.453125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
+    <col min="11" max="11" width="93.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" customWidth="1"/>
+    <col min="14" max="15" width="8.453125" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" customWidth="1"/>
+    <col min="18" max="18" width="20.453125" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" customWidth="1"/>
+    <col min="20" max="1013" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" customHeight="1">
@@ -30549,7 +30649,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:19" ht="114.75">
+    <row r="2" spans="1:19" ht="117">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30590,7 +30690,7 @@
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
     </row>
-    <row r="3" spans="1:19" ht="38.25">
+    <row r="3" spans="1:19" ht="39">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30649,7 +30749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.25">
+    <row r="4" spans="1:19" ht="14">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -30657,7 +30757,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:19" ht="14.25">
+    <row r="5" spans="1:19" ht="14">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -30665,7 +30765,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25">
+    <row r="6" spans="1:19" ht="14">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -30675,7 +30775,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:19" ht="14.25">
+    <row r="7" spans="1:19" ht="14">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30686,7 +30786,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:19" ht="14.25">
+    <row r="8" spans="1:19" ht="14">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30697,7 +30797,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:19" ht="14.25">
+    <row r="9" spans="1:19" ht="14">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30709,7 +30809,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:19" ht="14.25">
+    <row r="10" spans="1:19" ht="14">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30721,7 +30821,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:19" ht="14.25">
+    <row r="11" spans="1:19" ht="14">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30733,7 +30833,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:19" ht="14.25">
+    <row r="12" spans="1:19" ht="14">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30745,7 +30845,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:19" ht="14.25">
+    <row r="13" spans="1:19" ht="14">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30757,7 +30857,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:19" ht="14.25">
+    <row r="14" spans="1:19" ht="14">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30769,7 +30869,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:19" ht="14.25">
+    <row r="15" spans="1:19" ht="14">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30781,7 +30881,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:19" ht="14.25">
+    <row r="16" spans="1:19" ht="14">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30793,7 +30893,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14.25">
+    <row r="17" spans="6:19" ht="14">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30805,7 +30905,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14.25">
+    <row r="18" spans="6:19" ht="14">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30817,7 +30917,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14.25">
+    <row r="19" spans="6:19" ht="14">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -30827,7 +30927,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14.25">
+    <row r="20" spans="6:19" ht="14">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -30835,7 +30935,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14.25">
+    <row r="21" spans="6:19" ht="14">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30846,7 +30946,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14.25">
+    <row r="22" spans="6:19" ht="14">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30858,7 +30958,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14.25">
+    <row r="23" spans="6:19" ht="14">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -30870,7 +30970,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14.25">
+    <row r="24" spans="6:19" ht="14">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -30878,7 +30978,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14.25">
+    <row r="25" spans="6:19" ht="14">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -30889,7 +30989,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14.25">
+    <row r="26" spans="6:19" ht="14">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -30901,7 +31001,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14.25">
+    <row r="27" spans="6:19" ht="14">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -30912,7 +31012,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14.25">
+    <row r="28" spans="6:19" ht="14">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -30922,7 +31022,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14.25">
+    <row r="29" spans="6:19" ht="14">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -30933,7 +31033,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14.25">
+    <row r="30" spans="6:19" ht="14">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -30944,7 +31044,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14.25">
+    <row r="31" spans="6:19" ht="14">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -30955,7 +31055,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14.25">
+    <row r="32" spans="6:19" ht="14">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -30964,7 +31064,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14.25">
+    <row r="33" spans="6:19" ht="14">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -30973,7 +31073,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14.25">
+    <row r="34" spans="6:19" ht="14">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -30983,7 +31083,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14.25">
+    <row r="35" spans="6:19" ht="14">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -30992,7 +31092,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14.25">
+    <row r="36" spans="6:19" ht="14">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -31108,7 +31208,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14.25">
+    <row r="48" spans="6:19" ht="14">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -31199,26 +31299,26 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="58.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="58.453125" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="87.140625" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="87.1796875" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -31242,7 +31342,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:17" ht="57.95" customHeight="1">
+    <row r="2" spans="1:17" ht="58" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31291,7 +31391,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="38.25">
+    <row r="3" spans="1:17" ht="39">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -33349,29 +33449,29 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:XFD194"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD192"/>
+      <selection pane="bottomLeft" activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.1796875" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="30" t="s">
         <v>136</v>
       </c>
@@ -33385,7 +33485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93.95" customHeight="1">
+    <row r="2" spans="1:11" ht="94" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -33416,8 +33516,11 @@
       <c r="J2" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="25.5">
+      <c r="K2" s="22" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -33448,8 +33551,11 @@
       <c r="J3" s="26" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="26" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>1103</v>
       </c>
@@ -33467,7 +33573,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
@@ -33485,7 +33591,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>1103</v>
       </c>
@@ -33503,7 +33609,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -33523,7 +33629,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1103</v>
       </c>
@@ -33543,7 +33649,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>1103</v>
       </c>
@@ -33563,7 +33669,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>1103</v>
       </c>
@@ -33585,7 +33691,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>1103</v>
       </c>
@@ -33605,7 +33711,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>1103</v>
       </c>
@@ -33625,7 +33731,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>1103</v>
       </c>
@@ -33645,7 +33751,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>1103</v>
       </c>
@@ -33664,7 +33770,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>1103</v>
       </c>
@@ -33684,7 +33790,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>1103</v>
       </c>

</xml_diff>

<commit_message>
RET-0000: Post merge tidy up
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-englandwales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF576B99-775F-47A7-8355-F168B63163BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E4902A-FCBA-4581-B595-8E1361F12271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1905" yWindow="-18165" windowWidth="28800" windowHeight="15315" tabRatio="500" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="500" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="1154">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3625,6 +3625,12 @@
   <si>
     <t>ID that identifies the document category
 MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>Publish</t>
   </si>
 </sst>
 </file>
@@ -4380,7 +4386,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="277">
+  <cellXfs count="278">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4923,6 +4929,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -5404,14 +5411,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="256"/>
+    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="267" t="s">
         <v>1137</v>
       </c>
@@ -5419,7 +5426,7 @@
       <c r="C1" s="271"/>
       <c r="D1" s="270"/>
     </row>
-    <row r="2" spans="1:4" ht="88.5">
+    <row r="2" spans="1:4" ht="102.75">
       <c r="A2" s="269" t="s">
         <v>1133</v>
       </c>
@@ -5464,7 +5471,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="30" t="s">
@@ -5476,7 +5483,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:5" ht="65">
+    <row r="2" spans="1:5" ht="63.75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -5493,7 +5500,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13">
+    <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="276" t="s">
         <v>39</v>
       </c>
@@ -5523,20 +5530,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="239"/>
-    <col min="3" max="3" width="54.7265625" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7265625" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.26953125" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="239"/>
+    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7265625" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.81640625" style="239"/>
-    <col min="1026" max="16384" width="10.81640625" style="238"/>
+    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" style="239"/>
+    <col min="1026" max="16384" width="10.85546875" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -5562,7 +5569,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="52">
+    <row r="2" spans="1:13" ht="63.75">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -5597,7 +5604,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.5">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -5649,7 +5656,7 @@
       <c r="L4" s="240"/>
       <c r="M4" s="240"/>
     </row>
-    <row r="5" spans="1:13" ht="13">
+    <row r="5" spans="1:13">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="242"/>
@@ -5664,7 +5671,7 @@
       <c r="L5" s="240"/>
       <c r="M5" s="240"/>
     </row>
-    <row r="6" spans="1:13" ht="13">
+    <row r="6" spans="1:13">
       <c r="A6" s="241"/>
       <c r="B6" s="241"/>
       <c r="D6" s="240"/>
@@ -5678,7 +5685,7 @@
       <c r="L6" s="240"/>
       <c r="M6" s="240"/>
     </row>
-    <row r="7" spans="1:13" ht="13">
+    <row r="7" spans="1:13">
       <c r="A7" s="241"/>
       <c r="B7" s="241"/>
       <c r="D7" s="240"/>
@@ -5725,20 +5732,20 @@
       <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="6" width="53.81640625" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" customWidth="1"/>
     <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5765,7 +5772,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:15" ht="55" customHeight="1">
+    <row r="2" spans="1:15" ht="54.95" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -5808,7 +5815,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="52">
+    <row r="3" spans="1:15" ht="51">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -5949,7 +5956,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="13">
+    <row r="9" spans="1:15">
       <c r="A9" s="121" t="s">
         <v>1036</v>
       </c>
@@ -6040,7 +6047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13">
+    <row r="14" spans="1:15">
       <c r="A14" s="121" t="s">
         <v>1037</v>
       </c>
@@ -6205,7 +6212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13">
+    <row r="22" spans="1:9">
       <c r="A22" s="121" t="s">
         <v>1062</v>
       </c>
@@ -6250,7 +6257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13">
+    <row r="24" spans="1:9">
       <c r="A24" s="121" t="s">
         <v>1063</v>
       </c>
@@ -6291,7 +6298,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13">
+    <row r="26" spans="1:9">
       <c r="A26" s="121" t="s">
         <v>1023</v>
       </c>
@@ -6499,7 +6506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13">
+    <row r="36" spans="1:9">
       <c r="A36" s="121" t="s">
         <v>1018</v>
       </c>
@@ -6854,7 +6861,7 @@
       <c r="J50" s="43"/>
       <c r="K50" s="43"/>
     </row>
-    <row r="51" spans="1:11" ht="13">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -6881,7 +6888,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
     </row>
-    <row r="52" spans="1:11" ht="13">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -6908,7 +6915,7 @@
       <c r="J52" s="43"/>
       <c r="K52" s="43"/>
     </row>
-    <row r="53" spans="1:11" ht="13">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -7306,7 +7313,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="13">
+    <row r="69" spans="1:9">
       <c r="A69" s="121" t="s">
         <v>80</v>
       </c>
@@ -7327,7 +7334,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.15" customHeight="1">
+    <row r="70" spans="1:9" ht="14.1" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -7350,7 +7357,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="10" customHeight="1">
+    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -7556,7 +7563,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="13">
+    <row r="81" spans="1:14">
       <c r="A81" s="121" t="s">
         <v>1020</v>
       </c>
@@ -7647,7 +7654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="13">
+    <row r="85" spans="1:14">
       <c r="A85" s="121" t="s">
         <v>1056</v>
       </c>
@@ -7717,7 +7724,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="13">
+    <row r="88" spans="1:14">
       <c r="A88" s="121" t="s">
         <v>1040</v>
       </c>
@@ -7778,7 +7785,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="13">
+    <row r="91" spans="1:14">
       <c r="A91" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7799,7 +7806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="13">
+    <row r="92" spans="1:14">
       <c r="A92" s="121" t="s">
         <v>1065</v>
       </c>
@@ -7820,7 +7827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="13">
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
         <v>1014</v>
       </c>
@@ -7849,7 +7856,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="13">
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
         <v>1014</v>
       </c>
@@ -7875,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="13">
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
         <v>1014</v>
       </c>
@@ -7895,7 +7902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="13">
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
         <v>1014</v>
       </c>
@@ -7921,7 +7928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="13">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>1014</v>
       </c>
@@ -7941,7 +7948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="13">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>1014</v>
       </c>
@@ -8150,7 +8157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="13">
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
         <v>1014</v>
       </c>
@@ -8177,7 +8184,7 @@
       </c>
       <c r="O108" s="233"/>
     </row>
-    <row r="109" spans="1:15" ht="13">
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
         <v>1014</v>
       </c>
@@ -8218,7 +8225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="13">
+    <row r="111" spans="1:15">
       <c r="A111" s="121" t="s">
         <v>1014</v>
       </c>
@@ -8404,7 +8411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="13">
+    <row r="119" spans="1:13">
       <c r="A119" s="121" t="s">
         <v>1003</v>
       </c>
@@ -8508,7 +8515,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="13">
+    <row r="124" spans="1:13">
       <c r="A124" s="121" t="s">
         <v>998</v>
       </c>
@@ -8699,7 +8706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="13">
+    <row r="133" spans="1:9">
       <c r="A133" s="121" t="s">
         <v>1064</v>
       </c>
@@ -8780,7 +8787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="13">
+    <row r="137" spans="1:9">
       <c r="A137" s="121" t="s">
         <v>883</v>
       </c>
@@ -8981,7 +8988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="13">
+    <row r="147" spans="1:14">
       <c r="A147" s="121" t="s">
         <v>884</v>
       </c>
@@ -9065,7 +9072,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="13">
+    <row r="151" spans="1:14">
       <c r="A151" s="121" t="s">
         <v>885</v>
       </c>
@@ -9086,7 +9093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="13">
+    <row r="152" spans="1:14">
       <c r="A152" s="121" t="s">
         <v>1076</v>
       </c>
@@ -9107,7 +9114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="13">
+    <row r="153" spans="1:14">
       <c r="A153" s="121" t="s">
         <v>1066</v>
       </c>
@@ -9171,7 +9178,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="13">
+    <row r="156" spans="1:14">
       <c r="A156" s="121" t="s">
         <v>936</v>
       </c>
@@ -9239,7 +9246,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="13">
+    <row r="159" spans="1:14">
       <c r="A159" s="121" t="s">
         <v>946</v>
       </c>
@@ -9284,7 +9291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="13">
+    <row r="161" spans="1:9">
       <c r="A161" s="121" t="s">
         <v>953</v>
       </c>
@@ -9400,7 +9407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="13">
+    <row r="166" spans="1:9">
       <c r="A166" s="121" t="s">
         <v>956</v>
       </c>
@@ -9525,7 +9532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="13">
+    <row r="172" spans="1:9">
       <c r="A172" s="121" t="s">
         <v>986</v>
       </c>
@@ -11225,7 +11232,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="13">
+    <row r="243" spans="1:11">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -11251,7 +11258,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="13">
+    <row r="244" spans="1:11">
       <c r="A244" s="121" t="s">
         <v>0</v>
       </c>
@@ -11298,7 +11305,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
     </row>
-    <row r="246" spans="1:11" ht="13">
+    <row r="246" spans="1:11">
       <c r="A246" t="s">
         <v>861</v>
       </c>
@@ -11325,7 +11332,7 @@
       <c r="J246" s="43"/>
       <c r="K246" s="43"/>
     </row>
-    <row r="247" spans="1:11" ht="13">
+    <row r="247" spans="1:11">
       <c r="A247" t="s">
         <v>861</v>
       </c>
@@ -11352,7 +11359,7 @@
       <c r="J247" s="43"/>
       <c r="K247" s="43"/>
     </row>
-    <row r="248" spans="1:11" ht="13">
+    <row r="248" spans="1:11">
       <c r="A248" t="s">
         <v>861</v>
       </c>
@@ -11381,7 +11388,7 @@
       <c r="J248" s="43"/>
       <c r="K248" s="43"/>
     </row>
-    <row r="249" spans="1:11" ht="13">
+    <row r="249" spans="1:11">
       <c r="A249" t="s">
         <v>861</v>
       </c>
@@ -11410,7 +11417,7 @@
       <c r="J249" s="43"/>
       <c r="K249" s="43"/>
     </row>
-    <row r="250" spans="1:11" ht="13">
+    <row r="250" spans="1:11">
       <c r="A250" s="121" t="s">
         <v>861</v>
       </c>
@@ -11764,7 +11771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="13">
+    <row r="265" spans="1:14">
       <c r="A265" s="121" t="s">
         <v>1034</v>
       </c>
@@ -12028,7 +12035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="13">
+    <row r="275" spans="1:14">
       <c r="A275" s="121" t="s">
         <v>1033</v>
       </c>
@@ -12120,7 +12127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13">
+    <row r="279" spans="1:14" ht="13.5">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -12292,7 +12299,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="13">
+    <row r="287" spans="1:14">
       <c r="A287" t="s">
         <v>102</v>
       </c>
@@ -12315,7 +12322,7 @@
       <c r="J287" s="43"/>
       <c r="K287" s="43"/>
     </row>
-    <row r="288" spans="1:14" ht="13">
+    <row r="288" spans="1:14">
       <c r="A288" s="121" t="s">
         <v>102</v>
       </c>
@@ -12875,7 +12882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="13">
+    <row r="309" spans="1:9">
       <c r="A309" s="121" t="s">
         <v>103</v>
       </c>
@@ -12900,7 +12907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:9" ht="13">
+    <row r="310" spans="1:9">
       <c r="A310" s="121" t="s">
         <v>103</v>
       </c>
@@ -13390,7 +13397,7 @@
       <c r="G329" s="31"/>
       <c r="H329" s="31"/>
     </row>
-    <row r="330" spans="1:9" ht="13">
+    <row r="330" spans="1:9">
       <c r="A330" s="121"/>
       <c r="B330" s="121"/>
       <c r="C330" s="121"/>
@@ -13401,7 +13408,7 @@
       <c r="H330" s="205"/>
       <c r="I330" s="124"/>
     </row>
-    <row r="331" spans="1:9" ht="13">
+    <row r="331" spans="1:9">
       <c r="A331" s="121"/>
       <c r="B331" s="121"/>
       <c r="C331" s="121"/>
@@ -13417,7 +13424,7 @@
       <c r="G332" s="31"/>
       <c r="H332" s="31"/>
     </row>
-    <row r="333" spans="1:9" ht="13">
+    <row r="333" spans="1:9">
       <c r="A333" s="121"/>
       <c r="B333" s="121"/>
       <c r="C333" s="121"/>
@@ -13445,7 +13452,7 @@
       <c r="G336" s="31"/>
       <c r="H336" s="31"/>
     </row>
-    <row r="337" spans="1:9" ht="13">
+    <row r="337" spans="1:9">
       <c r="A337" s="121"/>
       <c r="B337" s="121"/>
       <c r="C337" s="121"/>
@@ -13479,7 +13486,7 @@
       <c r="G341" s="31"/>
       <c r="H341" s="31"/>
     </row>
-    <row r="342" spans="1:9" ht="13">
+    <row r="342" spans="1:9">
       <c r="A342" s="121"/>
       <c r="B342" s="121"/>
       <c r="C342" s="121"/>
@@ -13490,7 +13497,7 @@
       <c r="H342" s="205"/>
       <c r="I342" s="124"/>
     </row>
-    <row r="343" spans="1:9" ht="13">
+    <row r="343" spans="1:9">
       <c r="A343" s="105"/>
       <c r="B343" s="121"/>
       <c r="E343" s="117"/>
@@ -13498,7 +13505,7 @@
       <c r="G343" s="31"/>
       <c r="H343" s="31"/>
     </row>
-    <row r="344" spans="1:9" ht="13">
+    <row r="344" spans="1:9">
       <c r="A344" s="105"/>
       <c r="B344" s="121"/>
       <c r="E344" s="117"/>
@@ -13506,28 +13513,28 @@
       <c r="G344" s="31"/>
       <c r="H344" s="31"/>
     </row>
-    <row r="345" spans="1:9" ht="13">
+    <row r="345" spans="1:9">
       <c r="A345" s="105"/>
       <c r="E345" s="117"/>
       <c r="F345" s="31"/>
       <c r="G345" s="31"/>
       <c r="H345" s="31"/>
     </row>
-    <row r="346" spans="1:9" ht="13">
+    <row r="346" spans="1:9">
       <c r="A346" s="105"/>
       <c r="E346" s="117"/>
       <c r="F346" s="31"/>
       <c r="G346" s="31"/>
       <c r="H346" s="31"/>
     </row>
-    <row r="347" spans="1:9" ht="13">
+    <row r="347" spans="1:9">
       <c r="A347" s="105"/>
       <c r="E347" s="117"/>
       <c r="F347" s="31"/>
       <c r="G347" s="31"/>
       <c r="H347" s="31"/>
     </row>
-    <row r="348" spans="1:9" ht="13">
+    <row r="348" spans="1:9">
       <c r="A348" s="121"/>
       <c r="B348" s="121"/>
       <c r="C348" s="121"/>
@@ -14379,7 +14386,7 @@
       <c r="G474" s="31"/>
       <c r="H474" s="31"/>
     </row>
-    <row r="475" spans="1:9" ht="13">
+    <row r="475" spans="1:9">
       <c r="A475" s="121"/>
       <c r="B475" s="121"/>
       <c r="C475" s="121"/>
@@ -14390,7 +14397,7 @@
       <c r="H475" s="205"/>
       <c r="I475" s="124"/>
     </row>
-    <row r="476" spans="1:9" ht="13">
+    <row r="476" spans="1:9">
       <c r="A476" s="121"/>
       <c r="B476" s="121"/>
       <c r="C476" s="121"/>
@@ -14401,55 +14408,55 @@
       <c r="H476" s="31"/>
       <c r="I476" s="124"/>
     </row>
-    <row r="477" spans="1:9" ht="13">
+    <row r="477" spans="1:9">
       <c r="A477" s="105"/>
       <c r="E477" s="117"/>
       <c r="F477" s="105"/>
       <c r="G477" s="31"/>
     </row>
-    <row r="478" spans="1:9" ht="13">
+    <row r="478" spans="1:9">
       <c r="A478" s="105"/>
       <c r="E478" s="117"/>
       <c r="F478" s="105"/>
       <c r="G478" s="31"/>
     </row>
-    <row r="479" spans="1:9" ht="13">
+    <row r="479" spans="1:9">
       <c r="A479" s="105"/>
       <c r="E479" s="117"/>
       <c r="F479" s="105"/>
       <c r="G479" s="31"/>
     </row>
-    <row r="480" spans="1:9" ht="13">
+    <row r="480" spans="1:9">
       <c r="A480" s="105"/>
       <c r="E480" s="117"/>
       <c r="F480" s="105"/>
       <c r="G480" s="31"/>
     </row>
-    <row r="481" spans="1:8" ht="13">
+    <row r="481" spans="1:8">
       <c r="A481" s="105"/>
       <c r="E481" s="117"/>
       <c r="F481" s="105"/>
       <c r="G481" s="31"/>
     </row>
-    <row r="482" spans="1:8" ht="13">
+    <row r="482" spans="1:8">
       <c r="A482" s="105"/>
       <c r="E482" s="117"/>
       <c r="F482" s="105"/>
       <c r="G482" s="31"/>
     </row>
-    <row r="483" spans="1:8" ht="13">
+    <row r="483" spans="1:8">
       <c r="A483" s="105"/>
       <c r="E483" s="117"/>
       <c r="F483" s="105"/>
       <c r="G483" s="31"/>
     </row>
-    <row r="484" spans="1:8" ht="13">
+    <row r="484" spans="1:8">
       <c r="A484" s="105"/>
       <c r="E484" s="117"/>
       <c r="F484" s="105"/>
       <c r="G484" s="31"/>
     </row>
-    <row r="485" spans="1:8" ht="13">
+    <row r="485" spans="1:8">
       <c r="A485" s="105"/>
       <c r="E485" s="117"/>
       <c r="F485" s="105"/>
@@ -14565,7 +14572,7 @@
       <c r="G507" s="31"/>
       <c r="H507" s="31"/>
     </row>
-    <row r="508" spans="1:10" ht="13">
+    <row r="508" spans="1:10">
       <c r="A508" s="121"/>
       <c r="B508" s="121"/>
       <c r="C508" s="121"/>
@@ -14576,7 +14583,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13">
+    <row r="509" spans="1:10" ht="13.5">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -14587,7 +14594,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13">
+    <row r="510" spans="1:10" ht="13.5">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -14598,7 +14605,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13">
+    <row r="511" spans="1:10" ht="13.5">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -14680,7 +14687,7 @@
       <c r="G525" s="31"/>
       <c r="H525" s="31"/>
     </row>
-    <row r="526" spans="1:9" ht="13">
+    <row r="526" spans="1:9">
       <c r="A526" s="121"/>
       <c r="B526" s="121"/>
       <c r="C526" s="121"/>
@@ -14801,7 +14808,7 @@
       <c r="G546" s="31"/>
       <c r="H546" s="31"/>
     </row>
-    <row r="547" spans="1:9" ht="13">
+    <row r="547" spans="1:9">
       <c r="A547" s="121"/>
       <c r="B547" s="121"/>
       <c r="C547" s="121"/>
@@ -14888,7 +14895,7 @@
       <c r="G562" s="31"/>
       <c r="H562" s="31"/>
     </row>
-    <row r="563" spans="1:9" ht="13">
+    <row r="563" spans="1:9">
       <c r="A563" s="121"/>
       <c r="B563" s="121"/>
       <c r="C563" s="121"/>
@@ -14939,29 +14946,29 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EE7EEF-305D-1145-A07B-3D132F6E2765}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:K402"/>
+  <dimension ref="A1:L402"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1">
+    <row r="1" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -14980,7 +14987,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:11" ht="67" customHeight="1">
+    <row r="2" spans="1:12" ht="66.95" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -15006,8 +15013,11 @@
       <c r="I2" s="55" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="13">
+      <c r="L2" s="22" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
@@ -15041,8 +15051,11 @@
       <c r="K3" s="226" t="s">
         <v>1080</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="277" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15070,7 +15083,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15098,7 +15111,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15126,7 +15139,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15154,7 +15167,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15182,7 +15195,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15210,7 +15223,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15233,7 +15246,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15258,7 +15271,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15281,7 +15294,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15304,7 +15317,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15329,7 +15342,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="47" t="s">
         <v>1019</v>
       </c>
@@ -15354,7 +15367,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="47" t="s">
         <v>1019</v>
       </c>
@@ -21165,17 +21178,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -21189,7 +21202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="169">
+    <row r="2" spans="1:5" ht="165.75">
       <c r="A2" s="273" t="s">
         <v>14</v>
       </c>
@@ -21203,7 +21216,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="274" t="s">
         <v>19</v>
       </c>
@@ -21974,13 +21987,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.453125" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.453125" style="170"/>
+    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21997,7 +22010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="78">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -22011,7 +22024,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="173" t="s">
         <v>6</v>
       </c>
@@ -25946,19 +25959,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.453125" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" customWidth="1"/>
-    <col min="7" max="7" width="43.453125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="1021" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="29.5">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -25976,7 +25989,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="65.5">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26000,7 +26013,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26026,86 +26039,86 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5">
+    <row r="4" spans="1:8" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="133"/>
       <c r="G4" s="12"/>
       <c r="H4" s="128"/>
     </row>
-    <row r="5" spans="1:8" ht="14.5">
+    <row r="5" spans="1:8" ht="15">
       <c r="E5" s="7"/>
       <c r="F5" s="133"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" ht="14.5">
+    <row r="6" spans="1:8" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="133"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:8" ht="14.5">
+    <row r="7" spans="1:8" ht="15">
       <c r="E7" s="7"/>
       <c r="F7" s="133"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" ht="14.5">
+    <row r="8" spans="1:8" ht="15">
       <c r="E8" s="7"/>
       <c r="F8" s="133"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.5">
+    <row r="9" spans="1:8" ht="15">
       <c r="E9" s="7"/>
       <c r="F9" s="133"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="14.5">
+    <row r="10" spans="1:8" ht="15">
       <c r="E10" s="7"/>
       <c r="F10" s="133"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="14.5">
+    <row r="11" spans="1:8" ht="15">
       <c r="E11" s="7"/>
       <c r="F11" s="133"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="14.5">
+    <row r="12" spans="1:8" ht="15">
       <c r="E12" s="7"/>
       <c r="F12" s="133"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="14.5">
+    <row r="13" spans="1:8" ht="15">
       <c r="D13" s="202"/>
       <c r="E13" s="7"/>
       <c r="F13" s="133"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="14.5">
+    <row r="14" spans="1:8" ht="15">
       <c r="E14" s="7"/>
       <c r="F14" s="133"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="14.5">
+    <row r="15" spans="1:8" ht="15">
       <c r="C15" s="31"/>
       <c r="E15" s="7"/>
       <c r="F15" s="133"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="14.5">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="31"/>
       <c r="E16" s="7"/>
       <c r="F16" s="133"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:8" ht="14.5">
+    <row r="17" spans="2:8" ht="15">
       <c r="E17" s="7"/>
       <c r="F17" s="133"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:8" ht="14.5">
+    <row r="18" spans="2:8" ht="15">
       <c r="E18" s="7"/>
       <c r="F18" s="133"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:8" ht="14.5">
+    <row r="19" spans="2:8" ht="15">
       <c r="E19" s="7"/>
       <c r="H19" s="133"/>
     </row>
@@ -26146,15 +26159,15 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" customWidth="1"/>
-    <col min="7" max="7" width="29.453125" customWidth="1"/>
-    <col min="8" max="1013" width="8.453125" customWidth="1"/>
+    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
@@ -26174,7 +26187,7 @@
       <c r="F1" s="129"/>
       <c r="G1" s="130"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="87">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26195,7 +26208,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26303,19 +26316,19 @@
       <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="3" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="7" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" customWidth="1"/>
-    <col min="9" max="1022" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="72" t="s">
         <v>749</v>
       </c>
@@ -26333,7 +26346,7 @@
       <c r="G1" s="129"/>
       <c r="H1" s="130"/>
     </row>
-    <row r="2" spans="1:8" ht="78">
+    <row r="2" spans="1:8" ht="76.5">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26357,7 +26370,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26383,19 +26396,19 @@
         <v>763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5">
+    <row r="4" spans="1:8" ht="15">
       <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="107"/>
     </row>
-    <row r="6" spans="1:8" ht="14">
+    <row r="6" spans="1:8" ht="14.25">
       <c r="D6" s="114"/>
     </row>
-    <row r="7" spans="1:8" ht="14">
+    <row r="7" spans="1:8" ht="14.25">
       <c r="D7" s="114"/>
     </row>
-    <row r="8" spans="1:8" ht="14">
+    <row r="8" spans="1:8" ht="14.25">
       <c r="D8" s="114"/>
     </row>
     <row r="9" spans="1:8">
@@ -26455,15 +26468,15 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="3" width="27.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" customWidth="1"/>
-    <col min="8" max="1008" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
@@ -26483,7 +26496,7 @@
       <c r="F1" s="129"/>
       <c r="G1" s="130"/>
     </row>
-    <row r="2" spans="1:7" ht="87">
+    <row r="2" spans="1:7" ht="105">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26504,7 +26517,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
@@ -26527,7 +26540,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="D6" s="114"/>
     </row>
     <row r="10" spans="1:7">
@@ -26586,14 +26599,14 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.7265625" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.1796875" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="256"/>
+    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="256"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="267" t="s">
         <v>1134</v>
       </c>
@@ -26685,18 +26698,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="140"/>
+    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -26718,7 +26731,7 @@
       <c r="H1" s="139"/>
       <c r="I1" s="139"/>
     </row>
-    <row r="2" spans="1:9" ht="39">
+    <row r="2" spans="1:9" ht="38.25">
       <c r="A2" s="141"/>
       <c r="B2" s="141"/>
       <c r="C2" s="142" t="s">
@@ -26737,7 +26750,7 @@
       <c r="H2" s="141"/>
       <c r="I2" s="141"/>
     </row>
-    <row r="3" spans="1:9" ht="14.5">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="143" t="s">
         <v>19</v>
       </c>
@@ -26766,7 +26779,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.5">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="145"/>
       <c r="B4" s="146"/>
       <c r="C4" s="139"/>
@@ -26777,7 +26790,7 @@
       <c r="H4" s="146"/>
       <c r="I4" s="146"/>
     </row>
-    <row r="5" spans="1:9" ht="14.5">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="145"/>
       <c r="B5" s="146"/>
       <c r="C5" s="139"/>
@@ -26788,7 +26801,7 @@
       <c r="H5" s="139"/>
       <c r="I5" s="146"/>
     </row>
-    <row r="6" spans="1:9" ht="14.5">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="145"/>
       <c r="B6" s="146"/>
       <c r="C6" s="139"/>
@@ -26799,7 +26812,7 @@
       <c r="H6" s="139"/>
       <c r="I6" s="146"/>
     </row>
-    <row r="7" spans="1:9" ht="14.5">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="145"/>
       <c r="B7" s="146"/>
       <c r="C7" s="139"/>
@@ -26810,7 +26823,7 @@
       <c r="H7" s="139"/>
       <c r="I7" s="146"/>
     </row>
-    <row r="8" spans="1:9" ht="14.5">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="145"/>
       <c r="B8" s="146"/>
       <c r="C8" s="139"/>
@@ -26821,7 +26834,7 @@
       <c r="H8" s="139"/>
       <c r="I8" s="146"/>
     </row>
-    <row r="9" spans="1:9" ht="14.5">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="145"/>
       <c r="B9" s="146"/>
       <c r="C9" s="139"/>
@@ -26849,12 +26862,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.453125" customWidth="1"/>
+    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -26871,7 +26884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="65">
+    <row r="2" spans="1:4" ht="76.5">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -26882,7 +26895,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39">
+    <row r="3" spans="1:4" ht="38.25">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -26963,17 +26976,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.81640625" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.81640625" style="140"/>
+    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -26992,7 +27005,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="39">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -27012,7 +27025,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.75" customHeight="1">
+    <row r="3" spans="1:6" ht="13.7" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -27032,28 +27045,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1">
+    <row r="4" spans="1:6" ht="13.7" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1">
+    <row r="5" spans="1:6" ht="13.7" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1">
+    <row r="6" spans="1:6" ht="13.7" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1">
+    <row r="7" spans="1:6" ht="13.7" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1">
+    <row r="8" spans="1:6" ht="13.7" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27072,12 +27085,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -27094,7 +27107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="175.5">
+    <row r="2" spans="1:5" ht="178.5">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27111,7 +27124,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13">
+    <row r="3" spans="1:5">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -27162,12 +27175,12 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1">
@@ -27181,7 +27194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="78">
+    <row r="2" spans="1:3" ht="76.5">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -27192,7 +27205,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13">
+    <row r="3" spans="1:3">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -27251,14 +27264,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.453125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
+    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -27275,7 +27288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27289,7 +27302,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -28946,13 +28959,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.453125" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -28969,7 +28982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="63.75">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -28983,7 +28996,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>768</v>
       </c>
@@ -29438,12 +29451,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -29460,7 +29473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -29474,7 +29487,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4">
       <c r="A3" s="78" t="s">
         <v>39</v>
       </c>
@@ -29649,12 +29662,12 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="1014" width="10.453125" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="1014" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29672,7 +29685,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="143">
+    <row r="2" spans="1:6" ht="153">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -29692,7 +29705,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13">
+    <row r="3" spans="1:6">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -29737,14 +29750,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="5" width="21.1796875" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.81640625" customWidth="1"/>
-    <col min="8" max="1011" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -29766,7 +29779,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="195">
+    <row r="2" spans="1:9" ht="191.25">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29795,7 +29808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39">
+    <row r="3" spans="1:9" ht="38.25">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29863,14 +29876,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29889,7 +29902,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="91">
+    <row r="2" spans="1:6" ht="89.25">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29909,7 +29922,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -30003,19 +30016,19 @@
       <selection activeCell="A4" sqref="A4:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" customWidth="1"/>
-    <col min="11" max="1015" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="1015" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -30036,7 +30049,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="88">
+    <row r="2" spans="1:10" ht="102">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30068,7 +30081,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="39">
+    <row r="3" spans="1:10" ht="38.25">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30591,36 +30604,36 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BE1D59-106C-BF43-BA5D-A6515397BCBE}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="A4:XFD57"/>
+    <sheetView topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="55.453125" customWidth="1"/>
-    <col min="8" max="8" width="47.81640625" customWidth="1"/>
-    <col min="9" max="9" width="52.453125" customWidth="1"/>
-    <col min="10" max="10" width="81.453125" customWidth="1"/>
-    <col min="11" max="11" width="93.453125" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="23.453125" customWidth="1"/>
-    <col min="14" max="15" width="8.453125" customWidth="1"/>
-    <col min="16" max="16" width="18.453125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" customWidth="1"/>
-    <col min="18" max="18" width="20.453125" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" customWidth="1"/>
-    <col min="20" max="1013" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" customWidth="1"/>
+    <col min="10" max="10" width="81.42578125" customWidth="1"/>
+    <col min="11" max="11" width="93.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1">
+    <row r="1" spans="1:20" ht="18" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
@@ -30649,7 +30662,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:19" ht="117">
+    <row r="2" spans="1:20" ht="114.75">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30689,8 +30702,11 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
-    </row>
-    <row r="3" spans="1:19" ht="39">
+      <c r="T2" s="22" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="38.25">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30748,8 +30764,11 @@
       <c r="S3" s="26" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="14">
+      <c r="T3" s="277" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="14.25">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -30757,7 +30776,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:19" ht="14">
+    <row r="5" spans="1:20" ht="14.25">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -30765,7 +30784,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:19" ht="14">
+    <row r="6" spans="1:20" ht="14.25">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -30775,7 +30794,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:19" ht="14">
+    <row r="7" spans="1:20" ht="14.25">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30786,7 +30805,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:19" ht="14">
+    <row r="8" spans="1:20" ht="14.25">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30797,7 +30816,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:19" ht="14">
+    <row r="9" spans="1:20" ht="14.25">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30809,7 +30828,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:19" ht="14">
+    <row r="10" spans="1:20" ht="14.25">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30821,7 +30840,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:19" ht="14">
+    <row r="11" spans="1:20" ht="14.25">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30833,7 +30852,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:19" ht="14">
+    <row r="12" spans="1:20" ht="14.25">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30845,7 +30864,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:19" ht="14">
+    <row r="13" spans="1:20" ht="14.25">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30857,7 +30876,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:19" ht="14">
+    <row r="14" spans="1:20" ht="14.25">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30869,7 +30888,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:19" ht="14">
+    <row r="15" spans="1:20" ht="14.25">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30881,7 +30900,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:19" ht="14">
+    <row r="16" spans="1:20" ht="14.25">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30893,7 +30912,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14">
+    <row r="17" spans="6:19" ht="14.25">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30905,7 +30924,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14">
+    <row r="18" spans="6:19" ht="14.25">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30917,7 +30936,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14">
+    <row r="19" spans="6:19" ht="14.25">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -30927,7 +30946,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14">
+    <row r="20" spans="6:19" ht="14.25">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -30935,7 +30954,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14">
+    <row r="21" spans="6:19" ht="14.25">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30946,7 +30965,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14">
+    <row r="22" spans="6:19" ht="14.25">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30958,7 +30977,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14">
+    <row r="23" spans="6:19" ht="14.25">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -30970,7 +30989,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14">
+    <row r="24" spans="6:19" ht="14.25">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -30978,7 +30997,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14">
+    <row r="25" spans="6:19" ht="14.25">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -30989,7 +31008,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14">
+    <row r="26" spans="6:19" ht="14.25">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -31001,7 +31020,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14">
+    <row r="27" spans="6:19" ht="14.25">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -31012,7 +31031,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14">
+    <row r="28" spans="6:19" ht="14.25">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -31022,7 +31041,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14">
+    <row r="29" spans="6:19" ht="14.25">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -31033,7 +31052,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14">
+    <row r="30" spans="6:19" ht="14.25">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -31044,7 +31063,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14">
+    <row r="31" spans="6:19" ht="14.25">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -31055,7 +31074,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14">
+    <row r="32" spans="6:19" ht="14.25">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -31064,7 +31083,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14">
+    <row r="33" spans="6:19" ht="14.25">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -31073,7 +31092,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14">
+    <row r="34" spans="6:19" ht="14.25">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -31083,7 +31102,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14">
+    <row r="35" spans="6:19" ht="14.25">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -31092,7 +31111,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14">
+    <row r="36" spans="6:19" ht="14.25">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -31208,7 +31227,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14">
+    <row r="48" spans="6:19" ht="14.25">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -31297,31 +31316,31 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E75101-AE74-3B43-A771-FE940D099A52}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:Q217"/>
+  <dimension ref="A1:R217"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
-      <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="8" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="58.453125" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="58.42578125" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.453125" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="87.1796875" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="87.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18">
+    <row r="1" spans="1:18" ht="18">
       <c r="A1" s="30" t="s">
         <v>106</v>
       </c>
@@ -31342,7 +31361,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:17" ht="58" customHeight="1">
+    <row r="2" spans="1:18" ht="57.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31390,8 +31409,11 @@
       <c r="Q2" s="24" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="39">
+      <c r="R2" s="22" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -31443,8 +31465,11 @@
       <c r="Q3" s="26" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="277" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>1103</v>
       </c>
@@ -31475,7 +31500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
@@ -31505,7 +31530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>1103</v>
       </c>
@@ -31535,7 +31560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -31571,7 +31596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>1103</v>
       </c>
@@ -31607,7 +31632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>1103</v>
       </c>
@@ -31643,7 +31668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>1103</v>
       </c>
@@ -31679,7 +31704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>1103</v>
       </c>
@@ -31715,7 +31740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -31723,7 +31748,7 @@
       <c r="N12" s="42"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -31732,7 +31757,7 @@
       <c r="N13" s="42"/>
       <c r="O13" s="7"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -31740,7 +31765,7 @@
       <c r="N14" s="42"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -31748,7 +31773,7 @@
       <c r="N15" s="42"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -33449,26 +33474,26 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:XFD194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.1796875" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -33485,7 +33510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="94" customHeight="1">
+    <row r="2" spans="1:11" ht="93.95" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -33520,7 +33545,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13">
+    <row r="3" spans="1:11" ht="25.5">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Case flags V2.1 updates
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-englandwales\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmet.dede/dev/IntelliJ/ccd_definitions/et-ccd-definitions-englandwales/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E4902A-FCBA-4581-B595-8E1361F12271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833559D3-CD5A-7046-85D6-3AFCEA8019A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="500" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -52,7 +52,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$J$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseType!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseTypeTab!$A$3:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseTypeTab!$A$3:$K$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">ComplexTypes!$A$3:$N$563</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'EnglandWales Scrubbed'!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3733" uniqueCount="1155">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3631,6 +3631,9 @@
   </si>
   <si>
     <t>Publish</t>
+  </si>
+  <si>
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
   </si>
 </sst>
 </file>
@@ -5411,11 +5414,11 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.6640625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1640625" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="256"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -5426,7 +5429,7 @@
       <c r="C1" s="271"/>
       <c r="D1" s="270"/>
     </row>
-    <row r="2" spans="1:4" ht="102.75">
+    <row r="2" spans="1:4" ht="99">
       <c r="A2" s="269" t="s">
         <v>1133</v>
       </c>
@@ -5471,7 +5474,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="30" t="s">
@@ -5483,7 +5486,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:5" ht="63.75">
+    <row r="2" spans="1:5" ht="70">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -5500,7 +5503,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5">
+    <row r="3" spans="1:5" ht="14">
       <c r="A3" s="276" t="s">
         <v>39</v>
       </c>
@@ -5530,20 +5533,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="239" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="239"/>
-    <col min="3" max="3" width="54.7109375" style="239" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="239" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="239" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="239" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="239" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="239" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="239"/>
+    <col min="3" max="3" width="54.6640625" style="239" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="239" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="239" customWidth="1"/>
+    <col min="7" max="7" width="44.33203125" style="239" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="239" customWidth="1"/>
     <col min="9" max="9" width="37" style="239" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="239" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="239" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" style="239"/>
-    <col min="1026" max="16384" width="10.85546875" style="238"/>
+    <col min="10" max="10" width="43.6640625" style="239" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="239" customWidth="1"/>
+    <col min="12" max="1025" width="10.83203125" style="239"/>
+    <col min="1026" max="16384" width="10.83203125" style="238"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -5569,7 +5572,7 @@
       <c r="L1" s="240"/>
       <c r="M1" s="240"/>
     </row>
-    <row r="2" spans="1:13" ht="63.75">
+    <row r="2" spans="1:13" ht="56">
       <c r="A2" s="251" t="s">
         <v>14</v>
       </c>
@@ -5604,7 +5607,7 @@
       <c r="L2" s="247"/>
       <c r="M2" s="247"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75">
+    <row r="3" spans="1:13" ht="16">
       <c r="A3" s="246" t="s">
         <v>19</v>
       </c>
@@ -5732,20 +5735,20 @@
       <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="53.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
     <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5772,7 +5775,7 @@
       <c r="L1" s="44"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:15" ht="54.95" customHeight="1">
+    <row r="2" spans="1:15" ht="55" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>193</v>
       </c>
@@ -5815,7 +5818,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="51">
+    <row r="3" spans="1:15" ht="56">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -7334,7 +7337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.1" customHeight="1">
+    <row r="70" spans="1:9" ht="14" customHeight="1">
       <c r="A70" t="s">
         <v>1020</v>
       </c>
@@ -7357,7 +7360,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="9.9499999999999993" customHeight="1">
+    <row r="71" spans="1:9" ht="10" customHeight="1">
       <c r="A71" t="s">
         <v>1020</v>
       </c>
@@ -12127,7 +12130,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="13.5">
+    <row r="279" spans="1:14">
       <c r="A279" t="s">
         <v>102</v>
       </c>
@@ -14583,7 +14586,7 @@
       <c r="H508" s="205"/>
       <c r="I508" s="124"/>
     </row>
-    <row r="509" spans="1:10" ht="13.5">
+    <row r="509" spans="1:10">
       <c r="A509" s="121"/>
       <c r="B509" s="237"/>
       <c r="C509" s="121"/>
@@ -14594,7 +14597,7 @@
       <c r="I509" s="43"/>
       <c r="J509" s="43"/>
     </row>
-    <row r="510" spans="1:10" ht="13.5">
+    <row r="510" spans="1:10">
       <c r="A510" s="121"/>
       <c r="B510" s="237"/>
       <c r="C510" s="121"/>
@@ -14605,7 +14608,7 @@
       <c r="I510" s="124"/>
       <c r="J510" s="43"/>
     </row>
-    <row r="511" spans="1:10" ht="13.5">
+    <row r="511" spans="1:10">
       <c r="A511" s="121"/>
       <c r="B511" s="237"/>
       <c r="C511" s="121"/>
@@ -14954,21 +14957,21 @@
       <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:12" ht="40" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>691</v>
       </c>
@@ -14987,7 +14990,7 @@
       <c r="H1" s="54"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:12" ht="66.95" customHeight="1">
+    <row r="2" spans="1:12" ht="67" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>692</v>
       </c>
@@ -21178,17 +21181,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94120695-055A-489E-BBBE-B6C0A0852310}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -21202,7 +21205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165.75">
+    <row r="2" spans="1:5" ht="154">
       <c r="A2" s="273" t="s">
         <v>14</v>
       </c>
@@ -21987,13 +21990,13 @@
       <selection activeCell="A4" sqref="A4:XFD780"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="46" style="170" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="178" customWidth="1"/>
-    <col min="3" max="3" width="91.42578125" style="170" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="170" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="170"/>
+    <col min="2" max="2" width="28.83203125" style="178" customWidth="1"/>
+    <col min="3" max="3" width="91.5" style="170" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="170" customWidth="1"/>
+    <col min="5" max="16384" width="11.5" style="170"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -22010,7 +22013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="84">
       <c r="A2" s="171" t="s">
         <v>735</v>
       </c>
@@ -25959,19 +25962,19 @@
       <selection activeCell="A4" sqref="A4:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="1021" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="43.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="1021" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="36">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="19">
       <c r="A1" s="62" t="s">
         <v>741</v>
       </c>
@@ -25989,7 +25992,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="132"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="75">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="71">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26159,18 +26162,18 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="1013" width="8.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="8" max="1013" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="18">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="19">
       <c r="A1" s="62" t="s">
         <v>745</v>
       </c>
@@ -26187,7 +26190,7 @@
       <c r="F1" s="129"/>
       <c r="G1" s="130"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="90">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="80">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26316,19 +26319,19 @@
       <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="7" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="1022" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+    <col min="9" max="1022" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="19">
       <c r="A1" s="72" t="s">
         <v>749</v>
       </c>
@@ -26346,7 +26349,7 @@
       <c r="G1" s="129"/>
       <c r="H1" s="130"/>
     </row>
-    <row r="2" spans="1:8" ht="76.5">
+    <row r="2" spans="1:8" ht="84">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26402,13 +26405,13 @@
     <row r="5" spans="1:8">
       <c r="D5" s="107"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25">
+    <row r="6" spans="1:8" ht="14">
       <c r="D6" s="114"/>
     </row>
-    <row r="7" spans="1:8" ht="14.25">
+    <row r="7" spans="1:8" ht="14">
       <c r="D7" s="114"/>
     </row>
-    <row r="8" spans="1:8" ht="14.25">
+    <row r="8" spans="1:8" ht="14">
       <c r="D8" s="114"/>
     </row>
     <row r="9" spans="1:8">
@@ -26468,15 +26471,15 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="7" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="1008" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="1008" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
@@ -26496,7 +26499,7 @@
       <c r="F1" s="129"/>
       <c r="G1" s="130"/>
     </row>
-    <row r="2" spans="1:7" ht="105">
+    <row r="2" spans="1:7" ht="96">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -26540,7 +26543,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="6" spans="1:7" ht="14">
       <c r="D6" s="114"/>
     </row>
     <row r="10" spans="1:7">
@@ -26599,11 +26602,11 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="256" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="256"/>
+    <col min="1" max="2" width="10.6640625" style="257" customWidth="1"/>
+    <col min="3" max="1025" width="11.1640625" style="256" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="256"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -26620,7 +26623,7 @@
       <c r="I1" s="266"/>
       <c r="J1" s="265"/>
     </row>
-    <row r="2" spans="1:10" ht="409.5">
+    <row r="2" spans="1:10" ht="409.6">
       <c r="A2" s="263" t="s">
         <v>1133</v>
       </c>
@@ -26698,18 +26701,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="140" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="140" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="140" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="140" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="140" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="140" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="140" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="140" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="140"/>
+    <col min="1" max="1" width="31.83203125" style="140" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="140" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="140" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="140" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="140" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="140" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="140" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -26731,7 +26734,7 @@
       <c r="H1" s="139"/>
       <c r="I1" s="139"/>
     </row>
-    <row r="2" spans="1:9" ht="38.25">
+    <row r="2" spans="1:9" ht="42">
       <c r="A2" s="141"/>
       <c r="B2" s="141"/>
       <c r="C2" s="142" t="s">
@@ -26862,12 +26865,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="1013" width="10.42578125" customWidth="1"/>
+    <col min="4" max="1013" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -26884,7 +26887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="76.5">
+    <row r="2" spans="1:4" ht="70">
       <c r="B2" s="22" t="s">
         <v>751</v>
       </c>
@@ -26895,7 +26898,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.25">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -26976,17 +26979,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="140" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="140" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="140" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="140" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="140" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="140" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="140" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="140" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="140"/>
+    <col min="1" max="1" width="16.1640625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="140" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="140" customWidth="1"/>
+    <col min="4" max="4" width="28.5" style="140" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" style="140" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="140" customWidth="1"/>
+    <col min="8" max="1025" width="8.83203125" style="140" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -27005,7 +27008,7 @@
       <c r="E1" s="151"/>
       <c r="F1" s="151"/>
     </row>
-    <row r="2" spans="1:6" s="155" customFormat="1" ht="38.25">
+    <row r="2" spans="1:6" s="155" customFormat="1" ht="42">
       <c r="A2" s="152" t="s">
         <v>14</v>
       </c>
@@ -27025,7 +27028,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.7" customHeight="1">
+    <row r="3" spans="1:6" ht="13.75" customHeight="1">
       <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
@@ -27045,28 +27048,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.7" customHeight="1">
+    <row r="4" spans="1:6" ht="13.75" customHeight="1">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
     </row>
-    <row r="5" spans="1:6" ht="13.7" customHeight="1">
+    <row r="5" spans="1:6" ht="13.75" customHeight="1">
       <c r="A5" s="159"/>
       <c r="B5" s="159"/>
     </row>
-    <row r="6" spans="1:6" ht="13.7" customHeight="1">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1">
       <c r="A6" s="159"/>
       <c r="B6" s="159"/>
     </row>
-    <row r="7" spans="1:6" ht="13.7" customHeight="1">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1">
       <c r="A7" s="159"/>
       <c r="B7" s="159"/>
     </row>
-    <row r="8" spans="1:6" ht="13.7" customHeight="1">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1">
       <c r="A8" s="159"/>
       <c r="B8" s="159"/>
     </row>
-    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27085,12 +27088,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="775" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="7" customWidth="1"/>
+    <col min="4" max="775" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -27107,7 +27110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="178.5">
+    <row r="2" spans="1:5" ht="196">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -27175,12 +27178,12 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="773" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="7" customWidth="1"/>
+    <col min="4" max="773" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1">
@@ -27194,7 +27197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="76.5">
+    <row r="2" spans="1:3" ht="70">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -27264,14 +27267,14 @@
       <selection activeCell="A4" sqref="A4:XFD486"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
-    <col min="5" max="1011" width="8.42578125" customWidth="1"/>
-    <col min="1012" max="1015" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="49.5" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="7" customWidth="1"/>
+    <col min="5" max="1011" width="8.5" customWidth="1"/>
+    <col min="1012" max="1015" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -27288,7 +27291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -28959,13 +28962,13 @@
       <selection activeCell="A4" sqref="A4:XFD121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
-    <col min="5" max="774" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.5" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="7" customWidth="1"/>
+    <col min="5" max="774" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -28982,7 +28985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="63.75">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="23" t="s">
         <v>766</v>
       </c>
@@ -29451,12 +29454,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -29473,7 +29476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="23" t="s">
         <v>759</v>
       </c>
@@ -29662,12 +29665,12 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="1014" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="1014" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29685,7 +29688,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="153">
+    <row r="2" spans="1:6" ht="154">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -29750,14 +29753,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="58.85546875" customWidth="1"/>
-    <col min="8" max="1011" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="58.83203125" customWidth="1"/>
+    <col min="8" max="1011" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -29779,7 +29782,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="191.25">
+    <row r="2" spans="1:9" ht="210">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29808,7 +29811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25">
+    <row r="3" spans="1:9" ht="42">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29876,14 +29879,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1000" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="1000" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
@@ -29902,7 +29905,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="89.25">
+    <row r="2" spans="1:6" ht="98">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -29922,7 +29925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="28">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -30010,28 +30013,28 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD105"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
-    <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
-    <col min="11" max="1015" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
+    <col min="7" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="49.5" customWidth="1"/>
+    <col min="10" max="10" width="31" customWidth="1"/>
+    <col min="11" max="11" width="26.5" customWidth="1"/>
+    <col min="12" max="1014" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="30" t="s">
         <v>42</v>
       </c>
@@ -30045,11 +30048,11 @@
       <c r="E1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="31"/>
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
-    </row>
-    <row r="2" spans="1:10" ht="102">
+      <c r="J1" s="31"/>
+    </row>
+    <row r="2" spans="1:11" ht="196">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30068,20 +30071,23 @@
       <c r="F2" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="22" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25">
+    <row r="3" spans="1:11" ht="42">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30100,473 +30106,476 @@
       <c r="F3" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="I3" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="J3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="K3" s="36" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="D4" s="112"/>
       <c r="E4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="H4" s="7"/>
+      <c r="I4" s="37"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="E5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="37"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="H5" s="7"/>
+      <c r="I5" s="37"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="E6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="37"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="H6" s="7"/>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="E7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="E8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="E9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="E10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="H10" s="7"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="E11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="E12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="E13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="E14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="H14" s="7"/>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="E15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="H15" s="7"/>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="E16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="5:8">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="5:9">
       <c r="E17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="5:8">
+      <c r="H17" s="7"/>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="5:9">
       <c r="E18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="37"/>
-    </row>
-    <row r="19" spans="5:8">
+      <c r="H18" s="7"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="5:9">
       <c r="E19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="5:8">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="5:9">
       <c r="E20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="5:8">
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="5:9">
       <c r="E21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="37"/>
-    </row>
-    <row r="22" spans="5:8">
+      <c r="H21" s="7"/>
+      <c r="I21" s="37"/>
+    </row>
+    <row r="22" spans="5:9">
       <c r="E22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="37"/>
-    </row>
-    <row r="23" spans="5:8">
+      <c r="H22" s="7"/>
+      <c r="I22" s="37"/>
+    </row>
+    <row r="23" spans="5:9">
       <c r="E23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="5:8">
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="5:9">
       <c r="E24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="5:8">
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="5:9">
       <c r="E25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="5:8">
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="5:9">
       <c r="E26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="5:8">
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="5:9">
       <c r="E27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="37"/>
-    </row>
-    <row r="28" spans="5:8">
+      <c r="H27" s="7"/>
+      <c r="I27" s="37"/>
+    </row>
+    <row r="28" spans="5:9">
       <c r="E28" s="7"/>
       <c r="F28" s="105"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="37"/>
-    </row>
-    <row r="29" spans="5:8">
+      <c r="H28" s="7"/>
+      <c r="I28" s="37"/>
+    </row>
+    <row r="29" spans="5:9">
       <c r="E29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="37"/>
-    </row>
-    <row r="30" spans="5:8">
+      <c r="H29" s="7"/>
+      <c r="I29" s="37"/>
+    </row>
+    <row r="30" spans="5:9">
       <c r="E30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="37"/>
-    </row>
-    <row r="31" spans="5:8">
+      <c r="H30" s="7"/>
+      <c r="I30" s="37"/>
+    </row>
+    <row r="31" spans="5:9">
       <c r="E31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="37"/>
-    </row>
-    <row r="32" spans="5:8">
+      <c r="H31" s="7"/>
+      <c r="I31" s="37"/>
+    </row>
+    <row r="32" spans="5:9">
       <c r="E32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="37"/>
-    </row>
-    <row r="33" spans="5:9">
+      <c r="H32" s="7"/>
+      <c r="I32" s="37"/>
+    </row>
+    <row r="33" spans="5:10">
       <c r="E33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="37"/>
-    </row>
-    <row r="34" spans="5:9">
+      <c r="H33" s="7"/>
+      <c r="I33" s="37"/>
+    </row>
+    <row r="34" spans="5:10">
       <c r="E34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="37"/>
-    </row>
-    <row r="35" spans="5:9">
+      <c r="H34" s="7"/>
+      <c r="I34" s="37"/>
+    </row>
+    <row r="35" spans="5:10">
       <c r="E35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="37"/>
-    </row>
-    <row r="36" spans="5:9">
+      <c r="H35" s="7"/>
+      <c r="I35" s="37"/>
+    </row>
+    <row r="36" spans="5:10">
       <c r="E36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="37"/>
-    </row>
-    <row r="37" spans="5:9">
+      <c r="H36" s="7"/>
+      <c r="I36" s="37"/>
+    </row>
+    <row r="37" spans="5:10">
       <c r="E37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="37"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="37"/>
-    </row>
-    <row r="38" spans="5:9">
+      <c r="J37" s="37"/>
+    </row>
+    <row r="38" spans="5:10">
       <c r="E38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="37"/>
-    </row>
-    <row r="39" spans="5:9">
+      <c r="H38" s="7"/>
+      <c r="I38" s="37"/>
+    </row>
+    <row r="39" spans="5:10">
       <c r="E39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="37"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="37"/>
-    </row>
-    <row r="40" spans="5:9">
+      <c r="J39" s="37"/>
+    </row>
+    <row r="40" spans="5:10">
       <c r="E40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="I40" s="37"/>
-    </row>
-    <row r="41" spans="5:9">
+      <c r="H40" s="7"/>
+      <c r="J40" s="37"/>
+    </row>
+    <row r="41" spans="5:10">
       <c r="E41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="I41" s="37"/>
-    </row>
-    <row r="42" spans="5:9">
+      <c r="H41" s="7"/>
+      <c r="J41" s="37"/>
+    </row>
+    <row r="42" spans="5:10">
       <c r="E42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="37"/>
-    </row>
-    <row r="43" spans="5:9">
+      <c r="H42" s="7"/>
+      <c r="I42" s="37"/>
+    </row>
+    <row r="43" spans="5:10">
       <c r="E43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="37"/>
-    </row>
-    <row r="44" spans="5:9">
+      <c r="H43" s="7"/>
+      <c r="I43" s="37"/>
+    </row>
+    <row r="44" spans="5:10">
       <c r="E44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="37"/>
-    </row>
-    <row r="45" spans="5:9">
+      <c r="H44" s="7"/>
+      <c r="I44" s="37"/>
+    </row>
+    <row r="45" spans="5:10">
       <c r="E45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="37"/>
-    </row>
-    <row r="46" spans="5:9">
+      <c r="H45" s="7"/>
+      <c r="I45" s="37"/>
+    </row>
+    <row r="46" spans="5:10">
       <c r="E46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="37"/>
-    </row>
-    <row r="47" spans="5:9">
+      <c r="H46" s="7"/>
+      <c r="I46" s="37"/>
+    </row>
+    <row r="47" spans="5:10">
       <c r="E47" s="7"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="5:9">
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="5:10">
       <c r="E48" s="7"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="5:7">
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="5:8">
       <c r="E49" s="7"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="5:7">
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="5:8">
       <c r="E50" s="7"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="53" spans="5:7">
+      <c r="H50" s="7"/>
+    </row>
+    <row r="53" spans="5:8">
       <c r="E53" s="7"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="5:7">
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="5:8">
       <c r="E54" s="7"/>
-      <c r="G54" s="7"/>
-    </row>
-    <row r="55" spans="5:7">
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="5:8">
       <c r="E55" s="7"/>
-      <c r="G55" s="7"/>
-    </row>
-    <row r="56" spans="5:7">
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="5:8">
       <c r="E56" s="7"/>
-      <c r="G56" s="7"/>
-    </row>
-    <row r="57" spans="5:7">
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="5:8">
       <c r="E57" s="7"/>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="5:7">
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="5:8">
       <c r="E58" s="7"/>
-      <c r="G58" s="7"/>
-    </row>
-    <row r="59" spans="5:7">
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="5:8">
       <c r="E59" s="7"/>
-      <c r="G59" s="7"/>
-    </row>
-    <row r="60" spans="5:7">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="5:8">
       <c r="E60" s="7"/>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="5:7">
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="5:8">
       <c r="E61" s="7"/>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="5:7">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="5:8">
       <c r="E62" s="7"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="5:7">
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="5:8">
       <c r="E63" s="7"/>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="5:7">
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="5:8">
       <c r="E64" s="7"/>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="5:7">
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="5:8">
       <c r="E65" s="7"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="5:7">
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="5:8">
       <c r="E66" s="7"/>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="5:7">
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="5:8">
       <c r="E67" s="7"/>
-      <c r="G67" s="7"/>
-    </row>
-    <row r="68" spans="5:7">
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="5:8">
       <c r="E68" s="7"/>
-      <c r="G68" s="7"/>
-    </row>
-    <row r="69" spans="5:7">
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="5:8">
       <c r="E69" s="7"/>
-      <c r="G69" s="7"/>
-    </row>
-    <row r="70" spans="5:7">
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="5:8">
       <c r="E70" s="7"/>
-      <c r="G70" s="7"/>
-    </row>
-    <row r="71" spans="5:7">
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="5:8">
       <c r="E71" s="7"/>
-      <c r="G71" s="7"/>
-    </row>
-    <row r="72" spans="5:7">
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="5:8">
       <c r="E72" s="7"/>
-      <c r="G72" s="7"/>
-    </row>
-    <row r="73" spans="5:7">
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="5:8">
       <c r="E73" s="7"/>
-      <c r="G73" s="7"/>
-    </row>
-    <row r="74" spans="5:7">
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="5:8">
       <c r="E74" s="7"/>
-      <c r="G74" s="7"/>
-    </row>
-    <row r="75" spans="5:7">
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="5:8">
       <c r="E75" s="7"/>
-      <c r="G75" s="7"/>
-    </row>
-    <row r="76" spans="5:7">
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="5:8">
       <c r="E76" s="7"/>
-      <c r="G76" s="7"/>
-    </row>
-    <row r="77" spans="5:7">
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="5:8">
       <c r="E77" s="7"/>
-      <c r="G77" s="7"/>
-    </row>
-    <row r="78" spans="5:7">
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="5:8">
       <c r="E78" s="7"/>
-      <c r="G78" s="7"/>
-    </row>
-    <row r="79" spans="5:7">
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="5:8">
       <c r="E79" s="7"/>
-      <c r="G79" s="7"/>
-    </row>
-    <row r="80" spans="5:7">
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="5:8">
       <c r="E80" s="7"/>
-      <c r="G80" s="7"/>
-    </row>
-    <row r="81" spans="5:10">
+      <c r="H80" s="7"/>
+    </row>
+    <row r="81" spans="5:11">
       <c r="E81" s="7"/>
-      <c r="G81" s="7"/>
-    </row>
-    <row r="82" spans="5:10">
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="5:11">
       <c r="E82" s="7"/>
-      <c r="G82" s="7"/>
-    </row>
-    <row r="83" spans="5:10">
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="5:11">
       <c r="E83" s="7"/>
-      <c r="G83" s="7"/>
-    </row>
-    <row r="84" spans="5:10">
+      <c r="H83" s="7"/>
+    </row>
+    <row r="84" spans="5:11">
       <c r="E84" s="7"/>
-      <c r="G84" s="7"/>
-    </row>
-    <row r="85" spans="5:10">
+      <c r="H84" s="7"/>
+    </row>
+    <row r="85" spans="5:11">
       <c r="E85" s="7"/>
-      <c r="G85" s="7"/>
-    </row>
-    <row r="86" spans="5:10">
+      <c r="H85" s="7"/>
+    </row>
+    <row r="86" spans="5:11">
       <c r="E86" s="7"/>
-      <c r="G86" s="7"/>
-    </row>
-    <row r="87" spans="5:10">
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="5:11">
       <c r="E87" s="7"/>
-      <c r="G87" s="7"/>
-    </row>
-    <row r="88" spans="5:10">
+      <c r="H87" s="7"/>
+    </row>
+    <row r="88" spans="5:11">
       <c r="E88" s="7"/>
-      <c r="G88" s="7"/>
-    </row>
-    <row r="89" spans="5:10">
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="5:11">
       <c r="E89" s="7"/>
-      <c r="G89" s="7"/>
-    </row>
-    <row r="90" spans="5:10">
+      <c r="H89" s="7"/>
+    </row>
+    <row r="90" spans="5:11">
       <c r="E90" s="7"/>
-      <c r="G90" s="7"/>
-    </row>
-    <row r="92" spans="5:10">
+      <c r="H90" s="7"/>
+    </row>
+    <row r="92" spans="5:11">
       <c r="F92" s="31"/>
-      <c r="G92" s="7"/>
-      <c r="I92" s="31"/>
+      <c r="H92" s="7"/>
       <c r="J92" s="31"/>
-    </row>
-    <row r="93" spans="5:10">
+      <c r="K92" s="31"/>
+    </row>
+    <row r="93" spans="5:11">
       <c r="F93" s="31"/>
-      <c r="G93" s="7"/>
-      <c r="I93" s="31"/>
+      <c r="H93" s="7"/>
       <c r="J93" s="31"/>
-    </row>
-    <row r="94" spans="5:10">
+      <c r="K93" s="31"/>
+    </row>
+    <row r="94" spans="5:11">
       <c r="F94" s="31"/>
-      <c r="G94" s="7"/>
-      <c r="I94" s="31"/>
+      <c r="H94" s="7"/>
       <c r="J94" s="31"/>
-    </row>
-    <row r="95" spans="5:10">
+      <c r="K94" s="31"/>
+    </row>
+    <row r="95" spans="5:11">
       <c r="F95" s="31"/>
-      <c r="G95" s="7"/>
-      <c r="J95" s="31"/>
-    </row>
-    <row r="96" spans="5:10">
+      <c r="H95" s="7"/>
+      <c r="K95" s="31"/>
+    </row>
+    <row r="96" spans="5:11">
       <c r="F96" s="31"/>
-      <c r="G96" s="7"/>
-      <c r="J96" s="31"/>
-    </row>
-    <row r="97" spans="6:10">
+      <c r="H96" s="7"/>
+      <c r="K96" s="31"/>
+    </row>
+    <row r="97" spans="6:11">
       <c r="F97" s="31"/>
-      <c r="G97" s="7"/>
-      <c r="J97" s="31"/>
-    </row>
-    <row r="98" spans="6:10">
+      <c r="H97" s="7"/>
+      <c r="K97" s="31"/>
+    </row>
+    <row r="98" spans="6:11">
       <c r="F98" s="31"/>
-      <c r="G98" s="7"/>
-      <c r="J98" s="31"/>
-    </row>
-    <row r="99" spans="6:10">
+      <c r="H98" s="7"/>
+      <c r="K98" s="31"/>
+    </row>
+    <row r="99" spans="6:11">
       <c r="F99" s="31"/>
-      <c r="G99" s="7"/>
-      <c r="J99" s="31"/>
-    </row>
-    <row r="100" spans="6:10">
+      <c r="H99" s="7"/>
+      <c r="K99" s="31"/>
+    </row>
+    <row r="100" spans="6:11">
       <c r="F100" s="31"/>
-      <c r="G100" s="7"/>
-      <c r="J100" s="31"/>
-    </row>
-    <row r="101" spans="6:10">
+      <c r="H100" s="7"/>
+      <c r="K100" s="31"/>
+    </row>
+    <row r="101" spans="6:11">
       <c r="F101" s="31"/>
-      <c r="G101" s="7"/>
-    </row>
-    <row r="102" spans="6:10">
+      <c r="H101" s="7"/>
+    </row>
+    <row r="102" spans="6:11">
       <c r="F102" s="31"/>
-      <c r="G102" s="7"/>
-    </row>
-    <row r="103" spans="6:10">
+      <c r="H102" s="7"/>
+    </row>
+    <row r="103" spans="6:11">
       <c r="F103" s="31"/>
-      <c r="G103" s="7"/>
-    </row>
-    <row r="104" spans="6:10">
+      <c r="H103" s="7"/>
+    </row>
+    <row r="104" spans="6:11">
       <c r="F104" s="31"/>
-      <c r="G104" s="7"/>
-    </row>
-    <row r="105" spans="6:10">
-      <c r="G105" s="7"/>
-    </row>
-    <row r="108" spans="6:10">
+      <c r="H104" s="7"/>
+    </row>
+    <row r="105" spans="6:11">
+      <c r="H105" s="7"/>
+    </row>
+    <row r="108" spans="6:11">
       <c r="F108" s="105"/>
     </row>
-    <row r="109" spans="6:10">
+    <row r="109" spans="6:11">
       <c r="F109" s="105"/>
     </row>
-    <row r="110" spans="6:10">
+    <row r="110" spans="6:11">
       <c r="F110" s="105"/>
     </row>
-    <row r="111" spans="6:10">
+    <row r="111" spans="6:11">
       <c r="F111" s="105"/>
     </row>
-    <row r="112" spans="6:10">
+    <row r="112" spans="6:11">
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="6:6">
@@ -30591,7 +30600,7 @@
       <c r="F119" s="105"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J3" xr:uid="{561AF9F7-DEF4-214D-AC1D-3FA58FDFD9E6}"/>
+  <autoFilter ref="A3:K3" xr:uid="{561AF9F7-DEF4-214D-AC1D-3FA58FDFD9E6}"/>
   <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -30610,27 +30619,27 @@
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="15" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="55.42578125" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" customWidth="1"/>
-    <col min="10" max="10" width="81.42578125" customWidth="1"/>
-    <col min="11" max="11" width="93.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="15" width="8.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="1013" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="55.5" customWidth="1"/>
+    <col min="8" max="8" width="47.83203125" customWidth="1"/>
+    <col min="9" max="9" width="52.5" customWidth="1"/>
+    <col min="10" max="10" width="81.5" customWidth="1"/>
+    <col min="11" max="11" width="93.5" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="23.5" customWidth="1"/>
+    <col min="14" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="18.5" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.5" customWidth="1"/>
+    <col min="18" max="18" width="20.5" customWidth="1"/>
+    <col min="19" max="19" width="17.83203125" customWidth="1"/>
+    <col min="20" max="1013" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" customHeight="1">
@@ -30662,7 +30671,7 @@
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
     </row>
-    <row r="2" spans="1:20" ht="114.75">
+    <row r="2" spans="1:20" ht="126">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30706,7 +30715,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="38.25">
+    <row r="3" spans="1:20" ht="42">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30768,7 +30777,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14.25">
+    <row r="4" spans="1:20" ht="14">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
@@ -30776,7 +30785,7 @@
       <c r="R4" s="116"/>
       <c r="S4" s="116"/>
     </row>
-    <row r="5" spans="1:20" ht="14.25">
+    <row r="5" spans="1:20" ht="14">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -30784,7 +30793,7 @@
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
     </row>
-    <row r="6" spans="1:20" ht="14.25">
+    <row r="6" spans="1:20" ht="14">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
@@ -30794,7 +30803,7 @@
       <c r="R6" s="116"/>
       <c r="S6" s="116"/>
     </row>
-    <row r="7" spans="1:20" ht="14.25">
+    <row r="7" spans="1:20" ht="14">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30805,7 +30814,7 @@
       <c r="R7" s="116"/>
       <c r="S7" s="116"/>
     </row>
-    <row r="8" spans="1:20" ht="14.25">
+    <row r="8" spans="1:20" ht="14">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30816,7 +30825,7 @@
       <c r="R8" s="116"/>
       <c r="S8" s="116"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25">
+    <row r="9" spans="1:20" ht="14">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30828,7 +30837,7 @@
       <c r="R9" s="116"/>
       <c r="S9" s="116"/>
     </row>
-    <row r="10" spans="1:20" ht="14.25">
+    <row r="10" spans="1:20" ht="14">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30840,7 +30849,7 @@
       <c r="R10" s="116"/>
       <c r="S10" s="116"/>
     </row>
-    <row r="11" spans="1:20" ht="14.25">
+    <row r="11" spans="1:20" ht="14">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30852,7 +30861,7 @@
       <c r="R11" s="116"/>
       <c r="S11" s="116"/>
     </row>
-    <row r="12" spans="1:20" ht="14.25">
+    <row r="12" spans="1:20" ht="14">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30864,7 +30873,7 @@
       <c r="R12" s="116"/>
       <c r="S12" s="116"/>
     </row>
-    <row r="13" spans="1:20" ht="14.25">
+    <row r="13" spans="1:20" ht="14">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30876,7 +30885,7 @@
       <c r="R13" s="116"/>
       <c r="S13" s="116"/>
     </row>
-    <row r="14" spans="1:20" ht="14.25">
+    <row r="14" spans="1:20" ht="14">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30888,7 +30897,7 @@
       <c r="R14" s="116"/>
       <c r="S14" s="116"/>
     </row>
-    <row r="15" spans="1:20" ht="14.25">
+    <row r="15" spans="1:20" ht="14">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30900,7 +30909,7 @@
       <c r="R15" s="116"/>
       <c r="S15" s="116"/>
     </row>
-    <row r="16" spans="1:20" ht="14.25">
+    <row r="16" spans="1:20" ht="14">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30912,7 +30921,7 @@
       <c r="R16" s="116"/>
       <c r="S16" s="116"/>
     </row>
-    <row r="17" spans="6:19" ht="14.25">
+    <row r="17" spans="6:19" ht="14">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30924,7 +30933,7 @@
       <c r="R17" s="116"/>
       <c r="S17" s="116"/>
     </row>
-    <row r="18" spans="6:19" ht="14.25">
+    <row r="18" spans="6:19" ht="14">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30936,7 +30945,7 @@
       <c r="R18" s="116"/>
       <c r="S18" s="116"/>
     </row>
-    <row r="19" spans="6:19" ht="14.25">
+    <row r="19" spans="6:19" ht="14">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
@@ -30946,7 +30955,7 @@
       <c r="R19" s="116"/>
       <c r="S19" s="116"/>
     </row>
-    <row r="20" spans="6:19" ht="14.25">
+    <row r="20" spans="6:19" ht="14">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
@@ -30954,7 +30963,7 @@
       <c r="R20" s="116"/>
       <c r="S20" s="116"/>
     </row>
-    <row r="21" spans="6:19" ht="14.25">
+    <row r="21" spans="6:19" ht="14">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30965,7 +30974,7 @@
       <c r="R21" s="116"/>
       <c r="S21" s="116"/>
     </row>
-    <row r="22" spans="6:19" ht="14.25">
+    <row r="22" spans="6:19" ht="14">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30977,7 +30986,7 @@
       <c r="R22" s="116"/>
       <c r="S22" s="116"/>
     </row>
-    <row r="23" spans="6:19" ht="14.25">
+    <row r="23" spans="6:19" ht="14">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -30989,7 +30998,7 @@
       <c r="R23" s="116"/>
       <c r="S23" s="116"/>
     </row>
-    <row r="24" spans="6:19" ht="14.25">
+    <row r="24" spans="6:19" ht="14">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
@@ -30997,7 +31006,7 @@
       <c r="R24" s="116"/>
       <c r="S24" s="116"/>
     </row>
-    <row r="25" spans="6:19" ht="14.25">
+    <row r="25" spans="6:19" ht="14">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -31008,7 +31017,7 @@
       <c r="R25" s="116"/>
       <c r="S25" s="116"/>
     </row>
-    <row r="26" spans="6:19" ht="14.25">
+    <row r="26" spans="6:19" ht="14">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -31020,7 +31029,7 @@
       <c r="R26" s="116"/>
       <c r="S26" s="116"/>
     </row>
-    <row r="27" spans="6:19" ht="14.25">
+    <row r="27" spans="6:19" ht="14">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -31031,7 +31040,7 @@
       <c r="R27" s="116"/>
       <c r="S27" s="116"/>
     </row>
-    <row r="28" spans="6:19" ht="14.25">
+    <row r="28" spans="6:19" ht="14">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
@@ -31041,7 +31050,7 @@
       <c r="R28" s="116"/>
       <c r="S28" s="116"/>
     </row>
-    <row r="29" spans="6:19" ht="14.25">
+    <row r="29" spans="6:19" ht="14">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -31052,7 +31061,7 @@
       <c r="R29" s="116"/>
       <c r="S29" s="116"/>
     </row>
-    <row r="30" spans="6:19" ht="14.25">
+    <row r="30" spans="6:19" ht="14">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -31063,7 +31072,7 @@
       <c r="R30" s="116"/>
       <c r="S30" s="116"/>
     </row>
-    <row r="31" spans="6:19" ht="14.25">
+    <row r="31" spans="6:19" ht="14">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -31074,7 +31083,7 @@
       <c r="R31" s="116"/>
       <c r="S31" s="116"/>
     </row>
-    <row r="32" spans="6:19" ht="14.25">
+    <row r="32" spans="6:19" ht="14">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
@@ -31083,7 +31092,7 @@
       <c r="R32" s="116"/>
       <c r="S32" s="116"/>
     </row>
-    <row r="33" spans="6:19" ht="14.25">
+    <row r="33" spans="6:19" ht="14">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
@@ -31092,7 +31101,7 @@
       <c r="R33" s="116"/>
       <c r="S33" s="116"/>
     </row>
-    <row r="34" spans="6:19" ht="14.25">
+    <row r="34" spans="6:19" ht="14">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
@@ -31102,7 +31111,7 @@
       <c r="R34" s="116"/>
       <c r="S34" s="116"/>
     </row>
-    <row r="35" spans="6:19" ht="14.25">
+    <row r="35" spans="6:19" ht="14">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
@@ -31111,7 +31120,7 @@
       <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
     </row>
-    <row r="36" spans="6:19" ht="14.25">
+    <row r="36" spans="6:19" ht="14">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
@@ -31227,7 +31236,7 @@
       <c r="R47" s="116"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="6:19" ht="14.25">
+    <row r="48" spans="6:19" ht="14">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
@@ -31324,20 +31333,20 @@
       <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="58.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="58.5" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="87.140625" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.5" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="87.1640625" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18">
@@ -31361,7 +31370,7 @@
       <c r="P1" s="31"/>
       <c r="Q1" s="34"/>
     </row>
-    <row r="2" spans="1:18" ht="57.95" customHeight="1">
+    <row r="2" spans="1:18" ht="58" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -31413,7 +31422,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="38.25">
+    <row r="3" spans="1:18" ht="42">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -33480,20 +33489,20 @@
       <selection pane="bottomLeft" activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.140625" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -33510,7 +33519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="93.95" customHeight="1">
+    <row r="2" spans="1:11" ht="94" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -33545,7 +33554,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="25.5">
+    <row r="3" spans="1:11" ht="14">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
missing columns added to the base template
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/Projects/et-ccd-definitions-englandwales/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tensaybulcha/Documents/GitHub/Reformed-ET/et-ccd-definitions-englandwales/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D006DB-E7F5-FB4B-BED7-0FF0497F2668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51F886-9A3C-FB4B-9A59-BA1C8DAD725B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38640" windowHeight="20620" tabRatio="500" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55340" yWindow="600" windowWidth="35960" windowHeight="17400" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$U$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$R$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$L$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3735" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3741" uniqueCount="1161">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3640,6 +3640,21 @@
 Blank - True
 Yes/Y/True - True
 No/N/False - False</t>
+  </si>
+  <si>
+    <t>EnableForDeletion</t>
+  </si>
+  <si>
+    <t>Marker field for Case deletion when its Time to Live(TTL) value expires</t>
+  </si>
+  <si>
+    <t>SignificantEvent</t>
+  </si>
+  <si>
+    <t>TTLIncrement</t>
+  </si>
+  <si>
+    <t>Magnitude in number of days that a Time to Live(TTL) value is incremented by</t>
   </si>
 </sst>
 </file>
@@ -4065,7 +4080,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4102,8 +4117,20 @@
         <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -4376,6 +4403,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4395,7 +4448,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4942,6 +4995,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -14968,7 +15033,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L402"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
@@ -26620,14 +26685,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA7525E-209B-8C42-BE0F-EC2469EB923C}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="10.6640625" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.1640625" style="256" customWidth="1"/>
+    <col min="3" max="3" width="16" style="256" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="256" customWidth="1"/>
+    <col min="5" max="5" width="22" style="256" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="256" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="256" customWidth="1"/>
+    <col min="8" max="8" width="21" style="256" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="256" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="256" customWidth="1"/>
+    <col min="11" max="1025" width="11.1640625" style="256" customWidth="1"/>
     <col min="1026" max="16384" width="8.83203125" style="256"/>
   </cols>
   <sheetData>
@@ -29769,10 +29842,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -29782,10 +29855,12 @@
     <col min="4" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="58.83203125" customWidth="1"/>
-    <col min="8" max="1011" width="10.5" customWidth="1"/>
+    <col min="8" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="1011" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
@@ -29804,7 +29879,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="210">
+    <row r="2" spans="1:10" ht="210">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29832,8 +29907,11 @@
       <c r="I2" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="42">
+      <c r="J2" s="8" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="42">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29861,22 +29939,25 @@
       <c r="I3" s="26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="279" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="14"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="G4" s="99"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="14"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="G5" s="99"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="14"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -30629,10 +30710,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BE1D59-106C-BF43-BA5D-A6515397BCBE}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -30647,18 +30728,18 @@
     <col min="8" max="8" width="47.83203125" customWidth="1"/>
     <col min="9" max="9" width="52.5" customWidth="1"/>
     <col min="10" max="10" width="81.5" customWidth="1"/>
-    <col min="11" max="11" width="93.5" customWidth="1"/>
+    <col min="11" max="11" width="48.5" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
     <col min="13" max="13" width="23.5" customWidth="1"/>
     <col min="14" max="15" width="8.5" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.5" customWidth="1"/>
-    <col min="18" max="18" width="20.5" customWidth="1"/>
-    <col min="19" max="19" width="17.83203125" customWidth="1"/>
-    <col min="20" max="1013" width="8.5" customWidth="1"/>
+    <col min="16" max="18" width="18.5" style="7" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" customWidth="1"/>
+    <col min="22" max="1015" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1">
+    <row r="1" spans="1:22" ht="18" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
@@ -30683,11 +30764,13 @@
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
       <c r="S1" s="34"/>
-    </row>
-    <row r="2" spans="1:20" ht="126">
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+    </row>
+    <row r="2" spans="1:22" ht="126">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30724,14 +30807,20 @@
       <c r="P2" s="22" t="s">
         <v>1059</v>
       </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
+      <c r="Q2" s="22" t="s">
+        <v>1059</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>1160</v>
+      </c>
       <c r="S2" s="24"/>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="22" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="42">
+    <row r="3" spans="1:22" ht="42">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30777,49 +30866,57 @@
       <c r="O3" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="280" t="s">
         <v>93</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="282" t="s">
+        <v>1158</v>
+      </c>
+      <c r="R3" s="282" t="s">
+        <v>1159</v>
+      </c>
+      <c r="S3" s="281" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="T3" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="U3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="277" t="s">
+      <c r="V3" s="277" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14">
+    <row r="4" spans="1:22" ht="14">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
       <c r="M4" s="40"/>
-      <c r="R4" s="116"/>
-      <c r="S4" s="116"/>
-    </row>
-    <row r="5" spans="1:20" ht="14">
+      <c r="T4" s="116"/>
+      <c r="U4" s="116"/>
+    </row>
+    <row r="5" spans="1:22" ht="14">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
       <c r="M5" s="40"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-    </row>
-    <row r="6" spans="1:20" ht="14">
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+    </row>
+    <row r="6" spans="1:22" ht="14">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
       <c r="L6" s="31"/>
       <c r="M6" s="40"/>
       <c r="P6" s="40"/>
-      <c r="R6" s="116"/>
-      <c r="S6" s="116"/>
-    </row>
-    <row r="7" spans="1:20" ht="14">
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="T6" s="116"/>
+      <c r="U6" s="116"/>
+    </row>
+    <row r="7" spans="1:22" ht="14">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30827,10 +30924,10 @@
       <c r="J7" s="99"/>
       <c r="L7" s="31"/>
       <c r="M7" s="40"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="116"/>
-    </row>
-    <row r="8" spans="1:20" ht="14">
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+    </row>
+    <row r="8" spans="1:22" ht="14">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30838,10 +30935,10 @@
       <c r="J8" s="99"/>
       <c r="L8" s="31"/>
       <c r="M8" s="40"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-    </row>
-    <row r="9" spans="1:20" ht="14">
+      <c r="T8" s="116"/>
+      <c r="U8" s="116"/>
+    </row>
+    <row r="9" spans="1:22" ht="14">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30850,10 +30947,10 @@
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
       <c r="M9" s="40"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-    </row>
-    <row r="10" spans="1:20" ht="14">
+      <c r="T9" s="116"/>
+      <c r="U9" s="116"/>
+    </row>
+    <row r="10" spans="1:22" ht="14">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30862,10 +30959,10 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
       <c r="M10" s="40"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-    </row>
-    <row r="11" spans="1:20" ht="14">
+      <c r="T10" s="116"/>
+      <c r="U10" s="116"/>
+    </row>
+    <row r="11" spans="1:22" ht="14">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30874,10 +30971,10 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="40"/>
-      <c r="R11" s="116"/>
-      <c r="S11" s="116"/>
-    </row>
-    <row r="12" spans="1:20" ht="14">
+      <c r="T11" s="116"/>
+      <c r="U11" s="116"/>
+    </row>
+    <row r="12" spans="1:22" ht="14">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30886,10 +30983,10 @@
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
       <c r="M12" s="40"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="116"/>
-    </row>
-    <row r="13" spans="1:20" ht="14">
+      <c r="T12" s="116"/>
+      <c r="U12" s="116"/>
+    </row>
+    <row r="13" spans="1:22" ht="14">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30898,10 +30995,10 @@
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
       <c r="M13" s="40"/>
-      <c r="R13" s="116"/>
-      <c r="S13" s="116"/>
-    </row>
-    <row r="14" spans="1:20" ht="14">
+      <c r="T13" s="116"/>
+      <c r="U13" s="116"/>
+    </row>
+    <row r="14" spans="1:22" ht="14">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30910,10 +31007,10 @@
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
       <c r="M14" s="40"/>
-      <c r="R14" s="116"/>
-      <c r="S14" s="116"/>
-    </row>
-    <row r="15" spans="1:20" ht="14">
+      <c r="T14" s="116"/>
+      <c r="U14" s="116"/>
+    </row>
+    <row r="15" spans="1:22" ht="14">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30922,10 +31019,10 @@
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
       <c r="M15" s="40"/>
-      <c r="R15" s="116"/>
-      <c r="S15" s="116"/>
-    </row>
-    <row r="16" spans="1:20" ht="14">
+      <c r="T15" s="116"/>
+      <c r="U15" s="116"/>
+    </row>
+    <row r="16" spans="1:22" ht="14">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30934,10 +31031,10 @@
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
       <c r="M16" s="40"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="116"/>
-    </row>
-    <row r="17" spans="6:19" ht="14">
+      <c r="T16" s="116"/>
+      <c r="U16" s="116"/>
+    </row>
+    <row r="17" spans="6:21" ht="14">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30946,10 +31043,10 @@
       <c r="K17" s="77"/>
       <c r="L17" s="31"/>
       <c r="M17" s="40"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="116"/>
-    </row>
-    <row r="18" spans="6:19" ht="14">
+      <c r="T17" s="116"/>
+      <c r="U17" s="116"/>
+    </row>
+    <row r="18" spans="6:21" ht="14">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30958,28 +31055,28 @@
       <c r="K18" s="77"/>
       <c r="L18" s="31"/>
       <c r="M18" s="40"/>
-      <c r="R18" s="116"/>
-      <c r="S18" s="116"/>
-    </row>
-    <row r="19" spans="6:19" ht="14">
+      <c r="T18" s="116"/>
+      <c r="U18" s="116"/>
+    </row>
+    <row r="19" spans="6:21" ht="14">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
       <c r="M19" s="40"/>
-      <c r="R19" s="116"/>
-      <c r="S19" s="116"/>
-    </row>
-    <row r="20" spans="6:19" ht="14">
+      <c r="T19" s="116"/>
+      <c r="U19" s="116"/>
+    </row>
+    <row r="20" spans="6:21" ht="14">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
       <c r="M20" s="40"/>
-      <c r="R20" s="116"/>
-      <c r="S20" s="116"/>
-    </row>
-    <row r="21" spans="6:19" ht="14">
+      <c r="T20" s="116"/>
+      <c r="U20" s="116"/>
+    </row>
+    <row r="21" spans="6:21" ht="14">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30987,10 +31084,10 @@
       <c r="J21" s="116"/>
       <c r="L21" s="31"/>
       <c r="M21" s="40"/>
-      <c r="R21" s="116"/>
-      <c r="S21" s="116"/>
-    </row>
-    <row r="22" spans="6:19" ht="14">
+      <c r="T21" s="116"/>
+      <c r="U21" s="116"/>
+    </row>
+    <row r="22" spans="6:21" ht="14">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30999,10 +31096,10 @@
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
       <c r="M22" s="40"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="116"/>
-    </row>
-    <row r="23" spans="6:19" ht="14">
+      <c r="T22" s="116"/>
+      <c r="U22" s="116"/>
+    </row>
+    <row r="23" spans="6:21" ht="14">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -31011,18 +31108,20 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="40"/>
-      <c r="R23" s="116"/>
-      <c r="S23" s="116"/>
-    </row>
-    <row r="24" spans="6:19" ht="14">
+      <c r="T23" s="116"/>
+      <c r="U23" s="116"/>
+    </row>
+    <row r="24" spans="6:21" ht="14">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
       <c r="P24" s="40"/>
-      <c r="R24" s="116"/>
-      <c r="S24" s="116"/>
-    </row>
-    <row r="25" spans="6:19" ht="14">
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="T24" s="116"/>
+      <c r="U24" s="116"/>
+    </row>
+    <row r="25" spans="6:21" ht="14">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -31030,10 +31129,12 @@
       <c r="L25" s="31"/>
       <c r="M25" s="40"/>
       <c r="P25" s="40"/>
-      <c r="R25" s="116"/>
-      <c r="S25" s="116"/>
-    </row>
-    <row r="26" spans="6:19" ht="14">
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="T25" s="116"/>
+      <c r="U25" s="116"/>
+    </row>
+    <row r="26" spans="6:21" ht="14">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -31042,10 +31143,12 @@
       <c r="L26" s="31"/>
       <c r="M26" s="40"/>
       <c r="P26" s="40"/>
-      <c r="R26" s="116"/>
-      <c r="S26" s="116"/>
-    </row>
-    <row r="27" spans="6:19" ht="14">
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="T26" s="116"/>
+      <c r="U26" s="116"/>
+    </row>
+    <row r="27" spans="6:21" ht="14">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -31053,20 +31156,24 @@
       <c r="L27" s="31"/>
       <c r="M27" s="40"/>
       <c r="P27" s="40"/>
-      <c r="R27" s="116"/>
-      <c r="S27" s="116"/>
-    </row>
-    <row r="28" spans="6:19" ht="14">
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="T27" s="116"/>
+      <c r="U27" s="116"/>
+    </row>
+    <row r="28" spans="6:21" ht="14">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
       <c r="L28" s="31"/>
       <c r="M28" s="40"/>
       <c r="P28" s="40"/>
-      <c r="R28" s="116"/>
-      <c r="S28" s="116"/>
-    </row>
-    <row r="29" spans="6:19" ht="14">
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="T28" s="116"/>
+      <c r="U28" s="116"/>
+    </row>
+    <row r="29" spans="6:21" ht="14">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -31074,10 +31181,12 @@
       <c r="L29" s="31"/>
       <c r="M29" s="40"/>
       <c r="P29" s="40"/>
-      <c r="R29" s="116"/>
-      <c r="S29" s="116"/>
-    </row>
-    <row r="30" spans="6:19" ht="14">
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="T29" s="116"/>
+      <c r="U29" s="116"/>
+    </row>
+    <row r="30" spans="6:21" ht="14">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -31085,10 +31194,12 @@
       <c r="L30" s="31"/>
       <c r="M30" s="40"/>
       <c r="P30" s="40"/>
-      <c r="R30" s="116"/>
-      <c r="S30" s="116"/>
-    </row>
-    <row r="31" spans="6:19" ht="14">
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="T30" s="116"/>
+      <c r="U30" s="116"/>
+    </row>
+    <row r="31" spans="6:21" ht="14">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -31096,183 +31207,191 @@
       <c r="K31" s="99"/>
       <c r="L31" s="31"/>
       <c r="M31" s="40"/>
-      <c r="R31" s="116"/>
-      <c r="S31" s="116"/>
-    </row>
-    <row r="32" spans="6:19" ht="14">
+      <c r="T31" s="116"/>
+      <c r="U31" s="116"/>
+    </row>
+    <row r="32" spans="6:21" ht="14">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
       <c r="L32" s="31"/>
       <c r="M32" s="40"/>
-      <c r="R32" s="116"/>
-      <c r="S32" s="116"/>
-    </row>
-    <row r="33" spans="6:19" ht="14">
+      <c r="T32" s="116"/>
+      <c r="U32" s="116"/>
+    </row>
+    <row r="33" spans="6:21" ht="14">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
       <c r="M33" s="40"/>
       <c r="P33" s="40"/>
-      <c r="R33" s="116"/>
-      <c r="S33" s="116"/>
-    </row>
-    <row r="34" spans="6:19" ht="14">
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="T33" s="116"/>
+      <c r="U33" s="116"/>
+    </row>
+    <row r="34" spans="6:21" ht="14">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
       <c r="L34" s="31"/>
       <c r="M34" s="40"/>
       <c r="P34" s="40"/>
-      <c r="R34" s="116"/>
-      <c r="S34" s="116"/>
-    </row>
-    <row r="35" spans="6:19" ht="14">
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="T34" s="116"/>
+      <c r="U34" s="116"/>
+    </row>
+    <row r="35" spans="6:21" ht="14">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
       <c r="L35" s="31"/>
       <c r="M35" s="40"/>
-      <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
-    </row>
-    <row r="36" spans="6:19" ht="14">
+      <c r="U35" s="116"/>
+    </row>
+    <row r="36" spans="6:21" ht="14">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
       <c r="L36" s="31"/>
       <c r="M36" s="40"/>
-      <c r="Q36" s="116"/>
       <c r="S36" s="116"/>
-    </row>
-    <row r="37" spans="6:19">
+      <c r="U36" s="116"/>
+    </row>
+    <row r="37" spans="6:21">
       <c r="I37" s="77"/>
       <c r="J37" s="77"/>
       <c r="K37" s="77"/>
       <c r="M37" s="7"/>
-      <c r="Q37" s="116"/>
-      <c r="R37" s="116"/>
       <c r="S37" s="116"/>
-    </row>
-    <row r="38" spans="6:19">
+      <c r="T37" s="116"/>
+      <c r="U37" s="116"/>
+    </row>
+    <row r="38" spans="6:21">
       <c r="I38" s="77"/>
       <c r="J38" s="77"/>
       <c r="K38" s="77"/>
       <c r="M38" s="7"/>
-      <c r="Q38" s="116"/>
-      <c r="R38" s="116"/>
       <c r="S38" s="116"/>
-    </row>
-    <row r="39" spans="6:19">
+      <c r="T38" s="116"/>
+      <c r="U38" s="116"/>
+    </row>
+    <row r="39" spans="6:21">
       <c r="I39" s="77"/>
       <c r="J39" s="77"/>
       <c r="K39" s="77"/>
       <c r="M39" s="7"/>
-      <c r="Q39" s="116"/>
-      <c r="R39" s="116"/>
       <c r="S39" s="116"/>
-    </row>
-    <row r="40" spans="6:19">
+      <c r="T39" s="116"/>
+      <c r="U39" s="116"/>
+    </row>
+    <row r="40" spans="6:21">
       <c r="I40" s="77"/>
       <c r="J40" s="77"/>
       <c r="K40" s="77"/>
       <c r="M40" s="7"/>
-      <c r="Q40" s="116"/>
-      <c r="R40" s="116"/>
       <c r="S40" s="116"/>
-    </row>
-    <row r="41" spans="6:19">
+      <c r="T40" s="116"/>
+      <c r="U40" s="116"/>
+    </row>
+    <row r="41" spans="6:21">
       <c r="I41" s="77"/>
       <c r="J41" s="77"/>
       <c r="K41" s="77"/>
       <c r="M41" s="7"/>
-      <c r="Q41" s="116"/>
-      <c r="R41" s="116"/>
       <c r="S41" s="116"/>
-    </row>
-    <row r="42" spans="6:19">
+      <c r="T41" s="116"/>
+      <c r="U41" s="116"/>
+    </row>
+    <row r="42" spans="6:21">
       <c r="I42" s="77"/>
       <c r="J42" s="77"/>
       <c r="K42" s="77"/>
       <c r="L42" s="31"/>
       <c r="M42" s="7"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="116"/>
       <c r="S42" s="6"/>
-    </row>
-    <row r="43" spans="6:19">
+      <c r="T42" s="116"/>
+      <c r="U42" s="6"/>
+    </row>
+    <row r="43" spans="6:21">
       <c r="I43" s="77"/>
       <c r="J43" s="77"/>
       <c r="K43" s="77"/>
       <c r="L43" s="31"/>
       <c r="M43" s="108"/>
       <c r="P43" s="108"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="116"/>
+      <c r="Q43" s="108"/>
+      <c r="R43" s="108"/>
       <c r="S43" s="6"/>
-    </row>
-    <row r="44" spans="6:19">
+      <c r="T43" s="116"/>
+      <c r="U43" s="6"/>
+    </row>
+    <row r="44" spans="6:21">
       <c r="I44" s="77"/>
       <c r="J44" s="77"/>
       <c r="K44" s="77"/>
       <c r="L44" s="31"/>
       <c r="M44" s="7"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="116"/>
       <c r="S44" s="6"/>
-    </row>
-    <row r="45" spans="6:19">
+      <c r="T44" s="116"/>
+      <c r="U44" s="6"/>
+    </row>
+    <row r="45" spans="6:21">
       <c r="I45" s="77"/>
       <c r="J45" s="77"/>
       <c r="K45" s="77"/>
       <c r="L45" s="31"/>
       <c r="M45" s="7"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="116"/>
       <c r="S45" s="6"/>
-    </row>
-    <row r="46" spans="6:19">
+      <c r="T45" s="116"/>
+      <c r="U45" s="6"/>
+    </row>
+    <row r="46" spans="6:21">
       <c r="I46" s="77"/>
       <c r="J46" s="77"/>
       <c r="K46" s="77"/>
       <c r="L46" s="31"/>
       <c r="M46" s="7"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="116"/>
       <c r="S46" s="6"/>
-    </row>
-    <row r="47" spans="6:19">
+      <c r="T46" s="116"/>
+      <c r="U46" s="6"/>
+    </row>
+    <row r="47" spans="6:21">
       <c r="I47" s="77"/>
       <c r="J47" s="77"/>
       <c r="K47" s="77"/>
       <c r="L47" s="31"/>
       <c r="M47" s="108"/>
       <c r="P47" s="108"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="116"/>
+      <c r="Q47" s="108"/>
+      <c r="R47" s="108"/>
       <c r="S47" s="6"/>
-    </row>
-    <row r="48" spans="6:19" ht="14">
+      <c r="T47" s="116"/>
+      <c r="U47" s="6"/>
+    </row>
+    <row r="48" spans="6:21" ht="14">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
       <c r="K48" s="77"/>
       <c r="L48" s="31"/>
       <c r="M48" s="40"/>
-      <c r="Q48" s="116"/>
-      <c r="R48" s="77"/>
       <c r="S48" s="116"/>
-    </row>
-    <row r="49" spans="3:17">
+      <c r="T48" s="77"/>
+      <c r="U48" s="116"/>
+    </row>
+    <row r="49" spans="3:19">
       <c r="F49" s="107"/>
       <c r="I49" s="77"/>
       <c r="J49" s="77"/>
       <c r="K49" s="77"/>
       <c r="L49" s="31"/>
       <c r="M49" s="108"/>
-      <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="3:17">
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="3:19">
       <c r="C50" s="202"/>
       <c r="F50" s="107"/>
       <c r="I50" s="77"/>
@@ -31281,7 +31400,7 @@
       <c r="L50" s="31"/>
       <c r="M50" s="108"/>
     </row>
-    <row r="51" spans="3:17">
+    <row r="51" spans="3:19">
       <c r="F51" s="107"/>
       <c r="I51" s="77"/>
       <c r="J51" s="77"/>
@@ -31289,45 +31408,47 @@
       <c r="L51" s="31"/>
       <c r="M51" s="108"/>
     </row>
-    <row r="52" spans="3:17">
+    <row r="52" spans="3:19">
       <c r="I52" s="77"/>
       <c r="J52" s="199"/>
       <c r="K52" s="77"/>
       <c r="L52" s="31"/>
       <c r="M52" s="108"/>
     </row>
-    <row r="53" spans="3:17">
+    <row r="53" spans="3:19">
       <c r="I53" s="77"/>
       <c r="J53" s="77"/>
       <c r="K53" s="77"/>
       <c r="L53" s="31"/>
       <c r="M53" s="108"/>
     </row>
-    <row r="54" spans="3:17">
+    <row r="54" spans="3:19">
       <c r="I54" s="77"/>
       <c r="J54" s="77"/>
       <c r="K54" s="77"/>
       <c r="L54" s="31"/>
       <c r="M54" s="108"/>
     </row>
-    <row r="55" spans="3:17">
+    <row r="55" spans="3:19">
       <c r="I55" s="77"/>
       <c r="J55" s="77"/>
       <c r="K55" s="77"/>
       <c r="L55" s="31"/>
       <c r="M55" s="108"/>
     </row>
-    <row r="56" spans="3:17">
+    <row r="56" spans="3:19">
       <c r="C56" s="109"/>
       <c r="D56" s="109"/>
       <c r="J56" s="77"/>
       <c r="M56" s="108"/>
     </row>
-    <row r="57" spans="3:17">
+    <row r="57" spans="3:19">
       <c r="J57" s="77"/>
       <c r="L57" s="31"/>
       <c r="M57" s="108"/>
       <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31344,7 +31465,7 @@
   <dimension ref="A1:R217"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
@@ -33507,7 +33628,7 @@
   <dimension ref="A1:XFD194"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="L3" sqref="A3:L3"/>
     </sheetView>

</xml_diff>

<commit_message>
ttl related changes added (#1005)
* ttl related changes added

* missing columns added to the base template

* Update definitions/json/CaseEventToFields/CaseEventToFields.json

Co-authored-by: Harpreet Jhita <harpreet.jhita@justice.gov.uk>

* pr feedback changes

* ttl added to ET1Repped

* ttl is added for submitEt1Draft

* retain and dispose changes separated out

* Update definitions/json/CaseEvent/CaseEvent-ET1Repped.json

Co-authored-by: Harpreet Jhita <harpreet.jhita@justice.gov.uk>

* Update definitions/json/CaseEvent/CaseEvent-WA.json

Co-authored-by: Harpreet Jhita <harpreet.jhita@justice.gov.uk>

* prod and non-prod version separated for r&D changes

* role to access profiles for ttl separated out

* Updates to Configs for R&D

* event name shortened

long event name shortened to meet char limitation

* Update Auth

* Update CaseEvent with TTL

---------

Co-authored-by: Harpreet Jhita <harpreet.jhita@justice.gov.uk>
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/Projects/et-ccd-definitions-englandwales/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tensaybulcha/Documents/GitHub/Reformed-ET/et-ccd-definitions-englandwales/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D006DB-E7F5-FB4B-BED7-0FF0497F2668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51F886-9A3C-FB4B-9A59-BA1C8DAD725B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38640" windowHeight="20620" tabRatio="500" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55340" yWindow="600" windowWidth="35960" windowHeight="17400" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCriteria" sheetId="37" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseType!$A$3:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationComplexType!$A$3:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$S$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEvent!$A$3:$U$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEventToFields!$A$3:$R$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseField!$A$3:$L$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CaseRoles!$A$3:$F$3</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3735" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3741" uniqueCount="1161">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3640,6 +3640,21 @@
 Blank - True
 Yes/Y/True - True
 No/N/False - False</t>
+  </si>
+  <si>
+    <t>EnableForDeletion</t>
+  </si>
+  <si>
+    <t>Marker field for Case deletion when its Time to Live(TTL) value expires</t>
+  </si>
+  <si>
+    <t>SignificantEvent</t>
+  </si>
+  <si>
+    <t>TTLIncrement</t>
+  </si>
+  <si>
+    <t>Magnitude in number of days that a Time to Live(TTL) value is incremented by</t>
   </si>
 </sst>
 </file>
@@ -4065,7 +4080,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4102,8 +4117,20 @@
         <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -4376,6 +4403,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4395,7 +4448,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4942,6 +4995,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{B681C2DD-6984-1C44-A47B-9C3A32035367}"/>
@@ -14968,7 +15033,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L402"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
@@ -26620,14 +26685,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA7525E-209B-8C42-BE0F-EC2469EB923C}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="10.6640625" style="257" customWidth="1"/>
-    <col min="3" max="1025" width="11.1640625" style="256" customWidth="1"/>
+    <col min="3" max="3" width="16" style="256" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="256" customWidth="1"/>
+    <col min="5" max="5" width="22" style="256" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="256" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="256" customWidth="1"/>
+    <col min="8" max="8" width="21" style="256" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="256" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="256" customWidth="1"/>
+    <col min="11" max="1025" width="11.1640625" style="256" customWidth="1"/>
     <col min="1026" max="16384" width="8.83203125" style="256"/>
   </cols>
   <sheetData>
@@ -29769,10 +29842,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -29782,10 +29855,12 @@
     <col min="4" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="58.83203125" customWidth="1"/>
-    <col min="8" max="1011" width="10.5" customWidth="1"/>
+    <col min="8" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="1011" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
@@ -29804,7 +29879,7 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="210">
+    <row r="2" spans="1:10" ht="210">
       <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
@@ -29832,8 +29907,11 @@
       <c r="I2" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="42">
+      <c r="J2" s="8" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="42">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -29861,22 +29939,25 @@
       <c r="I3" s="26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="279" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="14"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="G4" s="99"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="14"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="G5" s="99"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="14"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -30629,10 +30710,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BE1D59-106C-BF43-BA5D-A6515397BCBE}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -30647,18 +30728,18 @@
     <col min="8" max="8" width="47.83203125" customWidth="1"/>
     <col min="9" max="9" width="52.5" customWidth="1"/>
     <col min="10" max="10" width="81.5" customWidth="1"/>
-    <col min="11" max="11" width="93.5" customWidth="1"/>
+    <col min="11" max="11" width="48.5" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
     <col min="13" max="13" width="23.5" customWidth="1"/>
     <col min="14" max="15" width="8.5" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.5" customWidth="1"/>
-    <col min="18" max="18" width="20.5" customWidth="1"/>
-    <col min="19" max="19" width="17.83203125" customWidth="1"/>
-    <col min="20" max="1013" width="8.5" customWidth="1"/>
+    <col min="16" max="18" width="18.5" style="7" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" customWidth="1"/>
+    <col min="22" max="1015" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1">
+    <row r="1" spans="1:22" ht="18" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
@@ -30683,11 +30764,13 @@
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
       <c r="S1" s="34"/>
-    </row>
-    <row r="2" spans="1:20" ht="126">
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+    </row>
+    <row r="2" spans="1:22" ht="126">
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
@@ -30724,14 +30807,20 @@
       <c r="P2" s="22" t="s">
         <v>1059</v>
       </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
+      <c r="Q2" s="22" t="s">
+        <v>1059</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>1160</v>
+      </c>
       <c r="S2" s="24"/>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="22" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="42">
+    <row r="3" spans="1:22" ht="42">
       <c r="A3" s="35" t="s">
         <v>39</v>
       </c>
@@ -30777,49 +30866,57 @@
       <c r="O3" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="280" t="s">
         <v>93</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="282" t="s">
+        <v>1158</v>
+      </c>
+      <c r="R3" s="282" t="s">
+        <v>1159</v>
+      </c>
+      <c r="S3" s="281" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="T3" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="U3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="277" t="s">
+      <c r="V3" s="277" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14">
+    <row r="4" spans="1:22" ht="14">
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
       <c r="L4" s="31"/>
       <c r="M4" s="40"/>
-      <c r="R4" s="116"/>
-      <c r="S4" s="116"/>
-    </row>
-    <row r="5" spans="1:20" ht="14">
+      <c r="T4" s="116"/>
+      <c r="U4" s="116"/>
+    </row>
+    <row r="5" spans="1:22" ht="14">
       <c r="F5" s="8"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
       <c r="M5" s="40"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-    </row>
-    <row r="6" spans="1:20" ht="14">
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+    </row>
+    <row r="6" spans="1:22" ht="14">
       <c r="F6" s="8"/>
       <c r="G6" s="202"/>
       <c r="I6" s="164"/>
       <c r="L6" s="31"/>
       <c r="M6" s="40"/>
       <c r="P6" s="40"/>
-      <c r="R6" s="116"/>
-      <c r="S6" s="116"/>
-    </row>
-    <row r="7" spans="1:20" ht="14">
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="T6" s="116"/>
+      <c r="U6" s="116"/>
+    </row>
+    <row r="7" spans="1:22" ht="14">
       <c r="F7" s="8"/>
       <c r="G7" s="224"/>
       <c r="H7" s="8"/>
@@ -30827,10 +30924,10 @@
       <c r="J7" s="99"/>
       <c r="L7" s="31"/>
       <c r="M7" s="40"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="116"/>
-    </row>
-    <row r="8" spans="1:20" ht="14">
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+    </row>
+    <row r="8" spans="1:22" ht="14">
       <c r="F8" s="8"/>
       <c r="G8" s="224"/>
       <c r="H8" s="8"/>
@@ -30838,10 +30935,10 @@
       <c r="J8" s="99"/>
       <c r="L8" s="31"/>
       <c r="M8" s="40"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-    </row>
-    <row r="9" spans="1:20" ht="14">
+      <c r="T8" s="116"/>
+      <c r="U8" s="116"/>
+    </row>
+    <row r="9" spans="1:22" ht="14">
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -30850,10 +30947,10 @@
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
       <c r="M9" s="40"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-    </row>
-    <row r="10" spans="1:20" ht="14">
+      <c r="T9" s="116"/>
+      <c r="U9" s="116"/>
+    </row>
+    <row r="10" spans="1:22" ht="14">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -30862,10 +30959,10 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
       <c r="M10" s="40"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-    </row>
-    <row r="11" spans="1:20" ht="14">
+      <c r="T10" s="116"/>
+      <c r="U10" s="116"/>
+    </row>
+    <row r="11" spans="1:22" ht="14">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -30874,10 +30971,10 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="40"/>
-      <c r="R11" s="116"/>
-      <c r="S11" s="116"/>
-    </row>
-    <row r="12" spans="1:20" ht="14">
+      <c r="T11" s="116"/>
+      <c r="U11" s="116"/>
+    </row>
+    <row r="12" spans="1:22" ht="14">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -30886,10 +30983,10 @@
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
       <c r="M12" s="40"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="116"/>
-    </row>
-    <row r="13" spans="1:20" ht="14">
+      <c r="T12" s="116"/>
+      <c r="U12" s="116"/>
+    </row>
+    <row r="13" spans="1:22" ht="14">
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -30898,10 +30995,10 @@
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
       <c r="M13" s="40"/>
-      <c r="R13" s="116"/>
-      <c r="S13" s="116"/>
-    </row>
-    <row r="14" spans="1:20" ht="14">
+      <c r="T13" s="116"/>
+      <c r="U13" s="116"/>
+    </row>
+    <row r="14" spans="1:22" ht="14">
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -30910,10 +31007,10 @@
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
       <c r="M14" s="40"/>
-      <c r="R14" s="116"/>
-      <c r="S14" s="116"/>
-    </row>
-    <row r="15" spans="1:20" ht="14">
+      <c r="T14" s="116"/>
+      <c r="U14" s="116"/>
+    </row>
+    <row r="15" spans="1:22" ht="14">
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -30922,10 +31019,10 @@
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
       <c r="M15" s="40"/>
-      <c r="R15" s="116"/>
-      <c r="S15" s="116"/>
-    </row>
-    <row r="16" spans="1:20" ht="14">
+      <c r="T15" s="116"/>
+      <c r="U15" s="116"/>
+    </row>
+    <row r="16" spans="1:22" ht="14">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -30934,10 +31031,10 @@
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
       <c r="M16" s="40"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="116"/>
-    </row>
-    <row r="17" spans="6:19" ht="14">
+      <c r="T16" s="116"/>
+      <c r="U16" s="116"/>
+    </row>
+    <row r="17" spans="6:21" ht="14">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -30946,10 +31043,10 @@
       <c r="K17" s="77"/>
       <c r="L17" s="31"/>
       <c r="M17" s="40"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="116"/>
-    </row>
-    <row r="18" spans="6:19" ht="14">
+      <c r="T17" s="116"/>
+      <c r="U17" s="116"/>
+    </row>
+    <row r="18" spans="6:21" ht="14">
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -30958,28 +31055,28 @@
       <c r="K18" s="77"/>
       <c r="L18" s="31"/>
       <c r="M18" s="40"/>
-      <c r="R18" s="116"/>
-      <c r="S18" s="116"/>
-    </row>
-    <row r="19" spans="6:19" ht="14">
+      <c r="T18" s="116"/>
+      <c r="U18" s="116"/>
+    </row>
+    <row r="19" spans="6:21" ht="14">
       <c r="F19" s="8"/>
       <c r="I19" s="232"/>
       <c r="J19" s="199"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
       <c r="M19" s="40"/>
-      <c r="R19" s="116"/>
-      <c r="S19" s="116"/>
-    </row>
-    <row r="20" spans="6:19" ht="14">
+      <c r="T19" s="116"/>
+      <c r="U19" s="116"/>
+    </row>
+    <row r="20" spans="6:21" ht="14">
       <c r="F20" s="8"/>
       <c r="J20" s="77"/>
       <c r="L20" s="31"/>
       <c r="M20" s="40"/>
-      <c r="R20" s="116"/>
-      <c r="S20" s="116"/>
-    </row>
-    <row r="21" spans="6:19" ht="14">
+      <c r="T20" s="116"/>
+      <c r="U20" s="116"/>
+    </row>
+    <row r="21" spans="6:21" ht="14">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -30987,10 +31084,10 @@
       <c r="J21" s="116"/>
       <c r="L21" s="31"/>
       <c r="M21" s="40"/>
-      <c r="R21" s="116"/>
-      <c r="S21" s="116"/>
-    </row>
-    <row r="22" spans="6:19" ht="14">
+      <c r="T21" s="116"/>
+      <c r="U21" s="116"/>
+    </row>
+    <row r="22" spans="6:21" ht="14">
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -30999,10 +31096,10 @@
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
       <c r="M22" s="40"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="116"/>
-    </row>
-    <row r="23" spans="6:19" ht="14">
+      <c r="T22" s="116"/>
+      <c r="U22" s="116"/>
+    </row>
+    <row r="23" spans="6:21" ht="14">
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -31011,18 +31108,20 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="40"/>
-      <c r="R23" s="116"/>
-      <c r="S23" s="116"/>
-    </row>
-    <row r="24" spans="6:19" ht="14">
+      <c r="T23" s="116"/>
+      <c r="U23" s="116"/>
+    </row>
+    <row r="24" spans="6:21" ht="14">
       <c r="J24" s="99"/>
       <c r="L24" s="31"/>
       <c r="M24" s="40"/>
       <c r="P24" s="40"/>
-      <c r="R24" s="116"/>
-      <c r="S24" s="116"/>
-    </row>
-    <row r="25" spans="6:19" ht="14">
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="T24" s="116"/>
+      <c r="U24" s="116"/>
+    </row>
+    <row r="25" spans="6:21" ht="14">
       <c r="F25" s="8"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
@@ -31030,10 +31129,12 @@
       <c r="L25" s="31"/>
       <c r="M25" s="40"/>
       <c r="P25" s="40"/>
-      <c r="R25" s="116"/>
-      <c r="S25" s="116"/>
-    </row>
-    <row r="26" spans="6:19" ht="14">
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="T25" s="116"/>
+      <c r="U25" s="116"/>
+    </row>
+    <row r="26" spans="6:21" ht="14">
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="I26" s="77"/>
@@ -31042,10 +31143,12 @@
       <c r="L26" s="31"/>
       <c r="M26" s="40"/>
       <c r="P26" s="40"/>
-      <c r="R26" s="116"/>
-      <c r="S26" s="116"/>
-    </row>
-    <row r="27" spans="6:19" ht="14">
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="T26" s="116"/>
+      <c r="U26" s="116"/>
+    </row>
+    <row r="27" spans="6:21" ht="14">
       <c r="F27" s="8"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
@@ -31053,20 +31156,24 @@
       <c r="L27" s="31"/>
       <c r="M27" s="40"/>
       <c r="P27" s="40"/>
-      <c r="R27" s="116"/>
-      <c r="S27" s="116"/>
-    </row>
-    <row r="28" spans="6:19" ht="14">
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="T27" s="116"/>
+      <c r="U27" s="116"/>
+    </row>
+    <row r="28" spans="6:21" ht="14">
       <c r="F28" s="8"/>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
       <c r="L28" s="31"/>
       <c r="M28" s="40"/>
       <c r="P28" s="40"/>
-      <c r="R28" s="116"/>
-      <c r="S28" s="116"/>
-    </row>
-    <row r="29" spans="6:19" ht="14">
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="T28" s="116"/>
+      <c r="U28" s="116"/>
+    </row>
+    <row r="29" spans="6:21" ht="14">
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="I29" s="77"/>
@@ -31074,10 +31181,12 @@
       <c r="L29" s="31"/>
       <c r="M29" s="40"/>
       <c r="P29" s="40"/>
-      <c r="R29" s="116"/>
-      <c r="S29" s="116"/>
-    </row>
-    <row r="30" spans="6:19" ht="14">
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="T29" s="116"/>
+      <c r="U29" s="116"/>
+    </row>
+    <row r="30" spans="6:21" ht="14">
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="77"/>
@@ -31085,10 +31194,12 @@
       <c r="L30" s="31"/>
       <c r="M30" s="40"/>
       <c r="P30" s="40"/>
-      <c r="R30" s="116"/>
-      <c r="S30" s="116"/>
-    </row>
-    <row r="31" spans="6:19" ht="14">
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="T30" s="116"/>
+      <c r="U30" s="116"/>
+    </row>
+    <row r="31" spans="6:21" ht="14">
       <c r="F31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="77"/>
@@ -31096,183 +31207,191 @@
       <c r="K31" s="99"/>
       <c r="L31" s="31"/>
       <c r="M31" s="40"/>
-      <c r="R31" s="116"/>
-      <c r="S31" s="116"/>
-    </row>
-    <row r="32" spans="6:19" ht="14">
+      <c r="T31" s="116"/>
+      <c r="U31" s="116"/>
+    </row>
+    <row r="32" spans="6:21" ht="14">
       <c r="G32" s="8"/>
       <c r="I32" s="164"/>
       <c r="K32" s="99"/>
       <c r="L32" s="31"/>
       <c r="M32" s="40"/>
-      <c r="R32" s="116"/>
-      <c r="S32" s="116"/>
-    </row>
-    <row r="33" spans="6:19" ht="14">
+      <c r="T32" s="116"/>
+      <c r="U32" s="116"/>
+    </row>
+    <row r="33" spans="6:21" ht="14">
       <c r="J33" s="77"/>
       <c r="K33" s="77"/>
       <c r="L33" s="31"/>
       <c r="M33" s="40"/>
       <c r="P33" s="40"/>
-      <c r="R33" s="116"/>
-      <c r="S33" s="116"/>
-    </row>
-    <row r="34" spans="6:19" ht="14">
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="T33" s="116"/>
+      <c r="U33" s="116"/>
+    </row>
+    <row r="34" spans="6:21" ht="14">
       <c r="G34" s="8"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
       <c r="L34" s="31"/>
       <c r="M34" s="40"/>
       <c r="P34" s="40"/>
-      <c r="R34" s="116"/>
-      <c r="S34" s="116"/>
-    </row>
-    <row r="35" spans="6:19" ht="14">
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="T34" s="116"/>
+      <c r="U34" s="116"/>
+    </row>
+    <row r="35" spans="6:21" ht="14">
       <c r="I35" s="77"/>
       <c r="J35" s="77"/>
       <c r="K35" s="77"/>
       <c r="L35" s="31"/>
       <c r="M35" s="40"/>
-      <c r="Q35" s="116"/>
       <c r="S35" s="116"/>
-    </row>
-    <row r="36" spans="6:19" ht="14">
+      <c r="U35" s="116"/>
+    </row>
+    <row r="36" spans="6:21" ht="14">
       <c r="I36" s="77"/>
       <c r="J36" s="77"/>
       <c r="K36" s="77"/>
       <c r="L36" s="31"/>
       <c r="M36" s="40"/>
-      <c r="Q36" s="116"/>
       <c r="S36" s="116"/>
-    </row>
-    <row r="37" spans="6:19">
+      <c r="U36" s="116"/>
+    </row>
+    <row r="37" spans="6:21">
       <c r="I37" s="77"/>
       <c r="J37" s="77"/>
       <c r="K37" s="77"/>
       <c r="M37" s="7"/>
-      <c r="Q37" s="116"/>
-      <c r="R37" s="116"/>
       <c r="S37" s="116"/>
-    </row>
-    <row r="38" spans="6:19">
+      <c r="T37" s="116"/>
+      <c r="U37" s="116"/>
+    </row>
+    <row r="38" spans="6:21">
       <c r="I38" s="77"/>
       <c r="J38" s="77"/>
       <c r="K38" s="77"/>
       <c r="M38" s="7"/>
-      <c r="Q38" s="116"/>
-      <c r="R38" s="116"/>
       <c r="S38" s="116"/>
-    </row>
-    <row r="39" spans="6:19">
+      <c r="T38" s="116"/>
+      <c r="U38" s="116"/>
+    </row>
+    <row r="39" spans="6:21">
       <c r="I39" s="77"/>
       <c r="J39" s="77"/>
       <c r="K39" s="77"/>
       <c r="M39" s="7"/>
-      <c r="Q39" s="116"/>
-      <c r="R39" s="116"/>
       <c r="S39" s="116"/>
-    </row>
-    <row r="40" spans="6:19">
+      <c r="T39" s="116"/>
+      <c r="U39" s="116"/>
+    </row>
+    <row r="40" spans="6:21">
       <c r="I40" s="77"/>
       <c r="J40" s="77"/>
       <c r="K40" s="77"/>
       <c r="M40" s="7"/>
-      <c r="Q40" s="116"/>
-      <c r="R40" s="116"/>
       <c r="S40" s="116"/>
-    </row>
-    <row r="41" spans="6:19">
+      <c r="T40" s="116"/>
+      <c r="U40" s="116"/>
+    </row>
+    <row r="41" spans="6:21">
       <c r="I41" s="77"/>
       <c r="J41" s="77"/>
       <c r="K41" s="77"/>
       <c r="M41" s="7"/>
-      <c r="Q41" s="116"/>
-      <c r="R41" s="116"/>
       <c r="S41" s="116"/>
-    </row>
-    <row r="42" spans="6:19">
+      <c r="T41" s="116"/>
+      <c r="U41" s="116"/>
+    </row>
+    <row r="42" spans="6:21">
       <c r="I42" s="77"/>
       <c r="J42" s="77"/>
       <c r="K42" s="77"/>
       <c r="L42" s="31"/>
       <c r="M42" s="7"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="116"/>
       <c r="S42" s="6"/>
-    </row>
-    <row r="43" spans="6:19">
+      <c r="T42" s="116"/>
+      <c r="U42" s="6"/>
+    </row>
+    <row r="43" spans="6:21">
       <c r="I43" s="77"/>
       <c r="J43" s="77"/>
       <c r="K43" s="77"/>
       <c r="L43" s="31"/>
       <c r="M43" s="108"/>
       <c r="P43" s="108"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="116"/>
+      <c r="Q43" s="108"/>
+      <c r="R43" s="108"/>
       <c r="S43" s="6"/>
-    </row>
-    <row r="44" spans="6:19">
+      <c r="T43" s="116"/>
+      <c r="U43" s="6"/>
+    </row>
+    <row r="44" spans="6:21">
       <c r="I44" s="77"/>
       <c r="J44" s="77"/>
       <c r="K44" s="77"/>
       <c r="L44" s="31"/>
       <c r="M44" s="7"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="116"/>
       <c r="S44" s="6"/>
-    </row>
-    <row r="45" spans="6:19">
+      <c r="T44" s="116"/>
+      <c r="U44" s="6"/>
+    </row>
+    <row r="45" spans="6:21">
       <c r="I45" s="77"/>
       <c r="J45" s="77"/>
       <c r="K45" s="77"/>
       <c r="L45" s="31"/>
       <c r="M45" s="7"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="116"/>
       <c r="S45" s="6"/>
-    </row>
-    <row r="46" spans="6:19">
+      <c r="T45" s="116"/>
+      <c r="U45" s="6"/>
+    </row>
+    <row r="46" spans="6:21">
       <c r="I46" s="77"/>
       <c r="J46" s="77"/>
       <c r="K46" s="77"/>
       <c r="L46" s="31"/>
       <c r="M46" s="7"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="116"/>
       <c r="S46" s="6"/>
-    </row>
-    <row r="47" spans="6:19">
+      <c r="T46" s="116"/>
+      <c r="U46" s="6"/>
+    </row>
+    <row r="47" spans="6:21">
       <c r="I47" s="77"/>
       <c r="J47" s="77"/>
       <c r="K47" s="77"/>
       <c r="L47" s="31"/>
       <c r="M47" s="108"/>
       <c r="P47" s="108"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="116"/>
+      <c r="Q47" s="108"/>
+      <c r="R47" s="108"/>
       <c r="S47" s="6"/>
-    </row>
-    <row r="48" spans="6:19" ht="14">
+      <c r="T47" s="116"/>
+      <c r="U47" s="6"/>
+    </row>
+    <row r="48" spans="6:21" ht="14">
       <c r="F48" s="107"/>
       <c r="I48" s="77"/>
       <c r="J48" s="77"/>
       <c r="K48" s="77"/>
       <c r="L48" s="31"/>
       <c r="M48" s="40"/>
-      <c r="Q48" s="116"/>
-      <c r="R48" s="77"/>
       <c r="S48" s="116"/>
-    </row>
-    <row r="49" spans="3:17">
+      <c r="T48" s="77"/>
+      <c r="U48" s="116"/>
+    </row>
+    <row r="49" spans="3:19">
       <c r="F49" s="107"/>
       <c r="I49" s="77"/>
       <c r="J49" s="77"/>
       <c r="K49" s="77"/>
       <c r="L49" s="31"/>
       <c r="M49" s="108"/>
-      <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="3:17">
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="3:19">
       <c r="C50" s="202"/>
       <c r="F50" s="107"/>
       <c r="I50" s="77"/>
@@ -31281,7 +31400,7 @@
       <c r="L50" s="31"/>
       <c r="M50" s="108"/>
     </row>
-    <row r="51" spans="3:17">
+    <row r="51" spans="3:19">
       <c r="F51" s="107"/>
       <c r="I51" s="77"/>
       <c r="J51" s="77"/>
@@ -31289,45 +31408,47 @@
       <c r="L51" s="31"/>
       <c r="M51" s="108"/>
     </row>
-    <row r="52" spans="3:17">
+    <row r="52" spans="3:19">
       <c r="I52" s="77"/>
       <c r="J52" s="199"/>
       <c r="K52" s="77"/>
       <c r="L52" s="31"/>
       <c r="M52" s="108"/>
     </row>
-    <row r="53" spans="3:17">
+    <row r="53" spans="3:19">
       <c r="I53" s="77"/>
       <c r="J53" s="77"/>
       <c r="K53" s="77"/>
       <c r="L53" s="31"/>
       <c r="M53" s="108"/>
     </row>
-    <row r="54" spans="3:17">
+    <row r="54" spans="3:19">
       <c r="I54" s="77"/>
       <c r="J54" s="77"/>
       <c r="K54" s="77"/>
       <c r="L54" s="31"/>
       <c r="M54" s="108"/>
     </row>
-    <row r="55" spans="3:17">
+    <row r="55" spans="3:19">
       <c r="I55" s="77"/>
       <c r="J55" s="77"/>
       <c r="K55" s="77"/>
       <c r="L55" s="31"/>
       <c r="M55" s="108"/>
     </row>
-    <row r="56" spans="3:17">
+    <row r="56" spans="3:19">
       <c r="C56" s="109"/>
       <c r="D56" s="109"/>
       <c r="J56" s="77"/>
       <c r="M56" s="108"/>
     </row>
-    <row r="57" spans="3:17">
+    <row r="57" spans="3:19">
       <c r="J57" s="77"/>
       <c r="L57" s="31"/>
       <c r="M57" s="108"/>
       <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31344,7 +31465,7 @@
   <dimension ref="A1:R217"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
@@ -33507,7 +33628,7 @@
   <dimension ref="A1:XFD194"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E23" sqref="E23"/>
       <selection pane="bottomLeft" activeCell="L3" sqref="A3:L3"/>
     </sheetView>

</xml_diff>